<commit_message>
[Admin] (Outlook) Map Signature APIs
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22711"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC569E17-4CBC-4A85-99A7-192CDBE25FDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514AB411-798F-465D-A184-9DB177A33EE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24180" yWindow="-18450" windowWidth="17280" windowHeight="8970" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="156">
   <si>
     <t>Class</t>
   </si>
@@ -466,6 +466,36 @@
   </si>
   <si>
     <t>outlook-attachments-get-attachment-content</t>
+  </si>
+  <si>
+    <t>isClientSignatureEnabledAsync</t>
+  </si>
+  <si>
+    <t>outlook-work-with-client-signatures</t>
+  </si>
+  <si>
+    <t>isClientSignatureEnabled</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>setSignatureAsync</t>
+  </si>
+  <si>
+    <t>setSignature</t>
+  </si>
+  <si>
+    <t>getComposeTypeAsync</t>
+  </si>
+  <si>
+    <t>getComposeType</t>
+  </si>
+  <si>
+    <t>disableClientSignatureAsync</t>
+  </si>
+  <si>
+    <t>disableClientSignature</t>
   </si>
 </sst>
 </file>
@@ -501,8 +531,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +571,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E146" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E146" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E152" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E152" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -873,11 +904,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3206,6 +3237,108 @@
         <v>4</v>
       </c>
     </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C147" s="1">
+        <v>2</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C148" s="1">
+        <v>2</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C149" s="1">
+        <v>2</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C150" s="1">
+        <v>2</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C151" s="1">
+        <v>2</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C152" s="1">
+        <v>2</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Admin] (Outlook) Map Signature APIs (#406)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22711"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC569E17-4CBC-4A85-99A7-192CDBE25FDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514AB411-798F-465D-A184-9DB177A33EE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24180" yWindow="-18450" windowWidth="17280" windowHeight="8970" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="156">
   <si>
     <t>Class</t>
   </si>
@@ -466,6 +466,36 @@
   </si>
   <si>
     <t>outlook-attachments-get-attachment-content</t>
+  </si>
+  <si>
+    <t>isClientSignatureEnabledAsync</t>
+  </si>
+  <si>
+    <t>outlook-work-with-client-signatures</t>
+  </si>
+  <si>
+    <t>isClientSignatureEnabled</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>setSignatureAsync</t>
+  </si>
+  <si>
+    <t>setSignature</t>
+  </si>
+  <si>
+    <t>getComposeTypeAsync</t>
+  </si>
+  <si>
+    <t>getComposeType</t>
+  </si>
+  <si>
+    <t>disableClientSignatureAsync</t>
+  </si>
+  <si>
+    <t>disableClientSignature</t>
   </si>
 </sst>
 </file>
@@ -501,8 +531,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +571,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E146" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E146" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E152" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E152" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -873,11 +904,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3206,6 +3237,108 @@
         <v>4</v>
       </c>
     </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C147" s="1">
+        <v>2</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C148" s="1">
+        <v>2</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C149" s="1">
+        <v>2</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C150" s="1">
+        <v>2</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C151" s="1">
+        <v>2</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C152" s="1">
+        <v>2</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Outlook] (to) Add how to set (Msg compose) (#417)
* [Outlook] (to) Add how to set

* Update file name
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514AB411-798F-465D-A184-9DB177A33EE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F88C06-5B13-4024-A7E9-963ABBCFD0A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="158">
   <si>
     <t>Class</t>
   </si>
@@ -201,9 +201,6 @@
     <t>to</t>
   </si>
   <si>
-    <t>outlook-recipients-and-attendees-get-to-message-compose</t>
-  </si>
-  <si>
     <t>getTo</t>
   </si>
   <si>
@@ -496,6 +493,15 @@
   </si>
   <si>
     <t>disableClientSignature</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-to-message-compose</t>
+  </si>
+  <si>
+    <t>setTo</t>
+  </si>
+  <si>
+    <t>setAsync</t>
   </si>
 </sst>
 </file>
@@ -571,8 +577,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E152" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E152" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E154" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E154" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -904,11 +910,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1242,10 +1248,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1273,10 +1279,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1318,10 +1324,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -1377,10 +1383,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1422,10 +1428,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -1467,10 +1473,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -1504,462 +1510,466 @@
         <v>56</v>
       </c>
       <c r="D37" t="s">
+        <v>155</v>
+      </c>
+      <c r="E37" t="s">
         <v>57</v>
-      </c>
-      <c r="E37" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" t="s">
         <v>57</v>
-      </c>
-      <c r="E38" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
         <v>56</v>
       </c>
+      <c r="C39" s="1"/>
       <c r="D39" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" t="s">
-        <v>58</v>
+        <v>155</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" t="s">
-        <v>142</v>
+      <c r="A40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="E40" t="s">
-        <v>63</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>142</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E41" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" t="s">
         <v>62</v>
-      </c>
-      <c r="E42" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" t="s">
         <v>62</v>
-      </c>
-      <c r="E43" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" t="s">
         <v>61</v>
       </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>62</v>
-      </c>
-      <c r="E44" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D45" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" t="s">
         <v>62</v>
-      </c>
-      <c r="E45" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>142</v>
+        <v>60</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
       </c>
       <c r="D46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" t="s">
         <v>62</v>
-      </c>
-      <c r="E46" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
+        <v>141</v>
+      </c>
+      <c r="D49" t="s">
         <v>61</v>
       </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s">
-        <v>62</v>
-      </c>
       <c r="E49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>142</v>
+        <v>60</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E51" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" t="s">
         <v>61</v>
       </c>
-      <c r="C54">
-        <v>2</v>
-      </c>
-      <c r="D54" t="s">
-        <v>62</v>
-      </c>
       <c r="E54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="B55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" t="s">
         <v>61</v>
       </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55" t="s">
-        <v>62</v>
-      </c>
       <c r="E55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E56" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>142</v>
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
+        <v>141</v>
+      </c>
+      <c r="D60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" t="s">
         <v>67</v>
-      </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s">
-        <v>62</v>
-      </c>
-      <c r="E60" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E61" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
+        <v>66</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E62" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s">
+        <v>141</v>
+      </c>
+      <c r="D65" t="s">
+        <v>61</v>
+      </c>
+      <c r="E65" t="s">
         <v>69</v>
-      </c>
-      <c r="C65">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s">
-        <v>62</v>
-      </c>
-      <c r="E65" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E66" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B67" t="s">
-        <v>142</v>
+        <v>68</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E67" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E68" t="s">
         <v>16</v>
@@ -1967,13 +1977,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E69" t="s">
         <v>16</v>
@@ -1981,16 +1991,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="D70" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E70" t="s">
         <v>16</v>
@@ -1998,36 +2005,33 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
+        <v>141</v>
       </c>
       <c r="D71" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E71" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E72" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -2035,16 +2039,16 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73" t="s">
+        <v>72</v>
+      </c>
+      <c r="E73" t="s">
         <v>73</v>
-      </c>
-      <c r="E73" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -2052,16 +2056,16 @@
         <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74" t="s">
+        <v>72</v>
+      </c>
+      <c r="E74" t="s">
         <v>73</v>
-      </c>
-      <c r="E74" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -2069,16 +2073,16 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E75" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -2086,16 +2090,16 @@
         <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2103,16 +2107,16 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E77" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2120,16 +2124,16 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2137,16 +2141,16 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E79" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2154,16 +2158,16 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E80" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2171,47 +2175,47 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>145</v>
+        <v>72</v>
       </c>
       <c r="E81" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>145</v>
+        <v>72</v>
       </c>
       <c r="E82" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C83">
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E83" t="s">
         <v>4</v>
@@ -2219,16 +2223,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C84">
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E84" t="s">
         <v>4</v>
@@ -2236,13 +2240,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B85" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="E85" t="s">
         <v>4</v>
@@ -2253,10 +2260,13 @@
         <v>21</v>
       </c>
       <c r="B86" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="E86" t="s">
         <v>4</v>
@@ -2264,269 +2274,263 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B87" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D87" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E87" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B88" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D88" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E88" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B89" t="s">
+        <v>83</v>
+      </c>
+      <c r="D89" t="s">
         <v>84</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>85</v>
-      </c>
-      <c r="E89" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B90" t="s">
+        <v>83</v>
+      </c>
+      <c r="D90" t="s">
         <v>84</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>85</v>
-      </c>
-      <c r="E90" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="B91" t="s">
-        <v>88</v>
-      </c>
-      <c r="C91">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="D91" t="s">
+        <v>84</v>
+      </c>
+      <c r="E91" t="s">
         <v>85</v>
-      </c>
-      <c r="E91" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="B92" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D92" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E92" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B93" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C93">
         <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E93" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D94" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E94" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E95" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B96" t="s">
+        <v>93</v>
+      </c>
+      <c r="D96" t="s">
         <v>94</v>
       </c>
-      <c r="D96" t="s">
-        <v>98</v>
-      </c>
       <c r="E96" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>87</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97" t="s">
         <v>94</v>
       </c>
-      <c r="D97" t="s">
-        <v>98</v>
-      </c>
       <c r="E97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B98" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D98" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E98" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D99" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E99" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B100" t="s">
+        <v>98</v>
+      </c>
+      <c r="D100" t="s">
         <v>99</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>100</v>
-      </c>
-      <c r="E100" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B101" t="s">
+        <v>98</v>
+      </c>
+      <c r="D101" t="s">
         <v>99</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>100</v>
-      </c>
-      <c r="E101" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
-      </c>
-      <c r="C102">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D102" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E102" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="B103" t="s">
-        <v>104</v>
-      </c>
-      <c r="C103">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D103" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E103" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B104" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C104">
         <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E104" t="s">
         <v>4</v>
@@ -2534,16 +2538,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E105" t="s">
         <v>4</v>
@@ -2551,36 +2555,36 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="B106" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E106" t="s">
-        <v>110</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B107" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E107" t="s">
-        <v>110</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2588,16 +2592,16 @@
         <v>19</v>
       </c>
       <c r="B108" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108" t="s">
         <v>111</v>
       </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
-      <c r="D108" t="s">
-        <v>112</v>
-      </c>
       <c r="E108" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -2605,16 +2609,16 @@
         <v>21</v>
       </c>
       <c r="B109" t="s">
+        <v>109</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109" t="s">
         <v>111</v>
       </c>
-      <c r="C109">
-        <v>1</v>
-      </c>
-      <c r="D109" t="s">
-        <v>112</v>
-      </c>
       <c r="E109" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2628,10 +2632,10 @@
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E110" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2645,58 +2649,58 @@
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E111" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B112" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E112" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E113" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C114">
         <v>2</v>
       </c>
       <c r="D114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E114" t="s">
         <v>11</v>
@@ -2704,16 +2708,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C115">
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E115" t="s">
         <v>11</v>
@@ -2721,50 +2725,50 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E116" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E117" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C118">
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E118" t="s">
         <v>4</v>
@@ -2772,16 +2776,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B119" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E119" t="s">
         <v>4</v>
@@ -2789,19 +2793,19 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B120" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E120" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2809,16 +2813,16 @@
         <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E121" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
@@ -2826,16 +2830,16 @@
         <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E122" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -2843,16 +2847,16 @@
         <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E123" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -2860,16 +2864,16 @@
         <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E124" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2877,16 +2881,16 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E125" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2894,16 +2898,16 @@
         <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E126" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2911,16 +2915,16 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E127" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2928,16 +2932,16 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
+        <v>120</v>
+      </c>
+      <c r="E128" t="s">
         <v>121</v>
-      </c>
-      <c r="E128" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2945,16 +2949,16 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
+        <v>120</v>
+      </c>
+      <c r="E129" t="s">
         <v>121</v>
-      </c>
-      <c r="E129" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2962,16 +2966,16 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E130" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2979,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E131" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -2996,16 +3000,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E132" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3013,61 +3017,64 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E133" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E134" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>129</v>
+        <v>125</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E135" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B136" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E136" t="s">
         <v>4</v>
@@ -3075,13 +3082,13 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B137" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D137" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E137" t="s">
         <v>4</v>
@@ -3089,13 +3096,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B138" t="s">
-        <v>129</v>
+        <v>115</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E138" t="s">
         <v>4</v>
@@ -3103,16 +3113,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B139" t="s">
-        <v>127</v>
-      </c>
-      <c r="C139">
-        <v>1</v>
+        <v>129</v>
       </c>
       <c r="D139" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E139" t="s">
         <v>4</v>
@@ -3120,16 +3127,13 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B140" t="s">
-        <v>132</v>
-      </c>
-      <c r="C140">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="D140" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E140" t="s">
         <v>4</v>
@@ -3137,16 +3141,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B141" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C141">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E141" t="s">
         <v>4</v>
@@ -3154,16 +3158,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="B142" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C142">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E142" t="s">
         <v>4</v>
@@ -3171,16 +3175,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="B143" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C143">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D143" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -3188,16 +3192,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="B144" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C144">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D144" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E144" t="s">
         <v>4</v>
@@ -3205,16 +3209,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B145" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="C145">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E145" t="s">
         <v>4</v>
@@ -3222,87 +3226,87 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B146" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E146" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A147" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C147" s="1">
-        <v>2</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>153</v>
+      <c r="A147" t="s">
+        <v>88</v>
+      </c>
+      <c r="B147" t="s">
+        <v>115</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
+      </c>
+      <c r="D147" t="s">
+        <v>137</v>
+      </c>
+      <c r="E147" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A148" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C148" s="1">
-        <v>2</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>151</v>
+      <c r="A148" t="s">
+        <v>88</v>
+      </c>
+      <c r="B148" t="s">
+        <v>138</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148" t="s">
+        <v>139</v>
+      </c>
+      <c r="E148" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C149" s="1">
         <v>2</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C150" s="1">
         <v>2</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -3310,16 +3314,16 @@
         <v>17</v>
       </c>
       <c r="B151" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C151" s="1">
+        <v>2</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C151" s="1">
-        <v>2</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="E151" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -3327,16 +3331,50 @@
         <v>20</v>
       </c>
       <c r="B152" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C152" s="1">
+        <v>2</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C152" s="1">
-        <v>2</v>
-      </c>
-      <c r="D152" s="1" t="s">
+      <c r="E152" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A153" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C153" s="1">
+        <v>2</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E153" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E152" s="1" t="s">
-        <v>148</v>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C154" s="1">
+        <v>2</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (cc) Add how to set cc (msg compose)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F88C06-5B13-4024-A7E9-963ABBCFD0A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4653D781-B58D-4ECE-9270-9ABC8CC3A8E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="159">
   <si>
     <t>Class</t>
   </si>
@@ -138,9 +138,6 @@
     <t>outlook-recipients-and-attendees-get-cc-message-read</t>
   </si>
   <si>
-    <t>outlook-recipients-and-attendees-get-cc-message-compose</t>
-  </si>
-  <si>
     <t>from</t>
   </si>
   <si>
@@ -502,6 +499,12 @@
   </si>
   <si>
     <t>setAsync</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-cc-message-compose</t>
+  </si>
+  <si>
+    <t>setCc</t>
   </si>
 </sst>
 </file>
@@ -577,8 +580,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E154" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E154" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E156" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E156" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -910,11 +913,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1248,10 +1251,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1271,7 +1274,7 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
@@ -1279,16 +1282,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
@@ -1296,241 +1299,241 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>157</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>156</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
         <v>37</v>
       </c>
-      <c r="D26" t="s">
-        <v>40</v>
-      </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>86</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>86</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>86</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>86</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1538,466 +1541,469 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" t="s">
-        <v>155</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>157</v>
+      <c r="A40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
-        <v>156</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C41" s="1"/>
       <c r="D41" t="s">
-        <v>58</v>
-      </c>
-      <c r="E41" t="s">
-        <v>57</v>
+        <v>154</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" t="s">
-        <v>141</v>
+      <c r="A42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>141</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" t="s">
         <v>61</v>
-      </c>
-      <c r="E44" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s">
         <v>61</v>
-      </c>
-      <c r="E45" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" t="s">
         <v>60</v>
       </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>61</v>
-      </c>
-      <c r="E46" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D47" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" t="s">
         <v>61</v>
-      </c>
-      <c r="E47" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" t="s">
         <v>61</v>
-      </c>
-      <c r="E48" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" t="s">
         <v>60</v>
       </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>61</v>
-      </c>
       <c r="E51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" t="s">
         <v>60</v>
       </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56" t="s">
-        <v>61</v>
-      </c>
       <c r="E56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B57" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" t="s">
         <v>60</v>
       </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57" t="s">
-        <v>61</v>
-      </c>
       <c r="E57" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E58" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" t="s">
         <v>66</v>
-      </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="D62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E62" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E63" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>141</v>
+        <v>65</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E64" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
+        <v>140</v>
+      </c>
+      <c r="D67" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" t="s">
         <v>68</v>
-      </c>
-      <c r="C67">
-        <v>2</v>
-      </c>
-      <c r="D67" t="s">
-        <v>61</v>
-      </c>
-      <c r="E67" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E68" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>141</v>
+        <v>67</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E69" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E70" t="s">
         <v>16</v>
@@ -2005,13 +2011,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E71" t="s">
         <v>16</v>
@@ -2019,16 +2025,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2036,36 +2039,33 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="D73" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E73" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E74" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -2073,16 +2073,16 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" t="s">
+        <v>71</v>
+      </c>
+      <c r="E75" t="s">
         <v>72</v>
-      </c>
-      <c r="E75" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -2090,16 +2090,16 @@
         <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" t="s">
+        <v>71</v>
+      </c>
+      <c r="E76" t="s">
         <v>72</v>
-      </c>
-      <c r="E76" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2107,16 +2107,16 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E77" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2124,16 +2124,16 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E78" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2141,16 +2141,16 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E79" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2158,16 +2158,16 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,16 +2175,16 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E81" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2192,16 +2192,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E82" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2209,47 +2209,47 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="E83" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="E84" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C85">
         <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E85" t="s">
         <v>4</v>
@@ -2257,16 +2257,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C86">
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E86" t="s">
         <v>4</v>
@@ -2274,13 +2274,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="E87" t="s">
         <v>4</v>
@@ -2291,10 +2294,13 @@
         <v>21</v>
       </c>
       <c r="B88" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="E88" t="s">
         <v>4</v>
@@ -2302,269 +2308,263 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D89" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E89" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D90" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E90" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B91" t="s">
+        <v>82</v>
+      </c>
+      <c r="D91" t="s">
         <v>83</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>84</v>
-      </c>
-      <c r="E91" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B92" t="s">
+        <v>82</v>
+      </c>
+      <c r="D92" t="s">
         <v>83</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>84</v>
-      </c>
-      <c r="E92" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B93" t="s">
-        <v>87</v>
-      </c>
-      <c r="C93">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="D93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E93" t="s">
         <v>84</v>
-      </c>
-      <c r="E93" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B94" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D94" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E94" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E95" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D96" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E96" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B97" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C97">
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E97" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B98" t="s">
+        <v>92</v>
+      </c>
+      <c r="D98" t="s">
         <v>93</v>
       </c>
-      <c r="D98" t="s">
-        <v>97</v>
-      </c>
       <c r="E98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="B99" t="s">
+        <v>86</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
         <v>93</v>
       </c>
-      <c r="D99" t="s">
-        <v>97</v>
-      </c>
       <c r="E99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B100" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D100" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E100" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B101" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D101" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E101" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
+        <v>97</v>
+      </c>
+      <c r="D102" t="s">
         <v>98</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>99</v>
-      </c>
-      <c r="E102" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B103" t="s">
+        <v>97</v>
+      </c>
+      <c r="D103" t="s">
         <v>98</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>99</v>
-      </c>
-      <c r="E103" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="B104" t="s">
-        <v>101</v>
-      </c>
-      <c r="C104">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="D104" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E104" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
-      </c>
-      <c r="C105">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="D105" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E105" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B106" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E106" t="s">
         <v>4</v>
@@ -2572,16 +2572,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E107" t="s">
         <v>4</v>
@@ -2589,36 +2589,36 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="B108" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E108" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C109">
         <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E109" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2626,16 +2626,16 @@
         <v>19</v>
       </c>
       <c r="B110" t="s">
+        <v>108</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
         <v>110</v>
       </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
-      <c r="D110" t="s">
-        <v>111</v>
-      </c>
       <c r="E110" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2643,16 +2643,16 @@
         <v>21</v>
       </c>
       <c r="B111" t="s">
+        <v>108</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111" t="s">
         <v>110</v>
       </c>
-      <c r="C111">
-        <v>1</v>
-      </c>
-      <c r="D111" t="s">
-        <v>111</v>
-      </c>
       <c r="E111" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2666,10 +2666,10 @@
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E112" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -2683,58 +2683,58 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E113" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C114">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E114" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C115">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E115" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C116">
         <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E116" t="s">
         <v>11</v>
@@ -2742,16 +2742,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B117" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C117">
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E117" t="s">
         <v>11</v>
@@ -2759,50 +2759,50 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B118" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E118" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B119" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E119" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E120" t="s">
         <v>4</v>
@@ -2810,16 +2810,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E121" t="s">
         <v>4</v>
@@ -2827,19 +2827,19 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B122" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E122" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -2847,16 +2847,16 @@
         <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E123" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -2864,16 +2864,16 @@
         <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E124" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2881,16 +2881,16 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E125" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2898,16 +2898,16 @@
         <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E126" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,16 +2915,16 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E127" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2932,16 +2932,16 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E128" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,16 +2949,16 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E129" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2966,16 +2966,16 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
+        <v>119</v>
+      </c>
+      <c r="E130" t="s">
         <v>120</v>
-      </c>
-      <c r="E130" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2983,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
+        <v>119</v>
+      </c>
+      <c r="E131" t="s">
         <v>120</v>
-      </c>
-      <c r="E131" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3000,16 +3000,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E132" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E133" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E134" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,61 +3051,64 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E135" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E136" t="s">
-        <v>4</v>
+        <v>124</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>128</v>
+        <v>124</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E137" t="s">
-        <v>4</v>
+        <v>124</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B138" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E138" t="s">
         <v>4</v>
@@ -3113,13 +3116,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B139" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D139" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E139" t="s">
         <v>4</v>
@@ -3127,13 +3130,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B140" t="s">
-        <v>128</v>
+        <v>114</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E140" t="s">
         <v>4</v>
@@ -3141,16 +3147,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B141" t="s">
-        <v>126</v>
-      </c>
-      <c r="C141">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="D141" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E141" t="s">
         <v>4</v>
@@ -3158,16 +3161,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B142" t="s">
-        <v>131</v>
-      </c>
-      <c r="C142">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D142" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E142" t="s">
         <v>4</v>
@@ -3175,16 +3175,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="B143" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C143">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -3192,16 +3192,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="B144" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C144">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E144" t="s">
         <v>4</v>
@@ -3209,16 +3209,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="B145" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D145" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E145" t="s">
         <v>4</v>
@@ -3226,16 +3226,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="B146" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D146" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E146" t="s">
         <v>4</v>
@@ -3243,16 +3243,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B147" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E147" t="s">
         <v>4</v>
@@ -3260,87 +3260,87 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B148" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A149" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C149" s="1">
-        <v>2</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>152</v>
+      <c r="A149" t="s">
+        <v>87</v>
+      </c>
+      <c r="B149" t="s">
+        <v>114</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
+      </c>
+      <c r="D149" t="s">
+        <v>136</v>
+      </c>
+      <c r="E149" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A150" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C150" s="1">
-        <v>2</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>150</v>
+      <c r="A150" t="s">
+        <v>87</v>
+      </c>
+      <c r="B150" t="s">
+        <v>137</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="D150" t="s">
+        <v>138</v>
+      </c>
+      <c r="E150" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C151" s="1">
         <v>2</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C152" s="1">
         <v>2</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3348,16 +3348,16 @@
         <v>17</v>
       </c>
       <c r="B153" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C153" s="1">
+        <v>2</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C153" s="1">
-        <v>2</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="E153" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -3365,16 +3365,50 @@
         <v>20</v>
       </c>
       <c r="B154" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C154" s="1">
+        <v>2</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C154" s="1">
-        <v>2</v>
-      </c>
-      <c r="D154" s="1" t="s">
+      <c r="E154" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C155" s="1">
+        <v>2</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E155" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E154" s="1" t="s">
-        <v>147</v>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C156" s="1">
+        <v>2</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (cc) Add how to set cc (msg compose) (#418)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F88C06-5B13-4024-A7E9-963ABBCFD0A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4653D781-B58D-4ECE-9270-9ABC8CC3A8E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="159">
   <si>
     <t>Class</t>
   </si>
@@ -138,9 +138,6 @@
     <t>outlook-recipients-and-attendees-get-cc-message-read</t>
   </si>
   <si>
-    <t>outlook-recipients-and-attendees-get-cc-message-compose</t>
-  </si>
-  <si>
     <t>from</t>
   </si>
   <si>
@@ -502,6 +499,12 @@
   </si>
   <si>
     <t>setAsync</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-cc-message-compose</t>
+  </si>
+  <si>
+    <t>setCc</t>
   </si>
 </sst>
 </file>
@@ -577,8 +580,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E154" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E154" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E156" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E156" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -910,11 +913,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1248,10 +1251,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1271,7 +1274,7 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
@@ -1279,16 +1282,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
@@ -1296,241 +1299,241 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>157</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>156</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
         <v>37</v>
       </c>
-      <c r="D26" t="s">
-        <v>40</v>
-      </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>86</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>86</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>86</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>86</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1538,466 +1541,469 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" t="s">
-        <v>155</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>157</v>
+      <c r="A40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
-        <v>156</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C41" s="1"/>
       <c r="D41" t="s">
-        <v>58</v>
-      </c>
-      <c r="E41" t="s">
-        <v>57</v>
+        <v>154</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" t="s">
-        <v>141</v>
+      <c r="A42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>141</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" t="s">
         <v>61</v>
-      </c>
-      <c r="E44" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s">
         <v>61</v>
-      </c>
-      <c r="E45" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" t="s">
         <v>60</v>
       </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>61</v>
-      </c>
-      <c r="E46" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D47" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" t="s">
         <v>61</v>
-      </c>
-      <c r="E47" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" t="s">
         <v>61</v>
-      </c>
-      <c r="E48" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" t="s">
         <v>60</v>
       </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>61</v>
-      </c>
       <c r="E51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" t="s">
         <v>60</v>
       </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56" t="s">
-        <v>61</v>
-      </c>
       <c r="E56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B57" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" t="s">
         <v>60</v>
       </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57" t="s">
-        <v>61</v>
-      </c>
       <c r="E57" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E58" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" t="s">
         <v>66</v>
-      </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="D62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E62" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E63" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>141</v>
+        <v>65</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E64" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
+        <v>140</v>
+      </c>
+      <c r="D67" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" t="s">
         <v>68</v>
-      </c>
-      <c r="C67">
-        <v>2</v>
-      </c>
-      <c r="D67" t="s">
-        <v>61</v>
-      </c>
-      <c r="E67" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E68" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>141</v>
+        <v>67</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E69" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E70" t="s">
         <v>16</v>
@@ -2005,13 +2011,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E71" t="s">
         <v>16</v>
@@ -2019,16 +2025,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="D72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2036,36 +2039,33 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="D73" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E73" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E74" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -2073,16 +2073,16 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" t="s">
+        <v>71</v>
+      </c>
+      <c r="E75" t="s">
         <v>72</v>
-      </c>
-      <c r="E75" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -2090,16 +2090,16 @@
         <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" t="s">
+        <v>71</v>
+      </c>
+      <c r="E76" t="s">
         <v>72</v>
-      </c>
-      <c r="E76" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2107,16 +2107,16 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E77" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2124,16 +2124,16 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E78" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2141,16 +2141,16 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E79" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2158,16 +2158,16 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,16 +2175,16 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E81" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2192,16 +2192,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E82" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2209,47 +2209,47 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="E83" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="E84" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C85">
         <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E85" t="s">
         <v>4</v>
@@ -2257,16 +2257,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C86">
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E86" t="s">
         <v>4</v>
@@ -2274,13 +2274,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="E87" t="s">
         <v>4</v>
@@ -2291,10 +2294,13 @@
         <v>21</v>
       </c>
       <c r="B88" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="E88" t="s">
         <v>4</v>
@@ -2302,269 +2308,263 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D89" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E89" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D90" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E90" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B91" t="s">
+        <v>82</v>
+      </c>
+      <c r="D91" t="s">
         <v>83</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>84</v>
-      </c>
-      <c r="E91" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B92" t="s">
+        <v>82</v>
+      </c>
+      <c r="D92" t="s">
         <v>83</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>84</v>
-      </c>
-      <c r="E92" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B93" t="s">
-        <v>87</v>
-      </c>
-      <c r="C93">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="D93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E93" t="s">
         <v>84</v>
-      </c>
-      <c r="E93" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B94" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D94" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E94" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E95" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D96" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E96" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B97" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C97">
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E97" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B98" t="s">
+        <v>92</v>
+      </c>
+      <c r="D98" t="s">
         <v>93</v>
       </c>
-      <c r="D98" t="s">
-        <v>97</v>
-      </c>
       <c r="E98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="B99" t="s">
+        <v>86</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
         <v>93</v>
       </c>
-      <c r="D99" t="s">
-        <v>97</v>
-      </c>
       <c r="E99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B100" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D100" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E100" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B101" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D101" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E101" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
+        <v>97</v>
+      </c>
+      <c r="D102" t="s">
         <v>98</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>99</v>
-      </c>
-      <c r="E102" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B103" t="s">
+        <v>97</v>
+      </c>
+      <c r="D103" t="s">
         <v>98</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>99</v>
-      </c>
-      <c r="E103" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="B104" t="s">
-        <v>101</v>
-      </c>
-      <c r="C104">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="D104" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E104" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
-      </c>
-      <c r="C105">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="D105" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E105" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B106" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E106" t="s">
         <v>4</v>
@@ -2572,16 +2572,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E107" t="s">
         <v>4</v>
@@ -2589,36 +2589,36 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="B108" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E108" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C109">
         <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E109" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2626,16 +2626,16 @@
         <v>19</v>
       </c>
       <c r="B110" t="s">
+        <v>108</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
         <v>110</v>
       </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
-      <c r="D110" t="s">
-        <v>111</v>
-      </c>
       <c r="E110" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2643,16 +2643,16 @@
         <v>21</v>
       </c>
       <c r="B111" t="s">
+        <v>108</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111" t="s">
         <v>110</v>
       </c>
-      <c r="C111">
-        <v>1</v>
-      </c>
-      <c r="D111" t="s">
-        <v>111</v>
-      </c>
       <c r="E111" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2666,10 +2666,10 @@
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E112" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -2683,58 +2683,58 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E113" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C114">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E114" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C115">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E115" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C116">
         <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E116" t="s">
         <v>11</v>
@@ -2742,16 +2742,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B117" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C117">
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E117" t="s">
         <v>11</v>
@@ -2759,50 +2759,50 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B118" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E118" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B119" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E119" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E120" t="s">
         <v>4</v>
@@ -2810,16 +2810,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E121" t="s">
         <v>4</v>
@@ -2827,19 +2827,19 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B122" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E122" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -2847,16 +2847,16 @@
         <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E123" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -2864,16 +2864,16 @@
         <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E124" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2881,16 +2881,16 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E125" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2898,16 +2898,16 @@
         <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E126" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,16 +2915,16 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E127" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2932,16 +2932,16 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E128" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,16 +2949,16 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E129" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2966,16 +2966,16 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
+        <v>119</v>
+      </c>
+      <c r="E130" t="s">
         <v>120</v>
-      </c>
-      <c r="E130" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2983,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
+        <v>119</v>
+      </c>
+      <c r="E131" t="s">
         <v>120</v>
-      </c>
-      <c r="E131" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3000,16 +3000,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E132" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E133" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E134" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,61 +3051,64 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E135" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E136" t="s">
-        <v>4</v>
+        <v>124</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>128</v>
+        <v>124</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E137" t="s">
-        <v>4</v>
+        <v>124</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B138" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E138" t="s">
         <v>4</v>
@@ -3113,13 +3116,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B139" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D139" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E139" t="s">
         <v>4</v>
@@ -3127,13 +3130,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B140" t="s">
-        <v>128</v>
+        <v>114</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E140" t="s">
         <v>4</v>
@@ -3141,16 +3147,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B141" t="s">
-        <v>126</v>
-      </c>
-      <c r="C141">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="D141" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E141" t="s">
         <v>4</v>
@@ -3158,16 +3161,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B142" t="s">
-        <v>131</v>
-      </c>
-      <c r="C142">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D142" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E142" t="s">
         <v>4</v>
@@ -3175,16 +3175,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="B143" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C143">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -3192,16 +3192,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="B144" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C144">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E144" t="s">
         <v>4</v>
@@ -3209,16 +3209,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="B145" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D145" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E145" t="s">
         <v>4</v>
@@ -3226,16 +3226,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="B146" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D146" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E146" t="s">
         <v>4</v>
@@ -3243,16 +3243,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B147" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E147" t="s">
         <v>4</v>
@@ -3260,87 +3260,87 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B148" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A149" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C149" s="1">
-        <v>2</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>152</v>
+      <c r="A149" t="s">
+        <v>87</v>
+      </c>
+      <c r="B149" t="s">
+        <v>114</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
+      </c>
+      <c r="D149" t="s">
+        <v>136</v>
+      </c>
+      <c r="E149" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A150" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C150" s="1">
-        <v>2</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>150</v>
+      <c r="A150" t="s">
+        <v>87</v>
+      </c>
+      <c r="B150" t="s">
+        <v>137</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="D150" t="s">
+        <v>138</v>
+      </c>
+      <c r="E150" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C151" s="1">
         <v>2</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C152" s="1">
         <v>2</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3348,16 +3348,16 @@
         <v>17</v>
       </c>
       <c r="B153" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C153" s="1">
+        <v>2</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C153" s="1">
-        <v>2</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="E153" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -3365,16 +3365,50 @@
         <v>20</v>
       </c>
       <c r="B154" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C154" s="1">
+        <v>2</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C154" s="1">
-        <v>2</v>
-      </c>
-      <c r="D154" s="1" t="s">
+      <c r="E154" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C155" s="1">
+        <v>2</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E155" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E154" s="1" t="s">
-        <v>147</v>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C156" s="1">
+        <v>2</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (bcc) Add how to set bcc (Message Compose)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4653D781-B58D-4ECE-9270-9ABC8CC3A8E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC206693-7000-458F-8CC4-DFA1EAB1C630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="160">
   <si>
     <t>Class</t>
   </si>
@@ -123,9 +123,6 @@
     <t>bcc</t>
   </si>
   <si>
-    <t>outlook-recipients-and-attendees-get-bcc-message-compose</t>
-  </si>
-  <si>
     <t>getBcc</t>
   </si>
   <si>
@@ -505,6 +502,12 @@
   </si>
   <si>
     <t>setCc</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-bcc-message-compose</t>
+  </si>
+  <si>
+    <t>setBcc</t>
   </si>
 </sst>
 </file>
@@ -580,8 +583,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E156" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E156" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E158" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E158" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -913,11 +916,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E156"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1243,27 +1246,27 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" t="s">
         <v>31</v>
-      </c>
-      <c r="E19" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" t="s">
         <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1271,30 +1274,30 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1302,269 +1305,269 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" t="s">
         <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>157</v>
-      </c>
-      <c r="E23" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
         <v>156</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>157</v>
-      </c>
       <c r="E24" t="s">
-        <v>158</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>155</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
         <v>36</v>
       </c>
-      <c r="D28" t="s">
-        <v>39</v>
-      </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>85</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E29" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E32" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>85</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>85</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>85</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>154</v>
+        <v>50</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1572,466 +1575,469 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>153</v>
+      </c>
+      <c r="E41" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" t="s">
-        <v>154</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>156</v>
+      <c r="A42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" t="s">
+        <v>85</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E42" t="s">
-        <v>155</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C43" s="1"/>
       <c r="D43" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" t="s">
-        <v>56</v>
+        <v>153</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" t="s">
-        <v>140</v>
+      <c r="A44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="E44" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" t="s">
         <v>60</v>
-      </c>
-      <c r="E46" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" t="s">
         <v>60</v>
-      </c>
-      <c r="E47" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" t="s">
         <v>59</v>
       </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>60</v>
-      </c>
-      <c r="E48" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D49" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" t="s">
         <v>60</v>
-      </c>
-      <c r="E49" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>140</v>
+        <v>58</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
       </c>
       <c r="D50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50" t="s">
         <v>60</v>
-      </c>
-      <c r="E50" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" t="s">
         <v>59</v>
       </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="D53" t="s">
-        <v>60</v>
-      </c>
       <c r="E53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E54" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E55" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
+        <v>139</v>
+      </c>
+      <c r="D58" t="s">
         <v>59</v>
       </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58" t="s">
-        <v>60</v>
-      </c>
       <c r="E58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" t="s">
         <v>59</v>
       </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s">
-        <v>60</v>
-      </c>
       <c r="E59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>140</v>
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>58</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E61" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" t="s">
         <v>65</v>
-      </c>
-      <c r="C64">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s">
-        <v>60</v>
-      </c>
-      <c r="E64" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E65" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>64</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E66" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B69" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" t="s">
+        <v>59</v>
+      </c>
+      <c r="E69" t="s">
         <v>67</v>
-      </c>
-      <c r="C69">
-        <v>2</v>
-      </c>
-      <c r="D69" t="s">
-        <v>60</v>
-      </c>
-      <c r="E69" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E70" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>66</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E71" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2039,13 +2045,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E73" t="s">
         <v>16</v>
@@ -2053,16 +2059,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
-      </c>
-      <c r="C74">
-        <v>2</v>
+        <v>139</v>
       </c>
       <c r="D74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E74" t="s">
         <v>16</v>
@@ -2070,36 +2073,33 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B75" t="s">
-        <v>70</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="D75" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E75" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B76" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E76" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2107,16 +2107,16 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
+        <v>70</v>
+      </c>
+      <c r="E77" t="s">
         <v>71</v>
-      </c>
-      <c r="E77" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2124,16 +2124,16 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" t="s">
+        <v>70</v>
+      </c>
+      <c r="E78" t="s">
         <v>71</v>
-      </c>
-      <c r="E78" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2141,16 +2141,16 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E79" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2158,16 +2158,16 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E80" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,16 +2175,16 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E81" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2192,16 +2192,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2209,16 +2209,16 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E83" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2226,16 +2226,16 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E84" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2243,47 +2243,47 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="E85" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="E86" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C87">
         <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E87" t="s">
         <v>4</v>
@@ -2291,16 +2291,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C88">
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E88" t="s">
         <v>4</v>
@@ -2308,13 +2308,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B89" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="E89" t="s">
         <v>4</v>
@@ -2325,10 +2328,13 @@
         <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="E90" t="s">
         <v>4</v>
@@ -2336,269 +2342,263 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B91" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D91" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E91" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B92" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D92" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E92" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
+        <v>81</v>
+      </c>
+      <c r="D93" t="s">
         <v>82</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>83</v>
-      </c>
-      <c r="E93" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B94" t="s">
+        <v>81</v>
+      </c>
+      <c r="D94" t="s">
         <v>82</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>83</v>
-      </c>
-      <c r="E94" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B95" t="s">
-        <v>86</v>
-      </c>
-      <c r="C95">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="D95" t="s">
+        <v>82</v>
+      </c>
+      <c r="E95" t="s">
         <v>83</v>
-      </c>
-      <c r="E95" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B96" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D96" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E96" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C97">
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E97" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D98" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E98" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B99" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E99" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B100" t="s">
+        <v>91</v>
+      </c>
+      <c r="D100" t="s">
         <v>92</v>
       </c>
-      <c r="D100" t="s">
-        <v>96</v>
-      </c>
       <c r="E100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B101" t="s">
+        <v>85</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
         <v>92</v>
       </c>
-      <c r="D101" t="s">
-        <v>96</v>
-      </c>
       <c r="E101" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B102" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D102" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E102" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B103" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D103" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E103" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B104" t="s">
+        <v>96</v>
+      </c>
+      <c r="D104" t="s">
         <v>97</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E104" t="s">
         <v>98</v>
-      </c>
-      <c r="E104" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B105" t="s">
+        <v>96</v>
+      </c>
+      <c r="D105" t="s">
         <v>97</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>98</v>
-      </c>
-      <c r="E105" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="B106" t="s">
-        <v>100</v>
-      </c>
-      <c r="C106">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="D106" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E106" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B107" t="s">
-        <v>102</v>
-      </c>
-      <c r="C107">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="D107" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E107" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B108" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E108" t="s">
         <v>4</v>
@@ -2606,16 +2606,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B109" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C109">
         <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E109" t="s">
         <v>4</v>
@@ -2623,36 +2623,36 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="B110" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E110" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B111" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E111" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2660,16 +2660,16 @@
         <v>19</v>
       </c>
       <c r="B112" t="s">
+        <v>107</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112" t="s">
         <v>109</v>
       </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
-      <c r="D112" t="s">
-        <v>110</v>
-      </c>
       <c r="E112" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -2677,16 +2677,16 @@
         <v>21</v>
       </c>
       <c r="B113" t="s">
+        <v>107</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113" t="s">
         <v>109</v>
       </c>
-      <c r="C113">
-        <v>1</v>
-      </c>
-      <c r="D113" t="s">
-        <v>110</v>
-      </c>
       <c r="E113" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2700,10 +2700,10 @@
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E114" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2717,58 +2717,58 @@
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E115" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B116" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E116" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B117" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C117">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E117" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C118">
         <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E118" t="s">
         <v>11</v>
@@ -2776,16 +2776,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B119" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C119">
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E119" t="s">
         <v>11</v>
@@ -2793,50 +2793,50 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E120" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E121" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B122" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E122" t="s">
         <v>4</v>
@@ -2844,16 +2844,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E123" t="s">
         <v>4</v>
@@ -2861,19 +2861,19 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B124" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E124" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2881,16 +2881,16 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E125" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2898,16 +2898,16 @@
         <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E126" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,16 +2915,16 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E127" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2932,16 +2932,16 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E128" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,16 +2949,16 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E129" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2966,16 +2966,16 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E130" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2983,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E131" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3000,16 +3000,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
+        <v>118</v>
+      </c>
+      <c r="E132" t="s">
         <v>119</v>
-      </c>
-      <c r="E132" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
+        <v>118</v>
+      </c>
+      <c r="E133" t="s">
         <v>119</v>
-      </c>
-      <c r="E133" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E134" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,16 +3051,16 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E135" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,16 +3068,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E136" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3085,61 +3085,64 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E137" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E138" t="s">
-        <v>4</v>
+        <v>123</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E139" t="s">
-        <v>4</v>
+        <v>123</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B140" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E140" t="s">
         <v>4</v>
@@ -3147,13 +3150,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B141" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D141" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E141" t="s">
         <v>4</v>
@@ -3161,13 +3164,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B142" t="s">
-        <v>127</v>
+        <v>113</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E142" t="s">
         <v>4</v>
@@ -3175,16 +3181,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B143" t="s">
-        <v>125</v>
-      </c>
-      <c r="C143">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D143" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -3192,16 +3195,13 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B144" t="s">
-        <v>130</v>
-      </c>
-      <c r="C144">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="D144" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E144" t="s">
         <v>4</v>
@@ -3209,16 +3209,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="B145" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C145">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E145" t="s">
         <v>4</v>
@@ -3226,16 +3226,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B146" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C146">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E146" t="s">
         <v>4</v>
@@ -3243,16 +3243,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="B147" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C147">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D147" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E147" t="s">
         <v>4</v>
@@ -3260,16 +3260,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="B148" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C148">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D148" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
@@ -3277,16 +3277,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B149" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E149" t="s">
         <v>4</v>
@@ -3294,87 +3294,87 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B150" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E150" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A151" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C151" s="1">
-        <v>2</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>151</v>
+      <c r="A151" t="s">
+        <v>86</v>
+      </c>
+      <c r="B151" t="s">
+        <v>113</v>
+      </c>
+      <c r="C151">
+        <v>2</v>
+      </c>
+      <c r="D151" t="s">
+        <v>135</v>
+      </c>
+      <c r="E151" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A152" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C152" s="1">
-        <v>2</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>149</v>
+      <c r="A152" t="s">
+        <v>86</v>
+      </c>
+      <c r="B152" t="s">
+        <v>136</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152" t="s">
+        <v>137</v>
+      </c>
+      <c r="E152" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C153" s="1">
         <v>2</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C154" s="1">
         <v>2</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3382,16 +3382,16 @@
         <v>17</v>
       </c>
       <c r="B155" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C155" s="1">
+        <v>2</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C155" s="1">
-        <v>2</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="E155" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3399,16 +3399,50 @@
         <v>20</v>
       </c>
       <c r="B156" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C156" s="1">
+        <v>2</v>
+      </c>
+      <c r="D156" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C156" s="1">
-        <v>2</v>
-      </c>
-      <c r="D156" s="1" t="s">
+      <c r="E156" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C157" s="1">
+        <v>2</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E157" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E156" s="1" t="s">
-        <v>146</v>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C158" s="1">
+        <v>2</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (bcc) Add how to set bcc (Message Compose) (#419)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4653D781-B58D-4ECE-9270-9ABC8CC3A8E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC206693-7000-458F-8CC4-DFA1EAB1C630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="160">
   <si>
     <t>Class</t>
   </si>
@@ -123,9 +123,6 @@
     <t>bcc</t>
   </si>
   <si>
-    <t>outlook-recipients-and-attendees-get-bcc-message-compose</t>
-  </si>
-  <si>
     <t>getBcc</t>
   </si>
   <si>
@@ -505,6 +502,12 @@
   </si>
   <si>
     <t>setCc</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-bcc-message-compose</t>
+  </si>
+  <si>
+    <t>setBcc</t>
   </si>
 </sst>
 </file>
@@ -580,8 +583,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E156" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E156" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E158" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E158" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -913,11 +916,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E156"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1243,27 +1246,27 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" t="s">
         <v>31</v>
-      </c>
-      <c r="E19" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" t="s">
         <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1271,30 +1274,30 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1302,269 +1305,269 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" t="s">
         <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>157</v>
-      </c>
-      <c r="E23" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
         <v>156</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>157</v>
-      </c>
       <c r="E24" t="s">
-        <v>158</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>155</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
         <v>36</v>
       </c>
-      <c r="D28" t="s">
-        <v>39</v>
-      </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>85</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E29" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E32" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>85</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>85</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>85</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>154</v>
+        <v>50</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1572,466 +1575,469 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>153</v>
+      </c>
+      <c r="E41" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" t="s">
-        <v>154</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>156</v>
+      <c r="A42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" t="s">
+        <v>85</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E42" t="s">
-        <v>155</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C43" s="1"/>
       <c r="D43" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" t="s">
-        <v>56</v>
+        <v>153</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" t="s">
-        <v>140</v>
+      <c r="A44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="E44" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" t="s">
         <v>60</v>
-      </c>
-      <c r="E46" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" t="s">
         <v>60</v>
-      </c>
-      <c r="E47" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" t="s">
         <v>59</v>
       </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>60</v>
-      </c>
-      <c r="E48" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D49" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" t="s">
         <v>60</v>
-      </c>
-      <c r="E49" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>140</v>
+        <v>58</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
       </c>
       <c r="D50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50" t="s">
         <v>60</v>
-      </c>
-      <c r="E50" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" t="s">
         <v>59</v>
       </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="D53" t="s">
-        <v>60</v>
-      </c>
       <c r="E53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E54" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E55" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
+        <v>139</v>
+      </c>
+      <c r="D58" t="s">
         <v>59</v>
       </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58" t="s">
-        <v>60</v>
-      </c>
       <c r="E58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" t="s">
         <v>59</v>
       </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s">
-        <v>60</v>
-      </c>
       <c r="E59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>140</v>
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>58</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E61" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" t="s">
         <v>65</v>
-      </c>
-      <c r="C64">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s">
-        <v>60</v>
-      </c>
-      <c r="E64" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E65" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>64</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E66" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B69" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" t="s">
+        <v>59</v>
+      </c>
+      <c r="E69" t="s">
         <v>67</v>
-      </c>
-      <c r="C69">
-        <v>2</v>
-      </c>
-      <c r="D69" t="s">
-        <v>60</v>
-      </c>
-      <c r="E69" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E70" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>66</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E71" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E72" t="s">
         <v>16</v>
@@ -2039,13 +2045,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E73" t="s">
         <v>16</v>
@@ -2053,16 +2059,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
-      </c>
-      <c r="C74">
-        <v>2</v>
+        <v>139</v>
       </c>
       <c r="D74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E74" t="s">
         <v>16</v>
@@ -2070,36 +2073,33 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B75" t="s">
-        <v>70</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="D75" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E75" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B76" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E76" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2107,16 +2107,16 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
+        <v>70</v>
+      </c>
+      <c r="E77" t="s">
         <v>71</v>
-      </c>
-      <c r="E77" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2124,16 +2124,16 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" t="s">
+        <v>70</v>
+      </c>
+      <c r="E78" t="s">
         <v>71</v>
-      </c>
-      <c r="E78" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2141,16 +2141,16 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E79" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2158,16 +2158,16 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E80" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,16 +2175,16 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E81" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2192,16 +2192,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2209,16 +2209,16 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E83" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2226,16 +2226,16 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E84" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2243,47 +2243,47 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="E85" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="E86" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C87">
         <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E87" t="s">
         <v>4</v>
@@ -2291,16 +2291,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C88">
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E88" t="s">
         <v>4</v>
@@ -2308,13 +2308,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B89" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="E89" t="s">
         <v>4</v>
@@ -2325,10 +2328,13 @@
         <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="E90" t="s">
         <v>4</v>
@@ -2336,269 +2342,263 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B91" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D91" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E91" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B92" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D92" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E92" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
+        <v>81</v>
+      </c>
+      <c r="D93" t="s">
         <v>82</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>83</v>
-      </c>
-      <c r="E93" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B94" t="s">
+        <v>81</v>
+      </c>
+      <c r="D94" t="s">
         <v>82</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>83</v>
-      </c>
-      <c r="E94" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B95" t="s">
-        <v>86</v>
-      </c>
-      <c r="C95">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="D95" t="s">
+        <v>82</v>
+      </c>
+      <c r="E95" t="s">
         <v>83</v>
-      </c>
-      <c r="E95" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B96" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D96" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E96" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C97">
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E97" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D98" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E98" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B99" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E99" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B100" t="s">
+        <v>91</v>
+      </c>
+      <c r="D100" t="s">
         <v>92</v>
       </c>
-      <c r="D100" t="s">
-        <v>96</v>
-      </c>
       <c r="E100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B101" t="s">
+        <v>85</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
         <v>92</v>
       </c>
-      <c r="D101" t="s">
-        <v>96</v>
-      </c>
       <c r="E101" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B102" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D102" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E102" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B103" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D103" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E103" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B104" t="s">
+        <v>96</v>
+      </c>
+      <c r="D104" t="s">
         <v>97</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E104" t="s">
         <v>98</v>
-      </c>
-      <c r="E104" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B105" t="s">
+        <v>96</v>
+      </c>
+      <c r="D105" t="s">
         <v>97</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>98</v>
-      </c>
-      <c r="E105" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="B106" t="s">
-        <v>100</v>
-      </c>
-      <c r="C106">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="D106" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E106" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B107" t="s">
-        <v>102</v>
-      </c>
-      <c r="C107">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="D107" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E107" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B108" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E108" t="s">
         <v>4</v>
@@ -2606,16 +2606,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B109" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C109">
         <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E109" t="s">
         <v>4</v>
@@ -2623,36 +2623,36 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="B110" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E110" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B111" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E111" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2660,16 +2660,16 @@
         <v>19</v>
       </c>
       <c r="B112" t="s">
+        <v>107</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112" t="s">
         <v>109</v>
       </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
-      <c r="D112" t="s">
-        <v>110</v>
-      </c>
       <c r="E112" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -2677,16 +2677,16 @@
         <v>21</v>
       </c>
       <c r="B113" t="s">
+        <v>107</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113" t="s">
         <v>109</v>
       </c>
-      <c r="C113">
-        <v>1</v>
-      </c>
-      <c r="D113" t="s">
-        <v>110</v>
-      </c>
       <c r="E113" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2700,10 +2700,10 @@
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E114" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2717,58 +2717,58 @@
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E115" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B116" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E116" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B117" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C117">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E117" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C118">
         <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E118" t="s">
         <v>11</v>
@@ -2776,16 +2776,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B119" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C119">
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E119" t="s">
         <v>11</v>
@@ -2793,50 +2793,50 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E120" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E121" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B122" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E122" t="s">
         <v>4</v>
@@ -2844,16 +2844,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E123" t="s">
         <v>4</v>
@@ -2861,19 +2861,19 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B124" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E124" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2881,16 +2881,16 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E125" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2898,16 +2898,16 @@
         <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E126" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,16 +2915,16 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E127" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2932,16 +2932,16 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E128" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,16 +2949,16 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E129" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2966,16 +2966,16 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E130" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2983,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E131" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3000,16 +3000,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
+        <v>118</v>
+      </c>
+      <c r="E132" t="s">
         <v>119</v>
-      </c>
-      <c r="E132" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
+        <v>118</v>
+      </c>
+      <c r="E133" t="s">
         <v>119</v>
-      </c>
-      <c r="E133" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E134" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,16 +3051,16 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E135" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,16 +3068,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E136" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3085,61 +3085,64 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E137" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E138" t="s">
-        <v>4</v>
+        <v>123</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E139" t="s">
-        <v>4</v>
+        <v>123</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B140" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E140" t="s">
         <v>4</v>
@@ -3147,13 +3150,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B141" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D141" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E141" t="s">
         <v>4</v>
@@ -3161,13 +3164,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B142" t="s">
-        <v>127</v>
+        <v>113</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E142" t="s">
         <v>4</v>
@@ -3175,16 +3181,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B143" t="s">
-        <v>125</v>
-      </c>
-      <c r="C143">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D143" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -3192,16 +3195,13 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B144" t="s">
-        <v>130</v>
-      </c>
-      <c r="C144">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="D144" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E144" t="s">
         <v>4</v>
@@ -3209,16 +3209,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="B145" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C145">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E145" t="s">
         <v>4</v>
@@ -3226,16 +3226,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B146" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C146">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E146" t="s">
         <v>4</v>
@@ -3243,16 +3243,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="B147" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C147">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D147" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E147" t="s">
         <v>4</v>
@@ -3260,16 +3260,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="B148" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C148">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D148" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
@@ -3277,16 +3277,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B149" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E149" t="s">
         <v>4</v>
@@ -3294,87 +3294,87 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B150" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E150" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A151" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C151" s="1">
-        <v>2</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>151</v>
+      <c r="A151" t="s">
+        <v>86</v>
+      </c>
+      <c r="B151" t="s">
+        <v>113</v>
+      </c>
+      <c r="C151">
+        <v>2</v>
+      </c>
+      <c r="D151" t="s">
+        <v>135</v>
+      </c>
+      <c r="E151" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A152" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C152" s="1">
-        <v>2</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>149</v>
+      <c r="A152" t="s">
+        <v>86</v>
+      </c>
+      <c r="B152" t="s">
+        <v>136</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152" t="s">
+        <v>137</v>
+      </c>
+      <c r="E152" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C153" s="1">
         <v>2</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C154" s="1">
         <v>2</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3382,16 +3382,16 @@
         <v>17</v>
       </c>
       <c r="B155" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C155" s="1">
+        <v>2</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C155" s="1">
-        <v>2</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="E155" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3399,16 +3399,50 @@
         <v>20</v>
       </c>
       <c r="B156" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C156" s="1">
+        <v>2</v>
+      </c>
+      <c r="D156" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C156" s="1">
-        <v>2</v>
-      </c>
-      <c r="D156" s="1" t="s">
+      <c r="E156" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C157" s="1">
+        <v>2</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E157" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E156" s="1" t="s">
-        <v>146</v>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C158" s="1">
+        <v>2</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (requiredAttendees) Add how to set (Appointment compose)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC206693-7000-458F-8CC4-DFA1EAB1C630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C3BBE1-7F22-449A-AF5A-62AC47D1A151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="161">
   <si>
     <t>Class</t>
   </si>
@@ -180,9 +180,6 @@
     <t>getRequiredAttendees</t>
   </si>
   <si>
-    <t>outlook-recipients-and-attendees-get-required-attendees-appointment-organizer</t>
-  </si>
-  <si>
     <t>sender</t>
   </si>
   <si>
@@ -508,6 +505,12 @@
   </si>
   <si>
     <t>setBcc</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-required-attendees-appointment-organizer</t>
+  </si>
+  <si>
+    <t>setRequiredAttendees</t>
   </si>
 </sst>
 </file>
@@ -583,8 +586,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E158" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E158" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E160" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E160" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -916,11 +919,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E158"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1246,7 +1249,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1254,16 +1257,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1277,27 +1280,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" t="s">
         <v>158</v>
-      </c>
-      <c r="E21" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" t="s">
         <v>158</v>
-      </c>
-      <c r="E22" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1308,7 +1311,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1316,16 +1319,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1339,27 +1342,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>155</v>
+      </c>
+      <c r="E25" t="s">
         <v>156</v>
-      </c>
-      <c r="E25" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>155</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>156</v>
-      </c>
-      <c r="E26" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1392,10 +1395,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1451,10 +1454,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1496,10 +1499,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -1533,7 +1536,7 @@
         <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>159</v>
       </c>
       <c r="E38" t="s">
         <v>49</v>
@@ -1541,16 +1544,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>159</v>
       </c>
       <c r="E39" t="s">
         <v>49</v>
@@ -1558,47 +1561,47 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>52</v>
+        <v>159</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>154</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E41" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="E42" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1606,466 +1609,469 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>155</v>
+      <c r="A44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E44" t="s">
-        <v>154</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C45" s="1"/>
       <c r="D45" t="s">
-        <v>56</v>
-      </c>
-      <c r="E45" t="s">
-        <v>55</v>
+        <v>152</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" t="s">
-        <v>139</v>
+      <c r="A46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="E46" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" t="s">
         <v>59</v>
-      </c>
-      <c r="E48" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D49" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" t="s">
         <v>59</v>
-      </c>
-      <c r="E49" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" t="s">
         <v>58</v>
       </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>59</v>
-      </c>
-      <c r="E50" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" t="s">
         <v>59</v>
-      </c>
-      <c r="E51" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
       </c>
       <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" t="s">
         <v>59</v>
-      </c>
-      <c r="E52" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" t="s">
         <v>58</v>
       </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55" t="s">
-        <v>59</v>
-      </c>
       <c r="E55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E56" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60" t="s">
         <v>58</v>
       </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s">
-        <v>59</v>
-      </c>
       <c r="E60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B61" t="s">
+        <v>138</v>
+      </c>
+      <c r="D61" t="s">
         <v>58</v>
       </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s">
-        <v>59</v>
-      </c>
       <c r="E61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E62" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E63" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" t="s">
+        <v>58</v>
+      </c>
+      <c r="E66" t="s">
         <v>64</v>
-      </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-      <c r="D66" t="s">
-        <v>59</v>
-      </c>
-      <c r="E66" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E67" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>63</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E68" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E71" t="s">
         <v>66</v>
-      </c>
-      <c r="C71">
-        <v>2</v>
-      </c>
-      <c r="D71" t="s">
-        <v>59</v>
-      </c>
-      <c r="E71" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B72" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E72" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B73" t="s">
-        <v>139</v>
+        <v>65</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E73" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E74" t="s">
         <v>16</v>
@@ -2073,13 +2079,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
@@ -2087,16 +2093,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>68</v>
-      </c>
-      <c r="C76">
-        <v>2</v>
+        <v>138</v>
       </c>
       <c r="D76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2104,36 +2107,33 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B77" t="s">
-        <v>69</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="D77" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E77" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E78" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2141,16 +2141,16 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" t="s">
+        <v>69</v>
+      </c>
+      <c r="E79" t="s">
         <v>70</v>
-      </c>
-      <c r="E79" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2158,16 +2158,16 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
+        <v>69</v>
+      </c>
+      <c r="E80" t="s">
         <v>70</v>
-      </c>
-      <c r="E80" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,16 +2175,16 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E81" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2192,16 +2192,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E82" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2209,16 +2209,16 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2226,16 +2226,16 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E84" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2243,16 +2243,16 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E85" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2260,16 +2260,16 @@
         <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E86" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2277,47 +2277,47 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E87" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E88" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C89">
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E89" t="s">
         <v>4</v>
@@ -2325,16 +2325,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C90">
         <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E90" t="s">
         <v>4</v>
@@ -2342,13 +2342,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B91" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2359,10 +2362,13 @@
         <v>21</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2370,269 +2376,263 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B93" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D93" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E93" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B94" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D94" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E94" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B95" t="s">
+        <v>80</v>
+      </c>
+      <c r="D95" t="s">
         <v>81</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>82</v>
-      </c>
-      <c r="E95" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B96" t="s">
+        <v>80</v>
+      </c>
+      <c r="D96" t="s">
         <v>81</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>82</v>
-      </c>
-      <c r="E96" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B97" t="s">
-        <v>85</v>
-      </c>
-      <c r="C97">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="D97" t="s">
+        <v>81</v>
+      </c>
+      <c r="E97" t="s">
         <v>82</v>
-      </c>
-      <c r="E97" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="B98" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D98" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E98" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E99" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B100" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D100" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E100" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B101" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E101" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
+        <v>90</v>
+      </c>
+      <c r="D102" t="s">
         <v>91</v>
       </c>
-      <c r="D102" t="s">
-        <v>95</v>
-      </c>
       <c r="E102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="B103" t="s">
+        <v>84</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s">
         <v>91</v>
       </c>
-      <c r="D103" t="s">
-        <v>95</v>
-      </c>
       <c r="E103" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B104" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D104" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E104" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D105" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E105" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B106" t="s">
+        <v>95</v>
+      </c>
+      <c r="D106" t="s">
         <v>96</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E106" t="s">
         <v>97</v>
-      </c>
-      <c r="E106" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B107" t="s">
+        <v>95</v>
+      </c>
+      <c r="D107" t="s">
         <v>96</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" t="s">
         <v>97</v>
-      </c>
-      <c r="E107" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B108" t="s">
-        <v>99</v>
-      </c>
-      <c r="C108">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="D108" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E108" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="B109" t="s">
-        <v>101</v>
-      </c>
-      <c r="C109">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="D109" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E109" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B110" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E110" t="s">
         <v>4</v>
@@ -2640,16 +2640,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B111" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E111" t="s">
         <v>4</v>
@@ -2657,36 +2657,36 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="B112" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E112" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="B113" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C113">
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E113" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2694,16 +2694,16 @@
         <v>19</v>
       </c>
       <c r="B114" t="s">
+        <v>106</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114" t="s">
         <v>108</v>
       </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-      <c r="D114" t="s">
-        <v>109</v>
-      </c>
       <c r="E114" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2711,16 +2711,16 @@
         <v>21</v>
       </c>
       <c r="B115" t="s">
+        <v>106</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115" t="s">
         <v>108</v>
       </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-      <c r="D115" t="s">
-        <v>109</v>
-      </c>
       <c r="E115" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2734,10 +2734,10 @@
         <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E116" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2751,58 +2751,58 @@
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E117" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B118" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C118">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E118" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B119" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E119" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B120" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C120">
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E120" t="s">
         <v>11</v>
@@ -2810,16 +2810,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
@@ -2827,50 +2827,50 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B122" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C122">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E122" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E123" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E124" t="s">
         <v>4</v>
@@ -2878,16 +2878,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B125" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E125" t="s">
         <v>4</v>
@@ -2895,19 +2895,19 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B126" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E126" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,16 +2915,16 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E127" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2932,16 +2932,16 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E128" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,16 +2949,16 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E129" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2966,16 +2966,16 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E130" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2983,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E131" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3000,16 +3000,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E132" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E133" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
+        <v>117</v>
+      </c>
+      <c r="E134" t="s">
         <v>118</v>
-      </c>
-      <c r="E134" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,16 +3051,16 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
+        <v>117</v>
+      </c>
+      <c r="E135" t="s">
         <v>118</v>
-      </c>
-      <c r="E135" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,16 +3068,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E136" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3085,16 +3085,16 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E137" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -3102,16 +3102,16 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E138" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3119,61 +3119,64 @@
         <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E139" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E140" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E141" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B142" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E142" t="s">
         <v>4</v>
@@ -3181,13 +3184,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B143" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D143" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -3195,13 +3198,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B144" t="s">
-        <v>126</v>
+        <v>112</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E144" t="s">
         <v>4</v>
@@ -3209,16 +3215,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B145" t="s">
-        <v>124</v>
-      </c>
-      <c r="C145">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="D145" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E145" t="s">
         <v>4</v>
@@ -3226,16 +3229,13 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B146" t="s">
-        <v>129</v>
-      </c>
-      <c r="C146">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="D146" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E146" t="s">
         <v>4</v>
@@ -3243,16 +3243,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B147" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E147" t="s">
         <v>4</v>
@@ -3260,16 +3260,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B148" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C148">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
@@ -3277,16 +3277,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="B149" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D149" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E149" t="s">
         <v>4</v>
@@ -3294,16 +3294,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B150" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C150">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D150" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E150" t="s">
         <v>4</v>
@@ -3311,16 +3311,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B151" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="C151">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E151" t="s">
         <v>4</v>
@@ -3328,87 +3328,87 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B152" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C152">
         <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E152" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A153" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C153" s="1">
-        <v>2</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>150</v>
+      <c r="A153" t="s">
+        <v>85</v>
+      </c>
+      <c r="B153" t="s">
+        <v>112</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153" t="s">
+        <v>134</v>
+      </c>
+      <c r="E153" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A154" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C154" s="1">
-        <v>2</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>148</v>
+      <c r="A154" t="s">
+        <v>85</v>
+      </c>
+      <c r="B154" t="s">
+        <v>135</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+      <c r="D154" t="s">
+        <v>136</v>
+      </c>
+      <c r="E154" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C155" s="1">
         <v>2</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C156" s="1">
         <v>2</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3416,16 +3416,16 @@
         <v>17</v>
       </c>
       <c r="B157" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C157" s="1">
+        <v>2</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C157" s="1">
-        <v>2</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="E157" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -3433,16 +3433,50 @@
         <v>20</v>
       </c>
       <c r="B158" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C158" s="1">
+        <v>2</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C158" s="1">
-        <v>2</v>
-      </c>
-      <c r="D158" s="1" t="s">
+      <c r="E158" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C159" s="1">
+        <v>2</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E159" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E158" s="1" t="s">
-        <v>145</v>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C160" s="1">
+        <v>2</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (requiredAttendees) Add how to set in Appointment Organizer mode (#420)
* [Outlook] (requiredAttendees) Add how to set (Appointment compose)

* Fix typo
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC206693-7000-458F-8CC4-DFA1EAB1C630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C3BBE1-7F22-449A-AF5A-62AC47D1A151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="161">
   <si>
     <t>Class</t>
   </si>
@@ -180,9 +180,6 @@
     <t>getRequiredAttendees</t>
   </si>
   <si>
-    <t>outlook-recipients-and-attendees-get-required-attendees-appointment-organizer</t>
-  </si>
-  <si>
     <t>sender</t>
   </si>
   <si>
@@ -508,6 +505,12 @@
   </si>
   <si>
     <t>setBcc</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-required-attendees-appointment-organizer</t>
+  </si>
+  <si>
+    <t>setRequiredAttendees</t>
   </si>
 </sst>
 </file>
@@ -583,8 +586,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E158" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E158" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E160" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E160" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -916,11 +919,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E158"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1246,7 +1249,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1254,16 +1257,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1277,27 +1280,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" t="s">
         <v>158</v>
-      </c>
-      <c r="E21" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" t="s">
         <v>158</v>
-      </c>
-      <c r="E22" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1308,7 +1311,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1316,16 +1319,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1339,27 +1342,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>155</v>
+      </c>
+      <c r="E25" t="s">
         <v>156</v>
-      </c>
-      <c r="E25" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>155</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>156</v>
-      </c>
-      <c r="E26" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1392,10 +1395,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1451,10 +1454,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1496,10 +1499,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -1533,7 +1536,7 @@
         <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>159</v>
       </c>
       <c r="E38" t="s">
         <v>49</v>
@@ -1541,16 +1544,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>159</v>
       </c>
       <c r="E39" t="s">
         <v>49</v>
@@ -1558,47 +1561,47 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>52</v>
+        <v>159</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>154</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E41" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="E42" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1606,466 +1609,469 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>155</v>
+      <c r="A44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E44" t="s">
-        <v>154</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C45" s="1"/>
       <c r="D45" t="s">
-        <v>56</v>
-      </c>
-      <c r="E45" t="s">
-        <v>55</v>
+        <v>152</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" t="s">
-        <v>139</v>
+      <c r="A46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="E46" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" t="s">
         <v>59</v>
-      </c>
-      <c r="E48" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D49" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" t="s">
         <v>59</v>
-      </c>
-      <c r="E49" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" t="s">
         <v>58</v>
       </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>59</v>
-      </c>
-      <c r="E50" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" t="s">
         <v>59</v>
-      </c>
-      <c r="E51" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
       </c>
       <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" t="s">
         <v>59</v>
-      </c>
-      <c r="E52" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" t="s">
         <v>58</v>
       </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55" t="s">
-        <v>59</v>
-      </c>
       <c r="E55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E56" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60" t="s">
         <v>58</v>
       </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s">
-        <v>59</v>
-      </c>
       <c r="E60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B61" t="s">
+        <v>138</v>
+      </c>
+      <c r="D61" t="s">
         <v>58</v>
       </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s">
-        <v>59</v>
-      </c>
       <c r="E61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E62" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E63" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" t="s">
+        <v>58</v>
+      </c>
+      <c r="E66" t="s">
         <v>64</v>
-      </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-      <c r="D66" t="s">
-        <v>59</v>
-      </c>
-      <c r="E66" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E67" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>63</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E68" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E71" t="s">
         <v>66</v>
-      </c>
-      <c r="C71">
-        <v>2</v>
-      </c>
-      <c r="D71" t="s">
-        <v>59</v>
-      </c>
-      <c r="E71" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B72" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E72" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B73" t="s">
-        <v>139</v>
+        <v>65</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E73" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E74" t="s">
         <v>16</v>
@@ -2073,13 +2079,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
@@ -2087,16 +2093,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>68</v>
-      </c>
-      <c r="C76">
-        <v>2</v>
+        <v>138</v>
       </c>
       <c r="D76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2104,36 +2107,33 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B77" t="s">
-        <v>69</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="D77" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E77" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E78" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2141,16 +2141,16 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" t="s">
+        <v>69</v>
+      </c>
+      <c r="E79" t="s">
         <v>70</v>
-      </c>
-      <c r="E79" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2158,16 +2158,16 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
+        <v>69</v>
+      </c>
+      <c r="E80" t="s">
         <v>70</v>
-      </c>
-      <c r="E80" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,16 +2175,16 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E81" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2192,16 +2192,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E82" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2209,16 +2209,16 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2226,16 +2226,16 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E84" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2243,16 +2243,16 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E85" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2260,16 +2260,16 @@
         <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E86" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2277,47 +2277,47 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E87" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E88" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C89">
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E89" t="s">
         <v>4</v>
@@ -2325,16 +2325,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C90">
         <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E90" t="s">
         <v>4</v>
@@ -2342,13 +2342,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B91" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2359,10 +2362,13 @@
         <v>21</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2370,269 +2376,263 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B93" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D93" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E93" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B94" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D94" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E94" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B95" t="s">
+        <v>80</v>
+      </c>
+      <c r="D95" t="s">
         <v>81</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>82</v>
-      </c>
-      <c r="E95" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B96" t="s">
+        <v>80</v>
+      </c>
+      <c r="D96" t="s">
         <v>81</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>82</v>
-      </c>
-      <c r="E96" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B97" t="s">
-        <v>85</v>
-      </c>
-      <c r="C97">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="D97" t="s">
+        <v>81</v>
+      </c>
+      <c r="E97" t="s">
         <v>82</v>
-      </c>
-      <c r="E97" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="B98" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D98" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E98" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E99" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B100" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D100" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E100" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B101" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E101" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
+        <v>90</v>
+      </c>
+      <c r="D102" t="s">
         <v>91</v>
       </c>
-      <c r="D102" t="s">
-        <v>95</v>
-      </c>
       <c r="E102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="B103" t="s">
+        <v>84</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s">
         <v>91</v>
       </c>
-      <c r="D103" t="s">
-        <v>95</v>
-      </c>
       <c r="E103" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B104" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D104" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E104" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D105" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E105" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B106" t="s">
+        <v>95</v>
+      </c>
+      <c r="D106" t="s">
         <v>96</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E106" t="s">
         <v>97</v>
-      </c>
-      <c r="E106" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B107" t="s">
+        <v>95</v>
+      </c>
+      <c r="D107" t="s">
         <v>96</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" t="s">
         <v>97</v>
-      </c>
-      <c r="E107" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B108" t="s">
-        <v>99</v>
-      </c>
-      <c r="C108">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="D108" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E108" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="B109" t="s">
-        <v>101</v>
-      </c>
-      <c r="C109">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="D109" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E109" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B110" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E110" t="s">
         <v>4</v>
@@ -2640,16 +2640,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B111" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E111" t="s">
         <v>4</v>
@@ -2657,36 +2657,36 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="B112" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E112" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="B113" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C113">
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E113" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2694,16 +2694,16 @@
         <v>19</v>
       </c>
       <c r="B114" t="s">
+        <v>106</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114" t="s">
         <v>108</v>
       </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-      <c r="D114" t="s">
-        <v>109</v>
-      </c>
       <c r="E114" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2711,16 +2711,16 @@
         <v>21</v>
       </c>
       <c r="B115" t="s">
+        <v>106</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115" t="s">
         <v>108</v>
       </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-      <c r="D115" t="s">
-        <v>109</v>
-      </c>
       <c r="E115" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2734,10 +2734,10 @@
         <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E116" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2751,58 +2751,58 @@
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E117" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B118" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C118">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E118" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B119" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E119" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B120" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C120">
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E120" t="s">
         <v>11</v>
@@ -2810,16 +2810,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
@@ -2827,50 +2827,50 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B122" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C122">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E122" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E123" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E124" t="s">
         <v>4</v>
@@ -2878,16 +2878,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B125" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E125" t="s">
         <v>4</v>
@@ -2895,19 +2895,19 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B126" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E126" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,16 +2915,16 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E127" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2932,16 +2932,16 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E128" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,16 +2949,16 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E129" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2966,16 +2966,16 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E130" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2983,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E131" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3000,16 +3000,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E132" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E133" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
+        <v>117</v>
+      </c>
+      <c r="E134" t="s">
         <v>118</v>
-      </c>
-      <c r="E134" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,16 +3051,16 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
+        <v>117</v>
+      </c>
+      <c r="E135" t="s">
         <v>118</v>
-      </c>
-      <c r="E135" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,16 +3068,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E136" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3085,16 +3085,16 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E137" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -3102,16 +3102,16 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E138" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3119,61 +3119,64 @@
         <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E139" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E140" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E141" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B142" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E142" t="s">
         <v>4</v>
@@ -3181,13 +3184,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B143" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D143" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -3195,13 +3198,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B144" t="s">
-        <v>126</v>
+        <v>112</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E144" t="s">
         <v>4</v>
@@ -3209,16 +3215,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B145" t="s">
-        <v>124</v>
-      </c>
-      <c r="C145">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="D145" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E145" t="s">
         <v>4</v>
@@ -3226,16 +3229,13 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B146" t="s">
-        <v>129</v>
-      </c>
-      <c r="C146">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="D146" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E146" t="s">
         <v>4</v>
@@ -3243,16 +3243,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B147" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E147" t="s">
         <v>4</v>
@@ -3260,16 +3260,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B148" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C148">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
@@ -3277,16 +3277,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="B149" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D149" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E149" t="s">
         <v>4</v>
@@ -3294,16 +3294,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B150" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C150">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D150" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E150" t="s">
         <v>4</v>
@@ -3311,16 +3311,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B151" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="C151">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E151" t="s">
         <v>4</v>
@@ -3328,87 +3328,87 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B152" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C152">
         <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E152" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A153" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C153" s="1">
-        <v>2</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>150</v>
+      <c r="A153" t="s">
+        <v>85</v>
+      </c>
+      <c r="B153" t="s">
+        <v>112</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153" t="s">
+        <v>134</v>
+      </c>
+      <c r="E153" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A154" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C154" s="1">
-        <v>2</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>148</v>
+      <c r="A154" t="s">
+        <v>85</v>
+      </c>
+      <c r="B154" t="s">
+        <v>135</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+      <c r="D154" t="s">
+        <v>136</v>
+      </c>
+      <c r="E154" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C155" s="1">
         <v>2</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C156" s="1">
         <v>2</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3416,16 +3416,16 @@
         <v>17</v>
       </c>
       <c r="B157" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C157" s="1">
+        <v>2</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C157" s="1">
-        <v>2</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="E157" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -3433,16 +3433,50 @@
         <v>20</v>
       </c>
       <c r="B158" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C158" s="1">
+        <v>2</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C158" s="1">
-        <v>2</v>
-      </c>
-      <c r="D158" s="1" t="s">
+      <c r="E158" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C159" s="1">
+        <v>2</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E159" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E158" s="1" t="s">
-        <v>145</v>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C160" s="1">
+        <v>2</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (optionalAttendees) Add how to set in Appointment Organizer mode
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C3BBE1-7F22-449A-AF5A-62AC47D1A151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA066B6-ABEE-49C4-9841-E7FA611B171D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="162">
   <si>
     <t>Class</t>
   </si>
@@ -156,9 +156,6 @@
     <t>getOptionalAttendees</t>
   </si>
   <si>
-    <t>outlook-recipients-and-attendees-get-optional-attendees-appointment-organizer</t>
-  </si>
-  <si>
     <t>organizer</t>
   </si>
   <si>
@@ -511,6 +508,12 @@
   </si>
   <si>
     <t>setRequiredAttendees</t>
+  </si>
+  <si>
+    <t>setOptionalAttendees</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-optional-attendees-appointment-organizer</t>
   </si>
 </sst>
 </file>
@@ -586,8 +589,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E160" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E160" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E162" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E162" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -919,11 +922,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1249,7 +1252,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1257,16 +1260,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1280,27 +1283,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" t="s">
         <v>157</v>
-      </c>
-      <c r="E21" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" t="s">
         <v>157</v>
-      </c>
-      <c r="E22" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1311,7 +1314,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1319,16 +1322,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1342,27 +1345,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" t="s">
         <v>155</v>
-      </c>
-      <c r="E25" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>154</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>155</v>
-      </c>
-      <c r="E26" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1395,10 +1398,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1446,7 +1449,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>161</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1454,16 +1457,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>161</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1471,92 +1474,92 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>161</v>
       </c>
       <c r="E34" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>153</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="E35" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>83</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1564,75 +1567,75 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E40" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E41" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>158</v>
       </c>
       <c r="E42" t="s">
-        <v>52</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>153</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="E43" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>152</v>
+        <v>50</v>
       </c>
       <c r="E44" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1640,466 +1643,469 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="1"/>
-      <c r="D45" t="s">
-        <v>152</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>153</v>
-      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>154</v>
+      <c r="A46" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" t="s">
+        <v>83</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E46" t="s">
-        <v>153</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C47" s="1"/>
       <c r="D47" t="s">
-        <v>55</v>
-      </c>
-      <c r="E47" t="s">
-        <v>54</v>
+        <v>151</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" t="s">
-        <v>138</v>
+      <c r="A48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
+        <v>151</v>
       </c>
       <c r="E48" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>138</v>
+        <v>52</v>
       </c>
       <c r="D49" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E49" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D50" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" t="s">
         <v>58</v>
-      </c>
-      <c r="E50" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D51" t="s">
+        <v>57</v>
+      </c>
+      <c r="E51" t="s">
         <v>58</v>
-      </c>
-      <c r="E51" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" t="s">
         <v>57</v>
       </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>58</v>
-      </c>
-      <c r="E52" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D53" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" t="s">
         <v>58</v>
-      </c>
-      <c r="E53" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
       </c>
       <c r="D54" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" t="s">
         <v>58</v>
-      </c>
-      <c r="E54" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="D57" t="s">
         <v>57</v>
       </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57" t="s">
-        <v>58</v>
-      </c>
       <c r="E57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
+        <v>137</v>
+      </c>
+      <c r="D62" t="s">
         <v>57</v>
       </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="D62" t="s">
-        <v>58</v>
-      </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D63" t="s">
         <v>57</v>
       </c>
-      <c r="C63">
-        <v>2</v>
-      </c>
-      <c r="D63" t="s">
-        <v>58</v>
-      </c>
       <c r="E63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E64" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E65" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D66" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
+        <v>137</v>
+      </c>
+      <c r="D68" t="s">
+        <v>57</v>
+      </c>
+      <c r="E68" t="s">
         <v>63</v>
-      </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
-      <c r="D68" t="s">
-        <v>58</v>
-      </c>
-      <c r="E68" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E69" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>62</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E70" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D72" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B73" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" t="s">
+        <v>57</v>
+      </c>
+      <c r="E73" t="s">
         <v>65</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73" t="s">
-        <v>58</v>
-      </c>
-      <c r="E73" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E74" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B75" t="s">
-        <v>138</v>
+        <v>64</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E75" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D76" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2107,13 +2113,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D77" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E77" t="s">
         <v>16</v>
@@ -2121,16 +2127,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>67</v>
-      </c>
-      <c r="C78">
-        <v>2</v>
+        <v>137</v>
       </c>
       <c r="D78" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E78" t="s">
         <v>16</v>
@@ -2138,36 +2141,33 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>68</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="D79" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E79" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B80" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E80" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,16 +2175,16 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" t="s">
+        <v>68</v>
+      </c>
+      <c r="E81" t="s">
         <v>69</v>
-      </c>
-      <c r="E81" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2192,16 +2192,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" t="s">
+        <v>68</v>
+      </c>
+      <c r="E82" t="s">
         <v>69</v>
-      </c>
-      <c r="E82" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2209,16 +2209,16 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E83" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2226,16 +2226,16 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E84" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2243,16 +2243,16 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E85" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2260,16 +2260,16 @@
         <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2277,16 +2277,16 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E87" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -2294,16 +2294,16 @@
         <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E88" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2311,47 +2311,47 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="E89" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="E90" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C91">
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2359,16 +2359,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C92">
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2376,13 +2376,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B93" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
@@ -2393,10 +2396,13 @@
         <v>21</v>
       </c>
       <c r="B94" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
@@ -2404,269 +2410,263 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D95" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E95" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B96" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D96" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E96" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B97" t="s">
+        <v>79</v>
+      </c>
+      <c r="D97" t="s">
         <v>80</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>81</v>
-      </c>
-      <c r="E97" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B98" t="s">
+        <v>79</v>
+      </c>
+      <c r="D98" t="s">
         <v>80</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>81</v>
-      </c>
-      <c r="E98" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B99" t="s">
-        <v>84</v>
-      </c>
-      <c r="C99">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D99" t="s">
+        <v>80</v>
+      </c>
+      <c r="E99" t="s">
         <v>81</v>
-      </c>
-      <c r="E99" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B100" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D100" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E100" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B101" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E101" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D102" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E102" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C103">
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E103" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B104" t="s">
+        <v>89</v>
+      </c>
+      <c r="D104" t="s">
         <v>90</v>
       </c>
-      <c r="D104" t="s">
-        <v>94</v>
-      </c>
       <c r="E104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="B105" t="s">
+        <v>83</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s">
         <v>90</v>
       </c>
-      <c r="D105" t="s">
-        <v>94</v>
-      </c>
       <c r="E105" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B106" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D106" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E106" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B107" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D107" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E107" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B108" t="s">
+        <v>94</v>
+      </c>
+      <c r="D108" t="s">
         <v>95</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" t="s">
         <v>96</v>
-      </c>
-      <c r="E108" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B109" t="s">
+        <v>94</v>
+      </c>
+      <c r="D109" t="s">
         <v>95</v>
       </c>
-      <c r="D109" t="s">
+      <c r="E109" t="s">
         <v>96</v>
-      </c>
-      <c r="E109" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>98</v>
-      </c>
-      <c r="C110">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="D110" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E110" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B111" t="s">
-        <v>100</v>
-      </c>
-      <c r="C111">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="D111" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E111" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B112" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E112" t="s">
         <v>4</v>
@@ -2674,16 +2674,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B113" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C113">
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E113" t="s">
         <v>4</v>
@@ -2691,36 +2691,36 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B114" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E114" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B115" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C115">
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E115" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2728,16 +2728,16 @@
         <v>19</v>
       </c>
       <c r="B116" t="s">
+        <v>105</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
         <v>107</v>
       </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-      <c r="D116" t="s">
-        <v>108</v>
-      </c>
       <c r="E116" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2745,16 +2745,16 @@
         <v>21</v>
       </c>
       <c r="B117" t="s">
+        <v>105</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117" t="s">
         <v>107</v>
       </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
-      <c r="D117" t="s">
-        <v>108</v>
-      </c>
       <c r="E117" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2768,10 +2768,10 @@
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E118" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -2785,58 +2785,58 @@
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E119" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B120" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C120">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E120" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E121" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C122">
         <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E122" t="s">
         <v>11</v>
@@ -2844,16 +2844,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C123">
         <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E123" t="s">
         <v>11</v>
@@ -2861,50 +2861,50 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C124">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E124" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C125">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D125" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E125" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E126" t="s">
         <v>4</v>
@@ -2912,16 +2912,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E127" t="s">
         <v>4</v>
@@ -2929,19 +2929,19 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E128" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,16 +2949,16 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E129" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2966,16 +2966,16 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E130" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2983,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E131" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3000,16 +3000,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E132" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E133" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E134" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,16 +3051,16 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E135" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,16 +3068,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
+        <v>116</v>
+      </c>
+      <c r="E136" t="s">
         <v>117</v>
-      </c>
-      <c r="E136" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3085,16 +3085,16 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
+        <v>116</v>
+      </c>
+      <c r="E137" t="s">
         <v>117</v>
-      </c>
-      <c r="E137" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -3102,16 +3102,16 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E138" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3119,16 +3119,16 @@
         <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E139" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -3136,16 +3136,16 @@
         <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E140" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -3153,61 +3153,64 @@
         <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C141">
         <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E141" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="B142" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E142" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B143" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E143" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B144" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E144" t="s">
         <v>4</v>
@@ -3215,13 +3218,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B145" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D145" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E145" t="s">
         <v>4</v>
@@ -3229,13 +3232,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B146" t="s">
-        <v>125</v>
+        <v>111</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E146" t="s">
         <v>4</v>
@@ -3243,16 +3249,13 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B147" t="s">
-        <v>123</v>
-      </c>
-      <c r="C147">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="D147" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E147" t="s">
         <v>4</v>
@@ -3260,16 +3263,13 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B148" t="s">
-        <v>128</v>
-      </c>
-      <c r="C148">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="D148" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
@@ -3277,16 +3277,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B149" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E149" t="s">
         <v>4</v>
@@ -3294,16 +3294,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="B150" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C150">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E150" t="s">
         <v>4</v>
@@ -3311,16 +3311,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="B151" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D151" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E151" t="s">
         <v>4</v>
@@ -3328,16 +3328,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C152">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E152" t="s">
         <v>4</v>
@@ -3345,16 +3345,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B153" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="C153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E153" t="s">
         <v>4</v>
@@ -3362,87 +3362,87 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B154" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E154" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A155" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C155" s="1">
-        <v>2</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>149</v>
+      <c r="A155" t="s">
+        <v>84</v>
+      </c>
+      <c r="B155" t="s">
+        <v>111</v>
+      </c>
+      <c r="C155">
+        <v>2</v>
+      </c>
+      <c r="D155" t="s">
+        <v>133</v>
+      </c>
+      <c r="E155" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C156" s="1">
-        <v>2</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>147</v>
+      <c r="A156" t="s">
+        <v>84</v>
+      </c>
+      <c r="B156" t="s">
+        <v>134</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156" t="s">
+        <v>135</v>
+      </c>
+      <c r="E156" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C157" s="1">
         <v>2</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C158" s="1">
         <v>2</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -3450,16 +3450,16 @@
         <v>17</v>
       </c>
       <c r="B159" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C159" s="1">
+        <v>2</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C159" s="1">
-        <v>2</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="E159" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -3467,16 +3467,50 @@
         <v>20</v>
       </c>
       <c r="B160" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C160" s="1">
+        <v>2</v>
+      </c>
+      <c r="D160" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C160" s="1">
-        <v>2</v>
-      </c>
-      <c r="D160" s="1" t="s">
+      <c r="E160" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C161" s="1">
+        <v>2</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E161" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E160" s="1" t="s">
-        <v>144</v>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C162" s="1">
+        <v>2</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (optionalAttendees) Add how to set in Appointment Organizer mode (#421)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C3BBE1-7F22-449A-AF5A-62AC47D1A151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA066B6-ABEE-49C4-9841-E7FA611B171D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="162">
   <si>
     <t>Class</t>
   </si>
@@ -156,9 +156,6 @@
     <t>getOptionalAttendees</t>
   </si>
   <si>
-    <t>outlook-recipients-and-attendees-get-optional-attendees-appointment-organizer</t>
-  </si>
-  <si>
     <t>organizer</t>
   </si>
   <si>
@@ -511,6 +508,12 @@
   </si>
   <si>
     <t>setRequiredAttendees</t>
+  </si>
+  <si>
+    <t>setOptionalAttendees</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-optional-attendees-appointment-organizer</t>
   </si>
 </sst>
 </file>
@@ -586,8 +589,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E160" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E160" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E162" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E162" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -919,11 +922,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1249,7 +1252,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1257,16 +1260,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1280,27 +1283,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" t="s">
         <v>157</v>
-      </c>
-      <c r="E21" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" t="s">
         <v>157</v>
-      </c>
-      <c r="E22" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1311,7 +1314,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1319,16 +1322,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1342,27 +1345,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" t="s">
         <v>155</v>
-      </c>
-      <c r="E25" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>154</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>155</v>
-      </c>
-      <c r="E26" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1395,10 +1398,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1446,7 +1449,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>161</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1454,16 +1457,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>161</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1471,92 +1474,92 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>161</v>
       </c>
       <c r="E34" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>153</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="E35" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>83</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1564,75 +1567,75 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E40" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E41" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>158</v>
       </c>
       <c r="E42" t="s">
-        <v>52</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>153</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="E43" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>152</v>
+        <v>50</v>
       </c>
       <c r="E44" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1640,466 +1643,469 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="1"/>
-      <c r="D45" t="s">
-        <v>152</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>153</v>
-      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>154</v>
+      <c r="A46" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" t="s">
+        <v>83</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E46" t="s">
-        <v>153</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C47" s="1"/>
       <c r="D47" t="s">
-        <v>55</v>
-      </c>
-      <c r="E47" t="s">
-        <v>54</v>
+        <v>151</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" t="s">
-        <v>138</v>
+      <c r="A48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
+        <v>151</v>
       </c>
       <c r="E48" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>138</v>
+        <v>52</v>
       </c>
       <c r="D49" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E49" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D50" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" t="s">
         <v>58</v>
-      </c>
-      <c r="E50" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D51" t="s">
+        <v>57</v>
+      </c>
+      <c r="E51" t="s">
         <v>58</v>
-      </c>
-      <c r="E51" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" t="s">
         <v>57</v>
       </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>58</v>
-      </c>
-      <c r="E52" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D53" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" t="s">
         <v>58</v>
-      </c>
-      <c r="E53" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
       </c>
       <c r="D54" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" t="s">
         <v>58</v>
-      </c>
-      <c r="E54" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="D57" t="s">
         <v>57</v>
       </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57" t="s">
-        <v>58</v>
-      </c>
       <c r="E57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
+        <v>137</v>
+      </c>
+      <c r="D62" t="s">
         <v>57</v>
       </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="D62" t="s">
-        <v>58</v>
-      </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D63" t="s">
         <v>57</v>
       </c>
-      <c r="C63">
-        <v>2</v>
-      </c>
-      <c r="D63" t="s">
-        <v>58</v>
-      </c>
       <c r="E63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E64" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E65" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D66" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
+        <v>137</v>
+      </c>
+      <c r="D68" t="s">
+        <v>57</v>
+      </c>
+      <c r="E68" t="s">
         <v>63</v>
-      </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
-      <c r="D68" t="s">
-        <v>58</v>
-      </c>
-      <c r="E68" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E69" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>62</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E70" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D72" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B73" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" t="s">
+        <v>57</v>
+      </c>
+      <c r="E73" t="s">
         <v>65</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73" t="s">
-        <v>58</v>
-      </c>
-      <c r="E73" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E74" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B75" t="s">
-        <v>138</v>
+        <v>64</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E75" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D76" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2107,13 +2113,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D77" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E77" t="s">
         <v>16</v>
@@ -2121,16 +2127,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>67</v>
-      </c>
-      <c r="C78">
-        <v>2</v>
+        <v>137</v>
       </c>
       <c r="D78" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E78" t="s">
         <v>16</v>
@@ -2138,36 +2141,33 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>68</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="D79" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E79" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B80" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E80" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,16 +2175,16 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" t="s">
+        <v>68</v>
+      </c>
+      <c r="E81" t="s">
         <v>69</v>
-      </c>
-      <c r="E81" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2192,16 +2192,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" t="s">
+        <v>68</v>
+      </c>
+      <c r="E82" t="s">
         <v>69</v>
-      </c>
-      <c r="E82" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2209,16 +2209,16 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E83" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2226,16 +2226,16 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E84" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2243,16 +2243,16 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E85" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2260,16 +2260,16 @@
         <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2277,16 +2277,16 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E87" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -2294,16 +2294,16 @@
         <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E88" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2311,47 +2311,47 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="E89" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="E90" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C91">
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2359,16 +2359,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C92">
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2376,13 +2376,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B93" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
@@ -2393,10 +2396,13 @@
         <v>21</v>
       </c>
       <c r="B94" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
@@ -2404,269 +2410,263 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D95" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E95" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B96" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D96" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E96" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B97" t="s">
+        <v>79</v>
+      </c>
+      <c r="D97" t="s">
         <v>80</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>81</v>
-      </c>
-      <c r="E97" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B98" t="s">
+        <v>79</v>
+      </c>
+      <c r="D98" t="s">
         <v>80</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>81</v>
-      </c>
-      <c r="E98" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B99" t="s">
-        <v>84</v>
-      </c>
-      <c r="C99">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D99" t="s">
+        <v>80</v>
+      </c>
+      <c r="E99" t="s">
         <v>81</v>
-      </c>
-      <c r="E99" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B100" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D100" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E100" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B101" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E101" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D102" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E102" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C103">
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E103" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B104" t="s">
+        <v>89</v>
+      </c>
+      <c r="D104" t="s">
         <v>90</v>
       </c>
-      <c r="D104" t="s">
-        <v>94</v>
-      </c>
       <c r="E104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="B105" t="s">
+        <v>83</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s">
         <v>90</v>
       </c>
-      <c r="D105" t="s">
-        <v>94</v>
-      </c>
       <c r="E105" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B106" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D106" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E106" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B107" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D107" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E107" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B108" t="s">
+        <v>94</v>
+      </c>
+      <c r="D108" t="s">
         <v>95</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" t="s">
         <v>96</v>
-      </c>
-      <c r="E108" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B109" t="s">
+        <v>94</v>
+      </c>
+      <c r="D109" t="s">
         <v>95</v>
       </c>
-      <c r="D109" t="s">
+      <c r="E109" t="s">
         <v>96</v>
-      </c>
-      <c r="E109" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>98</v>
-      </c>
-      <c r="C110">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="D110" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E110" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B111" t="s">
-        <v>100</v>
-      </c>
-      <c r="C111">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="D111" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E111" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B112" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E112" t="s">
         <v>4</v>
@@ -2674,16 +2674,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B113" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C113">
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E113" t="s">
         <v>4</v>
@@ -2691,36 +2691,36 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B114" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E114" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B115" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C115">
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E115" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2728,16 +2728,16 @@
         <v>19</v>
       </c>
       <c r="B116" t="s">
+        <v>105</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
         <v>107</v>
       </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-      <c r="D116" t="s">
-        <v>108</v>
-      </c>
       <c r="E116" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2745,16 +2745,16 @@
         <v>21</v>
       </c>
       <c r="B117" t="s">
+        <v>105</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117" t="s">
         <v>107</v>
       </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
-      <c r="D117" t="s">
-        <v>108</v>
-      </c>
       <c r="E117" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2768,10 +2768,10 @@
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E118" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -2785,58 +2785,58 @@
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E119" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B120" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C120">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E120" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E121" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C122">
         <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E122" t="s">
         <v>11</v>
@@ -2844,16 +2844,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C123">
         <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E123" t="s">
         <v>11</v>
@@ -2861,50 +2861,50 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C124">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E124" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C125">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D125" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E125" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E126" t="s">
         <v>4</v>
@@ -2912,16 +2912,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E127" t="s">
         <v>4</v>
@@ -2929,19 +2929,19 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E128" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,16 +2949,16 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E129" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2966,16 +2966,16 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E130" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2983,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E131" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3000,16 +3000,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E132" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E133" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E134" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,16 +3051,16 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E135" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,16 +3068,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
+        <v>116</v>
+      </c>
+      <c r="E136" t="s">
         <v>117</v>
-      </c>
-      <c r="E136" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3085,16 +3085,16 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
+        <v>116</v>
+      </c>
+      <c r="E137" t="s">
         <v>117</v>
-      </c>
-      <c r="E137" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -3102,16 +3102,16 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E138" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3119,16 +3119,16 @@
         <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E139" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -3136,16 +3136,16 @@
         <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E140" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -3153,61 +3153,64 @@
         <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C141">
         <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E141" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="B142" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E142" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B143" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E143" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B144" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E144" t="s">
         <v>4</v>
@@ -3215,13 +3218,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B145" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D145" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E145" t="s">
         <v>4</v>
@@ -3229,13 +3232,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B146" t="s">
-        <v>125</v>
+        <v>111</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E146" t="s">
         <v>4</v>
@@ -3243,16 +3249,13 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B147" t="s">
-        <v>123</v>
-      </c>
-      <c r="C147">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="D147" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E147" t="s">
         <v>4</v>
@@ -3260,16 +3263,13 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B148" t="s">
-        <v>128</v>
-      </c>
-      <c r="C148">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="D148" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
@@ -3277,16 +3277,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B149" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E149" t="s">
         <v>4</v>
@@ -3294,16 +3294,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="B150" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C150">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E150" t="s">
         <v>4</v>
@@ -3311,16 +3311,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="B151" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D151" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E151" t="s">
         <v>4</v>
@@ -3328,16 +3328,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C152">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E152" t="s">
         <v>4</v>
@@ -3345,16 +3345,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B153" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="C153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E153" t="s">
         <v>4</v>
@@ -3362,87 +3362,87 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B154" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E154" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A155" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C155" s="1">
-        <v>2</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>149</v>
+      <c r="A155" t="s">
+        <v>84</v>
+      </c>
+      <c r="B155" t="s">
+        <v>111</v>
+      </c>
+      <c r="C155">
+        <v>2</v>
+      </c>
+      <c r="D155" t="s">
+        <v>133</v>
+      </c>
+      <c r="E155" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C156" s="1">
-        <v>2</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>147</v>
+      <c r="A156" t="s">
+        <v>84</v>
+      </c>
+      <c r="B156" t="s">
+        <v>134</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156" t="s">
+        <v>135</v>
+      </c>
+      <c r="E156" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C157" s="1">
         <v>2</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C158" s="1">
         <v>2</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -3450,16 +3450,16 @@
         <v>17</v>
       </c>
       <c r="B159" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C159" s="1">
+        <v>2</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C159" s="1">
-        <v>2</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="E159" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -3467,16 +3467,50 @@
         <v>20</v>
       </c>
       <c r="B160" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C160" s="1">
+        <v>2</v>
+      </c>
+      <c r="D160" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C160" s="1">
-        <v>2</v>
-      </c>
-      <c r="D160" s="1" t="s">
+      <c r="E160" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C161" s="1">
+        <v>2</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E161" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E160" s="1" t="s">
-        <v>144</v>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C162" s="1">
+        <v>2</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (master categories) Add how to add and remove
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA066B6-ABEE-49C4-9841-E7FA611B171D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04A9757-9955-4589-9C11-9AB88D60E3BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="164">
   <si>
     <t>Class</t>
   </si>
@@ -288,9 +288,6 @@
     <t>masterCategories</t>
   </si>
   <si>
-    <t>outlook-categories-get-master-categories</t>
-  </si>
-  <si>
     <t>getMasterCategories</t>
   </si>
   <si>
@@ -514,6 +511,15 @@
   </si>
   <si>
     <t>outlook-recipients-and-attendees-get-set-optional-attendees-appointment-organizer</t>
+  </si>
+  <si>
+    <t>addMasterCategories</t>
+  </si>
+  <si>
+    <t>removeMasterCategories</t>
+  </si>
+  <si>
+    <t>outlook-categories-work-with-master-categories</t>
   </si>
 </sst>
 </file>
@@ -589,8 +595,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E162" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E162" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E166" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E166" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -922,11 +928,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33:D35"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D103" sqref="D103:D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,7 +1258,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1260,7 +1266,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
         <v>83</v>
@@ -1269,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1283,27 +1289,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" t="s">
         <v>156</v>
-      </c>
-      <c r="E21" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" t="s">
         <v>156</v>
-      </c>
-      <c r="E22" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1314,7 +1320,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1322,7 +1328,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
         <v>83</v>
@@ -1331,7 +1337,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1345,27 +1351,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" t="s">
         <v>154</v>
-      </c>
-      <c r="E25" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>153</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>154</v>
-      </c>
-      <c r="E26" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1398,7 +1404,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
         <v>83</v>
@@ -1449,7 +1455,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1457,7 +1463,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
         <v>83</v>
@@ -1466,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1480,27 +1486,27 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1533,7 +1539,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B38" t="s">
         <v>83</v>
@@ -1570,7 +1576,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
@@ -1578,7 +1584,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
         <v>83</v>
@@ -1587,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
@@ -1601,27 +1607,27 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" t="s">
         <v>158</v>
-      </c>
-      <c r="E42" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" t="s">
         <v>158</v>
-      </c>
-      <c r="E43" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1646,7 +1652,7 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
@@ -1654,7 +1660,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
         <v>83</v>
@@ -1663,7 +1669,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -1678,27 +1684,27 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" t="s">
         <v>151</v>
-      </c>
-      <c r="E48" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1720,7 +1726,7 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1734,7 +1740,7 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1748,7 +1754,7 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1762,7 +1768,7 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1793,7 +1799,7 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1807,7 +1813,7 @@
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -1821,7 +1827,7 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -1835,7 +1841,7 @@
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -1866,7 +1872,7 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D60" t="s">
         <v>57</v>
@@ -1880,7 +1886,7 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D61" t="s">
         <v>57</v>
@@ -1894,7 +1900,7 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D62" t="s">
         <v>57</v>
@@ -1908,7 +1914,7 @@
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D63" t="s">
         <v>57</v>
@@ -1956,7 +1962,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D66" t="s">
         <v>57</v>
@@ -1970,7 +1976,7 @@
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D67" t="s">
         <v>57</v>
@@ -1984,7 +1990,7 @@
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
         <v>57</v>
@@ -1998,7 +2004,7 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D69" t="s">
         <v>57</v>
@@ -2029,7 +2035,7 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D71" t="s">
         <v>57</v>
@@ -2043,7 +2049,7 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D72" t="s">
         <v>57</v>
@@ -2057,7 +2063,7 @@
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D73" t="s">
         <v>57</v>
@@ -2071,7 +2077,7 @@
         <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D74" t="s">
         <v>57</v>
@@ -2102,7 +2108,7 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D76" t="s">
         <v>57</v>
@@ -2116,7 +2122,7 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D77" t="s">
         <v>57</v>
@@ -2130,7 +2136,7 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -2144,7 +2150,7 @@
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D79" t="s">
         <v>57</v>
@@ -2351,7 +2357,7 @@
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2368,7 +2374,7 @@
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2385,7 +2391,7 @@
         <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
@@ -2402,7 +2408,7 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
@@ -2517,15 +2523,15 @@
         <v>85</v>
       </c>
       <c r="D102" t="s">
+        <v>163</v>
+      </c>
+      <c r="E102" t="s">
         <v>86</v>
-      </c>
-      <c r="E102" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B103" t="s">
         <v>83</v>
@@ -2534,69 +2540,72 @@
         <v>2</v>
       </c>
       <c r="D103" t="s">
+        <v>163</v>
+      </c>
+      <c r="E103" t="s">
         <v>86</v>
-      </c>
-      <c r="E103" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B104" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D104" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="E104" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B105" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C105">
         <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="E105" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B106" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D106" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="E106" t="s">
-        <v>91</v>
+        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="B107" t="s">
-        <v>89</v>
+        <v>66</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="E107" t="s">
-        <v>91</v>
+        <v>162</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2604,41 +2613,44 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D108" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E108" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>83</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E109" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B110" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D110" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E110" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2646,149 +2658,137 @@
         <v>21</v>
       </c>
       <c r="B111" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D111" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E111" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>97</v>
-      </c>
-      <c r="C112">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D112" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E112" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B113" t="s">
-        <v>99</v>
-      </c>
-      <c r="C113">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D113" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E113" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B114" t="s">
-        <v>101</v>
-      </c>
-      <c r="C114">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D114" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E114" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B115" t="s">
-        <v>103</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D115" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E115" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B116" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C116">
         <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E116" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B117" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C117">
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E117" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B118" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C118">
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E118" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B119" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E119" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2796,16 +2796,16 @@
         <v>19</v>
       </c>
       <c r="B120" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E120" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2813,67 +2813,67 @@
         <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E121" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E122" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E123" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C124">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E124" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2881,16 +2881,16 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E125" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2898,16 +2898,16 @@
         <v>17</v>
       </c>
       <c r="B126" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C126">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D126" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E126" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,16 +2915,16 @@
         <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D127" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E127" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2932,16 +2932,16 @@
         <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D128" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E128" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,67 +2949,67 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C129">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D129" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E129" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B130" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E130" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B131" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E131" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B132" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E132" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E133" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E134" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,16 +3051,16 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E135" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,16 +3068,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E136" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3085,16 +3085,16 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E137" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -3102,16 +3102,16 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E138" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3119,16 +3119,16 @@
         <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E139" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -3136,16 +3136,16 @@
         <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E140" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -3153,16 +3153,16 @@
         <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C141">
         <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E141" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -3170,16 +3170,16 @@
         <v>19</v>
       </c>
       <c r="B142" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E142" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -3187,78 +3187,84 @@
         <v>21</v>
       </c>
       <c r="B143" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C143">
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E143" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E144" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>124</v>
+        <v>118</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E145" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E146" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E147" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3266,10 +3272,13 @@
         <v>84</v>
       </c>
       <c r="B148" t="s">
-        <v>124</v>
+        <v>121</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
@@ -3280,13 +3289,10 @@
         <v>84</v>
       </c>
       <c r="B149" t="s">
+        <v>123</v>
+      </c>
+      <c r="D149" t="s">
         <v>122</v>
-      </c>
-      <c r="C149">
-        <v>1</v>
-      </c>
-      <c r="D149" t="s">
-        <v>126</v>
       </c>
       <c r="E149" t="s">
         <v>4</v>
@@ -3297,13 +3303,13 @@
         <v>84</v>
       </c>
       <c r="B150" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E150" t="s">
         <v>4</v>
@@ -3311,16 +3317,13 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B151" t="s">
-        <v>128</v>
-      </c>
-      <c r="C151">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="D151" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E151" t="s">
         <v>4</v>
@@ -3328,16 +3331,13 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="B152" t="s">
-        <v>128</v>
-      </c>
-      <c r="C152">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="D152" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E152" t="s">
         <v>4</v>
@@ -3348,13 +3348,13 @@
         <v>84</v>
       </c>
       <c r="B153" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C153">
         <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E153" t="s">
         <v>4</v>
@@ -3365,13 +3365,13 @@
         <v>84</v>
       </c>
       <c r="B154" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E154" t="s">
         <v>4</v>
@@ -3379,16 +3379,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B155" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="C155">
         <v>2</v>
       </c>
       <c r="D155" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E155" t="s">
         <v>4</v>
@@ -3396,121 +3396,189 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C156">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D156" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E156" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A157" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C157" s="1">
-        <v>2</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>148</v>
+      <c r="A157" t="s">
+        <v>84</v>
+      </c>
+      <c r="B157" t="s">
+        <v>129</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+      <c r="D157" t="s">
+        <v>130</v>
+      </c>
+      <c r="E157" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A158" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C158" s="1">
-        <v>2</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>146</v>
+      <c r="A158" t="s">
+        <v>84</v>
+      </c>
+      <c r="B158" t="s">
+        <v>129</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158" t="s">
+        <v>131</v>
+      </c>
+      <c r="E158" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A159" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C159" s="1">
-        <v>2</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>150</v>
+      <c r="A159" t="s">
+        <v>84</v>
+      </c>
+      <c r="B159" t="s">
+        <v>110</v>
+      </c>
+      <c r="C159">
+        <v>2</v>
+      </c>
+      <c r="D159" t="s">
+        <v>132</v>
+      </c>
+      <c r="E159" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A160" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C160" s="1">
-        <v>2</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>150</v>
+      <c r="A160" t="s">
+        <v>84</v>
+      </c>
+      <c r="B160" t="s">
+        <v>133</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+      <c r="D160" t="s">
+        <v>134</v>
+      </c>
+      <c r="E160" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B161" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C161" s="1">
+        <v>2</v>
+      </c>
+      <c r="D161" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C161" s="1">
-        <v>2</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="E161" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C162" s="1">
+        <v>2</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C163" s="1">
+        <v>2</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B164" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C164" s="1">
+        <v>2</v>
+      </c>
+      <c r="D164" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C162" s="1">
-        <v>2</v>
-      </c>
-      <c r="D162" s="1" t="s">
+      <c r="E164" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C165" s="1">
+        <v>2</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E165" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E162" s="1" t="s">
-        <v>143</v>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C166" s="1">
+        <v>2</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (master categories) Add how to add and remove (#422)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA066B6-ABEE-49C4-9841-E7FA611B171D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04A9757-9955-4589-9C11-9AB88D60E3BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="164">
   <si>
     <t>Class</t>
   </si>
@@ -288,9 +288,6 @@
     <t>masterCategories</t>
   </si>
   <si>
-    <t>outlook-categories-get-master-categories</t>
-  </si>
-  <si>
     <t>getMasterCategories</t>
   </si>
   <si>
@@ -514,6 +511,15 @@
   </si>
   <si>
     <t>outlook-recipients-and-attendees-get-set-optional-attendees-appointment-organizer</t>
+  </si>
+  <si>
+    <t>addMasterCategories</t>
+  </si>
+  <si>
+    <t>removeMasterCategories</t>
+  </si>
+  <si>
+    <t>outlook-categories-work-with-master-categories</t>
   </si>
 </sst>
 </file>
@@ -589,8 +595,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E162" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E162" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E166" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E166" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -922,11 +928,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33:D35"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D103" sqref="D103:D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,7 +1258,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1260,7 +1266,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
         <v>83</v>
@@ -1269,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1283,27 +1289,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" t="s">
         <v>156</v>
-      </c>
-      <c r="E21" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" t="s">
         <v>156</v>
-      </c>
-      <c r="E22" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1314,7 +1320,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1322,7 +1328,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
         <v>83</v>
@@ -1331,7 +1337,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1345,27 +1351,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" t="s">
         <v>154</v>
-      </c>
-      <c r="E25" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>153</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>154</v>
-      </c>
-      <c r="E26" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1398,7 +1404,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
         <v>83</v>
@@ -1449,7 +1455,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1457,7 +1463,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
         <v>83</v>
@@ -1466,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1480,27 +1486,27 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1533,7 +1539,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B38" t="s">
         <v>83</v>
@@ -1570,7 +1576,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
@@ -1578,7 +1584,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
         <v>83</v>
@@ -1587,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
@@ -1601,27 +1607,27 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" t="s">
         <v>158</v>
-      </c>
-      <c r="E42" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" t="s">
         <v>158</v>
-      </c>
-      <c r="E43" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1646,7 +1652,7 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
@@ -1654,7 +1660,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
         <v>83</v>
@@ -1663,7 +1669,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -1678,27 +1684,27 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" t="s">
         <v>151</v>
-      </c>
-      <c r="E48" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1720,7 +1726,7 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1734,7 +1740,7 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1748,7 +1754,7 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1762,7 +1768,7 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1793,7 +1799,7 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1807,7 +1813,7 @@
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -1821,7 +1827,7 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -1835,7 +1841,7 @@
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -1866,7 +1872,7 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D60" t="s">
         <v>57</v>
@@ -1880,7 +1886,7 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D61" t="s">
         <v>57</v>
@@ -1894,7 +1900,7 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D62" t="s">
         <v>57</v>
@@ -1908,7 +1914,7 @@
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D63" t="s">
         <v>57</v>
@@ -1956,7 +1962,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D66" t="s">
         <v>57</v>
@@ -1970,7 +1976,7 @@
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D67" t="s">
         <v>57</v>
@@ -1984,7 +1990,7 @@
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
         <v>57</v>
@@ -1998,7 +2004,7 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D69" t="s">
         <v>57</v>
@@ -2029,7 +2035,7 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D71" t="s">
         <v>57</v>
@@ -2043,7 +2049,7 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D72" t="s">
         <v>57</v>
@@ -2057,7 +2063,7 @@
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D73" t="s">
         <v>57</v>
@@ -2071,7 +2077,7 @@
         <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D74" t="s">
         <v>57</v>
@@ -2102,7 +2108,7 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D76" t="s">
         <v>57</v>
@@ -2116,7 +2122,7 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D77" t="s">
         <v>57</v>
@@ -2130,7 +2136,7 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -2144,7 +2150,7 @@
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D79" t="s">
         <v>57</v>
@@ -2351,7 +2357,7 @@
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2368,7 +2374,7 @@
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2385,7 +2391,7 @@
         <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
@@ -2402,7 +2408,7 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
@@ -2517,15 +2523,15 @@
         <v>85</v>
       </c>
       <c r="D102" t="s">
+        <v>163</v>
+      </c>
+      <c r="E102" t="s">
         <v>86</v>
-      </c>
-      <c r="E102" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B103" t="s">
         <v>83</v>
@@ -2534,69 +2540,72 @@
         <v>2</v>
       </c>
       <c r="D103" t="s">
+        <v>163</v>
+      </c>
+      <c r="E103" t="s">
         <v>86</v>
-      </c>
-      <c r="E103" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B104" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D104" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="E104" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B105" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C105">
         <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="E105" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B106" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D106" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="E106" t="s">
-        <v>91</v>
+        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="B107" t="s">
-        <v>89</v>
+        <v>66</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="E107" t="s">
-        <v>91</v>
+        <v>162</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2604,41 +2613,44 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D108" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E108" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>83</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E109" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B110" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D110" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E110" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2646,149 +2658,137 @@
         <v>21</v>
       </c>
       <c r="B111" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D111" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E111" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>97</v>
-      </c>
-      <c r="C112">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D112" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E112" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B113" t="s">
-        <v>99</v>
-      </c>
-      <c r="C113">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D113" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E113" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B114" t="s">
-        <v>101</v>
-      </c>
-      <c r="C114">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D114" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E114" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B115" t="s">
-        <v>103</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D115" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E115" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B116" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C116">
         <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E116" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B117" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C117">
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E117" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B118" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C118">
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E118" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B119" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E119" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2796,16 +2796,16 @@
         <v>19</v>
       </c>
       <c r="B120" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E120" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2813,67 +2813,67 @@
         <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E121" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E122" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E123" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C124">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E124" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2881,16 +2881,16 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E125" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2898,16 +2898,16 @@
         <v>17</v>
       </c>
       <c r="B126" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C126">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D126" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E126" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,16 +2915,16 @@
         <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D127" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E127" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2932,16 +2932,16 @@
         <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D128" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E128" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,67 +2949,67 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C129">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D129" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E129" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B130" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E130" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B131" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E131" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B132" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E132" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +3017,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E133" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3034,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E134" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,16 +3051,16 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E135" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,16 +3068,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E136" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3085,16 +3085,16 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E137" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -3102,16 +3102,16 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E138" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3119,16 +3119,16 @@
         <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E139" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -3136,16 +3136,16 @@
         <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E140" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -3153,16 +3153,16 @@
         <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C141">
         <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E141" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -3170,16 +3170,16 @@
         <v>19</v>
       </c>
       <c r="B142" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E142" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -3187,78 +3187,84 @@
         <v>21</v>
       </c>
       <c r="B143" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C143">
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E143" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E144" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>124</v>
+        <v>118</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E145" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E146" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E147" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3266,10 +3272,13 @@
         <v>84</v>
       </c>
       <c r="B148" t="s">
-        <v>124</v>
+        <v>121</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
@@ -3280,13 +3289,10 @@
         <v>84</v>
       </c>
       <c r="B149" t="s">
+        <v>123</v>
+      </c>
+      <c r="D149" t="s">
         <v>122</v>
-      </c>
-      <c r="C149">
-        <v>1</v>
-      </c>
-      <c r="D149" t="s">
-        <v>126</v>
       </c>
       <c r="E149" t="s">
         <v>4</v>
@@ -3297,13 +3303,13 @@
         <v>84</v>
       </c>
       <c r="B150" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E150" t="s">
         <v>4</v>
@@ -3311,16 +3317,13 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B151" t="s">
-        <v>128</v>
-      </c>
-      <c r="C151">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="D151" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E151" t="s">
         <v>4</v>
@@ -3328,16 +3331,13 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="B152" t="s">
-        <v>128</v>
-      </c>
-      <c r="C152">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="D152" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E152" t="s">
         <v>4</v>
@@ -3348,13 +3348,13 @@
         <v>84</v>
       </c>
       <c r="B153" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C153">
         <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E153" t="s">
         <v>4</v>
@@ -3365,13 +3365,13 @@
         <v>84</v>
       </c>
       <c r="B154" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E154" t="s">
         <v>4</v>
@@ -3379,16 +3379,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B155" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="C155">
         <v>2</v>
       </c>
       <c r="D155" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E155" t="s">
         <v>4</v>
@@ -3396,121 +3396,189 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C156">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D156" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E156" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A157" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C157" s="1">
-        <v>2</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>148</v>
+      <c r="A157" t="s">
+        <v>84</v>
+      </c>
+      <c r="B157" t="s">
+        <v>129</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+      <c r="D157" t="s">
+        <v>130</v>
+      </c>
+      <c r="E157" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A158" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C158" s="1">
-        <v>2</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>146</v>
+      <c r="A158" t="s">
+        <v>84</v>
+      </c>
+      <c r="B158" t="s">
+        <v>129</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158" t="s">
+        <v>131</v>
+      </c>
+      <c r="E158" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A159" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C159" s="1">
-        <v>2</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>150</v>
+      <c r="A159" t="s">
+        <v>84</v>
+      </c>
+      <c r="B159" t="s">
+        <v>110</v>
+      </c>
+      <c r="C159">
+        <v>2</v>
+      </c>
+      <c r="D159" t="s">
+        <v>132</v>
+      </c>
+      <c r="E159" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A160" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C160" s="1">
-        <v>2</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>150</v>
+      <c r="A160" t="s">
+        <v>84</v>
+      </c>
+      <c r="B160" t="s">
+        <v>133</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+      <c r="D160" t="s">
+        <v>134</v>
+      </c>
+      <c r="E160" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B161" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C161" s="1">
+        <v>2</v>
+      </c>
+      <c r="D161" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C161" s="1">
-        <v>2</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="E161" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C162" s="1">
+        <v>2</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C163" s="1">
+        <v>2</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B164" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C164" s="1">
+        <v>2</v>
+      </c>
+      <c r="D164" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C162" s="1">
-        <v>2</v>
-      </c>
-      <c r="D162" s="1" t="s">
+      <c r="E164" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C165" s="1">
+        <v>2</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E165" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E162" s="1" t="s">
-        <v>143</v>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C166" s="1">
+        <v>2</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (categories) Add how to add and remove categories from item
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04A9757-9955-4589-9C11-9AB88D60E3BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E448235A-FC74-488F-A89C-A6C89812F18A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="166">
   <si>
     <t>Class</t>
   </si>
@@ -270,9 +270,6 @@
     <t>categories</t>
   </si>
   <si>
-    <t>outlook-categories-get-categories</t>
-  </si>
-  <si>
     <t>getCategories</t>
   </si>
   <si>
@@ -520,6 +517,15 @@
   </si>
   <si>
     <t>outlook-categories-work-with-master-categories</t>
+  </si>
+  <si>
+    <t>addCategories</t>
+  </si>
+  <si>
+    <t>removeCategories</t>
+  </si>
+  <si>
+    <t>outlook-categories-work-with-categories</t>
   </si>
 </sst>
 </file>
@@ -595,8 +601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E166" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E166" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E176" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E176" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -928,11 +934,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D103" sqref="D103:D107"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98:D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,7 +1264,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1266,16 +1272,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1289,27 +1295,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" t="s">
         <v>155</v>
-      </c>
-      <c r="E21" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" t="s">
         <v>155</v>
-      </c>
-      <c r="E22" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1320,7 +1326,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1328,16 +1334,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1351,27 +1357,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" t="s">
         <v>153</v>
-      </c>
-      <c r="E25" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>152</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>153</v>
-      </c>
-      <c r="E26" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1404,10 +1410,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1455,7 +1461,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1463,16 +1469,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1486,27 +1492,27 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1539,10 +1545,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -1576,7 +1582,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
@@ -1584,16 +1590,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
@@ -1607,27 +1613,27 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E42" t="s">
         <v>157</v>
-      </c>
-      <c r="E42" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
+        <v>156</v>
+      </c>
+      <c r="E43" t="s">
         <v>157</v>
-      </c>
-      <c r="E43" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1652,7 +1658,7 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
@@ -1660,16 +1666,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -1684,27 +1690,27 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>149</v>
+      </c>
+      <c r="E48" t="s">
         <v>150</v>
-      </c>
-      <c r="E48" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1726,7 +1732,7 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1740,7 +1746,7 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1754,7 +1760,7 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1768,7 +1774,7 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1799,7 +1805,7 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1813,7 +1819,7 @@
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -1827,7 +1833,7 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -1841,7 +1847,7 @@
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -1872,7 +1878,7 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D60" t="s">
         <v>57</v>
@@ -1886,7 +1892,7 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D61" t="s">
         <v>57</v>
@@ -1900,7 +1906,7 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D62" t="s">
         <v>57</v>
@@ -1914,7 +1920,7 @@
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D63" t="s">
         <v>57</v>
@@ -1962,7 +1968,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D66" t="s">
         <v>57</v>
@@ -1976,7 +1982,7 @@
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D67" t="s">
         <v>57</v>
@@ -1990,7 +1996,7 @@
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D68" t="s">
         <v>57</v>
@@ -2004,7 +2010,7 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D69" t="s">
         <v>57</v>
@@ -2035,7 +2041,7 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D71" t="s">
         <v>57</v>
@@ -2049,7 +2055,7 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D72" t="s">
         <v>57</v>
@@ -2063,7 +2069,7 @@
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D73" t="s">
         <v>57</v>
@@ -2077,7 +2083,7 @@
         <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D74" t="s">
         <v>57</v>
@@ -2108,7 +2114,7 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D76" t="s">
         <v>57</v>
@@ -2122,7 +2128,7 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D77" t="s">
         <v>57</v>
@@ -2136,7 +2142,7 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -2150,7 +2156,7 @@
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D79" t="s">
         <v>57</v>
@@ -2357,7 +2363,7 @@
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2374,7 +2380,7 @@
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2391,7 +2397,7 @@
         <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
@@ -2408,7 +2414,7 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
@@ -2450,10 +2456,10 @@
         <v>79</v>
       </c>
       <c r="D97" t="s">
+        <v>165</v>
+      </c>
+      <c r="E97" t="s">
         <v>80</v>
-      </c>
-      <c r="E97" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -2464,10 +2470,10 @@
         <v>79</v>
       </c>
       <c r="D98" t="s">
+        <v>165</v>
+      </c>
+      <c r="E98" t="s">
         <v>80</v>
-      </c>
-      <c r="E98" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -2478,10 +2484,10 @@
         <v>79</v>
       </c>
       <c r="D99" t="s">
+        <v>165</v>
+      </c>
+      <c r="E99" t="s">
         <v>80</v>
-      </c>
-      <c r="E99" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -2492,303 +2498,297 @@
         <v>79</v>
       </c>
       <c r="D100" t="s">
+        <v>165</v>
+      </c>
+      <c r="E100" t="s">
         <v>80</v>
-      </c>
-      <c r="E100" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>81</v>
+      </c>
+      <c r="B101" t="s">
         <v>82</v>
       </c>
-      <c r="B101" t="s">
-        <v>83</v>
-      </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" t="s">
+        <v>165</v>
+      </c>
+      <c r="E101" t="s">
         <v>80</v>
-      </c>
-      <c r="E101" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D102" t="s">
+        <v>165</v>
+      </c>
+      <c r="E102" t="s">
         <v>163</v>
-      </c>
-      <c r="E102" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>83</v>
-      </c>
-      <c r="C103">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D103" t="s">
+        <v>165</v>
+      </c>
+      <c r="E103" t="s">
         <v>163</v>
-      </c>
-      <c r="E103" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B104" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D104" t="s">
+        <v>165</v>
+      </c>
+      <c r="E104" t="s">
         <v>163</v>
-      </c>
-      <c r="E104" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>56</v>
-      </c>
-      <c r="C105">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D105" t="s">
+        <v>165</v>
+      </c>
+      <c r="E105" t="s">
         <v>163</v>
-      </c>
-      <c r="E105" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B106" t="s">
-        <v>85</v>
+        <v>56</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
       </c>
       <c r="D106" t="s">
+        <v>165</v>
+      </c>
+      <c r="E106" t="s">
         <v>163</v>
-      </c>
-      <c r="E106" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>66</v>
-      </c>
-      <c r="C107">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D107" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E107" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B108" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D108" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="E108" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="B109" t="s">
-        <v>83</v>
-      </c>
-      <c r="C109">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D109" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="E109" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B110" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D110" t="s">
-        <v>92</v>
+        <v>165</v>
       </c>
       <c r="E110" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B111" t="s">
-        <v>88</v>
+        <v>66</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>92</v>
+        <v>165</v>
       </c>
       <c r="E111" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B112" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D112" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E112" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="B113" t="s">
-        <v>93</v>
+        <v>82</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E113" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B114" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E114" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B115" t="s">
-        <v>93</v>
+        <v>56</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E115" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>83</v>
+      </c>
+      <c r="B116" t="s">
         <v>84</v>
       </c>
-      <c r="B116" t="s">
-        <v>96</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
       <c r="D116" t="s">
-        <v>97</v>
+        <v>162</v>
       </c>
       <c r="E116" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B117" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="E117" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>100</v>
-      </c>
-      <c r="C118">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D118" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E118" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B119" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E119" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2796,16 +2796,13 @@
         <v>19</v>
       </c>
       <c r="B120" t="s">
-        <v>104</v>
-      </c>
-      <c r="C120">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E120" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2813,67 +2810,55 @@
         <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>104</v>
-      </c>
-      <c r="C121">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D121" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E121" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B122" t="s">
-        <v>105</v>
-      </c>
-      <c r="C122">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D122" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E122" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>105</v>
-      </c>
-      <c r="C123">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D123" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E123" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B124" t="s">
-        <v>104</v>
-      </c>
-      <c r="C124">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D124" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E124" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2881,135 +2866,132 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>104</v>
-      </c>
-      <c r="C125">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D125" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E125" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B126" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E126" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B127" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E127" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B128" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C128">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E128" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C129">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E129" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E130" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E131" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E132" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +2999,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E133" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3016,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E134" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,67 +3033,67 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E135" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E136" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B137" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E137" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B138" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C138">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E138" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3119,67 +3101,67 @@
         <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C139">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E139" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E140" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B141" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C141">
         <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E141" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B142" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E142" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -3187,16 +3169,16 @@
         <v>21</v>
       </c>
       <c r="B143" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C143">
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E143" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -3204,16 +3186,16 @@
         <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E144" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -3221,16 +3203,16 @@
         <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E145" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -3238,16 +3220,16 @@
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E146" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3255,191 +3237,200 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E147" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E148" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>123</v>
+        <v>113</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E149" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B150" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E150" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B151" t="s">
-        <v>124</v>
+        <v>115</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E151" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B152" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E152" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C153">
         <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E153" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E154" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B155" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C155">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D155" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E155" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B156" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C156">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D156" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E156" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C157">
         <v>1</v>
       </c>
       <c r="D157" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E157" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B158" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C158">
         <v>1</v>
       </c>
       <c r="D158" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E158" t="s">
         <v>4</v>
@@ -3447,16 +3438,13 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B159" t="s">
-        <v>110</v>
-      </c>
-      <c r="C159">
-        <v>2</v>
+        <v>122</v>
       </c>
       <c r="D159" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E159" t="s">
         <v>4</v>
@@ -3464,121 +3452,285 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B160" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="C160">
         <v>1</v>
       </c>
       <c r="D160" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E160" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A161" s="1" t="s">
+      <c r="A161" t="s">
+        <v>83</v>
+      </c>
+      <c r="B161" t="s">
+        <v>123</v>
+      </c>
+      <c r="D161" t="s">
+        <v>124</v>
+      </c>
+      <c r="E161" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>83</v>
+      </c>
+      <c r="B162" t="s">
+        <v>122</v>
+      </c>
+      <c r="D162" t="s">
+        <v>124</v>
+      </c>
+      <c r="E162" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>83</v>
+      </c>
+      <c r="B163" t="s">
+        <v>120</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+      <c r="D163" t="s">
+        <v>124</v>
+      </c>
+      <c r="E163" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>83</v>
+      </c>
+      <c r="B164" t="s">
+        <v>125</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+      <c r="D164" t="s">
+        <v>124</v>
+      </c>
+      <c r="E164" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>17</v>
+      </c>
+      <c r="B165" t="s">
+        <v>126</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165" t="s">
+        <v>127</v>
+      </c>
+      <c r="E165" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
         <v>20</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B166" t="s">
+        <v>126</v>
+      </c>
+      <c r="C166">
+        <v>2</v>
+      </c>
+      <c r="D166" t="s">
+        <v>127</v>
+      </c>
+      <c r="E166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>83</v>
+      </c>
+      <c r="B167" t="s">
+        <v>128</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167" t="s">
+        <v>129</v>
+      </c>
+      <c r="E167" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>83</v>
+      </c>
+      <c r="B168" t="s">
+        <v>128</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168" t="s">
+        <v>130</v>
+      </c>
+      <c r="E168" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>83</v>
+      </c>
+      <c r="B169" t="s">
+        <v>109</v>
+      </c>
+      <c r="C169">
+        <v>2</v>
+      </c>
+      <c r="D169" t="s">
+        <v>131</v>
+      </c>
+      <c r="E169" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>83</v>
+      </c>
+      <c r="B170" t="s">
+        <v>132</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+      <c r="D170" t="s">
+        <v>133</v>
+      </c>
+      <c r="E170" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C171" s="1">
+        <v>2</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E171" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C161" s="1">
-        <v>2</v>
-      </c>
-      <c r="D161" s="1" t="s">
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C172" s="1">
+        <v>2</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C173" s="1">
+        <v>2</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C174" s="1">
+        <v>2</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C175" s="1">
+        <v>2</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E175" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E161" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A162" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C162" s="1">
-        <v>2</v>
-      </c>
-      <c r="D162" s="1" t="s">
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C176" s="1">
+        <v>2</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E176" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A163" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C163" s="1">
-        <v>2</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A164" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C164" s="1">
-        <v>2</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A165" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C165" s="1">
-        <v>2</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A166" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C166" s="1">
-        <v>2</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (categories) Add how to add and remove categories from item (#423)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04A9757-9955-4589-9C11-9AB88D60E3BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E448235A-FC74-488F-A89C-A6C89812F18A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="166">
   <si>
     <t>Class</t>
   </si>
@@ -270,9 +270,6 @@
     <t>categories</t>
   </si>
   <si>
-    <t>outlook-categories-get-categories</t>
-  </si>
-  <si>
     <t>getCategories</t>
   </si>
   <si>
@@ -520,6 +517,15 @@
   </si>
   <si>
     <t>outlook-categories-work-with-master-categories</t>
+  </si>
+  <si>
+    <t>addCategories</t>
+  </si>
+  <si>
+    <t>removeCategories</t>
+  </si>
+  <si>
+    <t>outlook-categories-work-with-categories</t>
   </si>
 </sst>
 </file>
@@ -595,8 +601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E166" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E166" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E176" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E176" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -928,11 +934,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D103" sqref="D103:D107"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98:D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,7 +1264,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1266,16 +1272,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1289,27 +1295,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" t="s">
         <v>155</v>
-      </c>
-      <c r="E21" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" t="s">
         <v>155</v>
-      </c>
-      <c r="E22" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1320,7 +1326,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1328,16 +1334,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1351,27 +1357,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" t="s">
         <v>153</v>
-      </c>
-      <c r="E25" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>152</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>153</v>
-      </c>
-      <c r="E26" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1404,10 +1410,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1455,7 +1461,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1463,16 +1469,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1486,27 +1492,27 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1539,10 +1545,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -1576,7 +1582,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
@@ -1584,16 +1590,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
@@ -1607,27 +1613,27 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E42" t="s">
         <v>157</v>
-      </c>
-      <c r="E42" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
+        <v>156</v>
+      </c>
+      <c r="E43" t="s">
         <v>157</v>
-      </c>
-      <c r="E43" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1652,7 +1658,7 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
@@ -1660,16 +1666,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -1684,27 +1690,27 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>149</v>
+      </c>
+      <c r="E48" t="s">
         <v>150</v>
-      </c>
-      <c r="E48" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1726,7 +1732,7 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1740,7 +1746,7 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1754,7 +1760,7 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1768,7 +1774,7 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1799,7 +1805,7 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1813,7 +1819,7 @@
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -1827,7 +1833,7 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -1841,7 +1847,7 @@
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -1872,7 +1878,7 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D60" t="s">
         <v>57</v>
@@ -1886,7 +1892,7 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D61" t="s">
         <v>57</v>
@@ -1900,7 +1906,7 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D62" t="s">
         <v>57</v>
@@ -1914,7 +1920,7 @@
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D63" t="s">
         <v>57</v>
@@ -1962,7 +1968,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D66" t="s">
         <v>57</v>
@@ -1976,7 +1982,7 @@
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D67" t="s">
         <v>57</v>
@@ -1990,7 +1996,7 @@
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D68" t="s">
         <v>57</v>
@@ -2004,7 +2010,7 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D69" t="s">
         <v>57</v>
@@ -2035,7 +2041,7 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D71" t="s">
         <v>57</v>
@@ -2049,7 +2055,7 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D72" t="s">
         <v>57</v>
@@ -2063,7 +2069,7 @@
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D73" t="s">
         <v>57</v>
@@ -2077,7 +2083,7 @@
         <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D74" t="s">
         <v>57</v>
@@ -2108,7 +2114,7 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D76" t="s">
         <v>57</v>
@@ -2122,7 +2128,7 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D77" t="s">
         <v>57</v>
@@ -2136,7 +2142,7 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -2150,7 +2156,7 @@
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D79" t="s">
         <v>57</v>
@@ -2357,7 +2363,7 @@
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2374,7 +2380,7 @@
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2391,7 +2397,7 @@
         <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
@@ -2408,7 +2414,7 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
@@ -2450,10 +2456,10 @@
         <v>79</v>
       </c>
       <c r="D97" t="s">
+        <v>165</v>
+      </c>
+      <c r="E97" t="s">
         <v>80</v>
-      </c>
-      <c r="E97" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -2464,10 +2470,10 @@
         <v>79</v>
       </c>
       <c r="D98" t="s">
+        <v>165</v>
+      </c>
+      <c r="E98" t="s">
         <v>80</v>
-      </c>
-      <c r="E98" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -2478,10 +2484,10 @@
         <v>79</v>
       </c>
       <c r="D99" t="s">
+        <v>165</v>
+      </c>
+      <c r="E99" t="s">
         <v>80</v>
-      </c>
-      <c r="E99" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -2492,303 +2498,297 @@
         <v>79</v>
       </c>
       <c r="D100" t="s">
+        <v>165</v>
+      </c>
+      <c r="E100" t="s">
         <v>80</v>
-      </c>
-      <c r="E100" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>81</v>
+      </c>
+      <c r="B101" t="s">
         <v>82</v>
       </c>
-      <c r="B101" t="s">
-        <v>83</v>
-      </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" t="s">
+        <v>165</v>
+      </c>
+      <c r="E101" t="s">
         <v>80</v>
-      </c>
-      <c r="E101" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D102" t="s">
+        <v>165</v>
+      </c>
+      <c r="E102" t="s">
         <v>163</v>
-      </c>
-      <c r="E102" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>83</v>
-      </c>
-      <c r="C103">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D103" t="s">
+        <v>165</v>
+      </c>
+      <c r="E103" t="s">
         <v>163</v>
-      </c>
-      <c r="E103" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B104" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D104" t="s">
+        <v>165</v>
+      </c>
+      <c r="E104" t="s">
         <v>163</v>
-      </c>
-      <c r="E104" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>56</v>
-      </c>
-      <c r="C105">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D105" t="s">
+        <v>165</v>
+      </c>
+      <c r="E105" t="s">
         <v>163</v>
-      </c>
-      <c r="E105" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B106" t="s">
-        <v>85</v>
+        <v>56</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
       </c>
       <c r="D106" t="s">
+        <v>165</v>
+      </c>
+      <c r="E106" t="s">
         <v>163</v>
-      </c>
-      <c r="E106" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>66</v>
-      </c>
-      <c r="C107">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D107" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E107" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B108" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D108" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="E108" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="B109" t="s">
-        <v>83</v>
-      </c>
-      <c r="C109">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D109" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="E109" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B110" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D110" t="s">
-        <v>92</v>
+        <v>165</v>
       </c>
       <c r="E110" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B111" t="s">
-        <v>88</v>
+        <v>66</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>92</v>
+        <v>165</v>
       </c>
       <c r="E111" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B112" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D112" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E112" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="B113" t="s">
-        <v>93</v>
+        <v>82</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E113" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B114" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E114" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B115" t="s">
-        <v>93</v>
+        <v>56</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E115" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>83</v>
+      </c>
+      <c r="B116" t="s">
         <v>84</v>
       </c>
-      <c r="B116" t="s">
-        <v>96</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
       <c r="D116" t="s">
-        <v>97</v>
+        <v>162</v>
       </c>
       <c r="E116" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B117" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="E117" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>100</v>
-      </c>
-      <c r="C118">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D118" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E118" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B119" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E119" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2796,16 +2796,13 @@
         <v>19</v>
       </c>
       <c r="B120" t="s">
-        <v>104</v>
-      </c>
-      <c r="C120">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E120" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2813,67 +2810,55 @@
         <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>104</v>
-      </c>
-      <c r="C121">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D121" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E121" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B122" t="s">
-        <v>105</v>
-      </c>
-      <c r="C122">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D122" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E122" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>105</v>
-      </c>
-      <c r="C123">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D123" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E123" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B124" t="s">
-        <v>104</v>
-      </c>
-      <c r="C124">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D124" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E124" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2881,135 +2866,132 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>104</v>
-      </c>
-      <c r="C125">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D125" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E125" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B126" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E126" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B127" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E127" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B128" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C128">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E128" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C129">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E129" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E130" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E131" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E132" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,16 +2999,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E133" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,16 +3016,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E134" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,67 +3033,67 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E135" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E136" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B137" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E137" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B138" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C138">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E138" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -3119,67 +3101,67 @@
         <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C139">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E139" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E140" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B141" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C141">
         <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E141" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B142" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E142" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -3187,16 +3169,16 @@
         <v>21</v>
       </c>
       <c r="B143" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C143">
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E143" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -3204,16 +3186,16 @@
         <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E144" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -3221,16 +3203,16 @@
         <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E145" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -3238,16 +3220,16 @@
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E146" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3255,191 +3237,200 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E147" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E148" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>123</v>
+        <v>113</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E149" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B150" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E150" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B151" t="s">
-        <v>124</v>
+        <v>115</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E151" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B152" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E152" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C153">
         <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E153" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E154" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B155" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C155">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D155" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E155" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B156" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C156">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D156" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E156" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C157">
         <v>1</v>
       </c>
       <c r="D157" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E157" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B158" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C158">
         <v>1</v>
       </c>
       <c r="D158" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E158" t="s">
         <v>4</v>
@@ -3447,16 +3438,13 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B159" t="s">
-        <v>110</v>
-      </c>
-      <c r="C159">
-        <v>2</v>
+        <v>122</v>
       </c>
       <c r="D159" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E159" t="s">
         <v>4</v>
@@ -3464,121 +3452,285 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B160" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="C160">
         <v>1</v>
       </c>
       <c r="D160" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E160" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A161" s="1" t="s">
+      <c r="A161" t="s">
+        <v>83</v>
+      </c>
+      <c r="B161" t="s">
+        <v>123</v>
+      </c>
+      <c r="D161" t="s">
+        <v>124</v>
+      </c>
+      <c r="E161" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>83</v>
+      </c>
+      <c r="B162" t="s">
+        <v>122</v>
+      </c>
+      <c r="D162" t="s">
+        <v>124</v>
+      </c>
+      <c r="E162" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>83</v>
+      </c>
+      <c r="B163" t="s">
+        <v>120</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+      <c r="D163" t="s">
+        <v>124</v>
+      </c>
+      <c r="E163" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>83</v>
+      </c>
+      <c r="B164" t="s">
+        <v>125</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+      <c r="D164" t="s">
+        <v>124</v>
+      </c>
+      <c r="E164" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>17</v>
+      </c>
+      <c r="B165" t="s">
+        <v>126</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165" t="s">
+        <v>127</v>
+      </c>
+      <c r="E165" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
         <v>20</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B166" t="s">
+        <v>126</v>
+      </c>
+      <c r="C166">
+        <v>2</v>
+      </c>
+      <c r="D166" t="s">
+        <v>127</v>
+      </c>
+      <c r="E166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>83</v>
+      </c>
+      <c r="B167" t="s">
+        <v>128</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167" t="s">
+        <v>129</v>
+      </c>
+      <c r="E167" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>83</v>
+      </c>
+      <c r="B168" t="s">
+        <v>128</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168" t="s">
+        <v>130</v>
+      </c>
+      <c r="E168" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>83</v>
+      </c>
+      <c r="B169" t="s">
+        <v>109</v>
+      </c>
+      <c r="C169">
+        <v>2</v>
+      </c>
+      <c r="D169" t="s">
+        <v>131</v>
+      </c>
+      <c r="E169" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>83</v>
+      </c>
+      <c r="B170" t="s">
+        <v>132</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+      <c r="D170" t="s">
+        <v>133</v>
+      </c>
+      <c r="E170" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C171" s="1">
+        <v>2</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E171" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C161" s="1">
-        <v>2</v>
-      </c>
-      <c r="D161" s="1" t="s">
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C172" s="1">
+        <v>2</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C173" s="1">
+        <v>2</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C174" s="1">
+        <v>2</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C175" s="1">
+        <v>2</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E175" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E161" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A162" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C162" s="1">
-        <v>2</v>
-      </c>
-      <c r="D162" s="1" t="s">
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C176" s="1">
+        <v>2</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E176" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A163" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C163" s="1">
-        <v>2</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A164" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C164" s="1">
-        <v>2</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A165" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C165" s="1">
-        <v>2</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A166" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C166" s="1">
-        <v>2</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (attachments) Reference correct method overload
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E448235A-FC74-488F-A89C-A6C89812F18A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCCD278-93B7-44EA-8D66-94D511330E3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -937,8 +937,8 @@
   <dimension ref="A1:E176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D98" sqref="D98:D111"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2360,7 +2360,7 @@
         <v>76</v>
       </c>
       <c r="C91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91" t="s">
         <v>138</v>
@@ -2377,7 +2377,7 @@
         <v>76</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92" t="s">
         <v>138</v>
@@ -2394,7 +2394,7 @@
         <v>76</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D93" t="s">
         <v>138</v>
@@ -2411,7 +2411,7 @@
         <v>76</v>
       </c>
       <c r="C94">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D94" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
[Outlook] (attachments) Reference correct method overload (#425)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E448235A-FC74-488F-A89C-A6C89812F18A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCCD278-93B7-44EA-8D66-94D511330E3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -937,8 +937,8 @@
   <dimension ref="A1:E176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D98" sqref="D98:D111"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2360,7 +2360,7 @@
         <v>76</v>
       </c>
       <c r="C91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91" t="s">
         <v>138</v>
@@ -2377,7 +2377,7 @@
         <v>76</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92" t="s">
         <v>138</v>
@@ -2394,7 +2394,7 @@
         <v>76</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D93" t="s">
         <v>138</v>
@@ -2411,7 +2411,7 @@
         <v>76</v>
       </c>
       <c r="C94">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D94" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
[Outlook] (mapping) Include new snippets
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCCD278-93B7-44EA-8D66-94D511330E3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C007D39D-F6FA-4C70-8469-A70D3759D0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="179">
   <si>
     <t>Class</t>
   </si>
@@ -526,6 +526,45 @@
   </si>
   <si>
     <t>outlook-categories-work-with-categories</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-subject-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-subject-compose</t>
+  </si>
+  <si>
+    <t>internetMessageId</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-internet-message-id-read</t>
+  </si>
+  <si>
+    <t>itemClass</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-item-class-read</t>
+  </si>
+  <si>
+    <t>itemType</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-item-type</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-start-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-start-appointment-organizer</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -601,8 +640,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E176" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E176" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E195" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E195" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -934,11 +973,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E176"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3733,6 +3772,295 @@
         <v>141</v>
       </c>
     </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C182" s="1"/>
+      <c r="D182" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C183" s="1"/>
+      <c r="D183" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C184" s="1"/>
+      <c r="D184" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C185" s="1"/>
+      <c r="D185" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A186" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A187" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C187" s="1"/>
+      <c r="D187" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A188" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C188" s="1"/>
+      <c r="D188" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A189" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C189" s="1"/>
+      <c r="D189" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A190" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C190" s="1"/>
+      <c r="D190" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A191" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C191" s="1"/>
+      <c r="D191" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C192" s="1"/>
+      <c r="D192" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C193" s="1">
+        <v>2</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C194" s="1"/>
+      <c r="D194" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C195" s="1">
+        <v>2</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Outlook] (mapping) Include new snippets (#434)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCCD278-93B7-44EA-8D66-94D511330E3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C007D39D-F6FA-4C70-8469-A70D3759D0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="179">
   <si>
     <t>Class</t>
   </si>
@@ -526,6 +526,45 @@
   </si>
   <si>
     <t>outlook-categories-work-with-categories</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-subject-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-subject-compose</t>
+  </si>
+  <si>
+    <t>internetMessageId</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-internet-message-id-read</t>
+  </si>
+  <si>
+    <t>itemClass</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-item-class-read</t>
+  </si>
+  <si>
+    <t>itemType</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-item-type</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-start-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-start-appointment-organizer</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -601,8 +640,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E176" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E176" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E195" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E195" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -934,11 +973,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E176"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3733,6 +3772,295 @@
         <v>141</v>
       </c>
     </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C182" s="1"/>
+      <c r="D182" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C183" s="1"/>
+      <c r="D183" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C184" s="1"/>
+      <c r="D184" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C185" s="1"/>
+      <c r="D185" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A186" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A187" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C187" s="1"/>
+      <c r="D187" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A188" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C188" s="1"/>
+      <c r="D188" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A189" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C189" s="1"/>
+      <c r="D189" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A190" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C190" s="1"/>
+      <c r="D190" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A191" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C191" s="1"/>
+      <c r="D191" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C192" s="1"/>
+      <c r="D192" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C193" s="1">
+        <v>2</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C194" s="1"/>
+      <c r="D194" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C195" s="1">
+        <v>2</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Outlook] (recurrence) Clean up snippet (Read)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C007D39D-F6FA-4C70-8469-A70D3759D0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8EBDA1-17E0-4A61-B5F9-1B7CC20CF5BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -976,8 +976,8 @@
   <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2841,7 +2841,7 @@
         <v>91</v>
       </c>
       <c r="E120" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2855,7 +2855,7 @@
         <v>91</v>
       </c>
       <c r="E121" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Outlook] (recurrence) Clean up snippet (Read) (#446)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C007D39D-F6FA-4C70-8469-A70D3759D0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8EBDA1-17E0-4A61-B5F9-1B7CC20CF5BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -976,8 +976,8 @@
   <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2841,7 +2841,7 @@
         <v>91</v>
       </c>
       <c r="E120" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2855,7 +2855,7 @@
         <v>91</v>
       </c>
       <c r="E121" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Outlook] (recurrence) Add how to set (Appointment Organizer)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8EBDA1-17E0-4A61-B5F9-1B7CC20CF5BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA11D42-4033-4A71-ADCF-EB96E1EE4C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="186">
   <si>
     <t>Class</t>
   </si>
@@ -294,12 +294,6 @@
     <t>recurrence</t>
   </si>
   <si>
-    <t>outlook-recurrence-get-recurrence-appointment-organizer</t>
-  </si>
-  <si>
-    <t>getRecurrence</t>
-  </si>
-  <si>
     <t>Recurrence</t>
   </si>
   <si>
@@ -565,6 +559,33 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>outlook-recurrence-get-set-recurrence-appointment-organizer</t>
+  </si>
+  <si>
+    <t>normalizedSubject</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-normalized-subject-read</t>
+  </si>
+  <si>
+    <t>conversationId</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-conversation-id-message</t>
+  </si>
+  <si>
+    <t>dateTimeCreated</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-date-time-created-read</t>
+  </si>
+  <si>
+    <t>dateTimeModified</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-date-time-modified-read</t>
   </si>
 </sst>
 </file>
@@ -640,8 +661,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E195" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E195" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E205" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E205" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -973,11 +994,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,7 +1324,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1311,7 +1332,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
         <v>82</v>
@@ -1320,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1334,27 +1355,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1365,7 +1386,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1373,7 +1394,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
         <v>82</v>
@@ -1382,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1396,27 +1417,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" t="s">
         <v>151</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E26" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1449,7 +1470,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
         <v>82</v>
@@ -1500,7 +1521,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1508,7 +1529,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
         <v>82</v>
@@ -1517,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1531,27 +1552,27 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1584,7 +1605,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B38" t="s">
         <v>82</v>
@@ -1621,7 +1642,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
@@ -1629,7 +1650,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
         <v>82</v>
@@ -1638,7 +1659,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
@@ -1652,27 +1673,27 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1697,7 +1718,7 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
@@ -1705,7 +1726,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
         <v>82</v>
@@ -1714,7 +1735,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -1729,27 +1750,27 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E48" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1771,7 +1792,7 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1785,7 +1806,7 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1799,7 +1820,7 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1813,7 +1834,7 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1844,7 +1865,7 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1858,7 +1879,7 @@
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -1872,7 +1893,7 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -1886,7 +1907,7 @@
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -1917,7 +1938,7 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D60" t="s">
         <v>57</v>
@@ -1931,7 +1952,7 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D61" t="s">
         <v>57</v>
@@ -1945,7 +1966,7 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D62" t="s">
         <v>57</v>
@@ -1959,7 +1980,7 @@
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D63" t="s">
         <v>57</v>
@@ -2007,7 +2028,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D66" t="s">
         <v>57</v>
@@ -2021,7 +2042,7 @@
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D67" t="s">
         <v>57</v>
@@ -2035,7 +2056,7 @@
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D68" t="s">
         <v>57</v>
@@ -2049,7 +2070,7 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D69" t="s">
         <v>57</v>
@@ -2080,7 +2101,7 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D71" t="s">
         <v>57</v>
@@ -2094,7 +2115,7 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D72" t="s">
         <v>57</v>
@@ -2108,7 +2129,7 @@
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D73" t="s">
         <v>57</v>
@@ -2122,7 +2143,7 @@
         <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D74" t="s">
         <v>57</v>
@@ -2153,7 +2174,7 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D76" t="s">
         <v>57</v>
@@ -2167,7 +2188,7 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D77" t="s">
         <v>57</v>
@@ -2181,7 +2202,7 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -2195,7 +2216,7 @@
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D79" t="s">
         <v>57</v>
@@ -2402,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2419,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2436,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
@@ -2453,7 +2474,7 @@
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
@@ -2495,7 +2516,7 @@
         <v>79</v>
       </c>
       <c r="D97" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E97" t="s">
         <v>80</v>
@@ -2509,7 +2530,7 @@
         <v>79</v>
       </c>
       <c r="D98" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E98" t="s">
         <v>80</v>
@@ -2523,7 +2544,7 @@
         <v>79</v>
       </c>
       <c r="D99" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E99" t="s">
         <v>80</v>
@@ -2537,7 +2558,7 @@
         <v>79</v>
       </c>
       <c r="D100" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E100" t="s">
         <v>80</v>
@@ -2554,7 +2575,7 @@
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E101" t="s">
         <v>80</v>
@@ -2568,10 +2589,10 @@
         <v>79</v>
       </c>
       <c r="D102" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E102" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -2582,10 +2603,10 @@
         <v>79</v>
       </c>
       <c r="D103" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E103" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -2596,10 +2617,10 @@
         <v>79</v>
       </c>
       <c r="D104" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E104" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2610,10 +2631,10 @@
         <v>79</v>
       </c>
       <c r="D105" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E105" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -2627,10 +2648,10 @@
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E106" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -2641,10 +2662,10 @@
         <v>79</v>
       </c>
       <c r="D107" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E107" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2655,10 +2676,10 @@
         <v>79</v>
       </c>
       <c r="D108" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E108" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -2669,10 +2690,10 @@
         <v>79</v>
       </c>
       <c r="D109" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E109" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2683,10 +2704,10 @@
         <v>79</v>
       </c>
       <c r="D110" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E110" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2700,10 +2721,10 @@
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E111" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2714,7 +2735,7 @@
         <v>84</v>
       </c>
       <c r="D112" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E112" t="s">
         <v>85</v>
@@ -2731,7 +2752,7 @@
         <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E113" t="s">
         <v>85</v>
@@ -2745,10 +2766,10 @@
         <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E114" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2762,10 +2783,10 @@
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E115" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2776,10 +2797,10 @@
         <v>84</v>
       </c>
       <c r="D116" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E116" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2793,10 +2814,10 @@
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E117" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2807,15 +2828,15 @@
         <v>87</v>
       </c>
       <c r="D118" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="E118" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B119" t="s">
         <v>82</v>
@@ -2824,128 +2845,125 @@
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="E119" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B120" t="s">
         <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="E120" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B121" t="s">
-        <v>87</v>
+        <v>149</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="E121" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D122" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E122" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D123" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E123" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B124" t="s">
+        <v>90</v>
+      </c>
+      <c r="D124" t="s">
+        <v>91</v>
+      </c>
+      <c r="E124" t="s">
         <v>92</v>
-      </c>
-      <c r="D124" t="s">
-        <v>93</v>
-      </c>
-      <c r="E124" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B125" t="s">
+        <v>90</v>
+      </c>
+      <c r="D125" t="s">
+        <v>91</v>
+      </c>
+      <c r="E125" t="s">
         <v>92</v>
-      </c>
-      <c r="D125" t="s">
-        <v>93</v>
-      </c>
-      <c r="E125" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B126" t="s">
-        <v>95</v>
-      </c>
-      <c r="C126">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D126" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E126" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>97</v>
-      </c>
-      <c r="C127">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D127" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E127" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2953,13 +2971,13 @@
         <v>83</v>
       </c>
       <c r="B128" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E128" t="s">
         <v>4</v>
@@ -2970,13 +2988,13 @@
         <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E129" t="s">
         <v>4</v>
@@ -2984,36 +3002,36 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B130" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E130" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B131" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E131" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3021,16 +3039,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E132" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3038,16 +3056,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E133" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3055,16 +3073,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
+        <v>102</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134" t="s">
         <v>103</v>
       </c>
-      <c r="C134">
-        <v>1</v>
-      </c>
-      <c r="D134" t="s">
-        <v>106</v>
-      </c>
       <c r="E134" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3072,64 +3090,64 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
+        <v>102</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135" t="s">
         <v>103</v>
       </c>
-      <c r="C135">
-        <v>1</v>
-      </c>
-      <c r="D135" t="s">
-        <v>106</v>
-      </c>
       <c r="E135" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E136" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E137" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C138">
         <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E138" t="s">
         <v>11</v>
@@ -3137,16 +3155,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B139" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C139">
         <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E139" t="s">
         <v>11</v>
@@ -3154,50 +3172,50 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B140" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D140" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E140" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C141">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D141" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E141" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E142" t="s">
         <v>4</v>
@@ -3205,16 +3223,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B143" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C143">
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -3222,19 +3240,19 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B144" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E144" t="s">
-        <v>110</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -3242,16 +3260,16 @@
         <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E145" t="s">
-        <v>110</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -3259,16 +3277,16 @@
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E146" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3276,16 +3294,16 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E147" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3293,16 +3311,16 @@
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E148" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -3310,16 +3328,16 @@
         <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C149">
         <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E149" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -3327,16 +3345,16 @@
         <v>19</v>
       </c>
       <c r="B150" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E150" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -3344,16 +3362,16 @@
         <v>21</v>
       </c>
       <c r="B151" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C151">
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E151" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -3361,16 +3379,16 @@
         <v>19</v>
       </c>
       <c r="B152" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C152">
         <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E152" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3378,16 +3396,16 @@
         <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C153">
         <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E153" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -3395,16 +3413,16 @@
         <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E154" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3412,16 +3430,16 @@
         <v>21</v>
       </c>
       <c r="B155" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C155">
         <v>1</v>
       </c>
       <c r="D155" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E155" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3429,16 +3447,16 @@
         <v>19</v>
       </c>
       <c r="B156" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C156">
         <v>1</v>
       </c>
       <c r="D156" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E156" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3446,47 +3464,50 @@
         <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C157">
         <v>1</v>
       </c>
       <c r="D157" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E157" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B158" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C158">
         <v>1</v>
       </c>
       <c r="D158" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E158" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B159" t="s">
-        <v>122</v>
+        <v>117</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
       </c>
       <c r="D159" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E159" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -3494,13 +3515,13 @@
         <v>83</v>
       </c>
       <c r="B160" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C160">
         <v>1</v>
       </c>
       <c r="D160" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E160" t="s">
         <v>4</v>
@@ -3511,10 +3532,10 @@
         <v>83</v>
       </c>
       <c r="B161" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D161" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E161" t="s">
         <v>4</v>
@@ -3525,10 +3546,13 @@
         <v>83</v>
       </c>
       <c r="B162" t="s">
-        <v>122</v>
+        <v>107</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
       </c>
       <c r="D162" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E162" t="s">
         <v>4</v>
@@ -3539,13 +3563,10 @@
         <v>83</v>
       </c>
       <c r="B163" t="s">
-        <v>120</v>
-      </c>
-      <c r="C163">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="D163" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E163" t="s">
         <v>4</v>
@@ -3556,13 +3577,10 @@
         <v>83</v>
       </c>
       <c r="B164" t="s">
-        <v>125</v>
-      </c>
-      <c r="C164">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D164" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E164" t="s">
         <v>4</v>
@@ -3570,16 +3588,16 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B165" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D165" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E165" t="s">
         <v>4</v>
@@ -3587,16 +3605,16 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B166" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C166">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D166" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E166" t="s">
         <v>4</v>
@@ -3604,16 +3622,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="B167" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C167">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D167" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E167" t="s">
         <v>4</v>
@@ -3621,16 +3639,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B168" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C168">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D168" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E168" t="s">
         <v>4</v>
@@ -3641,13 +3659,13 @@
         <v>83</v>
       </c>
       <c r="B169" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="C169">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E169" t="s">
         <v>4</v>
@@ -3658,84 +3676,84 @@
         <v>83</v>
       </c>
       <c r="B170" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C170">
         <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E170" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A171" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C171" s="1">
-        <v>2</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>146</v>
+      <c r="A171" t="s">
+        <v>83</v>
+      </c>
+      <c r="B171" t="s">
+        <v>107</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>129</v>
+      </c>
+      <c r="E171" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A172" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C172" s="1">
-        <v>2</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>144</v>
+      <c r="A172" t="s">
+        <v>83</v>
+      </c>
+      <c r="B172" t="s">
+        <v>130</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172" t="s">
+        <v>131</v>
+      </c>
+      <c r="E172" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C173" s="1">
         <v>2</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C174" s="1">
         <v>2</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
@@ -3743,16 +3761,16 @@
         <v>17</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C175" s="1">
         <v>2</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
@@ -3760,58 +3778,62 @@
         <v>20</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C176" s="1">
         <v>2</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C177" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C177" s="1">
+        <v>2</v>
+      </c>
       <c r="D177" s="1" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C178" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C178" s="1">
+        <v>2</v>
+      </c>
       <c r="D178" s="1" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C179" s="1"/>
       <c r="D179" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>11</v>
@@ -3819,14 +3841,14 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C180" s="1"/>
       <c r="D180" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>11</v>
@@ -3837,14 +3859,14 @@
         <v>17</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C181" s="1"/>
       <c r="D181" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
@@ -3852,44 +3874,44 @@
         <v>20</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C182" s="1"/>
       <c r="D182" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C183" s="1"/>
       <c r="D183" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C184" s="1"/>
       <c r="D184" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
@@ -3897,11 +3919,11 @@
         <v>21</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C185" s="1"/>
       <c r="D185" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>11</v>
@@ -3909,14 +3931,14 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C186" s="1"/>
       <c r="D186" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>11</v>
@@ -3924,14 +3946,14 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C187" s="1"/>
       <c r="D187" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>11</v>
@@ -3939,14 +3961,14 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C188" s="1"/>
       <c r="D188" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>11</v>
@@ -3954,14 +3976,14 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C189" s="1"/>
       <c r="D189" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>11</v>
@@ -3969,14 +3991,14 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C190" s="1"/>
       <c r="D190" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>11</v>
@@ -3987,11 +4009,11 @@
         <v>21</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>11</v>
@@ -3999,14 +4021,14 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>11</v>
@@ -4014,16 +4036,14 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>178</v>
+        <v>21</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C193" s="1">
-        <v>2</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C193" s="1"/>
       <c r="D193" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>11</v>
@@ -4034,31 +4054,183 @@
         <v>17</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C194" s="1"/>
       <c r="D194" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C195" s="1">
+        <v>2</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C196" s="1"/>
+      <c r="D196" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C197" s="1">
+        <v>2</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C195" s="1">
-        <v>2</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>3</v>
+      <c r="C198" s="1"/>
+      <c r="D198" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A199" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C199" s="1"/>
+      <c r="D199" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A200" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C200" s="1"/>
+      <c r="D200" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C201" s="1"/>
+      <c r="D201" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C202" s="1"/>
+      <c r="D202" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C203" s="1"/>
+      <c r="D203" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C205" s="1"/>
+      <c r="D205" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (recurrence) Add how to set (Appointment Organizer) (#447)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8EBDA1-17E0-4A61-B5F9-1B7CC20CF5BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA11D42-4033-4A71-ADCF-EB96E1EE4C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="186">
   <si>
     <t>Class</t>
   </si>
@@ -294,12 +294,6 @@
     <t>recurrence</t>
   </si>
   <si>
-    <t>outlook-recurrence-get-recurrence-appointment-organizer</t>
-  </si>
-  <si>
-    <t>getRecurrence</t>
-  </si>
-  <si>
     <t>Recurrence</t>
   </si>
   <si>
@@ -565,6 +559,33 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>outlook-recurrence-get-set-recurrence-appointment-organizer</t>
+  </si>
+  <si>
+    <t>normalizedSubject</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-normalized-subject-read</t>
+  </si>
+  <si>
+    <t>conversationId</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-conversation-id-message</t>
+  </si>
+  <si>
+    <t>dateTimeCreated</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-date-time-created-read</t>
+  </si>
+  <si>
+    <t>dateTimeModified</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-date-time-modified-read</t>
   </si>
 </sst>
 </file>
@@ -640,8 +661,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E195" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E195" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E205" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E205" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -973,11 +994,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,7 +1324,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1311,7 +1332,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
         <v>82</v>
@@ -1320,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1334,27 +1355,27 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1365,7 +1386,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1373,7 +1394,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
         <v>82</v>
@@ -1382,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1396,27 +1417,27 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" t="s">
         <v>151</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E26" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1449,7 +1470,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
         <v>82</v>
@@ -1500,7 +1521,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1508,7 +1529,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
         <v>82</v>
@@ -1517,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1531,27 +1552,27 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1584,7 +1605,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B38" t="s">
         <v>82</v>
@@ -1621,7 +1642,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
@@ -1629,7 +1650,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
         <v>82</v>
@@ -1638,7 +1659,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
@@ -1652,27 +1673,27 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1697,7 +1718,7 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
@@ -1705,7 +1726,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
         <v>82</v>
@@ -1714,7 +1735,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -1729,27 +1750,27 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E48" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1771,7 +1792,7 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1785,7 +1806,7 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1799,7 +1820,7 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1813,7 +1834,7 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1844,7 +1865,7 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1858,7 +1879,7 @@
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -1872,7 +1893,7 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -1886,7 +1907,7 @@
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -1917,7 +1938,7 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D60" t="s">
         <v>57</v>
@@ -1931,7 +1952,7 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D61" t="s">
         <v>57</v>
@@ -1945,7 +1966,7 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D62" t="s">
         <v>57</v>
@@ -1959,7 +1980,7 @@
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D63" t="s">
         <v>57</v>
@@ -2007,7 +2028,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D66" t="s">
         <v>57</v>
@@ -2021,7 +2042,7 @@
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D67" t="s">
         <v>57</v>
@@ -2035,7 +2056,7 @@
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D68" t="s">
         <v>57</v>
@@ -2049,7 +2070,7 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D69" t="s">
         <v>57</v>
@@ -2080,7 +2101,7 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D71" t="s">
         <v>57</v>
@@ -2094,7 +2115,7 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D72" t="s">
         <v>57</v>
@@ -2108,7 +2129,7 @@
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D73" t="s">
         <v>57</v>
@@ -2122,7 +2143,7 @@
         <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D74" t="s">
         <v>57</v>
@@ -2153,7 +2174,7 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D76" t="s">
         <v>57</v>
@@ -2167,7 +2188,7 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D77" t="s">
         <v>57</v>
@@ -2181,7 +2202,7 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -2195,7 +2216,7 @@
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D79" t="s">
         <v>57</v>
@@ -2402,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E91" t="s">
         <v>4</v>
@@ -2419,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E92" t="s">
         <v>4</v>
@@ -2436,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
@@ -2453,7 +2474,7 @@
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
@@ -2495,7 +2516,7 @@
         <v>79</v>
       </c>
       <c r="D97" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E97" t="s">
         <v>80</v>
@@ -2509,7 +2530,7 @@
         <v>79</v>
       </c>
       <c r="D98" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E98" t="s">
         <v>80</v>
@@ -2523,7 +2544,7 @@
         <v>79</v>
       </c>
       <c r="D99" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E99" t="s">
         <v>80</v>
@@ -2537,7 +2558,7 @@
         <v>79</v>
       </c>
       <c r="D100" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E100" t="s">
         <v>80</v>
@@ -2554,7 +2575,7 @@
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E101" t="s">
         <v>80</v>
@@ -2568,10 +2589,10 @@
         <v>79</v>
       </c>
       <c r="D102" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E102" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -2582,10 +2603,10 @@
         <v>79</v>
       </c>
       <c r="D103" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E103" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -2596,10 +2617,10 @@
         <v>79</v>
       </c>
       <c r="D104" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E104" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2610,10 +2631,10 @@
         <v>79</v>
       </c>
       <c r="D105" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E105" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -2627,10 +2648,10 @@
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E106" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -2641,10 +2662,10 @@
         <v>79</v>
       </c>
       <c r="D107" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E107" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2655,10 +2676,10 @@
         <v>79</v>
       </c>
       <c r="D108" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E108" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -2669,10 +2690,10 @@
         <v>79</v>
       </c>
       <c r="D109" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E109" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2683,10 +2704,10 @@
         <v>79</v>
       </c>
       <c r="D110" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E110" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2700,10 +2721,10 @@
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E111" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2714,7 +2735,7 @@
         <v>84</v>
       </c>
       <c r="D112" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E112" t="s">
         <v>85</v>
@@ -2731,7 +2752,7 @@
         <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E113" t="s">
         <v>85</v>
@@ -2745,10 +2766,10 @@
         <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E114" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2762,10 +2783,10 @@
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E115" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2776,10 +2797,10 @@
         <v>84</v>
       </c>
       <c r="D116" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E116" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2793,10 +2814,10 @@
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E117" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2807,15 +2828,15 @@
         <v>87</v>
       </c>
       <c r="D118" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="E118" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B119" t="s">
         <v>82</v>
@@ -2824,128 +2845,125 @@
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="E119" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B120" t="s">
         <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="E120" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B121" t="s">
-        <v>87</v>
+        <v>149</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="E121" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D122" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E122" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D123" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E123" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B124" t="s">
+        <v>90</v>
+      </c>
+      <c r="D124" t="s">
+        <v>91</v>
+      </c>
+      <c r="E124" t="s">
         <v>92</v>
-      </c>
-      <c r="D124" t="s">
-        <v>93</v>
-      </c>
-      <c r="E124" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B125" t="s">
+        <v>90</v>
+      </c>
+      <c r="D125" t="s">
+        <v>91</v>
+      </c>
+      <c r="E125" t="s">
         <v>92</v>
-      </c>
-      <c r="D125" t="s">
-        <v>93</v>
-      </c>
-      <c r="E125" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B126" t="s">
-        <v>95</v>
-      </c>
-      <c r="C126">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D126" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E126" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>97</v>
-      </c>
-      <c r="C127">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D127" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E127" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2953,13 +2971,13 @@
         <v>83</v>
       </c>
       <c r="B128" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E128" t="s">
         <v>4</v>
@@ -2970,13 +2988,13 @@
         <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E129" t="s">
         <v>4</v>
@@ -2984,36 +3002,36 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B130" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E130" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B131" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E131" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3021,16 +3039,16 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E132" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3038,16 +3056,16 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E133" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3055,16 +3073,16 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
+        <v>102</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134" t="s">
         <v>103</v>
       </c>
-      <c r="C134">
-        <v>1</v>
-      </c>
-      <c r="D134" t="s">
-        <v>106</v>
-      </c>
       <c r="E134" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3072,64 +3090,64 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
+        <v>102</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135" t="s">
         <v>103</v>
       </c>
-      <c r="C135">
-        <v>1</v>
-      </c>
-      <c r="D135" t="s">
-        <v>106</v>
-      </c>
       <c r="E135" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E136" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E137" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C138">
         <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E138" t="s">
         <v>11</v>
@@ -3137,16 +3155,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B139" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C139">
         <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E139" t="s">
         <v>11</v>
@@ -3154,50 +3172,50 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B140" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D140" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E140" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C141">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D141" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E141" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E142" t="s">
         <v>4</v>
@@ -3205,16 +3223,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B143" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C143">
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -3222,19 +3240,19 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B144" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E144" t="s">
-        <v>110</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -3242,16 +3260,16 @@
         <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E145" t="s">
-        <v>110</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -3259,16 +3277,16 @@
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E146" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3276,16 +3294,16 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E147" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3293,16 +3311,16 @@
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E148" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -3310,16 +3328,16 @@
         <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C149">
         <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E149" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -3327,16 +3345,16 @@
         <v>19</v>
       </c>
       <c r="B150" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E150" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -3344,16 +3362,16 @@
         <v>21</v>
       </c>
       <c r="B151" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C151">
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E151" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -3361,16 +3379,16 @@
         <v>19</v>
       </c>
       <c r="B152" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C152">
         <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E152" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3378,16 +3396,16 @@
         <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C153">
         <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E153" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -3395,16 +3413,16 @@
         <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E154" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3412,16 +3430,16 @@
         <v>21</v>
       </c>
       <c r="B155" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C155">
         <v>1</v>
       </c>
       <c r="D155" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E155" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3429,16 +3447,16 @@
         <v>19</v>
       </c>
       <c r="B156" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C156">
         <v>1</v>
       </c>
       <c r="D156" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E156" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3446,47 +3464,50 @@
         <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C157">
         <v>1</v>
       </c>
       <c r="D157" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E157" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B158" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C158">
         <v>1</v>
       </c>
       <c r="D158" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E158" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B159" t="s">
-        <v>122</v>
+        <v>117</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
       </c>
       <c r="D159" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E159" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -3494,13 +3515,13 @@
         <v>83</v>
       </c>
       <c r="B160" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C160">
         <v>1</v>
       </c>
       <c r="D160" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E160" t="s">
         <v>4</v>
@@ -3511,10 +3532,10 @@
         <v>83</v>
       </c>
       <c r="B161" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D161" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E161" t="s">
         <v>4</v>
@@ -3525,10 +3546,13 @@
         <v>83</v>
       </c>
       <c r="B162" t="s">
-        <v>122</v>
+        <v>107</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
       </c>
       <c r="D162" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E162" t="s">
         <v>4</v>
@@ -3539,13 +3563,10 @@
         <v>83</v>
       </c>
       <c r="B163" t="s">
-        <v>120</v>
-      </c>
-      <c r="C163">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="D163" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E163" t="s">
         <v>4</v>
@@ -3556,13 +3577,10 @@
         <v>83</v>
       </c>
       <c r="B164" t="s">
-        <v>125</v>
-      </c>
-      <c r="C164">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D164" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E164" t="s">
         <v>4</v>
@@ -3570,16 +3588,16 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B165" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D165" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E165" t="s">
         <v>4</v>
@@ -3587,16 +3605,16 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B166" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C166">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D166" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E166" t="s">
         <v>4</v>
@@ -3604,16 +3622,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="B167" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C167">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D167" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E167" t="s">
         <v>4</v>
@@ -3621,16 +3639,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B168" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C168">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D168" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E168" t="s">
         <v>4</v>
@@ -3641,13 +3659,13 @@
         <v>83</v>
       </c>
       <c r="B169" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="C169">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E169" t="s">
         <v>4</v>
@@ -3658,84 +3676,84 @@
         <v>83</v>
       </c>
       <c r="B170" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C170">
         <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E170" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A171" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C171" s="1">
-        <v>2</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>146</v>
+      <c r="A171" t="s">
+        <v>83</v>
+      </c>
+      <c r="B171" t="s">
+        <v>107</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>129</v>
+      </c>
+      <c r="E171" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A172" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C172" s="1">
-        <v>2</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>144</v>
+      <c r="A172" t="s">
+        <v>83</v>
+      </c>
+      <c r="B172" t="s">
+        <v>130</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172" t="s">
+        <v>131</v>
+      </c>
+      <c r="E172" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C173" s="1">
         <v>2</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C174" s="1">
         <v>2</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
@@ -3743,16 +3761,16 @@
         <v>17</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C175" s="1">
         <v>2</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
@@ -3760,58 +3778,62 @@
         <v>20</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C176" s="1">
         <v>2</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C177" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C177" s="1">
+        <v>2</v>
+      </c>
       <c r="D177" s="1" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C178" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C178" s="1">
+        <v>2</v>
+      </c>
       <c r="D178" s="1" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C179" s="1"/>
       <c r="D179" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>11</v>
@@ -3819,14 +3841,14 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C180" s="1"/>
       <c r="D180" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>11</v>
@@ -3837,14 +3859,14 @@
         <v>17</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C181" s="1"/>
       <c r="D181" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
@@ -3852,44 +3874,44 @@
         <v>20</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C182" s="1"/>
       <c r="D182" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C183" s="1"/>
       <c r="D183" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C184" s="1"/>
       <c r="D184" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
@@ -3897,11 +3919,11 @@
         <v>21</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C185" s="1"/>
       <c r="D185" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>11</v>
@@ -3909,14 +3931,14 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C186" s="1"/>
       <c r="D186" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>11</v>
@@ -3924,14 +3946,14 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C187" s="1"/>
       <c r="D187" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>11</v>
@@ -3939,14 +3961,14 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C188" s="1"/>
       <c r="D188" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>11</v>
@@ -3954,14 +3976,14 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C189" s="1"/>
       <c r="D189" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>11</v>
@@ -3969,14 +3991,14 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C190" s="1"/>
       <c r="D190" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>11</v>
@@ -3987,11 +4009,11 @@
         <v>21</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>11</v>
@@ -3999,14 +4021,14 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>11</v>
@@ -4014,16 +4036,14 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>178</v>
+        <v>21</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C193" s="1">
-        <v>2</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C193" s="1"/>
       <c r="D193" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>11</v>
@@ -4034,31 +4054,183 @@
         <v>17</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C194" s="1"/>
       <c r="D194" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C195" s="1">
+        <v>2</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C196" s="1"/>
+      <c r="D196" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C197" s="1">
+        <v>2</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C195" s="1">
-        <v>2</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>3</v>
+      <c r="C198" s="1"/>
+      <c r="D198" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A199" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C199" s="1"/>
+      <c r="D199" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A200" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C200" s="1"/>
+      <c r="D200" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C201" s="1"/>
+      <c r="D201" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C202" s="1"/>
+      <c r="D202" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C203" s="1"/>
+      <c r="D203" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C205" s="1"/>
+      <c r="D205" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (mappings) Include missing mappings
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA11D42-4033-4A71-ADCF-EB96E1EE4C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32662DF7-2C08-4DD4-A350-DF6A1B85B790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="196">
   <si>
     <t>Class</t>
   </si>
@@ -586,6 +586,36 @@
   </si>
   <si>
     <t>outlook-other-item-apis-get-date-time-modified-read</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-end-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-end-appointment-organizer</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-location-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-location-appointment-organizer</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>enhancedLocation</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-add-remove-enhancedlocation-appointment</t>
+  </si>
+  <si>
+    <t>EnhancedLocation</t>
   </si>
 </sst>
 </file>
@@ -661,8 +691,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E205" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E205" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E223" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E223" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -994,11 +1024,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E205"/>
+  <dimension ref="A1:E223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A224" sqref="A224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4233,6 +4263,287 @@
         <v>11</v>
       </c>
     </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C206" s="1"/>
+      <c r="D206" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C207" s="1"/>
+      <c r="D207" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C208" s="1"/>
+      <c r="D208" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A209" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C209" s="1"/>
+      <c r="D209" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A210" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C210" s="1">
+        <v>2</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A211" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C211" s="1"/>
+      <c r="D211" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C212" s="1"/>
+      <c r="D212" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A213" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C213" s="1"/>
+      <c r="D213" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A214" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C214" s="1">
+        <v>2</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A215" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C215" s="1"/>
+      <c r="D215" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A216" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C216" s="1">
+        <v>2</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A217" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C217" s="1"/>
+      <c r="D217" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A218" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C218" s="1"/>
+      <c r="D218" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A219" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C219" s="1">
+        <v>2</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>17</v>
+      </c>
+      <c r="B220" t="s">
+        <v>193</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E220" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A221" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C221" s="1">
+        <v>2</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A222" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C222" s="1"/>
+      <c r="D222" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A223" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C223" s="1">
+        <v>2</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Outlook] (mappings) Include missing mappings (#449)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA11D42-4033-4A71-ADCF-EB96E1EE4C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32662DF7-2C08-4DD4-A350-DF6A1B85B790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="196">
   <si>
     <t>Class</t>
   </si>
@@ -586,6 +586,36 @@
   </si>
   <si>
     <t>outlook-other-item-apis-get-date-time-modified-read</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-end-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-end-appointment-organizer</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-location-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-location-appointment-organizer</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>enhancedLocation</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-add-remove-enhancedlocation-appointment</t>
+  </si>
+  <si>
+    <t>EnhancedLocation</t>
   </si>
 </sst>
 </file>
@@ -661,8 +691,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E205" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E205" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E223" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E223" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -994,11 +1024,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E205"/>
+  <dimension ref="A1:E223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A224" sqref="A224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4233,6 +4263,287 @@
         <v>11</v>
       </c>
     </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C206" s="1"/>
+      <c r="D206" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C207" s="1"/>
+      <c r="D207" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C208" s="1"/>
+      <c r="D208" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A209" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C209" s="1"/>
+      <c r="D209" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A210" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C210" s="1">
+        <v>2</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A211" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C211" s="1"/>
+      <c r="D211" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C212" s="1"/>
+      <c r="D212" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A213" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C213" s="1"/>
+      <c r="D213" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A214" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C214" s="1">
+        <v>2</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A215" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C215" s="1"/>
+      <c r="D215" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A216" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C216" s="1">
+        <v>2</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A217" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C217" s="1"/>
+      <c r="D217" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A218" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C218" s="1"/>
+      <c r="D218" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A219" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C219" s="1">
+        <v>2</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>17</v>
+      </c>
+      <c r="B220" t="s">
+        <v>193</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E220" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A221" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C221" s="1">
+        <v>2</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A222" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C222" s="1"/>
+      <c r="D222" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A223" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C223" s="1">
+        <v>2</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Outlook] (preview) Add mappings for new calendar properties (Compose)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32662DF7-2C08-4DD4-A350-DF6A1B85B790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AC4114-BFA7-4A4C-806C-6A71FA30BA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="205">
   <si>
     <t>Class</t>
   </si>
@@ -616,6 +616,33 @@
   </si>
   <si>
     <t>EnhancedLocation</t>
+  </si>
+  <si>
+    <t>getIsAllDayEvent</t>
+  </si>
+  <si>
+    <t>outlook-calendar-properties-apis</t>
+  </si>
+  <si>
+    <t>isAllDayEvent</t>
+  </si>
+  <si>
+    <t>IsAllDayEvent</t>
+  </si>
+  <si>
+    <t>setIsAllDayEventTrue</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>getSensitivity</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>setSensitivityConfidential</t>
   </si>
 </sst>
 </file>
@@ -691,8 +718,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E223" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E223" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E231" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E231" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1024,11 +1051,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E223"/>
+  <dimension ref="A1:E231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A224" sqref="A224"/>
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4544,6 +4571,134 @@
         <v>16</v>
       </c>
     </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A224" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C224" s="1"/>
+      <c r="D224" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A225" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C225" s="1">
+        <v>2</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A226" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C226" s="1"/>
+      <c r="D226" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A227" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C227" s="1">
+        <v>2</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A228" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C228" s="1"/>
+      <c r="D228" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A229" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C229" s="1">
+        <v>2</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A230" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C230" s="1"/>
+      <c r="D230" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A231" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C231" s="1">
+        <v>2</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Outlook] (preview) Add mappings for new calendar properties (Compose) (#451)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32662DF7-2C08-4DD4-A350-DF6A1B85B790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AC4114-BFA7-4A4C-806C-6A71FA30BA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="205">
   <si>
     <t>Class</t>
   </si>
@@ -616,6 +616,33 @@
   </si>
   <si>
     <t>EnhancedLocation</t>
+  </si>
+  <si>
+    <t>getIsAllDayEvent</t>
+  </si>
+  <si>
+    <t>outlook-calendar-properties-apis</t>
+  </si>
+  <si>
+    <t>isAllDayEvent</t>
+  </si>
+  <si>
+    <t>IsAllDayEvent</t>
+  </si>
+  <si>
+    <t>setIsAllDayEventTrue</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>getSensitivity</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>setSensitivityConfidential</t>
   </si>
 </sst>
 </file>
@@ -691,8 +718,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E223" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E223" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E231" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E231" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1024,11 +1051,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E223"/>
+  <dimension ref="A1:E231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A224" sqref="A224"/>
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4544,6 +4571,134 @@
         <v>16</v>
       </c>
     </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A224" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C224" s="1"/>
+      <c r="D224" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A225" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C225" s="1">
+        <v>2</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A226" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C226" s="1"/>
+      <c r="D226" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A227" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C227" s="1">
+        <v>2</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A228" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C228" s="1"/>
+      <c r="D228" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A229" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C229" s="1">
+        <v>2</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A230" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C230" s="1"/>
+      <c r="D230" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A231" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C231" s="1">
+        <v>2</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Outlook] Shows how to inline base64 image
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22919"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AC4114-BFA7-4A4C-806C-6A71FA30BA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D96EEB-2C83-4C18-8340-667664CF9D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="206">
   <si>
     <t>Class</t>
   </si>
@@ -456,193 +456,196 @@
     <t>setSignatureAsync</t>
   </si>
   <si>
+    <t>getComposeTypeAsync</t>
+  </si>
+  <si>
+    <t>getComposeType</t>
+  </si>
+  <si>
+    <t>disableClientSignatureAsync</t>
+  </si>
+  <si>
+    <t>disableClientSignature</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-to-message-compose</t>
+  </si>
+  <si>
+    <t>setTo</t>
+  </si>
+  <si>
+    <t>setAsync</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-cc-message-compose</t>
+  </si>
+  <si>
+    <t>setCc</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-bcc-message-compose</t>
+  </si>
+  <si>
+    <t>setBcc</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-required-attendees-appointment-organizer</t>
+  </si>
+  <si>
+    <t>setRequiredAttendees</t>
+  </si>
+  <si>
+    <t>setOptionalAttendees</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-optional-attendees-appointment-organizer</t>
+  </si>
+  <si>
+    <t>addMasterCategories</t>
+  </si>
+  <si>
+    <t>removeMasterCategories</t>
+  </si>
+  <si>
+    <t>outlook-categories-work-with-master-categories</t>
+  </si>
+  <si>
+    <t>addCategories</t>
+  </si>
+  <si>
+    <t>removeCategories</t>
+  </si>
+  <si>
+    <t>outlook-categories-work-with-categories</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-subject-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-subject-compose</t>
+  </si>
+  <si>
+    <t>internetMessageId</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-internet-message-id-read</t>
+  </si>
+  <si>
+    <t>itemClass</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-item-class-read</t>
+  </si>
+  <si>
+    <t>itemType</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-item-type</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-start-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-start-appointment-organizer</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>outlook-recurrence-get-set-recurrence-appointment-organizer</t>
+  </si>
+  <si>
+    <t>normalizedSubject</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-normalized-subject-read</t>
+  </si>
+  <si>
+    <t>conversationId</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-conversation-id-message</t>
+  </si>
+  <si>
+    <t>dateTimeCreated</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-date-time-created-read</t>
+  </si>
+  <si>
+    <t>dateTimeModified</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-date-time-modified-read</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-end-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-end-appointment-organizer</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-location-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-location-appointment-organizer</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>enhancedLocation</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-add-remove-enhancedlocation-appointment</t>
+  </si>
+  <si>
+    <t>EnhancedLocation</t>
+  </si>
+  <si>
+    <t>getIsAllDayEvent</t>
+  </si>
+  <si>
+    <t>outlook-calendar-properties-apis</t>
+  </si>
+  <si>
+    <t>isAllDayEvent</t>
+  </si>
+  <si>
+    <t>IsAllDayEvent</t>
+  </si>
+  <si>
+    <t>setIsAllDayEventTrue</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>getSensitivity</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>setSensitivityConfidential</t>
+  </si>
+  <si>
+    <t>setSignatureWithInlineImage</t>
+  </si>
+  <si>
     <t>setSignature</t>
-  </si>
-  <si>
-    <t>getComposeTypeAsync</t>
-  </si>
-  <si>
-    <t>getComposeType</t>
-  </si>
-  <si>
-    <t>disableClientSignatureAsync</t>
-  </si>
-  <si>
-    <t>disableClientSignature</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-to-message-compose</t>
-  </si>
-  <si>
-    <t>setTo</t>
-  </si>
-  <si>
-    <t>setAsync</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-cc-message-compose</t>
-  </si>
-  <si>
-    <t>setCc</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-bcc-message-compose</t>
-  </si>
-  <si>
-    <t>setBcc</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-required-attendees-appointment-organizer</t>
-  </si>
-  <si>
-    <t>setRequiredAttendees</t>
-  </si>
-  <si>
-    <t>setOptionalAttendees</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-optional-attendees-appointment-organizer</t>
-  </si>
-  <si>
-    <t>addMasterCategories</t>
-  </si>
-  <si>
-    <t>removeMasterCategories</t>
-  </si>
-  <si>
-    <t>outlook-categories-work-with-master-categories</t>
-  </si>
-  <si>
-    <t>addCategories</t>
-  </si>
-  <si>
-    <t>removeCategories</t>
-  </si>
-  <si>
-    <t>outlook-categories-work-with-categories</t>
-  </si>
-  <si>
-    <t>subject</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-subject-read</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-set-subject-compose</t>
-  </si>
-  <si>
-    <t>internetMessageId</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-internet-message-id-read</t>
-  </si>
-  <si>
-    <t>itemClass</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-item-class-read</t>
-  </si>
-  <si>
-    <t>itemType</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-item-type</t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-start-read</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-set-start-appointment-organizer</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>outlook-recurrence-get-set-recurrence-appointment-organizer</t>
-  </si>
-  <si>
-    <t>normalizedSubject</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-normalized-subject-read</t>
-  </si>
-  <si>
-    <t>conversationId</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-conversation-id-message</t>
-  </si>
-  <si>
-    <t>dateTimeCreated</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-date-time-created-read</t>
-  </si>
-  <si>
-    <t>dateTimeModified</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-date-time-modified-read</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-end-read</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-set-end-appointment-organizer</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-location-read</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-set-location-appointment-organizer</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>enhancedLocation</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-add-remove-enhancedlocation-appointment</t>
-  </si>
-  <si>
-    <t>EnhancedLocation</t>
-  </si>
-  <si>
-    <t>getIsAllDayEvent</t>
-  </si>
-  <si>
-    <t>outlook-calendar-properties-apis</t>
-  </si>
-  <si>
-    <t>isAllDayEvent</t>
-  </si>
-  <si>
-    <t>IsAllDayEvent</t>
-  </si>
-  <si>
-    <t>setIsAllDayEventTrue</t>
-  </si>
-  <si>
-    <t>sensitivity</t>
-  </si>
-  <si>
-    <t>getSensitivity</t>
-  </si>
-  <si>
-    <t>Sensitivity</t>
-  </si>
-  <si>
-    <t>setSensitivityConfidential</t>
   </si>
 </sst>
 </file>
@@ -718,8 +721,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E231" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E231" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E234" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E234" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1051,11 +1054,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E231"/>
+  <dimension ref="A1:E234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1381,7 +1384,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1398,7 +1401,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1412,10 +1415,10 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" t="s">
         <v>152</v>
-      </c>
-      <c r="E21" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1423,16 +1426,16 @@
         <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" t="s">
         <v>152</v>
-      </c>
-      <c r="E22" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1443,7 +1446,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1460,7 +1463,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1474,10 +1477,10 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" t="s">
         <v>150</v>
-      </c>
-      <c r="E25" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1485,16 +1488,16 @@
         <v>132</v>
       </c>
       <c r="B26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>149</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>150</v>
-      </c>
-      <c r="E26" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1578,7 +1581,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1595,7 +1598,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1609,10 +1612,10 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1620,16 +1623,16 @@
         <v>132</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1699,7 +1702,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
@@ -1716,7 +1719,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
@@ -1730,10 +1733,10 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" t="s">
         <v>154</v>
-      </c>
-      <c r="E42" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1741,16 +1744,16 @@
         <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" t="s">
         <v>154</v>
-      </c>
-      <c r="E43" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1775,7 +1778,7 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
@@ -1792,7 +1795,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -1807,10 +1810,10 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1818,16 +1821,16 @@
         <v>132</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" t="s">
         <v>147</v>
-      </c>
-      <c r="E48" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -2406,16 +2409,16 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C87">
-        <v>2</v>
-      </c>
-      <c r="D87" t="s">
-        <v>68</v>
+        <v>1</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>204</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -2423,16 +2426,16 @@
         <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C88">
-        <v>2</v>
-      </c>
-      <c r="D88" t="s">
-        <v>68</v>
+        <v>1</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="E88" t="s">
-        <v>11</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2440,16 +2443,16 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D89" t="s">
         <v>68</v>
       </c>
       <c r="E89" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -2457,16 +2460,16 @@
         <v>20</v>
       </c>
       <c r="B90" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
         <v>68</v>
       </c>
       <c r="E90" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -2474,38 +2477,38 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="E91" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B92" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="E92" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
         <v>76</v>
@@ -2522,7 +2525,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B94" t="s">
         <v>76</v>
@@ -2539,13 +2542,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B95" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="E95" t="s">
         <v>4</v>
@@ -2556,10 +2562,13 @@
         <v>21</v>
       </c>
       <c r="B96" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="E96" t="s">
         <v>4</v>
@@ -2567,41 +2576,41 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B97" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D97" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="E97" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B98" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D98" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="E98" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B99" t="s">
         <v>79</v>
       </c>
       <c r="D99" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E99" t="s">
         <v>80</v>
@@ -2609,13 +2618,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B100" t="s">
         <v>79</v>
       </c>
       <c r="D100" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E100" t="s">
         <v>80</v>
@@ -2623,16 +2632,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="B101" t="s">
-        <v>82</v>
-      </c>
-      <c r="C101">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D101" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E101" t="s">
         <v>80</v>
@@ -2640,179 +2646,179 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B102" t="s">
         <v>79</v>
       </c>
       <c r="D102" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E102" t="s">
-        <v>161</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B103" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E103" t="s">
-        <v>161</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B104" t="s">
         <v>79</v>
       </c>
       <c r="D104" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E104" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B105" t="s">
         <v>79</v>
       </c>
       <c r="D105" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E105" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="B106" t="s">
-        <v>56</v>
-      </c>
-      <c r="C106">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D106" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E106" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B107" t="s">
         <v>79</v>
       </c>
       <c r="D107" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E107" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B108" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E108" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B109" t="s">
         <v>79</v>
       </c>
       <c r="D109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E109" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B110" t="s">
         <v>79</v>
       </c>
       <c r="D110" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E110" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="B111" t="s">
-        <v>66</v>
-      </c>
-      <c r="C111">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D111" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E111" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B112" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D112" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E112" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B113" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C113">
         <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E113" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2823,10 +2829,10 @@
         <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E114" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2834,16 +2840,16 @@
         <v>86</v>
       </c>
       <c r="B115" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C115">
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E115" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2854,10 +2860,10 @@
         <v>84</v>
       </c>
       <c r="D116" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E116" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2865,47 +2871,47 @@
         <v>86</v>
       </c>
       <c r="B117" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C117">
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E117" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D118" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="E118" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B119" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C119">
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="E119" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2916,10 +2922,10 @@
         <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E120" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2927,77 +2933,80 @@
         <v>88</v>
       </c>
       <c r="B121" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E121" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B122" t="s">
         <v>87</v>
       </c>
       <c r="D122" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="E122" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B123" t="s">
-        <v>87</v>
+        <v>148</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="E123" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D124" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E124" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D125" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E125" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B126" t="s">
         <v>90</v>
@@ -3011,7 +3020,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B127" t="s">
         <v>90</v>
@@ -3025,36 +3034,30 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>93</v>
-      </c>
-      <c r="C128">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D128" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E128" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>95</v>
-      </c>
-      <c r="C129">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D129" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E129" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -3062,13 +3065,13 @@
         <v>83</v>
       </c>
       <c r="B130" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E130" t="s">
         <v>4</v>
@@ -3079,13 +3082,13 @@
         <v>83</v>
       </c>
       <c r="B131" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E131" t="s">
         <v>4</v>
@@ -3093,36 +3096,36 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B132" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E132" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B133" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E133" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3130,7 +3133,7 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -3139,7 +3142,7 @@
         <v>103</v>
       </c>
       <c r="E134" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3147,7 +3150,7 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -3156,7 +3159,7 @@
         <v>103</v>
       </c>
       <c r="E135" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3164,16 +3167,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E136" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3181,55 +3184,55 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E137" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C138">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E138" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E139" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B140" t="s">
         <v>106</v>
@@ -3246,7 +3249,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B141" t="s">
         <v>106</v>
@@ -3263,41 +3266,41 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B142" t="s">
         <v>106</v>
       </c>
       <c r="C142">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D142" t="s">
         <v>105</v>
       </c>
       <c r="E142" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B143" t="s">
         <v>106</v>
       </c>
       <c r="C143">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D143" t="s">
         <v>105</v>
       </c>
       <c r="E143" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B144" t="s">
         <v>106</v>
@@ -3314,7 +3317,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B145" t="s">
         <v>106</v>
@@ -3331,19 +3334,19 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B146" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E146" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3351,16 +3354,16 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E147" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3368,7 +3371,7 @@
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -3377,7 +3380,7 @@
         <v>109</v>
       </c>
       <c r="E148" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -3385,7 +3388,7 @@
         <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -3394,7 +3397,7 @@
         <v>109</v>
       </c>
       <c r="E149" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -3402,16 +3405,16 @@
         <v>19</v>
       </c>
       <c r="B150" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E150" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -3419,16 +3422,16 @@
         <v>21</v>
       </c>
       <c r="B151" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C151">
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E151" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -3436,7 +3439,7 @@
         <v>19</v>
       </c>
       <c r="B152" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -3445,7 +3448,7 @@
         <v>112</v>
       </c>
       <c r="E152" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3453,7 +3456,7 @@
         <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -3462,7 +3465,7 @@
         <v>112</v>
       </c>
       <c r="E153" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -3470,7 +3473,7 @@
         <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -3479,7 +3482,7 @@
         <v>112</v>
       </c>
       <c r="E154" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3487,7 +3490,7 @@
         <v>21</v>
       </c>
       <c r="B155" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -3496,7 +3499,7 @@
         <v>112</v>
       </c>
       <c r="E155" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3504,16 +3507,16 @@
         <v>19</v>
       </c>
       <c r="B156" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C156">
         <v>1</v>
       </c>
       <c r="D156" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E156" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3521,16 +3524,16 @@
         <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C157">
         <v>1</v>
       </c>
       <c r="D157" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E157" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -3538,7 +3541,7 @@
         <v>19</v>
       </c>
       <c r="B158" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -3547,7 +3550,7 @@
         <v>116</v>
       </c>
       <c r="E158" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -3555,7 +3558,7 @@
         <v>21</v>
       </c>
       <c r="B159" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -3564,38 +3567,41 @@
         <v>116</v>
       </c>
       <c r="E159" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B160" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C160">
         <v>1</v>
       </c>
       <c r="D160" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E160" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B161" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
       </c>
       <c r="D161" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E161" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
@@ -3603,7 +3609,7 @@
         <v>83</v>
       </c>
       <c r="B162" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C162">
         <v>1</v>
@@ -3620,10 +3626,10 @@
         <v>83</v>
       </c>
       <c r="B163" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D163" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E163" t="s">
         <v>4</v>
@@ -3634,10 +3640,13 @@
         <v>83</v>
       </c>
       <c r="B164" t="s">
-        <v>120</v>
+        <v>107</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
       </c>
       <c r="D164" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E164" t="s">
         <v>4</v>
@@ -3648,10 +3657,7 @@
         <v>83</v>
       </c>
       <c r="B165" t="s">
-        <v>118</v>
-      </c>
-      <c r="C165">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="D165" t="s">
         <v>122</v>
@@ -3665,10 +3671,7 @@
         <v>83</v>
       </c>
       <c r="B166" t="s">
-        <v>123</v>
-      </c>
-      <c r="C166">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D166" t="s">
         <v>122</v>
@@ -3679,16 +3682,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B167" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C167">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D167" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E167" t="s">
         <v>4</v>
@@ -3696,16 +3699,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B168" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C168">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D168" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E168" t="s">
         <v>4</v>
@@ -3713,16 +3716,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="B169" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C169">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D169" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E169" t="s">
         <v>4</v>
@@ -3730,16 +3733,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B170" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C170">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D170" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E170" t="s">
         <v>4</v>
@@ -3750,13 +3753,13 @@
         <v>83</v>
       </c>
       <c r="B171" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="C171">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E171" t="s">
         <v>4</v>
@@ -3767,58 +3770,58 @@
         <v>83</v>
       </c>
       <c r="B172" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C172">
         <v>1</v>
       </c>
       <c r="D172" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E172" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A173" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C173" s="1">
-        <v>2</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>144</v>
+      <c r="A173" t="s">
+        <v>83</v>
+      </c>
+      <c r="B173" t="s">
+        <v>107</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+      <c r="D173" t="s">
+        <v>129</v>
+      </c>
+      <c r="E173" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A174" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C174" s="1">
-        <v>2</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>142</v>
+      <c r="A174" t="s">
+        <v>83</v>
+      </c>
+      <c r="B174" t="s">
+        <v>130</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+      <c r="D174" t="s">
+        <v>131</v>
+      </c>
+      <c r="E174" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C175" s="1">
         <v>2</v>
@@ -3827,32 +3830,32 @@
         <v>138</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C176" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C177" s="1">
         <v>2</v>
@@ -3861,15 +3864,15 @@
         <v>138</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>139</v>
+        <v>205</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C178" s="1">
         <v>2</v>
@@ -3878,64 +3881,70 @@
         <v>138</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C179" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="C179" s="1">
+        <v>2</v>
+      </c>
       <c r="D179" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C180" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C180" s="1">
+        <v>2</v>
+      </c>
       <c r="D180" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C181" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C181" s="1">
+        <v>2</v>
+      </c>
       <c r="D181" s="1" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C182" s="1"/>
       <c r="D182" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>11</v>
@@ -3943,44 +3952,44 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C183" s="1"/>
       <c r="D183" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C184" s="1"/>
       <c r="D184" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C185" s="1"/>
       <c r="D185" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>11</v>
@@ -3988,44 +3997,44 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C186" s="1"/>
       <c r="D186" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C187" s="1"/>
       <c r="D187" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C188" s="1"/>
       <c r="D188" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>11</v>
@@ -4036,11 +4045,11 @@
         <v>19</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C189" s="1"/>
       <c r="D189" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>11</v>
@@ -4048,14 +4057,14 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C190" s="1"/>
       <c r="D190" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>11</v>
@@ -4063,14 +4072,14 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>11</v>
@@ -4081,11 +4090,11 @@
         <v>19</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>11</v>
@@ -4093,14 +4102,14 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C193" s="1"/>
       <c r="D193" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>11</v>
@@ -4108,14 +4117,14 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C194" s="1"/>
       <c r="D194" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>11</v>
@@ -4123,16 +4132,14 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>176</v>
+        <v>19</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C195" s="1">
-        <v>2</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C195" s="1"/>
       <c r="D195" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>11</v>
@@ -4140,46 +4147,46 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C196" s="1"/>
       <c r="D196" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C197" s="1">
-        <v>2</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C198" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C198" s="1">
+        <v>2</v>
+      </c>
       <c r="D198" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>11</v>
@@ -4187,44 +4194,46 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C199" s="1"/>
       <c r="D199" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>20</v>
+        <v>175</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C200" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C200" s="1">
+        <v>2</v>
+      </c>
       <c r="D200" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C201" s="1"/>
       <c r="D201" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>11</v>
@@ -4232,14 +4241,14 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C202" s="1"/>
       <c r="D202" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>11</v>
@@ -4247,14 +4256,14 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C203" s="1"/>
       <c r="D203" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>11</v>
@@ -4262,14 +4271,14 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>11</v>
@@ -4277,14 +4286,14 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>11</v>
@@ -4292,14 +4301,14 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>11</v>
@@ -4307,14 +4316,14 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>11</v>
@@ -4322,14 +4331,14 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C208" s="1"/>
       <c r="D208" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>11</v>
@@ -4337,46 +4346,44 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C209" s="1"/>
       <c r="D209" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
-        <v>176</v>
+        <v>21</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C210" s="1">
-        <v>2</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C210" s="1"/>
       <c r="D210" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>11</v>
@@ -4384,46 +4391,46 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C212" s="1"/>
       <c r="D212" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>17</v>
+        <v>175</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C213" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C213" s="1">
+        <v>2</v>
+      </c>
       <c r="D213" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>192</v>
+        <v>19</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C214" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>11</v>
@@ -4431,46 +4438,46 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
-        <v>192</v>
+        <v>17</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C216" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C217" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C217" s="1">
+        <v>2</v>
+      </c>
       <c r="D217" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>11</v>
@@ -4478,225 +4485,272 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C218" s="1"/>
       <c r="D218" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="C219" s="1">
         <v>2</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E219" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A220" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E220" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A220" t="s">
-        <v>17</v>
-      </c>
-      <c r="B220" t="s">
-        <v>193</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E220" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
-        <v>195</v>
+        <v>19</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C221" s="1">
-        <v>2</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C221" s="1"/>
       <c r="D221" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B222" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C222" s="1">
+        <v>2</v>
+      </c>
+      <c r="D222" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C222" s="1"/>
-      <c r="D222" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="E222" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A223" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C223" s="1">
-        <v>2</v>
+      <c r="A223" t="s">
+        <v>17</v>
+      </c>
+      <c r="B223" t="s">
+        <v>192</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>16</v>
+        <v>193</v>
+      </c>
+      <c r="E223" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C224" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="C224" s="1">
+        <v>2</v>
+      </c>
       <c r="D224" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>196</v>
+        <v>69</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>199</v>
+        <v>17</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C225" s="1">
-        <v>2</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C225" s="1"/>
       <c r="D225" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>196</v>
+        <v>16</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C226" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="C226" s="1">
+        <v>2</v>
+      </c>
       <c r="D226" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>200</v>
+        <v>16</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
-        <v>199</v>
+        <v>17</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C227" s="1">
-        <v>2</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="C227" s="1"/>
       <c r="D227" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
-        <v>17</v>
+        <v>198</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C228" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C228" s="1">
+        <v>2</v>
+      </c>
       <c r="D228" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
-        <v>203</v>
+        <v>17</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C229" s="1">
-        <v>2</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="C229" s="1"/>
       <c r="D229" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
-        <v>17</v>
+        <v>198</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C230" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C230" s="1">
+        <v>2</v>
+      </c>
       <c r="D230" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C231" s="1"/>
+      <c r="D231" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A232" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C232" s="1">
+        <v>2</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A233" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C233" s="1"/>
+      <c r="D233" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E233" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B231" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C231" s="1">
-        <v>2</v>
-      </c>
-      <c r="D231" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>204</v>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A234" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C234" s="1">
+        <v>2</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] Shows how to inline base64 image (#457)
* [Outlook] Shows how to inline base64 image

* Add comment based on feedback
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22919"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AC4114-BFA7-4A4C-806C-6A71FA30BA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D96EEB-2C83-4C18-8340-667664CF9D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="206">
   <si>
     <t>Class</t>
   </si>
@@ -456,193 +456,196 @@
     <t>setSignatureAsync</t>
   </si>
   <si>
+    <t>getComposeTypeAsync</t>
+  </si>
+  <si>
+    <t>getComposeType</t>
+  </si>
+  <si>
+    <t>disableClientSignatureAsync</t>
+  </si>
+  <si>
+    <t>disableClientSignature</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-to-message-compose</t>
+  </si>
+  <si>
+    <t>setTo</t>
+  </si>
+  <si>
+    <t>setAsync</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-cc-message-compose</t>
+  </si>
+  <si>
+    <t>setCc</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-bcc-message-compose</t>
+  </si>
+  <si>
+    <t>setBcc</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-required-attendees-appointment-organizer</t>
+  </si>
+  <si>
+    <t>setRequiredAttendees</t>
+  </si>
+  <si>
+    <t>setOptionalAttendees</t>
+  </si>
+  <si>
+    <t>outlook-recipients-and-attendees-get-set-optional-attendees-appointment-organizer</t>
+  </si>
+  <si>
+    <t>addMasterCategories</t>
+  </si>
+  <si>
+    <t>removeMasterCategories</t>
+  </si>
+  <si>
+    <t>outlook-categories-work-with-master-categories</t>
+  </si>
+  <si>
+    <t>addCategories</t>
+  </si>
+  <si>
+    <t>removeCategories</t>
+  </si>
+  <si>
+    <t>outlook-categories-work-with-categories</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-subject-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-subject-compose</t>
+  </si>
+  <si>
+    <t>internetMessageId</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-internet-message-id-read</t>
+  </si>
+  <si>
+    <t>itemClass</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-item-class-read</t>
+  </si>
+  <si>
+    <t>itemType</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-item-type</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-start-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-start-appointment-organizer</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>outlook-recurrence-get-set-recurrence-appointment-organizer</t>
+  </si>
+  <si>
+    <t>normalizedSubject</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-normalized-subject-read</t>
+  </si>
+  <si>
+    <t>conversationId</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-conversation-id-message</t>
+  </si>
+  <si>
+    <t>dateTimeCreated</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-date-time-created-read</t>
+  </si>
+  <si>
+    <t>dateTimeModified</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-date-time-modified-read</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-end-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-end-appointment-organizer</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-location-read</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-set-location-appointment-organizer</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>enhancedLocation</t>
+  </si>
+  <si>
+    <t>outlook-other-item-apis-get-add-remove-enhancedlocation-appointment</t>
+  </si>
+  <si>
+    <t>EnhancedLocation</t>
+  </si>
+  <si>
+    <t>getIsAllDayEvent</t>
+  </si>
+  <si>
+    <t>outlook-calendar-properties-apis</t>
+  </si>
+  <si>
+    <t>isAllDayEvent</t>
+  </si>
+  <si>
+    <t>IsAllDayEvent</t>
+  </si>
+  <si>
+    <t>setIsAllDayEventTrue</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>getSensitivity</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>setSensitivityConfidential</t>
+  </si>
+  <si>
+    <t>setSignatureWithInlineImage</t>
+  </si>
+  <si>
     <t>setSignature</t>
-  </si>
-  <si>
-    <t>getComposeTypeAsync</t>
-  </si>
-  <si>
-    <t>getComposeType</t>
-  </si>
-  <si>
-    <t>disableClientSignatureAsync</t>
-  </si>
-  <si>
-    <t>disableClientSignature</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-to-message-compose</t>
-  </si>
-  <si>
-    <t>setTo</t>
-  </si>
-  <si>
-    <t>setAsync</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-cc-message-compose</t>
-  </si>
-  <si>
-    <t>setCc</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-bcc-message-compose</t>
-  </si>
-  <si>
-    <t>setBcc</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-required-attendees-appointment-organizer</t>
-  </si>
-  <si>
-    <t>setRequiredAttendees</t>
-  </si>
-  <si>
-    <t>setOptionalAttendees</t>
-  </si>
-  <si>
-    <t>outlook-recipients-and-attendees-get-set-optional-attendees-appointment-organizer</t>
-  </si>
-  <si>
-    <t>addMasterCategories</t>
-  </si>
-  <si>
-    <t>removeMasterCategories</t>
-  </si>
-  <si>
-    <t>outlook-categories-work-with-master-categories</t>
-  </si>
-  <si>
-    <t>addCategories</t>
-  </si>
-  <si>
-    <t>removeCategories</t>
-  </si>
-  <si>
-    <t>outlook-categories-work-with-categories</t>
-  </si>
-  <si>
-    <t>subject</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-subject-read</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-set-subject-compose</t>
-  </si>
-  <si>
-    <t>internetMessageId</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-internet-message-id-read</t>
-  </si>
-  <si>
-    <t>itemClass</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-item-class-read</t>
-  </si>
-  <si>
-    <t>itemType</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-item-type</t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-start-read</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-set-start-appointment-organizer</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>outlook-recurrence-get-set-recurrence-appointment-organizer</t>
-  </si>
-  <si>
-    <t>normalizedSubject</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-normalized-subject-read</t>
-  </si>
-  <si>
-    <t>conversationId</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-conversation-id-message</t>
-  </si>
-  <si>
-    <t>dateTimeCreated</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-date-time-created-read</t>
-  </si>
-  <si>
-    <t>dateTimeModified</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-date-time-modified-read</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-end-read</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-set-end-appointment-organizer</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-location-read</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-set-location-appointment-organizer</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>enhancedLocation</t>
-  </si>
-  <si>
-    <t>outlook-other-item-apis-get-add-remove-enhancedlocation-appointment</t>
-  </si>
-  <si>
-    <t>EnhancedLocation</t>
-  </si>
-  <si>
-    <t>getIsAllDayEvent</t>
-  </si>
-  <si>
-    <t>outlook-calendar-properties-apis</t>
-  </si>
-  <si>
-    <t>isAllDayEvent</t>
-  </si>
-  <si>
-    <t>IsAllDayEvent</t>
-  </si>
-  <si>
-    <t>setIsAllDayEventTrue</t>
-  </si>
-  <si>
-    <t>sensitivity</t>
-  </si>
-  <si>
-    <t>getSensitivity</t>
-  </si>
-  <si>
-    <t>Sensitivity</t>
-  </si>
-  <si>
-    <t>setSensitivityConfidential</t>
   </si>
 </sst>
 </file>
@@ -718,8 +721,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E231" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E231" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E234" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E234" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1051,11 +1054,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E231"/>
+  <dimension ref="A1:E234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1381,7 +1384,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
@@ -1398,7 +1401,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1412,10 +1415,10 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" t="s">
         <v>152</v>
-      </c>
-      <c r="E21" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1423,16 +1426,16 @@
         <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" t="s">
         <v>152</v>
-      </c>
-      <c r="E22" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1443,7 +1446,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1460,7 +1463,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1474,10 +1477,10 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" t="s">
         <v>150</v>
-      </c>
-      <c r="E25" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1485,16 +1488,16 @@
         <v>132</v>
       </c>
       <c r="B26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>149</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>150</v>
-      </c>
-      <c r="E26" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1578,7 +1581,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1595,7 +1598,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1609,10 +1612,10 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1620,16 +1623,16 @@
         <v>132</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1699,7 +1702,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
@@ -1716,7 +1719,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
@@ -1730,10 +1733,10 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" t="s">
         <v>154</v>
-      </c>
-      <c r="E42" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1741,16 +1744,16 @@
         <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" t="s">
         <v>154</v>
-      </c>
-      <c r="E43" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1775,7 +1778,7 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
@@ -1792,7 +1795,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -1807,10 +1810,10 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1818,16 +1821,16 @@
         <v>132</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" t="s">
         <v>147</v>
-      </c>
-      <c r="E48" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -2406,16 +2409,16 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C87">
-        <v>2</v>
-      </c>
-      <c r="D87" t="s">
-        <v>68</v>
+        <v>1</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>204</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -2423,16 +2426,16 @@
         <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C88">
-        <v>2</v>
-      </c>
-      <c r="D88" t="s">
-        <v>68</v>
+        <v>1</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="E88" t="s">
-        <v>11</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2440,16 +2443,16 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D89" t="s">
         <v>68</v>
       </c>
       <c r="E89" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -2457,16 +2460,16 @@
         <v>20</v>
       </c>
       <c r="B90" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
         <v>68</v>
       </c>
       <c r="E90" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -2474,38 +2477,38 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="E91" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B92" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="E92" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
         <v>76</v>
@@ -2522,7 +2525,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B94" t="s">
         <v>76</v>
@@ -2539,13 +2542,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B95" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="E95" t="s">
         <v>4</v>
@@ -2556,10 +2562,13 @@
         <v>21</v>
       </c>
       <c r="B96" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="E96" t="s">
         <v>4</v>
@@ -2567,41 +2576,41 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B97" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D97" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="E97" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B98" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D98" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="E98" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B99" t="s">
         <v>79</v>
       </c>
       <c r="D99" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E99" t="s">
         <v>80</v>
@@ -2609,13 +2618,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B100" t="s">
         <v>79</v>
       </c>
       <c r="D100" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E100" t="s">
         <v>80</v>
@@ -2623,16 +2632,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="B101" t="s">
-        <v>82</v>
-      </c>
-      <c r="C101">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D101" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E101" t="s">
         <v>80</v>
@@ -2640,179 +2646,179 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B102" t="s">
         <v>79</v>
       </c>
       <c r="D102" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E102" t="s">
-        <v>161</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B103" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E103" t="s">
-        <v>161</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B104" t="s">
         <v>79</v>
       </c>
       <c r="D104" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E104" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B105" t="s">
         <v>79</v>
       </c>
       <c r="D105" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E105" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="B106" t="s">
-        <v>56</v>
-      </c>
-      <c r="C106">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D106" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E106" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B107" t="s">
         <v>79</v>
       </c>
       <c r="D107" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E107" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B108" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E108" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B109" t="s">
         <v>79</v>
       </c>
       <c r="D109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E109" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B110" t="s">
         <v>79</v>
       </c>
       <c r="D110" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E110" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="B111" t="s">
-        <v>66</v>
-      </c>
-      <c r="C111">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D111" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E111" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B112" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D112" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E112" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B113" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C113">
         <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E113" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2823,10 +2829,10 @@
         <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E114" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2834,16 +2840,16 @@
         <v>86</v>
       </c>
       <c r="B115" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C115">
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E115" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2854,10 +2860,10 @@
         <v>84</v>
       </c>
       <c r="D116" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E116" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2865,47 +2871,47 @@
         <v>86</v>
       </c>
       <c r="B117" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C117">
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E117" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D118" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="E118" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B119" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C119">
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="E119" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2916,10 +2922,10 @@
         <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E120" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2927,77 +2933,80 @@
         <v>88</v>
       </c>
       <c r="B121" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E121" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B122" t="s">
         <v>87</v>
       </c>
       <c r="D122" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="E122" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B123" t="s">
-        <v>87</v>
+        <v>148</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="E123" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D124" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E124" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D125" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E125" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B126" t="s">
         <v>90</v>
@@ -3011,7 +3020,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B127" t="s">
         <v>90</v>
@@ -3025,36 +3034,30 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>93</v>
-      </c>
-      <c r="C128">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D128" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E128" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>95</v>
-      </c>
-      <c r="C129">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D129" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E129" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -3062,13 +3065,13 @@
         <v>83</v>
       </c>
       <c r="B130" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E130" t="s">
         <v>4</v>
@@ -3079,13 +3082,13 @@
         <v>83</v>
       </c>
       <c r="B131" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E131" t="s">
         <v>4</v>
@@ -3093,36 +3096,36 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B132" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E132" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B133" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E133" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -3130,7 +3133,7 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -3139,7 +3142,7 @@
         <v>103</v>
       </c>
       <c r="E134" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -3147,7 +3150,7 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -3156,7 +3159,7 @@
         <v>103</v>
       </c>
       <c r="E135" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -3164,16 +3167,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E136" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -3181,55 +3184,55 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E137" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C138">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E138" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E139" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B140" t="s">
         <v>106</v>
@@ -3246,7 +3249,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B141" t="s">
         <v>106</v>
@@ -3263,41 +3266,41 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B142" t="s">
         <v>106</v>
       </c>
       <c r="C142">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D142" t="s">
         <v>105</v>
       </c>
       <c r="E142" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B143" t="s">
         <v>106</v>
       </c>
       <c r="C143">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D143" t="s">
         <v>105</v>
       </c>
       <c r="E143" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B144" t="s">
         <v>106</v>
@@ -3314,7 +3317,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B145" t="s">
         <v>106</v>
@@ -3331,19 +3334,19 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B146" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E146" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3351,16 +3354,16 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E147" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3368,7 +3371,7 @@
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -3377,7 +3380,7 @@
         <v>109</v>
       </c>
       <c r="E148" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -3385,7 +3388,7 @@
         <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -3394,7 +3397,7 @@
         <v>109</v>
       </c>
       <c r="E149" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -3402,16 +3405,16 @@
         <v>19</v>
       </c>
       <c r="B150" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E150" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -3419,16 +3422,16 @@
         <v>21</v>
       </c>
       <c r="B151" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C151">
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E151" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -3436,7 +3439,7 @@
         <v>19</v>
       </c>
       <c r="B152" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -3445,7 +3448,7 @@
         <v>112</v>
       </c>
       <c r="E152" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3453,7 +3456,7 @@
         <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -3462,7 +3465,7 @@
         <v>112</v>
       </c>
       <c r="E153" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -3470,7 +3473,7 @@
         <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -3479,7 +3482,7 @@
         <v>112</v>
       </c>
       <c r="E154" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3487,7 +3490,7 @@
         <v>21</v>
       </c>
       <c r="B155" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -3496,7 +3499,7 @@
         <v>112</v>
       </c>
       <c r="E155" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3504,16 +3507,16 @@
         <v>19</v>
       </c>
       <c r="B156" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C156">
         <v>1</v>
       </c>
       <c r="D156" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E156" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3521,16 +3524,16 @@
         <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C157">
         <v>1</v>
       </c>
       <c r="D157" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E157" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -3538,7 +3541,7 @@
         <v>19</v>
       </c>
       <c r="B158" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -3547,7 +3550,7 @@
         <v>116</v>
       </c>
       <c r="E158" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -3555,7 +3558,7 @@
         <v>21</v>
       </c>
       <c r="B159" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -3564,38 +3567,41 @@
         <v>116</v>
       </c>
       <c r="E159" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B160" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C160">
         <v>1</v>
       </c>
       <c r="D160" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E160" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B161" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
       </c>
       <c r="D161" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E161" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
@@ -3603,7 +3609,7 @@
         <v>83</v>
       </c>
       <c r="B162" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C162">
         <v>1</v>
@@ -3620,10 +3626,10 @@
         <v>83</v>
       </c>
       <c r="B163" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D163" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E163" t="s">
         <v>4</v>
@@ -3634,10 +3640,13 @@
         <v>83</v>
       </c>
       <c r="B164" t="s">
-        <v>120</v>
+        <v>107</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
       </c>
       <c r="D164" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E164" t="s">
         <v>4</v>
@@ -3648,10 +3657,7 @@
         <v>83</v>
       </c>
       <c r="B165" t="s">
-        <v>118</v>
-      </c>
-      <c r="C165">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="D165" t="s">
         <v>122</v>
@@ -3665,10 +3671,7 @@
         <v>83</v>
       </c>
       <c r="B166" t="s">
-        <v>123</v>
-      </c>
-      <c r="C166">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D166" t="s">
         <v>122</v>
@@ -3679,16 +3682,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B167" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C167">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D167" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E167" t="s">
         <v>4</v>
@@ -3696,16 +3699,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B168" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C168">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D168" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E168" t="s">
         <v>4</v>
@@ -3713,16 +3716,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="B169" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C169">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D169" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E169" t="s">
         <v>4</v>
@@ -3730,16 +3733,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B170" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C170">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D170" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E170" t="s">
         <v>4</v>
@@ -3750,13 +3753,13 @@
         <v>83</v>
       </c>
       <c r="B171" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="C171">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E171" t="s">
         <v>4</v>
@@ -3767,58 +3770,58 @@
         <v>83</v>
       </c>
       <c r="B172" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C172">
         <v>1</v>
       </c>
       <c r="D172" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E172" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A173" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C173" s="1">
-        <v>2</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>144</v>
+      <c r="A173" t="s">
+        <v>83</v>
+      </c>
+      <c r="B173" t="s">
+        <v>107</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+      <c r="D173" t="s">
+        <v>129</v>
+      </c>
+      <c r="E173" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A174" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C174" s="1">
-        <v>2</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>142</v>
+      <c r="A174" t="s">
+        <v>83</v>
+      </c>
+      <c r="B174" t="s">
+        <v>130</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+      <c r="D174" t="s">
+        <v>131</v>
+      </c>
+      <c r="E174" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C175" s="1">
         <v>2</v>
@@ -3827,32 +3830,32 @@
         <v>138</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C176" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C177" s="1">
         <v>2</v>
@@ -3861,15 +3864,15 @@
         <v>138</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>139</v>
+        <v>205</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C178" s="1">
         <v>2</v>
@@ -3878,64 +3881,70 @@
         <v>138</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C179" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="C179" s="1">
+        <v>2</v>
+      </c>
       <c r="D179" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C180" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C180" s="1">
+        <v>2</v>
+      </c>
       <c r="D180" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C181" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C181" s="1">
+        <v>2</v>
+      </c>
       <c r="D181" s="1" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C182" s="1"/>
       <c r="D182" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>11</v>
@@ -3943,44 +3952,44 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C183" s="1"/>
       <c r="D183" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C184" s="1"/>
       <c r="D184" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C185" s="1"/>
       <c r="D185" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>11</v>
@@ -3988,44 +3997,44 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C186" s="1"/>
       <c r="D186" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C187" s="1"/>
       <c r="D187" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C188" s="1"/>
       <c r="D188" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>11</v>
@@ -4036,11 +4045,11 @@
         <v>19</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C189" s="1"/>
       <c r="D189" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>11</v>
@@ -4048,14 +4057,14 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C190" s="1"/>
       <c r="D190" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>11</v>
@@ -4063,14 +4072,14 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>11</v>
@@ -4081,11 +4090,11 @@
         <v>19</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>11</v>
@@ -4093,14 +4102,14 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C193" s="1"/>
       <c r="D193" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>11</v>
@@ -4108,14 +4117,14 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C194" s="1"/>
       <c r="D194" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>11</v>
@@ -4123,16 +4132,14 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>176</v>
+        <v>19</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C195" s="1">
-        <v>2</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C195" s="1"/>
       <c r="D195" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>11</v>
@@ -4140,46 +4147,46 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C196" s="1"/>
       <c r="D196" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C197" s="1">
-        <v>2</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C198" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C198" s="1">
+        <v>2</v>
+      </c>
       <c r="D198" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>11</v>
@@ -4187,44 +4194,46 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C199" s="1"/>
       <c r="D199" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>20</v>
+        <v>175</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C200" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C200" s="1">
+        <v>2</v>
+      </c>
       <c r="D200" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C201" s="1"/>
       <c r="D201" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>11</v>
@@ -4232,14 +4241,14 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C202" s="1"/>
       <c r="D202" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>11</v>
@@ -4247,14 +4256,14 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C203" s="1"/>
       <c r="D203" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>11</v>
@@ -4262,14 +4271,14 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>11</v>
@@ -4277,14 +4286,14 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>11</v>
@@ -4292,14 +4301,14 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>11</v>
@@ -4307,14 +4316,14 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>11</v>
@@ -4322,14 +4331,14 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C208" s="1"/>
       <c r="D208" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>11</v>
@@ -4337,46 +4346,44 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C209" s="1"/>
       <c r="D209" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
-        <v>176</v>
+        <v>21</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C210" s="1">
-        <v>2</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C210" s="1"/>
       <c r="D210" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>11</v>
@@ -4384,46 +4391,46 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C212" s="1"/>
       <c r="D212" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>17</v>
+        <v>175</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C213" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C213" s="1">
+        <v>2</v>
+      </c>
       <c r="D213" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>192</v>
+        <v>19</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C214" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>11</v>
@@ -4431,46 +4438,46 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
-        <v>192</v>
+        <v>17</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C216" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C217" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C217" s="1">
+        <v>2</v>
+      </c>
       <c r="D217" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>11</v>
@@ -4478,225 +4485,272 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C218" s="1"/>
       <c r="D218" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="C219" s="1">
         <v>2</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E219" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A220" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E220" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A220" t="s">
-        <v>17</v>
-      </c>
-      <c r="B220" t="s">
-        <v>193</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E220" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
-        <v>195</v>
+        <v>19</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C221" s="1">
-        <v>2</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C221" s="1"/>
       <c r="D221" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B222" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C222" s="1">
+        <v>2</v>
+      </c>
+      <c r="D222" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C222" s="1"/>
-      <c r="D222" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="E222" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A223" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C223" s="1">
-        <v>2</v>
+      <c r="A223" t="s">
+        <v>17</v>
+      </c>
+      <c r="B223" t="s">
+        <v>192</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>16</v>
+        <v>193</v>
+      </c>
+      <c r="E223" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C224" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="C224" s="1">
+        <v>2</v>
+      </c>
       <c r="D224" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>196</v>
+        <v>69</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>199</v>
+        <v>17</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C225" s="1">
-        <v>2</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C225" s="1"/>
       <c r="D225" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>196</v>
+        <v>16</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C226" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="C226" s="1">
+        <v>2</v>
+      </c>
       <c r="D226" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>200</v>
+        <v>16</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
-        <v>199</v>
+        <v>17</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C227" s="1">
-        <v>2</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="C227" s="1"/>
       <c r="D227" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
-        <v>17</v>
+        <v>198</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C228" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C228" s="1">
+        <v>2</v>
+      </c>
       <c r="D228" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
-        <v>203</v>
+        <v>17</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C229" s="1">
-        <v>2</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="C229" s="1"/>
       <c r="D229" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
-        <v>17</v>
+        <v>198</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C230" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C230" s="1">
+        <v>2</v>
+      </c>
       <c r="D230" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C231" s="1"/>
+      <c r="D231" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A232" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C232" s="1">
+        <v>2</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A233" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C233" s="1"/>
+      <c r="D233" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E233" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B231" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C231" s="1">
-        <v>2</v>
-      </c>
-      <c r="D231" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>204</v>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A234" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C234" s="1">
+        <v>2</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (display) Map async snippets
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D96EEB-2C83-4C18-8340-667664CF9D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A6676-9F57-4FB3-B8E0-BAFB2A21DC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="213">
   <si>
     <t>Class</t>
   </si>
@@ -646,6 +646,27 @@
   </si>
   <si>
     <t>setSignature</t>
+  </si>
+  <si>
+    <t>displayAppointmentFormAsync</t>
+  </si>
+  <si>
+    <t>displayMessageFormAsync</t>
+  </si>
+  <si>
+    <t>displayNewAppointmentFormAsync</t>
+  </si>
+  <si>
+    <t>displayNewMessageFormAsync</t>
+  </si>
+  <si>
+    <t>displayReplyFormAsync</t>
+  </si>
+  <si>
+    <t>displayReplyAllFormAsync</t>
+  </si>
+  <si>
+    <t>runAsync</t>
   </si>
 </sst>
 </file>
@@ -721,8 +742,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E234" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E234" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E244" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E244" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1054,11 +1075,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E234"/>
+  <dimension ref="A1:E244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D88" sqref="D88"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3232,121 +3253,121 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B140" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="C140">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E140" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B141" t="s">
-        <v>106</v>
+        <v>207</v>
       </c>
       <c r="C141">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E141" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B142" t="s">
-        <v>106</v>
+        <v>208</v>
       </c>
       <c r="C142">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E142" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B143" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="C143">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E143" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E144" t="s">
-        <v>4</v>
+        <v>210</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E145" t="s">
-        <v>4</v>
+        <v>210</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>106</v>
+        <v>211</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E146" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3354,16 +3375,16 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>106</v>
+        <v>211</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E147" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3371,16 +3392,16 @@
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E148" t="s">
-        <v>108</v>
+        <v>212</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -3388,67 +3409,67 @@
         <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="C149">
         <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E149" t="s">
-        <v>108</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B150" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C150">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D150" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E150" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B151" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D151" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E151" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C152">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E152" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3456,67 +3477,67 @@
         <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C153">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D153" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E153" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B154" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E154" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B155" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C155">
         <v>1</v>
       </c>
       <c r="D155" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E155" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C156">
         <v>1</v>
       </c>
       <c r="D156" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E156" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3524,16 +3545,16 @@
         <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C157">
         <v>1</v>
       </c>
       <c r="D157" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E157" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -3541,16 +3562,16 @@
         <v>19</v>
       </c>
       <c r="B158" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C158">
         <v>1</v>
       </c>
       <c r="D158" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E158" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -3558,16 +3579,16 @@
         <v>21</v>
       </c>
       <c r="B159" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C159">
         <v>1</v>
       </c>
       <c r="D159" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E159" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -3575,16 +3596,16 @@
         <v>19</v>
       </c>
       <c r="B160" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C160">
         <v>1</v>
       </c>
       <c r="D160" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E160" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
@@ -3592,177 +3613,186 @@
         <v>21</v>
       </c>
       <c r="B161" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C161">
         <v>1</v>
       </c>
       <c r="D161" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E161" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B162" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C162">
         <v>1</v>
       </c>
       <c r="D162" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E162" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B163" t="s">
-        <v>120</v>
+        <v>111</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
       </c>
       <c r="D163" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E163" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B164" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C164">
         <v>1</v>
       </c>
       <c r="D164" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E164" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B165" t="s">
-        <v>121</v>
+        <v>113</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
       </c>
       <c r="D165" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E165" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B166" t="s">
-        <v>120</v>
+        <v>114</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
       </c>
       <c r="D166" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E166" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B167" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C167">
         <v>1</v>
       </c>
       <c r="D167" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E167" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B168" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C168">
         <v>1</v>
       </c>
       <c r="D168" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E168" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B169" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C169">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E169" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B170" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C170">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E170" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B171" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C171">
         <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="E171" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
@@ -3770,13 +3800,13 @@
         <v>83</v>
       </c>
       <c r="B172" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C172">
         <v>1</v>
       </c>
       <c r="D172" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E172" t="s">
         <v>4</v>
@@ -3787,13 +3817,10 @@
         <v>83</v>
       </c>
       <c r="B173" t="s">
-        <v>107</v>
-      </c>
-      <c r="C173">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="D173" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E173" t="s">
         <v>4</v>
@@ -3804,180 +3831,180 @@
         <v>83</v>
       </c>
       <c r="B174" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C174">
         <v>1</v>
       </c>
       <c r="D174" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E174" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A175" s="1" t="s">
+      <c r="A175" t="s">
+        <v>83</v>
+      </c>
+      <c r="B175" t="s">
+        <v>121</v>
+      </c>
+      <c r="D175" t="s">
+        <v>122</v>
+      </c>
+      <c r="E175" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>83</v>
+      </c>
+      <c r="B176" t="s">
+        <v>120</v>
+      </c>
+      <c r="D176" t="s">
+        <v>122</v>
+      </c>
+      <c r="E176" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>83</v>
+      </c>
+      <c r="B177" t="s">
+        <v>118</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177" t="s">
+        <v>122</v>
+      </c>
+      <c r="E177" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>83</v>
+      </c>
+      <c r="B178" t="s">
+        <v>123</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+      <c r="D178" t="s">
+        <v>122</v>
+      </c>
+      <c r="E178" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>17</v>
+      </c>
+      <c r="B179" t="s">
+        <v>124</v>
+      </c>
+      <c r="C179">
+        <v>2</v>
+      </c>
+      <c r="D179" t="s">
+        <v>125</v>
+      </c>
+      <c r="E179" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
         <v>20</v>
       </c>
-      <c r="B175" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C175" s="1">
-        <v>2</v>
-      </c>
-      <c r="D175" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A176" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C176" s="1">
-        <v>1</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A177" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C177" s="1">
-        <v>2</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A178" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C178" s="1">
-        <v>2</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A179" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C179" s="1">
-        <v>2</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A180" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C180" s="1">
-        <v>2</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>139</v>
+      <c r="B180" t="s">
+        <v>124</v>
+      </c>
+      <c r="C180">
+        <v>2</v>
+      </c>
+      <c r="D180" t="s">
+        <v>125</v>
+      </c>
+      <c r="E180" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A181" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C181" s="1">
-        <v>2</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>139</v>
+      <c r="A181" t="s">
+        <v>83</v>
+      </c>
+      <c r="B181" t="s">
+        <v>126</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181" t="s">
+        <v>127</v>
+      </c>
+      <c r="E181" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A182" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C182" s="1"/>
-      <c r="D182" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>11</v>
+      <c r="A182" t="s">
+        <v>83</v>
+      </c>
+      <c r="B182" t="s">
+        <v>126</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="D182" t="s">
+        <v>128</v>
+      </c>
+      <c r="E182" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A183" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C183" s="1"/>
-      <c r="D183" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>11</v>
+      <c r="A183" t="s">
+        <v>83</v>
+      </c>
+      <c r="B183" t="s">
+        <v>107</v>
+      </c>
+      <c r="C183">
+        <v>2</v>
+      </c>
+      <c r="D183" t="s">
+        <v>129</v>
+      </c>
+      <c r="E183" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A184" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C184" s="1"/>
-      <c r="D184" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>11</v>
+      <c r="A184" t="s">
+        <v>83</v>
+      </c>
+      <c r="B184" t="s">
+        <v>130</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184" t="s">
+        <v>131</v>
+      </c>
+      <c r="E184" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
@@ -3985,104 +4012,118 @@
         <v>20</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C185" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="C185" s="1">
+        <v>2</v>
+      </c>
       <c r="D185" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C186" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="C186" s="1">
+        <v>1</v>
+      </c>
       <c r="D186" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C187" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="C187" s="1">
+        <v>2</v>
+      </c>
       <c r="D187" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>3</v>
+        <v>205</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C188" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="C188" s="1">
+        <v>2</v>
+      </c>
       <c r="D188" s="1" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C189" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="C189" s="1">
+        <v>2</v>
+      </c>
       <c r="D189" s="1" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C190" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C190" s="1">
+        <v>2</v>
+      </c>
       <c r="D190" s="1" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C191" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C191" s="1">
+        <v>2</v>
+      </c>
       <c r="D191" s="1" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
@@ -4090,11 +4131,11 @@
         <v>19</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>11</v>
@@ -4102,14 +4143,14 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C193" s="1"/>
       <c r="D193" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>11</v>
@@ -4117,14 +4158,14 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C194" s="1"/>
       <c r="D194" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>11</v>
@@ -4132,14 +4173,14 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C195" s="1"/>
       <c r="D195" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>11</v>
@@ -4147,46 +4188,44 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C196" s="1"/>
       <c r="D196" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C198" s="1">
-        <v>2</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C198" s="1"/>
       <c r="D198" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>11</v>
@@ -4194,46 +4233,44 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C199" s="1"/>
       <c r="D199" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C200" s="1">
-        <v>2</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C200" s="1"/>
       <c r="D200" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C201" s="1"/>
       <c r="D201" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>11</v>
@@ -4241,14 +4278,14 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C202" s="1"/>
       <c r="D202" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>11</v>
@@ -4259,11 +4296,11 @@
         <v>20</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C203" s="1"/>
       <c r="D203" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>11</v>
@@ -4274,11 +4311,11 @@
         <v>21</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>11</v>
@@ -4289,11 +4326,11 @@
         <v>19</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>11</v>
@@ -4304,11 +4341,11 @@
         <v>21</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>11</v>
@@ -4316,14 +4353,14 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>11</v>
@@ -4331,14 +4368,16 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C208" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C208" s="1">
+        <v>2</v>
+      </c>
       <c r="D208" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>11</v>
@@ -4346,44 +4385,46 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C209" s="1"/>
       <c r="D209" s="1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C210" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C210" s="1">
+        <v>2</v>
+      </c>
       <c r="D210" s="1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>11</v>
@@ -4391,46 +4432,44 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C212" s="1"/>
       <c r="D212" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>175</v>
+        <v>20</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C213" s="1">
-        <v>2</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="C213" s="1"/>
       <c r="D213" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>11</v>
@@ -4438,14 +4477,14 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>11</v>
@@ -4453,14 +4492,14 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>11</v>
@@ -4468,16 +4507,14 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C217" s="1">
-        <v>2</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>11</v>
@@ -4485,46 +4522,44 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C218" s="1"/>
       <c r="D218" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C219" s="1">
-        <v>2</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C219" s="1"/>
       <c r="D219" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C220" s="1"/>
       <c r="D220" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>11</v>
@@ -4532,14 +4567,14 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C221" s="1"/>
       <c r="D221" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E221" s="1" t="s">
         <v>11</v>
@@ -4547,166 +4582,163 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
-        <v>194</v>
+        <v>17</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C222" s="1">
-        <v>2</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C222" s="1"/>
       <c r="D222" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A223" t="s">
-        <v>17</v>
-      </c>
-      <c r="B223" t="s">
-        <v>192</v>
+      <c r="A223" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C223" s="1">
+        <v>2</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E223" t="s">
-        <v>69</v>
+        <v>187</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
-        <v>194</v>
+        <v>19</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C224" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C224" s="1"/>
       <c r="D224" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C225" s="1"/>
       <c r="D225" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
-        <v>194</v>
+        <v>17</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C226" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C226" s="1"/>
       <c r="D226" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C227" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C227" s="1">
+        <v>2</v>
+      </c>
       <c r="D227" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>195</v>
+        <v>11</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
-        <v>198</v>
+        <v>17</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C228" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C228" s="1"/>
       <c r="D228" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>195</v>
+        <v>3</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C229" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C229" s="1">
+        <v>2</v>
+      </c>
       <c r="D229" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>199</v>
+        <v>3</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
-        <v>198</v>
+        <v>17</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C230" s="1">
-        <v>2</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C230" s="1"/>
       <c r="D230" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>199</v>
+        <v>11</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C231" s="1"/>
       <c r="D231" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>82</v>
@@ -4715,41 +4747,200 @@
         <v>2</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A233" s="1" t="s">
+      <c r="A233" t="s">
         <v>17</v>
       </c>
-      <c r="B233" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C233" s="1"/>
+      <c r="B233" t="s">
+        <v>192</v>
+      </c>
       <c r="D233" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
+      </c>
+      <c r="E233" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C234" s="1">
+        <v>2</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A235" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C235" s="1"/>
+      <c r="D235" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A236" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C236" s="1">
+        <v>2</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A237" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C237" s="1"/>
+      <c r="D237" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A238" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C238" s="1">
+        <v>2</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A239" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C239" s="1"/>
+      <c r="D239" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A240" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C240" s="1">
+        <v>2</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A241" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C241" s="1"/>
+      <c r="D241" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A242" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B234" s="1" t="s">
+      <c r="B242" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C242" s="1">
+        <v>2</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A243" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C243" s="1"/>
+      <c r="D243" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A244" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B244" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C234" s="1">
-        <v>2</v>
-      </c>
-      <c r="D234" s="1" t="s">
+      <c r="C244" s="1">
+        <v>2</v>
+      </c>
+      <c r="D244" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E234" s="1" t="s">
+      <c r="E244" s="1" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Outlook] (display) Map async snippets (#462)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D96EEB-2C83-4C18-8340-667664CF9D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A6676-9F57-4FB3-B8E0-BAFB2A21DC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="213">
   <si>
     <t>Class</t>
   </si>
@@ -646,6 +646,27 @@
   </si>
   <si>
     <t>setSignature</t>
+  </si>
+  <si>
+    <t>displayAppointmentFormAsync</t>
+  </si>
+  <si>
+    <t>displayMessageFormAsync</t>
+  </si>
+  <si>
+    <t>displayNewAppointmentFormAsync</t>
+  </si>
+  <si>
+    <t>displayNewMessageFormAsync</t>
+  </si>
+  <si>
+    <t>displayReplyFormAsync</t>
+  </si>
+  <si>
+    <t>displayReplyAllFormAsync</t>
+  </si>
+  <si>
+    <t>runAsync</t>
   </si>
 </sst>
 </file>
@@ -721,8 +742,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E234" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E234" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E244" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E244" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1054,11 +1075,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E234"/>
+  <dimension ref="A1:E244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D88" sqref="D88"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3232,121 +3253,121 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B140" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="C140">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E140" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B141" t="s">
-        <v>106</v>
+        <v>207</v>
       </c>
       <c r="C141">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E141" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B142" t="s">
-        <v>106</v>
+        <v>208</v>
       </c>
       <c r="C142">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E142" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B143" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="C143">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E143" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E144" t="s">
-        <v>4</v>
+        <v>210</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E145" t="s">
-        <v>4</v>
+        <v>210</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>106</v>
+        <v>211</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E146" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3354,16 +3375,16 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>106</v>
+        <v>211</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E147" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3371,16 +3392,16 @@
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E148" t="s">
-        <v>108</v>
+        <v>212</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -3388,67 +3409,67 @@
         <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="C149">
         <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E149" t="s">
-        <v>108</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B150" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C150">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D150" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E150" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B151" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D151" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E151" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C152">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E152" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3456,67 +3477,67 @@
         <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C153">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D153" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E153" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B154" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C154">
         <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E154" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B155" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C155">
         <v>1</v>
       </c>
       <c r="D155" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E155" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C156">
         <v>1</v>
       </c>
       <c r="D156" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E156" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3524,16 +3545,16 @@
         <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C157">
         <v>1</v>
       </c>
       <c r="D157" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E157" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -3541,16 +3562,16 @@
         <v>19</v>
       </c>
       <c r="B158" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C158">
         <v>1</v>
       </c>
       <c r="D158" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E158" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -3558,16 +3579,16 @@
         <v>21</v>
       </c>
       <c r="B159" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C159">
         <v>1</v>
       </c>
       <c r="D159" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E159" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -3575,16 +3596,16 @@
         <v>19</v>
       </c>
       <c r="B160" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C160">
         <v>1</v>
       </c>
       <c r="D160" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E160" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
@@ -3592,177 +3613,186 @@
         <v>21</v>
       </c>
       <c r="B161" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C161">
         <v>1</v>
       </c>
       <c r="D161" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E161" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B162" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C162">
         <v>1</v>
       </c>
       <c r="D162" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E162" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B163" t="s">
-        <v>120</v>
+        <v>111</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
       </c>
       <c r="D163" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E163" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B164" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C164">
         <v>1</v>
       </c>
       <c r="D164" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E164" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B165" t="s">
-        <v>121</v>
+        <v>113</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
       </c>
       <c r="D165" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E165" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B166" t="s">
-        <v>120</v>
+        <v>114</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
       </c>
       <c r="D166" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E166" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B167" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C167">
         <v>1</v>
       </c>
       <c r="D167" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E167" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B168" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C168">
         <v>1</v>
       </c>
       <c r="D168" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E168" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B169" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C169">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E169" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B170" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C170">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E170" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="B171" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C171">
         <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="E171" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
@@ -3770,13 +3800,13 @@
         <v>83</v>
       </c>
       <c r="B172" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C172">
         <v>1</v>
       </c>
       <c r="D172" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E172" t="s">
         <v>4</v>
@@ -3787,13 +3817,10 @@
         <v>83</v>
       </c>
       <c r="B173" t="s">
-        <v>107</v>
-      </c>
-      <c r="C173">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="D173" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E173" t="s">
         <v>4</v>
@@ -3804,180 +3831,180 @@
         <v>83</v>
       </c>
       <c r="B174" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C174">
         <v>1</v>
       </c>
       <c r="D174" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E174" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A175" s="1" t="s">
+      <c r="A175" t="s">
+        <v>83</v>
+      </c>
+      <c r="B175" t="s">
+        <v>121</v>
+      </c>
+      <c r="D175" t="s">
+        <v>122</v>
+      </c>
+      <c r="E175" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>83</v>
+      </c>
+      <c r="B176" t="s">
+        <v>120</v>
+      </c>
+      <c r="D176" t="s">
+        <v>122</v>
+      </c>
+      <c r="E176" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>83</v>
+      </c>
+      <c r="B177" t="s">
+        <v>118</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177" t="s">
+        <v>122</v>
+      </c>
+      <c r="E177" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>83</v>
+      </c>
+      <c r="B178" t="s">
+        <v>123</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+      <c r="D178" t="s">
+        <v>122</v>
+      </c>
+      <c r="E178" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>17</v>
+      </c>
+      <c r="B179" t="s">
+        <v>124</v>
+      </c>
+      <c r="C179">
+        <v>2</v>
+      </c>
+      <c r="D179" t="s">
+        <v>125</v>
+      </c>
+      <c r="E179" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
         <v>20</v>
       </c>
-      <c r="B175" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C175" s="1">
-        <v>2</v>
-      </c>
-      <c r="D175" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A176" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C176" s="1">
-        <v>1</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A177" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C177" s="1">
-        <v>2</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A178" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C178" s="1">
-        <v>2</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A179" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C179" s="1">
-        <v>2</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A180" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C180" s="1">
-        <v>2</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>139</v>
+      <c r="B180" t="s">
+        <v>124</v>
+      </c>
+      <c r="C180">
+        <v>2</v>
+      </c>
+      <c r="D180" t="s">
+        <v>125</v>
+      </c>
+      <c r="E180" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A181" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C181" s="1">
-        <v>2</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>139</v>
+      <c r="A181" t="s">
+        <v>83</v>
+      </c>
+      <c r="B181" t="s">
+        <v>126</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181" t="s">
+        <v>127</v>
+      </c>
+      <c r="E181" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A182" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C182" s="1"/>
-      <c r="D182" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>11</v>
+      <c r="A182" t="s">
+        <v>83</v>
+      </c>
+      <c r="B182" t="s">
+        <v>126</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="D182" t="s">
+        <v>128</v>
+      </c>
+      <c r="E182" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A183" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C183" s="1"/>
-      <c r="D183" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>11</v>
+      <c r="A183" t="s">
+        <v>83</v>
+      </c>
+      <c r="B183" t="s">
+        <v>107</v>
+      </c>
+      <c r="C183">
+        <v>2</v>
+      </c>
+      <c r="D183" t="s">
+        <v>129</v>
+      </c>
+      <c r="E183" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A184" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C184" s="1"/>
-      <c r="D184" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>11</v>
+      <c r="A184" t="s">
+        <v>83</v>
+      </c>
+      <c r="B184" t="s">
+        <v>130</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184" t="s">
+        <v>131</v>
+      </c>
+      <c r="E184" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
@@ -3985,104 +4012,118 @@
         <v>20</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C185" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="C185" s="1">
+        <v>2</v>
+      </c>
       <c r="D185" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C186" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="C186" s="1">
+        <v>1</v>
+      </c>
       <c r="D186" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C187" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="C187" s="1">
+        <v>2</v>
+      </c>
       <c r="D187" s="1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>3</v>
+        <v>205</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C188" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="C188" s="1">
+        <v>2</v>
+      </c>
       <c r="D188" s="1" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C189" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="C189" s="1">
+        <v>2</v>
+      </c>
       <c r="D189" s="1" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C190" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C190" s="1">
+        <v>2</v>
+      </c>
       <c r="D190" s="1" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C191" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C191" s="1">
+        <v>2</v>
+      </c>
       <c r="D191" s="1" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
@@ -4090,11 +4131,11 @@
         <v>19</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>11</v>
@@ -4102,14 +4143,14 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C193" s="1"/>
       <c r="D193" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>11</v>
@@ -4117,14 +4158,14 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C194" s="1"/>
       <c r="D194" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>11</v>
@@ -4132,14 +4173,14 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C195" s="1"/>
       <c r="D195" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>11</v>
@@ -4147,46 +4188,44 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C196" s="1"/>
       <c r="D196" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C198" s="1">
-        <v>2</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C198" s="1"/>
       <c r="D198" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>11</v>
@@ -4194,46 +4233,44 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C199" s="1"/>
       <c r="D199" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C200" s="1">
-        <v>2</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C200" s="1"/>
       <c r="D200" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C201" s="1"/>
       <c r="D201" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>11</v>
@@ -4241,14 +4278,14 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C202" s="1"/>
       <c r="D202" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>11</v>
@@ -4259,11 +4296,11 @@
         <v>20</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C203" s="1"/>
       <c r="D203" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>11</v>
@@ -4274,11 +4311,11 @@
         <v>21</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>11</v>
@@ -4289,11 +4326,11 @@
         <v>19</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>11</v>
@@ -4304,11 +4341,11 @@
         <v>21</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>11</v>
@@ -4316,14 +4353,14 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>11</v>
@@ -4331,14 +4368,16 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C208" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C208" s="1">
+        <v>2</v>
+      </c>
       <c r="D208" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>11</v>
@@ -4346,44 +4385,46 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C209" s="1"/>
       <c r="D209" s="1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C210" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C210" s="1">
+        <v>2</v>
+      </c>
       <c r="D210" s="1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>11</v>
@@ -4391,46 +4432,44 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C212" s="1"/>
       <c r="D212" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>175</v>
+        <v>20</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C213" s="1">
-        <v>2</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="C213" s="1"/>
       <c r="D213" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>11</v>
@@ -4438,14 +4477,14 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>11</v>
@@ -4453,14 +4492,14 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>11</v>
@@ -4468,16 +4507,14 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C217" s="1">
-        <v>2</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>11</v>
@@ -4485,46 +4522,44 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C218" s="1"/>
       <c r="D218" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C219" s="1">
-        <v>2</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C219" s="1"/>
       <c r="D219" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C220" s="1"/>
       <c r="D220" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>11</v>
@@ -4532,14 +4567,14 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C221" s="1"/>
       <c r="D221" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E221" s="1" t="s">
         <v>11</v>
@@ -4547,166 +4582,163 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
-        <v>194</v>
+        <v>17</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C222" s="1">
-        <v>2</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C222" s="1"/>
       <c r="D222" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A223" t="s">
-        <v>17</v>
-      </c>
-      <c r="B223" t="s">
-        <v>192</v>
+      <c r="A223" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C223" s="1">
+        <v>2</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E223" t="s">
-        <v>69</v>
+        <v>187</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
-        <v>194</v>
+        <v>19</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C224" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C224" s="1"/>
       <c r="D224" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C225" s="1"/>
       <c r="D225" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
-        <v>194</v>
+        <v>17</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C226" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C226" s="1"/>
       <c r="D226" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C227" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C227" s="1">
+        <v>2</v>
+      </c>
       <c r="D227" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>195</v>
+        <v>11</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
-        <v>198</v>
+        <v>17</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C228" s="1">
-        <v>2</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C228" s="1"/>
       <c r="D228" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>195</v>
+        <v>3</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C229" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C229" s="1">
+        <v>2</v>
+      </c>
       <c r="D229" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>199</v>
+        <v>3</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
-        <v>198</v>
+        <v>17</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C230" s="1">
-        <v>2</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C230" s="1"/>
       <c r="D230" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>199</v>
+        <v>11</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C231" s="1"/>
       <c r="D231" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>82</v>
@@ -4715,41 +4747,200 @@
         <v>2</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A233" s="1" t="s">
+      <c r="A233" t="s">
         <v>17</v>
       </c>
-      <c r="B233" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C233" s="1"/>
+      <c r="B233" t="s">
+        <v>192</v>
+      </c>
       <c r="D233" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
+      </c>
+      <c r="E233" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C234" s="1">
+        <v>2</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A235" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C235" s="1"/>
+      <c r="D235" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A236" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C236" s="1">
+        <v>2</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A237" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C237" s="1"/>
+      <c r="D237" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A238" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C238" s="1">
+        <v>2</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A239" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C239" s="1"/>
+      <c r="D239" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A240" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C240" s="1">
+        <v>2</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A241" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C241" s="1"/>
+      <c r="D241" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A242" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B234" s="1" t="s">
+      <c r="B242" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C242" s="1">
+        <v>2</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A243" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C243" s="1"/>
+      <c r="D243" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A244" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B244" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C234" s="1">
-        <v>2</v>
-      </c>
-      <c r="D234" s="1" t="s">
+      <c r="C244" s="1">
+        <v>2</v>
+      </c>
+      <c r="D244" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E234" s="1" t="s">
+      <c r="E244" s="1" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Outlook] Map sessionData snippets
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23203"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A6676-9F57-4FB3-B8E0-BAFB2A21DC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66099875-5D3E-418A-9675-657606F947F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="222">
   <si>
     <t>Class</t>
   </si>
@@ -667,6 +667,33 @@
   </si>
   <si>
     <t>runAsync</t>
+  </si>
+  <si>
+    <t>sessionData</t>
+  </si>
+  <si>
+    <t>outlook-session-data-apis</t>
+  </si>
+  <si>
+    <t>getAllSessionData</t>
+  </si>
+  <si>
+    <t>SessionData</t>
+  </si>
+  <si>
+    <t>setSessionData</t>
+  </si>
+  <si>
+    <t>getSessionData</t>
+  </si>
+  <si>
+    <t>removeSessionData</t>
+  </si>
+  <si>
+    <t>clearAsync</t>
+  </si>
+  <si>
+    <t>clearSessionData</t>
   </si>
 </sst>
 </file>
@@ -742,8 +769,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E244" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E244" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E251" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E251" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1075,11 +1102,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E244"/>
+  <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E150" sqref="E150"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E251" sqref="E251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4944,6 +4971,121 @@
         <v>203</v>
       </c>
     </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A245" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C245" s="1"/>
+      <c r="D245" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A246" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C246" s="1"/>
+      <c r="D246" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A247" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C247" s="1">
+        <v>1</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A248" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C248" s="1">
+        <v>1</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A249" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C249" s="1">
+        <v>1</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A250" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C250" s="1">
+        <v>1</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A251" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C251" s="1">
+        <v>1</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Outlook] Map sessionData snippets (#475)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23203"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A6676-9F57-4FB3-B8E0-BAFB2A21DC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66099875-5D3E-418A-9675-657606F947F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="222">
   <si>
     <t>Class</t>
   </si>
@@ -667,6 +667,33 @@
   </si>
   <si>
     <t>runAsync</t>
+  </si>
+  <si>
+    <t>sessionData</t>
+  </si>
+  <si>
+    <t>outlook-session-data-apis</t>
+  </si>
+  <si>
+    <t>getAllSessionData</t>
+  </si>
+  <si>
+    <t>SessionData</t>
+  </si>
+  <si>
+    <t>setSessionData</t>
+  </si>
+  <si>
+    <t>getSessionData</t>
+  </si>
+  <si>
+    <t>removeSessionData</t>
+  </si>
+  <si>
+    <t>clearAsync</t>
+  </si>
+  <si>
+    <t>clearSessionData</t>
   </si>
 </sst>
 </file>
@@ -742,8 +769,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E244" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E244" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E251" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E251" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1075,11 +1102,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E244"/>
+  <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E150" sqref="E150"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E251" sqref="E251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4944,6 +4971,121 @@
         <v>203</v>
       </c>
     </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A245" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C245" s="1"/>
+      <c r="D245" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A246" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C246" s="1"/>
+      <c r="D246" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A247" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C247" s="1">
+        <v>1</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A248" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C248" s="1">
+        <v>1</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A249" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C249" s="1">
+        <v>1</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A250" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C250" s="1">
+        <v>1</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A251" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C251" s="1">
+        <v>1</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Outlook] (SessionData) Map to overloads
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23208"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66099875-5D3E-418A-9675-657606F947F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F923A3D6-574D-4181-AC36-8F099926817E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -1106,7 +1106,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E251" sqref="E251"/>
+      <selection pane="bottomLeft" activeCell="C247" sqref="C247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5009,7 +5009,7 @@
         <v>148</v>
       </c>
       <c r="C247" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>214</v>
@@ -5060,7 +5060,7 @@
         <v>66</v>
       </c>
       <c r="C250" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D250" s="1" t="s">
         <v>214</v>
@@ -5077,7 +5077,7 @@
         <v>220</v>
       </c>
       <c r="C251" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D251" s="1" t="s">
         <v>214</v>

</xml_diff>

<commit_message>
[Outlook] (SessionData) Map to overloads (#479)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23208"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66099875-5D3E-418A-9675-657606F947F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F923A3D6-574D-4181-AC36-8F099926817E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -1106,7 +1106,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E251" sqref="E251"/>
+      <selection pane="bottomLeft" activeCell="C247" sqref="C247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5009,7 +5009,7 @@
         <v>148</v>
       </c>
       <c r="C247" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>214</v>
@@ -5060,7 +5060,7 @@
         <v>66</v>
       </c>
       <c r="C250" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D250" s="1" t="s">
         <v>214</v>
@@ -5077,7 +5077,7 @@
         <v>220</v>
       </c>
       <c r="C251" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D251" s="1" t="s">
         <v>214</v>

</xml_diff>

<commit_message>
[Outlook] (delegate) Update snippet with appointment example
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23324"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F923A3D6-574D-4181-AC36-8F099926817E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA9E246-E756-41CA-AAD2-289042B4C3B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="224">
   <si>
     <t>Class</t>
   </si>
@@ -694,6 +694,12 @@
   </si>
   <si>
     <t>clearSessionData</t>
+  </si>
+  <si>
+    <t>runOnAppointment</t>
+  </si>
+  <si>
+    <t>runOnMessage</t>
   </si>
 </sst>
 </file>
@@ -1105,8 +1111,8 @@
   <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C247" sqref="C247"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3530,7 +3536,7 @@
         <v>105</v>
       </c>
       <c r="E154" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3547,7 +3553,7 @@
         <v>105</v>
       </c>
       <c r="E155" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3564,7 +3570,7 @@
         <v>105</v>
       </c>
       <c r="E156" t="s">
-        <v>4</v>
+        <v>223</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3581,7 +3587,7 @@
         <v>105</v>
       </c>
       <c r="E157" t="s">
-        <v>4</v>
+        <v>223</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Outlook] (delegate) Update snippet with appointment example (#495)
* [Outlook] (delegate) Update snippet with appointment example

* Update based on feedback

* Clarify
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23324"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F923A3D6-574D-4181-AC36-8F099926817E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA9E246-E756-41CA-AAD2-289042B4C3B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="224">
   <si>
     <t>Class</t>
   </si>
@@ -694,6 +694,12 @@
   </si>
   <si>
     <t>clearSessionData</t>
+  </si>
+  <si>
+    <t>runOnAppointment</t>
+  </si>
+  <si>
+    <t>runOnMessage</t>
   </si>
 </sst>
 </file>
@@ -1105,8 +1111,8 @@
   <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C247" sqref="C247"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3530,7 +3536,7 @@
         <v>105</v>
       </c>
       <c r="E154" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3547,7 +3553,7 @@
         <v>105</v>
       </c>
       <c r="E155" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3564,7 +3570,7 @@
         <v>105</v>
       </c>
       <c r="E156" t="s">
-        <v>4</v>
+        <v>223</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3581,7 +3587,7 @@
         <v>105</v>
       </c>
       <c r="E157" t="s">
-        <v>4</v>
+        <v>223</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Outlook] Clean up (#503)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23424"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA9E246-E756-41CA-AAD2-289042B4C3B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413DD66C-57A4-4D87-AC9C-187B5F85416F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -1111,8 +1111,8 @@
   <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E157" sqref="E157"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1590,7 +1590,7 @@
         <v>82</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
         <v>36</v>
@@ -1725,7 +1725,7 @@
         <v>82</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
         <v>45</v>
@@ -1965,7 +1965,7 @@
         <v>56</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" t="s">
         <v>57</v>
@@ -2038,7 +2038,7 @@
         <v>56</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" t="s">
         <v>57</v>
@@ -2111,7 +2111,7 @@
         <v>56</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" t="s">
         <v>57</v>
@@ -2128,7 +2128,7 @@
         <v>56</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65" t="s">
         <v>57</v>
@@ -2201,7 +2201,7 @@
         <v>62</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D70" t="s">
         <v>57</v>
@@ -2274,7 +2274,7 @@
         <v>64</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D75" t="s">
         <v>57</v>
@@ -2347,7 +2347,7 @@
         <v>66</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D80" t="s">
         <v>57</v>
@@ -2500,7 +2500,7 @@
         <v>74</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89" t="s">
         <v>68</v>
@@ -2517,7 +2517,7 @@
         <v>74</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D90" t="s">
         <v>68</v>
@@ -2793,7 +2793,7 @@
         <v>56</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D108" t="s">
         <v>162</v>
@@ -2866,7 +2866,7 @@
         <v>66</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D113" t="s">
         <v>162</v>
@@ -2928,7 +2928,7 @@
         <v>56</v>
       </c>
       <c r="C117">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D117" t="s">
         <v>159</v>
@@ -2959,7 +2959,7 @@
         <v>66</v>
       </c>
       <c r="C119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D119" t="s">
         <v>159</v>
@@ -2990,7 +2990,7 @@
         <v>82</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D121" t="s">
         <v>176</v>
@@ -3021,7 +3021,7 @@
         <v>148</v>
       </c>
       <c r="C123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D123" t="s">
         <v>176</v>
@@ -4082,7 +4082,7 @@
         <v>141</v>
       </c>
       <c r="C187" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>138</v>
@@ -4099,7 +4099,7 @@
         <v>144</v>
       </c>
       <c r="C188" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>138</v>
@@ -4116,7 +4116,7 @@
         <v>144</v>
       </c>
       <c r="C189" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>138</v>
@@ -4133,7 +4133,7 @@
         <v>137</v>
       </c>
       <c r="C190" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>138</v>
@@ -4150,7 +4150,7 @@
         <v>137</v>
       </c>
       <c r="C191" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>138</v>
@@ -4439,7 +4439,7 @@
         <v>148</v>
       </c>
       <c r="C210" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>174</v>
@@ -4636,7 +4636,7 @@
         <v>148</v>
       </c>
       <c r="C223" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>187</v>
@@ -4730,7 +4730,7 @@
         <v>148</v>
       </c>
       <c r="C229" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>190</v>
@@ -4777,7 +4777,7 @@
         <v>82</v>
       </c>
       <c r="C232" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>193</v>
@@ -4808,7 +4808,7 @@
         <v>56</v>
       </c>
       <c r="C234" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D234" s="1" t="s">
         <v>193</v>
@@ -4840,7 +4840,7 @@
         <v>66</v>
       </c>
       <c r="C236" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D236" s="1" t="s">
         <v>193</v>
@@ -4904,7 +4904,7 @@
         <v>148</v>
       </c>
       <c r="C240" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>196</v>
@@ -4968,7 +4968,7 @@
         <v>148</v>
       </c>
       <c r="C244" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D244" s="1" t="s">
         <v>196</v>
@@ -5015,7 +5015,7 @@
         <v>148</v>
       </c>
       <c r="C247" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>214</v>
@@ -5066,7 +5066,7 @@
         <v>66</v>
       </c>
       <c r="C250" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D250" s="1" t="s">
         <v>214</v>
@@ -5083,7 +5083,7 @@
         <v>220</v>
       </c>
       <c r="C251" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D251" s="1" t="s">
         <v>214</v>

</xml_diff>

<commit_message>
[Outlook] Couple other items
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23424"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413DD66C-57A4-4D87-AC9C-187B5F85416F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1A3475-AC00-45A2-B2F4-0E470FCEA49A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -1112,7 +1112,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,7 +1353,7 @@
         <v>25</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
@@ -1370,7 +1370,7 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
[Outlook] Couple other items (#504)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23424"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413DD66C-57A4-4D87-AC9C-187B5F85416F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1A3475-AC00-45A2-B2F4-0E470FCEA49A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -1112,7 +1112,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,7 +1353,7 @@
         <v>25</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
@@ -1370,7 +1370,7 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
[Outlook] (internet headers) Add snippets
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23616"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1A3475-AC00-45A2-B2F4-0E470FCEA49A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBA7D82-CB4D-4079-9C38-11B608C064FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="232">
   <si>
     <t>Class</t>
   </si>
@@ -700,6 +700,30 @@
   </si>
   <si>
     <t>runOnMessage</t>
+  </si>
+  <si>
+    <t>getAllInternetHeadersAsync</t>
+  </si>
+  <si>
+    <t>outlook-mime-headers-get-internet-headers-message-read</t>
+  </si>
+  <si>
+    <t>internetHeaders</t>
+  </si>
+  <si>
+    <t>outlook-mime-headers-manage-custom-internet-headers-message-compose</t>
+  </si>
+  <si>
+    <t>getSelectedCustomHeaders</t>
+  </si>
+  <si>
+    <t>InternetHeaders</t>
+  </si>
+  <si>
+    <t>removeSelectedCustomHeaders</t>
+  </si>
+  <si>
+    <t>setCustomHeaders</t>
   </si>
 </sst>
 </file>
@@ -775,8 +799,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E251" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E251" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E256" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E256" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1108,11 +1132,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E256" sqref="E256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5092,6 +5116,89 @@
         <v>221</v>
       </c>
     </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A252" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C252" s="1">
+        <v>1</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A253" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C253" s="1"/>
+      <c r="D253" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A254" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C254" s="1">
+        <v>1</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A255" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C255" s="1">
+        <v>1</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A256" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C256" s="1">
+        <v>1</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5099,4 +5206,10 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
[Outlook] (internet headers) Add snippets (#510)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23616"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1A3475-AC00-45A2-B2F4-0E470FCEA49A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBA7D82-CB4D-4079-9C38-11B608C064FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="232">
   <si>
     <t>Class</t>
   </si>
@@ -700,6 +700,30 @@
   </si>
   <si>
     <t>runOnMessage</t>
+  </si>
+  <si>
+    <t>getAllInternetHeadersAsync</t>
+  </si>
+  <si>
+    <t>outlook-mime-headers-get-internet-headers-message-read</t>
+  </si>
+  <si>
+    <t>internetHeaders</t>
+  </si>
+  <si>
+    <t>outlook-mime-headers-manage-custom-internet-headers-message-compose</t>
+  </si>
+  <si>
+    <t>getSelectedCustomHeaders</t>
+  </si>
+  <si>
+    <t>InternetHeaders</t>
+  </si>
+  <si>
+    <t>removeSelectedCustomHeaders</t>
+  </si>
+  <si>
+    <t>setCustomHeaders</t>
   </si>
 </sst>
 </file>
@@ -775,8 +799,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E251" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E251" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E256" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E256" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -1108,11 +1132,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E256" sqref="E256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5092,6 +5116,89 @@
         <v>221</v>
       </c>
     </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A252" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C252" s="1">
+        <v>1</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A253" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C253" s="1"/>
+      <c r="D253" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A254" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C254" s="1">
+        <v>1</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A255" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C255" s="1">
+        <v>1</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A256" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C256" s="1">
+        <v>1</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5099,4 +5206,10 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
[Outlook] Requirement set 1.11
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23616"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBA7D82-CB4D-4079-9C38-11B608C064FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3DD14-2B04-44B9-AC66-9CD296F768C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -672,9 +672,6 @@
     <t>sessionData</t>
   </si>
   <si>
-    <t>outlook-session-data-apis</t>
-  </si>
-  <si>
     <t>getAllSessionData</t>
   </si>
   <si>
@@ -724,6 +721,9 @@
   </si>
   <si>
     <t>setCustomHeaders</t>
+  </si>
+  <si>
+    <t>outlook-event-based-activation-session-data-apis</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1136,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E256" sqref="E256"/>
+      <selection pane="bottomLeft" activeCell="D244" sqref="D244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3560,7 +3560,7 @@
         <v>105</v>
       </c>
       <c r="E154" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3577,7 +3577,7 @@
         <v>105</v>
       </c>
       <c r="E155" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3594,7 +3594,7 @@
         <v>105</v>
       </c>
       <c r="E156" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3611,7 +3611,7 @@
         <v>105</v>
       </c>
       <c r="E157" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -5010,10 +5010,10 @@
       </c>
       <c r="C245" s="1"/>
       <c r="D245" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E245" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
@@ -5025,15 +5025,15 @@
       </c>
       <c r="C246" s="1"/>
       <c r="D246" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E246" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>148</v>
@@ -5042,15 +5042,15 @@
         <v>1</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>82</v>
@@ -5059,15 +5059,15 @@
         <v>1</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>62</v>
@@ -5076,15 +5076,15 @@
         <v>1</v>
       </c>
       <c r="D249" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E249" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>66</v>
@@ -5093,27 +5093,27 @@
         <v>1</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B251" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C251" s="1">
+        <v>1</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E251" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="C251" s="1">
-        <v>1</v>
-      </c>
-      <c r="D251" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
@@ -5121,13 +5121,13 @@
         <v>21</v>
       </c>
       <c r="B252" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C252" s="1">
+        <v>1</v>
+      </c>
+      <c r="D252" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C252" s="1">
-        <v>1</v>
-      </c>
-      <c r="D252" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="E252" s="1" t="s">
         <v>4</v>
@@ -5138,19 +5138,19 @@
         <v>20</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C253" s="1"/>
       <c r="D253" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E253" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>82</v>
@@ -5159,15 +5159,15 @@
         <v>1</v>
       </c>
       <c r="D254" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E254" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>66</v>
@@ -5176,15 +5176,15 @@
         <v>1</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>148</v>
@@ -5193,10 +5193,10 @@
         <v>1</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] Requirement set 1.11 (#572)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23616"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBA7D82-CB4D-4079-9C38-11B608C064FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3DD14-2B04-44B9-AC66-9CD296F768C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -672,9 +672,6 @@
     <t>sessionData</t>
   </si>
   <si>
-    <t>outlook-session-data-apis</t>
-  </si>
-  <si>
     <t>getAllSessionData</t>
   </si>
   <si>
@@ -724,6 +721,9 @@
   </si>
   <si>
     <t>setCustomHeaders</t>
+  </si>
+  <si>
+    <t>outlook-event-based-activation-session-data-apis</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1136,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E256" sqref="E256"/>
+      <selection pane="bottomLeft" activeCell="D244" sqref="D244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3560,7 +3560,7 @@
         <v>105</v>
       </c>
       <c r="E154" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3577,7 +3577,7 @@
         <v>105</v>
       </c>
       <c r="E155" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3594,7 +3594,7 @@
         <v>105</v>
       </c>
       <c r="E156" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3611,7 +3611,7 @@
         <v>105</v>
       </c>
       <c r="E157" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -5010,10 +5010,10 @@
       </c>
       <c r="C245" s="1"/>
       <c r="D245" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E245" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
@@ -5025,15 +5025,15 @@
       </c>
       <c r="C246" s="1"/>
       <c r="D246" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E246" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>148</v>
@@ -5042,15 +5042,15 @@
         <v>1</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>82</v>
@@ -5059,15 +5059,15 @@
         <v>1</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>62</v>
@@ -5076,15 +5076,15 @@
         <v>1</v>
       </c>
       <c r="D249" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E249" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>66</v>
@@ -5093,27 +5093,27 @@
         <v>1</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B251" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C251" s="1">
+        <v>1</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E251" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="C251" s="1">
-        <v>1</v>
-      </c>
-      <c r="D251" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
@@ -5121,13 +5121,13 @@
         <v>21</v>
       </c>
       <c r="B252" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C252" s="1">
+        <v>1</v>
+      </c>
+      <c r="D252" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C252" s="1">
-        <v>1</v>
-      </c>
-      <c r="D252" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="E252" s="1" t="s">
         <v>4</v>
@@ -5138,19 +5138,19 @@
         <v>20</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C253" s="1"/>
       <c r="D253" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E253" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>82</v>
@@ -5159,15 +5159,15 @@
         <v>1</v>
       </c>
       <c r="D254" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E254" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>66</v>
@@ -5176,15 +5176,15 @@
         <v>1</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>148</v>
@@ -5193,10 +5193,10 @@
         <v>1</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replace sample with recent snippet
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25414"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3DD14-2B04-44B9-AC66-9CD296F768C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BA4FB5-7635-42A4-B18A-554A349261C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="38475" yWindow="1695" windowWidth="28800" windowHeight="17145" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -411,9 +411,6 @@
     <t>makeEwsRequestAsync</t>
   </si>
   <si>
-    <t>outlook-tokens-and-service-calls-make-ews-request-async</t>
-  </si>
-  <si>
     <t>outlook-tokens-and-service-calls-send-message-using-make-ews-request-async</t>
   </si>
   <si>
@@ -724,6 +721,9 @@
   </si>
   <si>
     <t>outlook-event-based-activation-session-data-apis</t>
+  </si>
+  <si>
+    <t>outlook-tokens-and-service-calls-get-icaluid-as-attendee</t>
   </si>
 </sst>
 </file>
@@ -759,9 +759,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,20 +1134,20 @@
   <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D244" sqref="D244"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="74.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1233,7 +1232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1318,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1335,7 +1334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1352,7 +1351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1369,7 +1368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1386,7 +1385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1437,7 +1436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1454,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1462,15 +1461,15 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
         <v>82</v>
@@ -1479,13 +1478,13 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1493,30 +1492,30 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
         <v>151</v>
       </c>
-      <c r="E21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" t="s">
         <v>151</v>
       </c>
-      <c r="E22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1524,15 +1523,15 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
         <v>82</v>
@@ -1541,13 +1540,13 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1555,30 +1554,30 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" t="s">
         <v>149</v>
       </c>
-      <c r="E25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" t="s">
         <v>149</v>
       </c>
-      <c r="E26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1592,7 +1591,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1606,9 +1605,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
         <v>82</v>
@@ -1623,7 +1622,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1651,7 +1650,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1659,15 +1658,15 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B33" t="s">
         <v>82</v>
@@ -1676,13 +1675,13 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1690,30 +1689,30 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1727,7 +1726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1741,9 +1740,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B38" t="s">
         <v>82</v>
@@ -1758,7 +1757,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1772,7 +1771,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1780,15 +1779,15 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
         <v>82</v>
@@ -1797,13 +1796,13 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1811,30 +1810,30 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" t="s">
         <v>153</v>
       </c>
-      <c r="E42" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" t="s">
         <v>153</v>
       </c>
-      <c r="E43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -1856,15 +1855,15 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B46" t="s">
         <v>82</v>
@@ -1873,45 +1872,44 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>20</v>
       </c>
       <c r="B47" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="1"/>
       <c r="D47" t="s">
+        <v>145</v>
+      </c>
+      <c r="E47" t="s">
         <v>146</v>
       </c>
-      <c r="E47" s="1" t="s">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" t="s">
         <v>146</v>
       </c>
-      <c r="E48" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -1925,12 +1923,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1939,12 +1937,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1953,12 +1951,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1967,12 +1965,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1981,7 +1979,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1998,12 +1996,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -2012,12 +2010,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -2026,12 +2024,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -2040,12 +2038,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -2054,7 +2052,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -2071,12 +2069,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D60" t="s">
         <v>57</v>
@@ -2085,12 +2083,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D61" t="s">
         <v>57</v>
@@ -2099,12 +2097,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D62" t="s">
         <v>57</v>
@@ -2113,12 +2111,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D63" t="s">
         <v>57</v>
@@ -2127,7 +2125,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -2144,7 +2142,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -2161,12 +2159,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D66" t="s">
         <v>57</v>
@@ -2175,12 +2173,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D67" t="s">
         <v>57</v>
@@ -2189,12 +2187,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D68" t="s">
         <v>57</v>
@@ -2203,12 +2201,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D69" t="s">
         <v>57</v>
@@ -2217,7 +2215,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -2234,12 +2232,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D71" t="s">
         <v>57</v>
@@ -2248,12 +2246,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D72" t="s">
         <v>57</v>
@@ -2262,12 +2260,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D73" t="s">
         <v>57</v>
@@ -2276,12 +2274,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D74" t="s">
         <v>57</v>
@@ -2290,7 +2288,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -2307,12 +2305,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D76" t="s">
         <v>57</v>
@@ -2321,12 +2319,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D77" t="s">
         <v>57</v>
@@ -2335,12 +2333,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -2349,12 +2347,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D79" t="s">
         <v>57</v>
@@ -2363,7 +2361,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -2380,7 +2378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -2397,7 +2395,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>20</v>
       </c>
@@ -2414,7 +2412,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -2431,7 +2429,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>20</v>
       </c>
@@ -2448,7 +2446,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -2465,7 +2463,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>20</v>
       </c>
@@ -2482,7 +2480,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -2492,14 +2490,14 @@
       <c r="C87">
         <v>1</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>138</v>
+      <c r="D87" t="s">
+        <v>137</v>
       </c>
       <c r="E87" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>20</v>
       </c>
@@ -2509,14 +2507,14 @@
       <c r="C88">
         <v>1</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>138</v>
+      <c r="D88" t="s">
+        <v>137</v>
       </c>
       <c r="E88" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -2533,7 +2531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -2550,7 +2548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -2567,7 +2565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>20</v>
       </c>
@@ -2584,7 +2582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -2595,13 +2593,13 @@
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -2612,13 +2610,13 @@
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>20</v>
       </c>
@@ -2629,13 +2627,13 @@
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E95" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>21</v>
       </c>
@@ -2646,13 +2644,13 @@
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>19</v>
       </c>
@@ -2666,7 +2664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>21</v>
       </c>
@@ -2680,7 +2678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>17</v>
       </c>
@@ -2688,13 +2686,13 @@
         <v>79</v>
       </c>
       <c r="D99" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E99" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>19</v>
       </c>
@@ -2702,13 +2700,13 @@
         <v>79</v>
       </c>
       <c r="D100" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E100" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>20</v>
       </c>
@@ -2716,13 +2714,13 @@
         <v>79</v>
       </c>
       <c r="D101" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E101" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>21</v>
       </c>
@@ -2730,13 +2728,13 @@
         <v>79</v>
       </c>
       <c r="D102" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E102" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>81</v>
       </c>
@@ -2747,13 +2745,13 @@
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E103" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>17</v>
       </c>
@@ -2761,13 +2759,13 @@
         <v>79</v>
       </c>
       <c r="D104" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E104" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>19</v>
       </c>
@@ -2775,13 +2773,13 @@
         <v>79</v>
       </c>
       <c r="D105" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E105" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>20</v>
       </c>
@@ -2789,13 +2787,13 @@
         <v>79</v>
       </c>
       <c r="D106" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E106" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>21</v>
       </c>
@@ -2803,13 +2801,13 @@
         <v>79</v>
       </c>
       <c r="D107" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E107" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>81</v>
       </c>
@@ -2820,13 +2818,13 @@
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E108" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>17</v>
       </c>
@@ -2834,13 +2832,13 @@
         <v>79</v>
       </c>
       <c r="D109" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E109" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>19</v>
       </c>
@@ -2848,13 +2846,13 @@
         <v>79</v>
       </c>
       <c r="D110" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E110" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>20</v>
       </c>
@@ -2862,13 +2860,13 @@
         <v>79</v>
       </c>
       <c r="D111" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E111" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>21</v>
       </c>
@@ -2876,13 +2874,13 @@
         <v>79</v>
       </c>
       <c r="D112" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E112" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>81</v>
       </c>
@@ -2893,13 +2891,13 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E113" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>83</v>
       </c>
@@ -2907,13 +2905,13 @@
         <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E114" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>86</v>
       </c>
@@ -2924,13 +2922,13 @@
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E115" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>83</v>
       </c>
@@ -2938,13 +2936,13 @@
         <v>84</v>
       </c>
       <c r="D116" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E116" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>86</v>
       </c>
@@ -2955,13 +2953,13 @@
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E117" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>83</v>
       </c>
@@ -2969,13 +2967,13 @@
         <v>84</v>
       </c>
       <c r="D118" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E118" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>86</v>
       </c>
@@ -2986,13 +2984,13 @@
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E119" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>17</v>
       </c>
@@ -3000,13 +2998,13 @@
         <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E120" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>88</v>
       </c>
@@ -3017,13 +3015,13 @@
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>17</v>
       </c>
@@ -3031,30 +3029,30 @@
         <v>87</v>
       </c>
       <c r="D122" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E122" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>88</v>
       </c>
       <c r="B123" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E123" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>19</v>
       </c>
@@ -3068,7 +3066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>21</v>
       </c>
@@ -3082,7 +3080,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>17</v>
       </c>
@@ -3096,7 +3094,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>19</v>
       </c>
@@ -3110,7 +3108,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>20</v>
       </c>
@@ -3124,7 +3122,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>21</v>
       </c>
@@ -3138,7 +3136,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>83</v>
       </c>
@@ -3155,7 +3153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>83</v>
       </c>
@@ -3172,7 +3170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>83</v>
       </c>
@@ -3189,7 +3187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>83</v>
       </c>
@@ -3206,7 +3204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -3223,7 +3221,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>21</v>
       </c>
@@ -3240,7 +3238,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>19</v>
       </c>
@@ -3257,7 +3255,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>21</v>
       </c>
@@ -3274,7 +3272,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>19</v>
       </c>
@@ -3291,7 +3289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>21</v>
       </c>
@@ -3308,12 +3306,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>83</v>
       </c>
       <c r="B140" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -3322,15 +3320,15 @@
         <v>94</v>
       </c>
       <c r="E140" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>83</v>
       </c>
       <c r="B141" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -3339,15 +3337,15 @@
         <v>96</v>
       </c>
       <c r="E141" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>83</v>
       </c>
       <c r="B142" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -3356,15 +3354,15 @@
         <v>98</v>
       </c>
       <c r="E142" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>83</v>
       </c>
       <c r="B143" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -3373,15 +3371,15 @@
         <v>100</v>
       </c>
       <c r="E143" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -3390,15 +3388,15 @@
         <v>103</v>
       </c>
       <c r="E144" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -3407,15 +3405,15 @@
         <v>103</v>
       </c>
       <c r="E145" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -3424,15 +3422,15 @@
         <v>103</v>
       </c>
       <c r="E146" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -3441,15 +3439,15 @@
         <v>103</v>
       </c>
       <c r="E147" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -3458,15 +3456,15 @@
         <v>104</v>
       </c>
       <c r="E148" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -3475,10 +3473,10 @@
         <v>104</v>
       </c>
       <c r="E149" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>17</v>
       </c>
@@ -3495,7 +3493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>19</v>
       </c>
@@ -3512,7 +3510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>20</v>
       </c>
@@ -3529,7 +3527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>21</v>
       </c>
@@ -3546,7 +3544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>17</v>
       </c>
@@ -3560,10 +3558,10 @@
         <v>105</v>
       </c>
       <c r="E154" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>19</v>
       </c>
@@ -3577,10 +3575,10 @@
         <v>105</v>
       </c>
       <c r="E155" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>20</v>
       </c>
@@ -3594,10 +3592,10 @@
         <v>105</v>
       </c>
       <c r="E156" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>21</v>
       </c>
@@ -3611,10 +3609,10 @@
         <v>105</v>
       </c>
       <c r="E157" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>19</v>
       </c>
@@ -3631,7 +3629,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>21</v>
       </c>
@@ -3648,7 +3646,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>19</v>
       </c>
@@ -3665,7 +3663,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>21</v>
       </c>
@@ -3682,7 +3680,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>19</v>
       </c>
@@ -3699,7 +3697,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>21</v>
       </c>
@@ -3716,7 +3714,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>19</v>
       </c>
@@ -3733,7 +3731,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>21</v>
       </c>
@@ -3750,7 +3748,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>19</v>
       </c>
@@ -3767,7 +3765,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>21</v>
       </c>
@@ -3784,7 +3782,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>19</v>
       </c>
@@ -3801,7 +3799,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>21</v>
       </c>
@@ -3818,7 +3816,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>19</v>
       </c>
@@ -3835,7 +3833,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>21</v>
       </c>
@@ -3852,7 +3850,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>83</v>
       </c>
@@ -3869,7 +3867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>83</v>
       </c>
@@ -3883,7 +3881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>83</v>
       </c>
@@ -3900,7 +3898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>83</v>
       </c>
@@ -3914,7 +3912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>83</v>
       </c>
@@ -3928,7 +3926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>83</v>
       </c>
@@ -3945,7 +3943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>83</v>
       </c>
@@ -3962,7 +3960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>17</v>
       </c>
@@ -3979,7 +3977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>20</v>
       </c>
@@ -3996,7 +3994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>83</v>
       </c>
@@ -4007,13 +4005,13 @@
         <v>1</v>
       </c>
       <c r="D181" t="s">
-        <v>127</v>
+        <v>231</v>
       </c>
       <c r="E181" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>83</v>
       </c>
@@ -4024,13 +4022,13 @@
         <v>1</v>
       </c>
       <c r="D182" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E182" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>83</v>
       </c>
@@ -4041,1162 +4039,1119 @@
         <v>2</v>
       </c>
       <c r="D183" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E183" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>83</v>
       </c>
       <c r="B184" t="s">
+        <v>129</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184" t="s">
         <v>130</v>
-      </c>
-      <c r="C184">
-        <v>1</v>
-      </c>
-      <c r="D184" t="s">
-        <v>131</v>
       </c>
       <c r="E184" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A185" s="1" t="s">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>20</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B185" t="s">
+        <v>141</v>
+      </c>
+      <c r="C185">
+        <v>2</v>
+      </c>
+      <c r="D185" t="s">
+        <v>137</v>
+      </c>
+      <c r="E185" t="s">
         <v>142</v>
       </c>
-      <c r="C185" s="1">
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>139</v>
+      </c>
+      <c r="B186" t="s">
+        <v>140</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="D186" t="s">
+        <v>137</v>
+      </c>
+      <c r="E186" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>139</v>
+      </c>
+      <c r="B187" t="s">
+        <v>140</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+      <c r="D187" t="s">
+        <v>137</v>
+      </c>
+      <c r="E187" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>17</v>
+      </c>
+      <c r="B188" t="s">
+        <v>143</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+      <c r="D188" t="s">
+        <v>137</v>
+      </c>
+      <c r="E188" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>20</v>
+      </c>
+      <c r="B189" t="s">
+        <v>143</v>
+      </c>
+      <c r="C189">
+        <v>1</v>
+      </c>
+      <c r="D189" t="s">
+        <v>137</v>
+      </c>
+      <c r="E189" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>17</v>
+      </c>
+      <c r="B190" t="s">
+        <v>136</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+      <c r="D190" t="s">
+        <v>137</v>
+      </c>
+      <c r="E190" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>20</v>
+      </c>
+      <c r="B191" t="s">
+        <v>136</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191" t="s">
+        <v>137</v>
+      </c>
+      <c r="E191" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>19</v>
+      </c>
+      <c r="B192" t="s">
+        <v>162</v>
+      </c>
+      <c r="D192" t="s">
+        <v>163</v>
+      </c>
+      <c r="E192" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>21</v>
+      </c>
+      <c r="B193" t="s">
+        <v>162</v>
+      </c>
+      <c r="D193" t="s">
+        <v>163</v>
+      </c>
+      <c r="E193" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>17</v>
+      </c>
+      <c r="B194" t="s">
+        <v>162</v>
+      </c>
+      <c r="D194" t="s">
+        <v>164</v>
+      </c>
+      <c r="E194" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>20</v>
+      </c>
+      <c r="B195" t="s">
+        <v>162</v>
+      </c>
+      <c r="D195" t="s">
+        <v>164</v>
+      </c>
+      <c r="E195" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>17</v>
+      </c>
+      <c r="B196" t="s">
+        <v>162</v>
+      </c>
+      <c r="D196" t="s">
+        <v>164</v>
+      </c>
+      <c r="E196" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>20</v>
+      </c>
+      <c r="B197" t="s">
+        <v>162</v>
+      </c>
+      <c r="D197" t="s">
+        <v>164</v>
+      </c>
+      <c r="E197" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>21</v>
+      </c>
+      <c r="B198" t="s">
+        <v>165</v>
+      </c>
+      <c r="D198" t="s">
+        <v>166</v>
+      </c>
+      <c r="E198" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>19</v>
+      </c>
+      <c r="B199" t="s">
+        <v>167</v>
+      </c>
+      <c r="D199" t="s">
+        <v>168</v>
+      </c>
+      <c r="E199" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>21</v>
+      </c>
+      <c r="B200" t="s">
+        <v>167</v>
+      </c>
+      <c r="D200" t="s">
+        <v>168</v>
+      </c>
+      <c r="E200" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>17</v>
+      </c>
+      <c r="B201" t="s">
+        <v>169</v>
+      </c>
+      <c r="D201" t="s">
+        <v>170</v>
+      </c>
+      <c r="E201" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>19</v>
+      </c>
+      <c r="B202" t="s">
+        <v>169</v>
+      </c>
+      <c r="D202" t="s">
+        <v>170</v>
+      </c>
+      <c r="E202" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>20</v>
+      </c>
+      <c r="B203" t="s">
+        <v>169</v>
+      </c>
+      <c r="D203" t="s">
+        <v>170</v>
+      </c>
+      <c r="E203" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>21</v>
+      </c>
+      <c r="B204" t="s">
+        <v>169</v>
+      </c>
+      <c r="D204" t="s">
+        <v>170</v>
+      </c>
+      <c r="E204" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>19</v>
+      </c>
+      <c r="B205" t="s">
+        <v>171</v>
+      </c>
+      <c r="D205" t="s">
+        <v>172</v>
+      </c>
+      <c r="E205" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>21</v>
+      </c>
+      <c r="B206" t="s">
+        <v>171</v>
+      </c>
+      <c r="D206" t="s">
+        <v>172</v>
+      </c>
+      <c r="E206" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>17</v>
+      </c>
+      <c r="B207" t="s">
+        <v>171</v>
+      </c>
+      <c r="D207" t="s">
+        <v>173</v>
+      </c>
+      <c r="E207" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>174</v>
+      </c>
+      <c r="B208" t="s">
+        <v>82</v>
+      </c>
+      <c r="C208">
         <v>2</v>
       </c>
-      <c r="D185" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A186" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C186" s="1">
-        <v>1</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A187" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C187" s="1">
-        <v>1</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A188" s="1" t="s">
+      <c r="D208" t="s">
+        <v>173</v>
+      </c>
+      <c r="E208" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>17</v>
       </c>
-      <c r="B188" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C188" s="1">
-        <v>1</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A189" s="1" t="s">
+      <c r="B209" t="s">
+        <v>171</v>
+      </c>
+      <c r="D209" t="s">
+        <v>173</v>
+      </c>
+      <c r="E209" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>174</v>
+      </c>
+      <c r="B210" t="s">
+        <v>147</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+      <c r="D210" t="s">
+        <v>173</v>
+      </c>
+      <c r="E210" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>19</v>
+      </c>
+      <c r="B211" t="s">
+        <v>176</v>
+      </c>
+      <c r="D211" t="s">
+        <v>177</v>
+      </c>
+      <c r="E211" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>21</v>
+      </c>
+      <c r="B212" t="s">
+        <v>176</v>
+      </c>
+      <c r="D212" t="s">
+        <v>177</v>
+      </c>
+      <c r="E212" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>20</v>
       </c>
-      <c r="B189" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C189" s="1">
-        <v>1</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A190" s="1" t="s">
+      <c r="B213" t="s">
+        <v>178</v>
+      </c>
+      <c r="D213" t="s">
+        <v>179</v>
+      </c>
+      <c r="E213" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>21</v>
+      </c>
+      <c r="B214" t="s">
+        <v>178</v>
+      </c>
+      <c r="D214" t="s">
+        <v>179</v>
+      </c>
+      <c r="E214" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>19</v>
+      </c>
+      <c r="B215" t="s">
+        <v>180</v>
+      </c>
+      <c r="D215" t="s">
+        <v>181</v>
+      </c>
+      <c r="E215" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>21</v>
+      </c>
+      <c r="B216" t="s">
+        <v>180</v>
+      </c>
+      <c r="D216" t="s">
+        <v>181</v>
+      </c>
+      <c r="E216" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>19</v>
+      </c>
+      <c r="B217" t="s">
+        <v>182</v>
+      </c>
+      <c r="D217" t="s">
+        <v>183</v>
+      </c>
+      <c r="E217" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>21</v>
+      </c>
+      <c r="B218" t="s">
+        <v>182</v>
+      </c>
+      <c r="D218" t="s">
+        <v>183</v>
+      </c>
+      <c r="E218" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>19</v>
+      </c>
+      <c r="B219" t="s">
+        <v>184</v>
+      </c>
+      <c r="D219" t="s">
+        <v>185</v>
+      </c>
+      <c r="E219" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>21</v>
+      </c>
+      <c r="B220" t="s">
+        <v>184</v>
+      </c>
+      <c r="D220" t="s">
+        <v>185</v>
+      </c>
+      <c r="E220" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>17</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C190" s="1">
-        <v>1</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A191" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C191" s="1">
-        <v>1</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A192" s="1" t="s">
+      <c r="B221" t="s">
+        <v>184</v>
+      </c>
+      <c r="D221" t="s">
+        <v>186</v>
+      </c>
+      <c r="E221" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>17</v>
+      </c>
+      <c r="B222" t="s">
+        <v>184</v>
+      </c>
+      <c r="D222" t="s">
+        <v>186</v>
+      </c>
+      <c r="E222" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>174</v>
+      </c>
+      <c r="B223" t="s">
+        <v>147</v>
+      </c>
+      <c r="C223">
+        <v>1</v>
+      </c>
+      <c r="D223" t="s">
+        <v>186</v>
+      </c>
+      <c r="E223" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>19</v>
       </c>
-      <c r="B192" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C192" s="1"/>
-      <c r="D192" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E192" s="1" t="s">
+      <c r="B224" t="s">
+        <v>187</v>
+      </c>
+      <c r="D224" t="s">
+        <v>188</v>
+      </c>
+      <c r="E224" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A193" s="1" t="s">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>21</v>
       </c>
-      <c r="B193" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C193" s="1"/>
-      <c r="D193" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E193" s="1" t="s">
+      <c r="B225" t="s">
+        <v>187</v>
+      </c>
+      <c r="D225" t="s">
+        <v>188</v>
+      </c>
+      <c r="E225" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A194" s="1" t="s">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>17</v>
       </c>
-      <c r="B194" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C194" s="1"/>
-      <c r="D194" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E194" s="1" t="s">
+      <c r="B226" t="s">
+        <v>187</v>
+      </c>
+      <c r="D226" t="s">
+        <v>189</v>
+      </c>
+      <c r="E226" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A195" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C195" s="1"/>
-      <c r="D195" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E195" s="1" t="s">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>190</v>
+      </c>
+      <c r="B227" t="s">
+        <v>82</v>
+      </c>
+      <c r="C227">
+        <v>2</v>
+      </c>
+      <c r="D227" t="s">
+        <v>189</v>
+      </c>
+      <c r="E227" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A196" s="1" t="s">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>17</v>
       </c>
-      <c r="B196" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C196" s="1"/>
-      <c r="D196" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E196" s="1" t="s">
+      <c r="B228" t="s">
+        <v>187</v>
+      </c>
+      <c r="D228" t="s">
+        <v>189</v>
+      </c>
+      <c r="E228" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A197" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C197" s="1"/>
-      <c r="D197" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E197" s="1" t="s">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>190</v>
+      </c>
+      <c r="B229" t="s">
+        <v>147</v>
+      </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+      <c r="D229" t="s">
+        <v>189</v>
+      </c>
+      <c r="E229" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A198" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C198" s="1"/>
-      <c r="D198" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E198" s="1" t="s">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>17</v>
+      </c>
+      <c r="B230" t="s">
+        <v>191</v>
+      </c>
+      <c r="D230" t="s">
+        <v>192</v>
+      </c>
+      <c r="E230" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A199" s="1" t="s">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
         <v>19</v>
       </c>
-      <c r="B199" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C199" s="1"/>
-      <c r="D199" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E199" s="1" t="s">
+      <c r="B231" t="s">
+        <v>191</v>
+      </c>
+      <c r="D231" t="s">
+        <v>192</v>
+      </c>
+      <c r="E231" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A200" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C200" s="1"/>
-      <c r="D200" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E200" s="1" t="s">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>193</v>
+      </c>
+      <c r="B232" t="s">
+        <v>82</v>
+      </c>
+      <c r="C232">
+        <v>1</v>
+      </c>
+      <c r="D232" t="s">
+        <v>192</v>
+      </c>
+      <c r="E232" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A201" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C201" s="1"/>
-      <c r="D201" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A202" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C202" s="1"/>
-      <c r="D202" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E202" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A203" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C203" s="1"/>
-      <c r="D203" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A204" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C204" s="1"/>
-      <c r="D204" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A205" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C205" s="1"/>
-      <c r="D205" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A206" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C206" s="1"/>
-      <c r="D206" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A207" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C207" s="1"/>
-      <c r="D207" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A208" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C208" s="1">
-        <v>2</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A209" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C209" s="1"/>
-      <c r="D209" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A210" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C210" s="1">
-        <v>1</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A211" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C211" s="1"/>
-      <c r="D211" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A212" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C212" s="1"/>
-      <c r="D212" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A213" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C213" s="1"/>
-      <c r="D213" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A214" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C214" s="1"/>
-      <c r="D214" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A215" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C215" s="1"/>
-      <c r="D215" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A216" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C216" s="1"/>
-      <c r="D216" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A217" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C217" s="1"/>
-      <c r="D217" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A218" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C218" s="1"/>
-      <c r="D218" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E218" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A219" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C219" s="1"/>
-      <c r="D219" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A220" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C220" s="1"/>
-      <c r="D220" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A221" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C221" s="1"/>
-      <c r="D221" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A222" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C222" s="1"/>
-      <c r="D222" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A223" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C223" s="1">
-        <v>1</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A224" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C224" s="1"/>
-      <c r="D224" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A225" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C225" s="1"/>
-      <c r="D225" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A226" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C226" s="1"/>
-      <c r="D226" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A227" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C227" s="1">
-        <v>2</v>
-      </c>
-      <c r="D227" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A228" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C228" s="1"/>
-      <c r="D228" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A229" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C229" s="1">
-        <v>1</v>
-      </c>
-      <c r="D229" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A230" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B230" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C230" s="1"/>
-      <c r="D230" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A231" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C231" s="1"/>
-      <c r="D231" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A232" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C232" s="1">
-        <v>1</v>
-      </c>
-      <c r="D232" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>17</v>
       </c>
       <c r="B233" t="s">
+        <v>191</v>
+      </c>
+      <c r="D233" t="s">
         <v>192</v>
-      </c>
-      <c r="D233" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="E233" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A234" s="1" t="s">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>193</v>
+      </c>
+      <c r="B234" t="s">
+        <v>56</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+      <c r="D234" t="s">
+        <v>192</v>
+      </c>
+      <c r="E234" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>17</v>
+      </c>
+      <c r="B235" t="s">
+        <v>191</v>
+      </c>
+      <c r="D235" t="s">
+        <v>192</v>
+      </c>
+      <c r="E235" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>193</v>
+      </c>
+      <c r="B236" t="s">
+        <v>66</v>
+      </c>
+      <c r="C236">
+        <v>1</v>
+      </c>
+      <c r="D236" t="s">
+        <v>192</v>
+      </c>
+      <c r="E236" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>17</v>
+      </c>
+      <c r="B237" t="s">
+        <v>196</v>
+      </c>
+      <c r="D237" t="s">
+        <v>195</v>
+      </c>
+      <c r="E237" t="s">
         <v>194</v>
       </c>
-      <c r="B234" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C234" s="1">
-        <v>1</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A235" s="1" t="s">
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>197</v>
+      </c>
+      <c r="B238" t="s">
+        <v>82</v>
+      </c>
+      <c r="C238">
+        <v>2</v>
+      </c>
+      <c r="D238" t="s">
+        <v>195</v>
+      </c>
+      <c r="E238" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
         <v>17</v>
       </c>
-      <c r="B235" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C235" s="1"/>
-      <c r="D235" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A236" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B236" s="1" t="s">
+      <c r="B239" t="s">
+        <v>196</v>
+      </c>
+      <c r="D239" t="s">
+        <v>195</v>
+      </c>
+      <c r="E239" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>197</v>
+      </c>
+      <c r="B240" t="s">
+        <v>147</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240" t="s">
+        <v>195</v>
+      </c>
+      <c r="E240" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>17</v>
+      </c>
+      <c r="B241" t="s">
+        <v>199</v>
+      </c>
+      <c r="D241" t="s">
+        <v>195</v>
+      </c>
+      <c r="E241" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>201</v>
+      </c>
+      <c r="B242" t="s">
+        <v>82</v>
+      </c>
+      <c r="C242">
+        <v>2</v>
+      </c>
+      <c r="D242" t="s">
+        <v>195</v>
+      </c>
+      <c r="E242" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>17</v>
+      </c>
+      <c r="B243" t="s">
+        <v>199</v>
+      </c>
+      <c r="D243" t="s">
+        <v>195</v>
+      </c>
+      <c r="E243" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>201</v>
+      </c>
+      <c r="B244" t="s">
+        <v>147</v>
+      </c>
+      <c r="C244">
+        <v>1</v>
+      </c>
+      <c r="D244" t="s">
+        <v>195</v>
+      </c>
+      <c r="E244" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>17</v>
+      </c>
+      <c r="B245" t="s">
+        <v>212</v>
+      </c>
+      <c r="D245" t="s">
+        <v>230</v>
+      </c>
+      <c r="E245" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>20</v>
+      </c>
+      <c r="B246" t="s">
+        <v>212</v>
+      </c>
+      <c r="D246" t="s">
+        <v>230</v>
+      </c>
+      <c r="E246" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>214</v>
+      </c>
+      <c r="B247" t="s">
+        <v>147</v>
+      </c>
+      <c r="C247">
+        <v>1</v>
+      </c>
+      <c r="D247" t="s">
+        <v>230</v>
+      </c>
+      <c r="E247" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>214</v>
+      </c>
+      <c r="B248" t="s">
+        <v>82</v>
+      </c>
+      <c r="C248">
+        <v>1</v>
+      </c>
+      <c r="D248" t="s">
+        <v>230</v>
+      </c>
+      <c r="E248" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>214</v>
+      </c>
+      <c r="B249" t="s">
+        <v>62</v>
+      </c>
+      <c r="C249">
+        <v>1</v>
+      </c>
+      <c r="D249" t="s">
+        <v>230</v>
+      </c>
+      <c r="E249" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>214</v>
+      </c>
+      <c r="B250" t="s">
         <v>66</v>
       </c>
-      <c r="C236" s="1">
-        <v>1</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A237" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C237" s="1"/>
-      <c r="D237" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A238" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B238" s="1" t="s">
+      <c r="C250">
+        <v>1</v>
+      </c>
+      <c r="D250" t="s">
+        <v>230</v>
+      </c>
+      <c r="E250" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>214</v>
+      </c>
+      <c r="B251" t="s">
+        <v>218</v>
+      </c>
+      <c r="C251">
+        <v>1</v>
+      </c>
+      <c r="D251" t="s">
+        <v>230</v>
+      </c>
+      <c r="E251" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>21</v>
+      </c>
+      <c r="B252" t="s">
+        <v>222</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+      <c r="D252" t="s">
+        <v>223</v>
+      </c>
+      <c r="E252" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>20</v>
+      </c>
+      <c r="B253" t="s">
+        <v>224</v>
+      </c>
+      <c r="D253" t="s">
+        <v>225</v>
+      </c>
+      <c r="E253" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>227</v>
+      </c>
+      <c r="B254" t="s">
         <v>82</v>
       </c>
-      <c r="C238" s="1">
-        <v>2</v>
-      </c>
-      <c r="D238" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A239" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C239" s="1"/>
-      <c r="D239" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A240" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C240" s="1">
-        <v>1</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A241" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C241" s="1"/>
-      <c r="D241" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A242" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B242" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C242" s="1">
-        <v>2</v>
-      </c>
-      <c r="D242" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A243" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C243" s="1"/>
-      <c r="D243" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A244" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C244" s="1">
-        <v>1</v>
-      </c>
-      <c r="D244" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A245" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B245" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C245" s="1"/>
-      <c r="D245" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A246" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C246" s="1"/>
-      <c r="D246" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A247" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C247" s="1">
-        <v>1</v>
-      </c>
-      <c r="D247" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A248" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C248" s="1">
-        <v>1</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A249" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C249" s="1">
-        <v>1</v>
-      </c>
-      <c r="D249" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A250" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B250" s="1" t="s">
+      <c r="C254">
+        <v>1</v>
+      </c>
+      <c r="D254" t="s">
+        <v>225</v>
+      </c>
+      <c r="E254" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>227</v>
+      </c>
+      <c r="B255" t="s">
         <v>66</v>
       </c>
-      <c r="C250" s="1">
-        <v>1</v>
-      </c>
-      <c r="D250" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A251" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C251" s="1">
-        <v>1</v>
-      </c>
-      <c r="D251" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A252" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C252" s="1">
-        <v>1</v>
-      </c>
-      <c r="D252" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A253" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B253" s="1" t="s">
+      <c r="C255">
+        <v>1</v>
+      </c>
+      <c r="D255" t="s">
         <v>225</v>
       </c>
-      <c r="C253" s="1"/>
-      <c r="D253" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E253" s="1" t="s">
+      <c r="E255" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A254" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B254" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C254" s="1">
-        <v>1</v>
-      </c>
-      <c r="D254" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A255" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C255" s="1">
-        <v>1</v>
-      </c>
-      <c r="D255" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E255" s="1" t="s">
+      <c r="B256" t="s">
+        <v>147</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
+      <c r="D256" t="s">
+        <v>225</v>
+      </c>
+      <c r="E256" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A256" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C256" s="1">
-        <v>1</v>
-      </c>
-      <c r="D256" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] (makeEwsRequestAsync) Replace sample with recent snippet (#656)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25414"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3DD14-2B04-44B9-AC66-9CD296F768C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BA4FB5-7635-42A4-B18A-554A349261C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="38475" yWindow="1695" windowWidth="28800" windowHeight="17145" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -411,9 +411,6 @@
     <t>makeEwsRequestAsync</t>
   </si>
   <si>
-    <t>outlook-tokens-and-service-calls-make-ews-request-async</t>
-  </si>
-  <si>
     <t>outlook-tokens-and-service-calls-send-message-using-make-ews-request-async</t>
   </si>
   <si>
@@ -724,6 +721,9 @@
   </si>
   <si>
     <t>outlook-event-based-activation-session-data-apis</t>
+  </si>
+  <si>
+    <t>outlook-tokens-and-service-calls-get-icaluid-as-attendee</t>
   </si>
 </sst>
 </file>
@@ -759,9 +759,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,20 +1134,20 @@
   <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D244" sqref="D244"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="74.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1233,7 +1232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1318,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1335,7 +1334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1352,7 +1351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1369,7 +1368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1386,7 +1385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1437,7 +1436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1454,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1462,15 +1461,15 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
         <v>82</v>
@@ -1479,13 +1478,13 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1493,30 +1492,30 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
         <v>151</v>
       </c>
-      <c r="E21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" t="s">
         <v>151</v>
       </c>
-      <c r="E22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1524,15 +1523,15 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
         <v>82</v>
@@ -1541,13 +1540,13 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1555,30 +1554,30 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" t="s">
         <v>149</v>
       </c>
-      <c r="E25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" t="s">
         <v>149</v>
       </c>
-      <c r="E26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1592,7 +1591,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1606,9 +1605,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
         <v>82</v>
@@ -1623,7 +1622,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1651,7 +1650,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1659,15 +1658,15 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B33" t="s">
         <v>82</v>
@@ -1676,13 +1675,13 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1690,30 +1689,30 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1727,7 +1726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1741,9 +1740,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B38" t="s">
         <v>82</v>
@@ -1758,7 +1757,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1772,7 +1771,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1780,15 +1779,15 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
         <v>82</v>
@@ -1797,13 +1796,13 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1811,30 +1810,30 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" t="s">
         <v>153</v>
       </c>
-      <c r="E42" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" t="s">
         <v>153</v>
       </c>
-      <c r="E43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -1856,15 +1855,15 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B46" t="s">
         <v>82</v>
@@ -1873,45 +1872,44 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>20</v>
       </c>
       <c r="B47" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="1"/>
       <c r="D47" t="s">
+        <v>145</v>
+      </c>
+      <c r="E47" t="s">
         <v>146</v>
       </c>
-      <c r="E47" s="1" t="s">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" t="s">
         <v>146</v>
       </c>
-      <c r="E48" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -1925,12 +1923,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1939,12 +1937,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1953,12 +1951,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1967,12 +1965,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1981,7 +1979,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1998,12 +1996,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -2012,12 +2010,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -2026,12 +2024,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -2040,12 +2038,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -2054,7 +2052,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -2071,12 +2069,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D60" t="s">
         <v>57</v>
@@ -2085,12 +2083,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D61" t="s">
         <v>57</v>
@@ -2099,12 +2097,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D62" t="s">
         <v>57</v>
@@ -2113,12 +2111,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D63" t="s">
         <v>57</v>
@@ -2127,7 +2125,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -2144,7 +2142,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -2161,12 +2159,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D66" t="s">
         <v>57</v>
@@ -2175,12 +2173,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D67" t="s">
         <v>57</v>
@@ -2189,12 +2187,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D68" t="s">
         <v>57</v>
@@ -2203,12 +2201,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D69" t="s">
         <v>57</v>
@@ -2217,7 +2215,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -2234,12 +2232,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D71" t="s">
         <v>57</v>
@@ -2248,12 +2246,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D72" t="s">
         <v>57</v>
@@ -2262,12 +2260,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D73" t="s">
         <v>57</v>
@@ -2276,12 +2274,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D74" t="s">
         <v>57</v>
@@ -2290,7 +2288,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -2307,12 +2305,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D76" t="s">
         <v>57</v>
@@ -2321,12 +2319,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D77" t="s">
         <v>57</v>
@@ -2335,12 +2333,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -2349,12 +2347,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D79" t="s">
         <v>57</v>
@@ -2363,7 +2361,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -2380,7 +2378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -2397,7 +2395,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>20</v>
       </c>
@@ -2414,7 +2412,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -2431,7 +2429,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>20</v>
       </c>
@@ -2448,7 +2446,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -2465,7 +2463,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>20</v>
       </c>
@@ -2482,7 +2480,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -2492,14 +2490,14 @@
       <c r="C87">
         <v>1</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>138</v>
+      <c r="D87" t="s">
+        <v>137</v>
       </c>
       <c r="E87" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>20</v>
       </c>
@@ -2509,14 +2507,14 @@
       <c r="C88">
         <v>1</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>138</v>
+      <c r="D88" t="s">
+        <v>137</v>
       </c>
       <c r="E88" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -2533,7 +2531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -2550,7 +2548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -2567,7 +2565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>20</v>
       </c>
@@ -2584,7 +2582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -2595,13 +2593,13 @@
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -2612,13 +2610,13 @@
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E94" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>20</v>
       </c>
@@ -2629,13 +2627,13 @@
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E95" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>21</v>
       </c>
@@ -2646,13 +2644,13 @@
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>19</v>
       </c>
@@ -2666,7 +2664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>21</v>
       </c>
@@ -2680,7 +2678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>17</v>
       </c>
@@ -2688,13 +2686,13 @@
         <v>79</v>
       </c>
       <c r="D99" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E99" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>19</v>
       </c>
@@ -2702,13 +2700,13 @@
         <v>79</v>
       </c>
       <c r="D100" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E100" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>20</v>
       </c>
@@ -2716,13 +2714,13 @@
         <v>79</v>
       </c>
       <c r="D101" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E101" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>21</v>
       </c>
@@ -2730,13 +2728,13 @@
         <v>79</v>
       </c>
       <c r="D102" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E102" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>81</v>
       </c>
@@ -2747,13 +2745,13 @@
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E103" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>17</v>
       </c>
@@ -2761,13 +2759,13 @@
         <v>79</v>
       </c>
       <c r="D104" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E104" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>19</v>
       </c>
@@ -2775,13 +2773,13 @@
         <v>79</v>
       </c>
       <c r="D105" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E105" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>20</v>
       </c>
@@ -2789,13 +2787,13 @@
         <v>79</v>
       </c>
       <c r="D106" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E106" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>21</v>
       </c>
@@ -2803,13 +2801,13 @@
         <v>79</v>
       </c>
       <c r="D107" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E107" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>81</v>
       </c>
@@ -2820,13 +2818,13 @@
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E108" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>17</v>
       </c>
@@ -2834,13 +2832,13 @@
         <v>79</v>
       </c>
       <c r="D109" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E109" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>19</v>
       </c>
@@ -2848,13 +2846,13 @@
         <v>79</v>
       </c>
       <c r="D110" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E110" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>20</v>
       </c>
@@ -2862,13 +2860,13 @@
         <v>79</v>
       </c>
       <c r="D111" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E111" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>21</v>
       </c>
@@ -2876,13 +2874,13 @@
         <v>79</v>
       </c>
       <c r="D112" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E112" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>81</v>
       </c>
@@ -2893,13 +2891,13 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E113" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>83</v>
       </c>
@@ -2907,13 +2905,13 @@
         <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E114" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>86</v>
       </c>
@@ -2924,13 +2922,13 @@
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E115" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>83</v>
       </c>
@@ -2938,13 +2936,13 @@
         <v>84</v>
       </c>
       <c r="D116" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E116" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>86</v>
       </c>
@@ -2955,13 +2953,13 @@
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E117" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>83</v>
       </c>
@@ -2969,13 +2967,13 @@
         <v>84</v>
       </c>
       <c r="D118" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E118" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>86</v>
       </c>
@@ -2986,13 +2984,13 @@
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E119" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>17</v>
       </c>
@@ -3000,13 +2998,13 @@
         <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E120" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>88</v>
       </c>
@@ -3017,13 +3015,13 @@
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>17</v>
       </c>
@@ -3031,30 +3029,30 @@
         <v>87</v>
       </c>
       <c r="D122" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E122" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>88</v>
       </c>
       <c r="B123" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E123" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>19</v>
       </c>
@@ -3068,7 +3066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>21</v>
       </c>
@@ -3082,7 +3080,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>17</v>
       </c>
@@ -3096,7 +3094,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>19</v>
       </c>
@@ -3110,7 +3108,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>20</v>
       </c>
@@ -3124,7 +3122,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>21</v>
       </c>
@@ -3138,7 +3136,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>83</v>
       </c>
@@ -3155,7 +3153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>83</v>
       </c>
@@ -3172,7 +3170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>83</v>
       </c>
@@ -3189,7 +3187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>83</v>
       </c>
@@ -3206,7 +3204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -3223,7 +3221,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>21</v>
       </c>
@@ -3240,7 +3238,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>19</v>
       </c>
@@ -3257,7 +3255,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>21</v>
       </c>
@@ -3274,7 +3272,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>19</v>
       </c>
@@ -3291,7 +3289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>21</v>
       </c>
@@ -3308,12 +3306,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>83</v>
       </c>
       <c r="B140" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -3322,15 +3320,15 @@
         <v>94</v>
       </c>
       <c r="E140" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>83</v>
       </c>
       <c r="B141" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -3339,15 +3337,15 @@
         <v>96</v>
       </c>
       <c r="E141" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>83</v>
       </c>
       <c r="B142" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -3356,15 +3354,15 @@
         <v>98</v>
       </c>
       <c r="E142" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>83</v>
       </c>
       <c r="B143" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -3373,15 +3371,15 @@
         <v>100</v>
       </c>
       <c r="E143" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -3390,15 +3388,15 @@
         <v>103</v>
       </c>
       <c r="E144" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -3407,15 +3405,15 @@
         <v>103</v>
       </c>
       <c r="E145" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -3424,15 +3422,15 @@
         <v>103</v>
       </c>
       <c r="E146" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -3441,15 +3439,15 @@
         <v>103</v>
       </c>
       <c r="E147" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -3458,15 +3456,15 @@
         <v>104</v>
       </c>
       <c r="E148" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -3475,10 +3473,10 @@
         <v>104</v>
       </c>
       <c r="E149" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>17</v>
       </c>
@@ -3495,7 +3493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>19</v>
       </c>
@@ -3512,7 +3510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>20</v>
       </c>
@@ -3529,7 +3527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>21</v>
       </c>
@@ -3546,7 +3544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>17</v>
       </c>
@@ -3560,10 +3558,10 @@
         <v>105</v>
       </c>
       <c r="E154" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>19</v>
       </c>
@@ -3577,10 +3575,10 @@
         <v>105</v>
       </c>
       <c r="E155" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>20</v>
       </c>
@@ -3594,10 +3592,10 @@
         <v>105</v>
       </c>
       <c r="E156" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>21</v>
       </c>
@@ -3611,10 +3609,10 @@
         <v>105</v>
       </c>
       <c r="E157" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>19</v>
       </c>
@@ -3631,7 +3629,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>21</v>
       </c>
@@ -3648,7 +3646,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>19</v>
       </c>
@@ -3665,7 +3663,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>21</v>
       </c>
@@ -3682,7 +3680,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>19</v>
       </c>
@@ -3699,7 +3697,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>21</v>
       </c>
@@ -3716,7 +3714,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>19</v>
       </c>
@@ -3733,7 +3731,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>21</v>
       </c>
@@ -3750,7 +3748,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>19</v>
       </c>
@@ -3767,7 +3765,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>21</v>
       </c>
@@ -3784,7 +3782,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>19</v>
       </c>
@@ -3801,7 +3799,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>21</v>
       </c>
@@ -3818,7 +3816,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>19</v>
       </c>
@@ -3835,7 +3833,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>21</v>
       </c>
@@ -3852,7 +3850,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>83</v>
       </c>
@@ -3869,7 +3867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>83</v>
       </c>
@@ -3883,7 +3881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>83</v>
       </c>
@@ -3900,7 +3898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>83</v>
       </c>
@@ -3914,7 +3912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>83</v>
       </c>
@@ -3928,7 +3926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>83</v>
       </c>
@@ -3945,7 +3943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>83</v>
       </c>
@@ -3962,7 +3960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>17</v>
       </c>
@@ -3979,7 +3977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>20</v>
       </c>
@@ -3996,7 +3994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>83</v>
       </c>
@@ -4007,13 +4005,13 @@
         <v>1</v>
       </c>
       <c r="D181" t="s">
-        <v>127</v>
+        <v>231</v>
       </c>
       <c r="E181" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>83</v>
       </c>
@@ -4024,13 +4022,13 @@
         <v>1</v>
       </c>
       <c r="D182" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E182" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>83</v>
       </c>
@@ -4041,1162 +4039,1119 @@
         <v>2</v>
       </c>
       <c r="D183" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E183" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>83</v>
       </c>
       <c r="B184" t="s">
+        <v>129</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184" t="s">
         <v>130</v>
-      </c>
-      <c r="C184">
-        <v>1</v>
-      </c>
-      <c r="D184" t="s">
-        <v>131</v>
       </c>
       <c r="E184" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A185" s="1" t="s">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>20</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B185" t="s">
+        <v>141</v>
+      </c>
+      <c r="C185">
+        <v>2</v>
+      </c>
+      <c r="D185" t="s">
+        <v>137</v>
+      </c>
+      <c r="E185" t="s">
         <v>142</v>
       </c>
-      <c r="C185" s="1">
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>139</v>
+      </c>
+      <c r="B186" t="s">
+        <v>140</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="D186" t="s">
+        <v>137</v>
+      </c>
+      <c r="E186" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>139</v>
+      </c>
+      <c r="B187" t="s">
+        <v>140</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+      <c r="D187" t="s">
+        <v>137</v>
+      </c>
+      <c r="E187" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>17</v>
+      </c>
+      <c r="B188" t="s">
+        <v>143</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+      <c r="D188" t="s">
+        <v>137</v>
+      </c>
+      <c r="E188" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>20</v>
+      </c>
+      <c r="B189" t="s">
+        <v>143</v>
+      </c>
+      <c r="C189">
+        <v>1</v>
+      </c>
+      <c r="D189" t="s">
+        <v>137</v>
+      </c>
+      <c r="E189" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>17</v>
+      </c>
+      <c r="B190" t="s">
+        <v>136</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+      <c r="D190" t="s">
+        <v>137</v>
+      </c>
+      <c r="E190" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>20</v>
+      </c>
+      <c r="B191" t="s">
+        <v>136</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191" t="s">
+        <v>137</v>
+      </c>
+      <c r="E191" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>19</v>
+      </c>
+      <c r="B192" t="s">
+        <v>162</v>
+      </c>
+      <c r="D192" t="s">
+        <v>163</v>
+      </c>
+      <c r="E192" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>21</v>
+      </c>
+      <c r="B193" t="s">
+        <v>162</v>
+      </c>
+      <c r="D193" t="s">
+        <v>163</v>
+      </c>
+      <c r="E193" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>17</v>
+      </c>
+      <c r="B194" t="s">
+        <v>162</v>
+      </c>
+      <c r="D194" t="s">
+        <v>164</v>
+      </c>
+      <c r="E194" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>20</v>
+      </c>
+      <c r="B195" t="s">
+        <v>162</v>
+      </c>
+      <c r="D195" t="s">
+        <v>164</v>
+      </c>
+      <c r="E195" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>17</v>
+      </c>
+      <c r="B196" t="s">
+        <v>162</v>
+      </c>
+      <c r="D196" t="s">
+        <v>164</v>
+      </c>
+      <c r="E196" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>20</v>
+      </c>
+      <c r="B197" t="s">
+        <v>162</v>
+      </c>
+      <c r="D197" t="s">
+        <v>164</v>
+      </c>
+      <c r="E197" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>21</v>
+      </c>
+      <c r="B198" t="s">
+        <v>165</v>
+      </c>
+      <c r="D198" t="s">
+        <v>166</v>
+      </c>
+      <c r="E198" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>19</v>
+      </c>
+      <c r="B199" t="s">
+        <v>167</v>
+      </c>
+      <c r="D199" t="s">
+        <v>168</v>
+      </c>
+      <c r="E199" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>21</v>
+      </c>
+      <c r="B200" t="s">
+        <v>167</v>
+      </c>
+      <c r="D200" t="s">
+        <v>168</v>
+      </c>
+      <c r="E200" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>17</v>
+      </c>
+      <c r="B201" t="s">
+        <v>169</v>
+      </c>
+      <c r="D201" t="s">
+        <v>170</v>
+      </c>
+      <c r="E201" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>19</v>
+      </c>
+      <c r="B202" t="s">
+        <v>169</v>
+      </c>
+      <c r="D202" t="s">
+        <v>170</v>
+      </c>
+      <c r="E202" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>20</v>
+      </c>
+      <c r="B203" t="s">
+        <v>169</v>
+      </c>
+      <c r="D203" t="s">
+        <v>170</v>
+      </c>
+      <c r="E203" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>21</v>
+      </c>
+      <c r="B204" t="s">
+        <v>169</v>
+      </c>
+      <c r="D204" t="s">
+        <v>170</v>
+      </c>
+      <c r="E204" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>19</v>
+      </c>
+      <c r="B205" t="s">
+        <v>171</v>
+      </c>
+      <c r="D205" t="s">
+        <v>172</v>
+      </c>
+      <c r="E205" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>21</v>
+      </c>
+      <c r="B206" t="s">
+        <v>171</v>
+      </c>
+      <c r="D206" t="s">
+        <v>172</v>
+      </c>
+      <c r="E206" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>17</v>
+      </c>
+      <c r="B207" t="s">
+        <v>171</v>
+      </c>
+      <c r="D207" t="s">
+        <v>173</v>
+      </c>
+      <c r="E207" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>174</v>
+      </c>
+      <c r="B208" t="s">
+        <v>82</v>
+      </c>
+      <c r="C208">
         <v>2</v>
       </c>
-      <c r="D185" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A186" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C186" s="1">
-        <v>1</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A187" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C187" s="1">
-        <v>1</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A188" s="1" t="s">
+      <c r="D208" t="s">
+        <v>173</v>
+      </c>
+      <c r="E208" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>17</v>
       </c>
-      <c r="B188" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C188" s="1">
-        <v>1</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A189" s="1" t="s">
+      <c r="B209" t="s">
+        <v>171</v>
+      </c>
+      <c r="D209" t="s">
+        <v>173</v>
+      </c>
+      <c r="E209" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>174</v>
+      </c>
+      <c r="B210" t="s">
+        <v>147</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+      <c r="D210" t="s">
+        <v>173</v>
+      </c>
+      <c r="E210" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>19</v>
+      </c>
+      <c r="B211" t="s">
+        <v>176</v>
+      </c>
+      <c r="D211" t="s">
+        <v>177</v>
+      </c>
+      <c r="E211" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>21</v>
+      </c>
+      <c r="B212" t="s">
+        <v>176</v>
+      </c>
+      <c r="D212" t="s">
+        <v>177</v>
+      </c>
+      <c r="E212" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>20</v>
       </c>
-      <c r="B189" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C189" s="1">
-        <v>1</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A190" s="1" t="s">
+      <c r="B213" t="s">
+        <v>178</v>
+      </c>
+      <c r="D213" t="s">
+        <v>179</v>
+      </c>
+      <c r="E213" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>21</v>
+      </c>
+      <c r="B214" t="s">
+        <v>178</v>
+      </c>
+      <c r="D214" t="s">
+        <v>179</v>
+      </c>
+      <c r="E214" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>19</v>
+      </c>
+      <c r="B215" t="s">
+        <v>180</v>
+      </c>
+      <c r="D215" t="s">
+        <v>181</v>
+      </c>
+      <c r="E215" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>21</v>
+      </c>
+      <c r="B216" t="s">
+        <v>180</v>
+      </c>
+      <c r="D216" t="s">
+        <v>181</v>
+      </c>
+      <c r="E216" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>19</v>
+      </c>
+      <c r="B217" t="s">
+        <v>182</v>
+      </c>
+      <c r="D217" t="s">
+        <v>183</v>
+      </c>
+      <c r="E217" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>21</v>
+      </c>
+      <c r="B218" t="s">
+        <v>182</v>
+      </c>
+      <c r="D218" t="s">
+        <v>183</v>
+      </c>
+      <c r="E218" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>19</v>
+      </c>
+      <c r="B219" t="s">
+        <v>184</v>
+      </c>
+      <c r="D219" t="s">
+        <v>185</v>
+      </c>
+      <c r="E219" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>21</v>
+      </c>
+      <c r="B220" t="s">
+        <v>184</v>
+      </c>
+      <c r="D220" t="s">
+        <v>185</v>
+      </c>
+      <c r="E220" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>17</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C190" s="1">
-        <v>1</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A191" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C191" s="1">
-        <v>1</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A192" s="1" t="s">
+      <c r="B221" t="s">
+        <v>184</v>
+      </c>
+      <c r="D221" t="s">
+        <v>186</v>
+      </c>
+      <c r="E221" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>17</v>
+      </c>
+      <c r="B222" t="s">
+        <v>184</v>
+      </c>
+      <c r="D222" t="s">
+        <v>186</v>
+      </c>
+      <c r="E222" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>174</v>
+      </c>
+      <c r="B223" t="s">
+        <v>147</v>
+      </c>
+      <c r="C223">
+        <v>1</v>
+      </c>
+      <c r="D223" t="s">
+        <v>186</v>
+      </c>
+      <c r="E223" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>19</v>
       </c>
-      <c r="B192" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C192" s="1"/>
-      <c r="D192" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E192" s="1" t="s">
+      <c r="B224" t="s">
+        <v>187</v>
+      </c>
+      <c r="D224" t="s">
+        <v>188</v>
+      </c>
+      <c r="E224" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A193" s="1" t="s">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>21</v>
       </c>
-      <c r="B193" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C193" s="1"/>
-      <c r="D193" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E193" s="1" t="s">
+      <c r="B225" t="s">
+        <v>187</v>
+      </c>
+      <c r="D225" t="s">
+        <v>188</v>
+      </c>
+      <c r="E225" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A194" s="1" t="s">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>17</v>
       </c>
-      <c r="B194" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C194" s="1"/>
-      <c r="D194" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E194" s="1" t="s">
+      <c r="B226" t="s">
+        <v>187</v>
+      </c>
+      <c r="D226" t="s">
+        <v>189</v>
+      </c>
+      <c r="E226" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A195" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C195" s="1"/>
-      <c r="D195" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E195" s="1" t="s">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>190</v>
+      </c>
+      <c r="B227" t="s">
+        <v>82</v>
+      </c>
+      <c r="C227">
+        <v>2</v>
+      </c>
+      <c r="D227" t="s">
+        <v>189</v>
+      </c>
+      <c r="E227" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A196" s="1" t="s">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>17</v>
       </c>
-      <c r="B196" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C196" s="1"/>
-      <c r="D196" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E196" s="1" t="s">
+      <c r="B228" t="s">
+        <v>187</v>
+      </c>
+      <c r="D228" t="s">
+        <v>189</v>
+      </c>
+      <c r="E228" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A197" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C197" s="1"/>
-      <c r="D197" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E197" s="1" t="s">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>190</v>
+      </c>
+      <c r="B229" t="s">
+        <v>147</v>
+      </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+      <c r="D229" t="s">
+        <v>189</v>
+      </c>
+      <c r="E229" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A198" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C198" s="1"/>
-      <c r="D198" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E198" s="1" t="s">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>17</v>
+      </c>
+      <c r="B230" t="s">
+        <v>191</v>
+      </c>
+      <c r="D230" t="s">
+        <v>192</v>
+      </c>
+      <c r="E230" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A199" s="1" t="s">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
         <v>19</v>
       </c>
-      <c r="B199" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C199" s="1"/>
-      <c r="D199" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E199" s="1" t="s">
+      <c r="B231" t="s">
+        <v>191</v>
+      </c>
+      <c r="D231" t="s">
+        <v>192</v>
+      </c>
+      <c r="E231" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A200" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C200" s="1"/>
-      <c r="D200" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E200" s="1" t="s">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>193</v>
+      </c>
+      <c r="B232" t="s">
+        <v>82</v>
+      </c>
+      <c r="C232">
+        <v>1</v>
+      </c>
+      <c r="D232" t="s">
+        <v>192</v>
+      </c>
+      <c r="E232" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A201" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C201" s="1"/>
-      <c r="D201" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A202" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C202" s="1"/>
-      <c r="D202" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E202" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A203" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C203" s="1"/>
-      <c r="D203" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A204" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C204" s="1"/>
-      <c r="D204" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A205" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C205" s="1"/>
-      <c r="D205" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A206" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C206" s="1"/>
-      <c r="D206" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A207" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C207" s="1"/>
-      <c r="D207" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A208" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C208" s="1">
-        <v>2</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A209" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C209" s="1"/>
-      <c r="D209" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A210" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C210" s="1">
-        <v>1</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A211" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C211" s="1"/>
-      <c r="D211" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A212" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C212" s="1"/>
-      <c r="D212" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A213" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C213" s="1"/>
-      <c r="D213" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A214" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C214" s="1"/>
-      <c r="D214" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A215" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C215" s="1"/>
-      <c r="D215" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A216" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C216" s="1"/>
-      <c r="D216" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A217" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C217" s="1"/>
-      <c r="D217" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A218" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C218" s="1"/>
-      <c r="D218" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E218" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A219" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C219" s="1"/>
-      <c r="D219" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A220" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C220" s="1"/>
-      <c r="D220" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A221" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C221" s="1"/>
-      <c r="D221" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A222" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C222" s="1"/>
-      <c r="D222" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A223" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C223" s="1">
-        <v>1</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A224" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C224" s="1"/>
-      <c r="D224" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A225" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C225" s="1"/>
-      <c r="D225" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A226" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C226" s="1"/>
-      <c r="D226" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A227" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C227" s="1">
-        <v>2</v>
-      </c>
-      <c r="D227" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A228" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C228" s="1"/>
-      <c r="D228" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A229" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C229" s="1">
-        <v>1</v>
-      </c>
-      <c r="D229" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A230" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B230" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C230" s="1"/>
-      <c r="D230" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A231" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C231" s="1"/>
-      <c r="D231" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A232" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C232" s="1">
-        <v>1</v>
-      </c>
-      <c r="D232" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>17</v>
       </c>
       <c r="B233" t="s">
+        <v>191</v>
+      </c>
+      <c r="D233" t="s">
         <v>192</v>
-      </c>
-      <c r="D233" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="E233" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A234" s="1" t="s">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>193</v>
+      </c>
+      <c r="B234" t="s">
+        <v>56</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+      <c r="D234" t="s">
+        <v>192</v>
+      </c>
+      <c r="E234" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>17</v>
+      </c>
+      <c r="B235" t="s">
+        <v>191</v>
+      </c>
+      <c r="D235" t="s">
+        <v>192</v>
+      </c>
+      <c r="E235" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>193</v>
+      </c>
+      <c r="B236" t="s">
+        <v>66</v>
+      </c>
+      <c r="C236">
+        <v>1</v>
+      </c>
+      <c r="D236" t="s">
+        <v>192</v>
+      </c>
+      <c r="E236" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>17</v>
+      </c>
+      <c r="B237" t="s">
+        <v>196</v>
+      </c>
+      <c r="D237" t="s">
+        <v>195</v>
+      </c>
+      <c r="E237" t="s">
         <v>194</v>
       </c>
-      <c r="B234" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C234" s="1">
-        <v>1</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A235" s="1" t="s">
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>197</v>
+      </c>
+      <c r="B238" t="s">
+        <v>82</v>
+      </c>
+      <c r="C238">
+        <v>2</v>
+      </c>
+      <c r="D238" t="s">
+        <v>195</v>
+      </c>
+      <c r="E238" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
         <v>17</v>
       </c>
-      <c r="B235" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C235" s="1"/>
-      <c r="D235" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A236" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B236" s="1" t="s">
+      <c r="B239" t="s">
+        <v>196</v>
+      </c>
+      <c r="D239" t="s">
+        <v>195</v>
+      </c>
+      <c r="E239" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>197</v>
+      </c>
+      <c r="B240" t="s">
+        <v>147</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240" t="s">
+        <v>195</v>
+      </c>
+      <c r="E240" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>17</v>
+      </c>
+      <c r="B241" t="s">
+        <v>199</v>
+      </c>
+      <c r="D241" t="s">
+        <v>195</v>
+      </c>
+      <c r="E241" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>201</v>
+      </c>
+      <c r="B242" t="s">
+        <v>82</v>
+      </c>
+      <c r="C242">
+        <v>2</v>
+      </c>
+      <c r="D242" t="s">
+        <v>195</v>
+      </c>
+      <c r="E242" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>17</v>
+      </c>
+      <c r="B243" t="s">
+        <v>199</v>
+      </c>
+      <c r="D243" t="s">
+        <v>195</v>
+      </c>
+      <c r="E243" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>201</v>
+      </c>
+      <c r="B244" t="s">
+        <v>147</v>
+      </c>
+      <c r="C244">
+        <v>1</v>
+      </c>
+      <c r="D244" t="s">
+        <v>195</v>
+      </c>
+      <c r="E244" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>17</v>
+      </c>
+      <c r="B245" t="s">
+        <v>212</v>
+      </c>
+      <c r="D245" t="s">
+        <v>230</v>
+      </c>
+      <c r="E245" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>20</v>
+      </c>
+      <c r="B246" t="s">
+        <v>212</v>
+      </c>
+      <c r="D246" t="s">
+        <v>230</v>
+      </c>
+      <c r="E246" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>214</v>
+      </c>
+      <c r="B247" t="s">
+        <v>147</v>
+      </c>
+      <c r="C247">
+        <v>1</v>
+      </c>
+      <c r="D247" t="s">
+        <v>230</v>
+      </c>
+      <c r="E247" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>214</v>
+      </c>
+      <c r="B248" t="s">
+        <v>82</v>
+      </c>
+      <c r="C248">
+        <v>1</v>
+      </c>
+      <c r="D248" t="s">
+        <v>230</v>
+      </c>
+      <c r="E248" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>214</v>
+      </c>
+      <c r="B249" t="s">
+        <v>62</v>
+      </c>
+      <c r="C249">
+        <v>1</v>
+      </c>
+      <c r="D249" t="s">
+        <v>230</v>
+      </c>
+      <c r="E249" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>214</v>
+      </c>
+      <c r="B250" t="s">
         <v>66</v>
       </c>
-      <c r="C236" s="1">
-        <v>1</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A237" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C237" s="1"/>
-      <c r="D237" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A238" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B238" s="1" t="s">
+      <c r="C250">
+        <v>1</v>
+      </c>
+      <c r="D250" t="s">
+        <v>230</v>
+      </c>
+      <c r="E250" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>214</v>
+      </c>
+      <c r="B251" t="s">
+        <v>218</v>
+      </c>
+      <c r="C251">
+        <v>1</v>
+      </c>
+      <c r="D251" t="s">
+        <v>230</v>
+      </c>
+      <c r="E251" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>21</v>
+      </c>
+      <c r="B252" t="s">
+        <v>222</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+      <c r="D252" t="s">
+        <v>223</v>
+      </c>
+      <c r="E252" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>20</v>
+      </c>
+      <c r="B253" t="s">
+        <v>224</v>
+      </c>
+      <c r="D253" t="s">
+        <v>225</v>
+      </c>
+      <c r="E253" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>227</v>
+      </c>
+      <c r="B254" t="s">
         <v>82</v>
       </c>
-      <c r="C238" s="1">
-        <v>2</v>
-      </c>
-      <c r="D238" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A239" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C239" s="1"/>
-      <c r="D239" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A240" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C240" s="1">
-        <v>1</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A241" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C241" s="1"/>
-      <c r="D241" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A242" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B242" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C242" s="1">
-        <v>2</v>
-      </c>
-      <c r="D242" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A243" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C243" s="1"/>
-      <c r="D243" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A244" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C244" s="1">
-        <v>1</v>
-      </c>
-      <c r="D244" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A245" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B245" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C245" s="1"/>
-      <c r="D245" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A246" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C246" s="1"/>
-      <c r="D246" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A247" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C247" s="1">
-        <v>1</v>
-      </c>
-      <c r="D247" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A248" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C248" s="1">
-        <v>1</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A249" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C249" s="1">
-        <v>1</v>
-      </c>
-      <c r="D249" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A250" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B250" s="1" t="s">
+      <c r="C254">
+        <v>1</v>
+      </c>
+      <c r="D254" t="s">
+        <v>225</v>
+      </c>
+      <c r="E254" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>227</v>
+      </c>
+      <c r="B255" t="s">
         <v>66</v>
       </c>
-      <c r="C250" s="1">
-        <v>1</v>
-      </c>
-      <c r="D250" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A251" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C251" s="1">
-        <v>1</v>
-      </c>
-      <c r="D251" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A252" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C252" s="1">
-        <v>1</v>
-      </c>
-      <c r="D252" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A253" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B253" s="1" t="s">
+      <c r="C255">
+        <v>1</v>
+      </c>
+      <c r="D255" t="s">
         <v>225</v>
       </c>
-      <c r="C253" s="1"/>
-      <c r="D253" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E253" s="1" t="s">
+      <c r="E255" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A254" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B254" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C254" s="1">
-        <v>1</v>
-      </c>
-      <c r="D254" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A255" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C255" s="1">
-        <v>1</v>
-      </c>
-      <c r="D255" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E255" s="1" t="s">
+      <c r="B256" t="s">
+        <v>147</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
+      <c r="D256" t="s">
+        <v>225</v>
+      </c>
+      <c r="E256" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A256" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C256" s="1">
-        <v>1</v>
-      </c>
-      <c r="D256" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Outlook] Add MailboxEnums to enum names
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25519"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573EEB92-EB70-4023-A64F-7D50B497C831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605E840B-88E4-453B-8FA2-3B255470EF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-90" windowWidth="38640" windowHeight="23520" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -726,31 +726,31 @@
     <t>outlook-tokens-and-service-calls-get-icaluid-as-attendee</t>
   </si>
   <si>
-    <t>AppointmentSensitivity</t>
-  </si>
-  <si>
     <t>enum</t>
   </si>
   <si>
-    <t>AttachmentContentFormat</t>
-  </si>
-  <si>
     <t>handleAttachmentsCallback</t>
   </si>
   <si>
-    <t>CategoryColor</t>
-  </si>
-  <si>
-    <t>DelegatePermissions</t>
-  </si>
-  <si>
-    <t>EntityType</t>
-  </si>
-  <si>
-    <t>LocationType</t>
-  </si>
-  <si>
-    <t>RestVersion</t>
+    <t>MailboxEnums.AppointmentSensitivity</t>
+  </si>
+  <si>
+    <t>MailboxEnums.AttachmentContentFormat</t>
+  </si>
+  <si>
+    <t>MailboxEnums.CategoryColor</t>
+  </si>
+  <si>
+    <t>MailboxEnums.DelegatePermissions</t>
+  </si>
+  <si>
+    <t>MailboxEnums.EntityType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.LocationType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.RestVersion</t>
   </si>
 </sst>
 </file>
@@ -1165,20 +1165,20 @@
   <dimension ref="A1:E263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="74.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>19</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>19</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>19</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>19</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>19</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>19</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>19</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -2599,201 +2599,213 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>232</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>233</v>
+        <v>139</v>
+      </c>
+      <c r="B95" t="s">
+        <v>140</v>
+      </c>
+      <c r="C95" s="1">
+        <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="E95" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>234</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>233</v>
+        <v>139</v>
+      </c>
+      <c r="B96" t="s">
+        <v>140</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E96" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="B97" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="C97" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="E97" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="B98" t="s">
-        <v>140</v>
+        <v>56</v>
       </c>
       <c r="C98" s="1">
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="E98" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>81</v>
       </c>
       <c r="B99" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C99" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D99" t="s">
         <v>161</v>
       </c>
       <c r="E99" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="B100" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="C100" s="1">
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="E100" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="B101" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="C101" s="1">
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="E101" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>236</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>233</v>
+        <v>14</v>
+      </c>
+      <c r="B102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>158</v>
+        <v>15</v>
       </c>
       <c r="E102" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>15</v>
+        <v>192</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="B104" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C104" s="1">
         <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>15</v>
+        <v>192</v>
       </c>
       <c r="E104" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C105" s="1">
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>15</v>
+        <v>192</v>
       </c>
       <c r="E105" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>237</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>233</v>
+        <v>133</v>
+      </c>
+      <c r="B106" t="s">
+        <v>82</v>
+      </c>
+      <c r="C106" s="1">
+        <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="E106" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="B107" t="s">
         <v>82</v>
@@ -2802,606 +2814,591 @@
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="B108" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C108" s="1">
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="E108" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="C109" s="1">
         <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="E109" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>238</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>233</v>
+        <v>197</v>
+      </c>
+      <c r="B110" t="s">
+        <v>82</v>
+      </c>
+      <c r="C110" s="1">
+        <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>109</v>
+        <v>195</v>
       </c>
       <c r="E110" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>133</v>
+        <v>197</v>
       </c>
       <c r="B111" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C111" s="1">
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
       <c r="E111" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="B112" t="s">
         <v>82</v>
       </c>
       <c r="C112" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D112" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="E112" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="B113" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="C113" s="1">
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="E113" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>227</v>
+        <v>83</v>
       </c>
       <c r="B114" t="s">
-        <v>147</v>
-      </c>
-      <c r="C114" s="1">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>225</v>
+        <v>158</v>
       </c>
       <c r="E114" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>197</v>
+        <v>83</v>
       </c>
       <c r="B115" t="s">
-        <v>82</v>
-      </c>
-      <c r="C115" s="1">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D115" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="E115" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>197</v>
+        <v>83</v>
       </c>
       <c r="B116" t="s">
-        <v>147</v>
-      </c>
-      <c r="C116" s="1">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D116" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="E116" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>190</v>
+        <v>83</v>
       </c>
       <c r="B117" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C117" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>189</v>
+        <v>94</v>
       </c>
       <c r="E117" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>190</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="E118" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>239</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>233</v>
+        <v>83</v>
+      </c>
+      <c r="B119" t="s">
+        <v>97</v>
+      </c>
+      <c r="C119" s="1">
+        <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>192</v>
+        <v>98</v>
       </c>
       <c r="E119" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>83</v>
       </c>
       <c r="B120" t="s">
-        <v>84</v>
+        <v>99</v>
+      </c>
+      <c r="C120" s="1">
+        <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="E120" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>83</v>
       </c>
       <c r="B121" t="s">
-        <v>84</v>
+        <v>205</v>
+      </c>
+      <c r="C121" s="1">
+        <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="E121" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>83</v>
       </c>
       <c r="B122" t="s">
-        <v>84</v>
+        <v>206</v>
+      </c>
+      <c r="C122" s="1">
+        <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>158</v>
+        <v>96</v>
       </c>
       <c r="E122" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>83</v>
       </c>
       <c r="B123" t="s">
-        <v>93</v>
+        <v>207</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E123" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>83</v>
       </c>
       <c r="B124" t="s">
-        <v>95</v>
+        <v>208</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E124" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>83</v>
       </c>
       <c r="B125" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="E125" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>83</v>
       </c>
       <c r="B126" t="s">
-        <v>99</v>
-      </c>
-      <c r="C126" s="1">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D126" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="E126" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>83</v>
       </c>
       <c r="B127" t="s">
-        <v>205</v>
+        <v>107</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="E127" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>83</v>
       </c>
       <c r="B128" t="s">
-        <v>206</v>
-      </c>
-      <c r="C128" s="1">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="D128" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="E128" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>207</v>
-      </c>
-      <c r="C129" s="1">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D129" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="E129" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>83</v>
       </c>
       <c r="B130" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="E130" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>83</v>
       </c>
       <c r="B131" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C131" s="1">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E131" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>83</v>
       </c>
       <c r="B132" t="s">
-        <v>120</v>
+        <v>126</v>
+      </c>
+      <c r="C132" s="1">
+        <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>119</v>
+        <v>231</v>
       </c>
       <c r="E132" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>83</v>
       </c>
       <c r="B133" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="C133" s="1">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="E133" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>83</v>
       </c>
       <c r="B134" t="s">
-        <v>121</v>
+        <v>107</v>
+      </c>
+      <c r="C134" s="1">
+        <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E134" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>83</v>
       </c>
       <c r="B135" t="s">
-        <v>120</v>
+        <v>129</v>
+      </c>
+      <c r="C135" s="1">
+        <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="E135" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>83</v>
-      </c>
-      <c r="B136" t="s">
-        <v>118</v>
-      </c>
-      <c r="C136" s="1">
-        <v>1</v>
+        <v>234</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="D136" t="s">
-        <v>122</v>
+        <v>195</v>
       </c>
       <c r="E136" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>235</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D137" t="s">
+        <v>135</v>
+      </c>
+      <c r="E137" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>236</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D138" t="s">
+        <v>158</v>
+      </c>
+      <c r="E138" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>237</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D139" t="s">
+        <v>105</v>
+      </c>
+      <c r="E139" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>238</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D140" t="s">
+        <v>109</v>
+      </c>
+      <c r="E140" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>239</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D141" t="s">
+        <v>192</v>
+      </c>
+      <c r="E141" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>240</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D142" t="s">
+        <v>119</v>
+      </c>
+      <c r="E142" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>83</v>
-      </c>
-      <c r="B137" t="s">
-        <v>123</v>
-      </c>
-      <c r="C137" s="1">
-        <v>1</v>
-      </c>
-      <c r="D137" t="s">
-        <v>122</v>
-      </c>
-      <c r="E137" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>83</v>
-      </c>
-      <c r="B138" t="s">
-        <v>126</v>
-      </c>
-      <c r="C138" s="1">
-        <v>1</v>
-      </c>
-      <c r="D138" t="s">
-        <v>231</v>
-      </c>
-      <c r="E138" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>83</v>
-      </c>
-      <c r="B139" t="s">
-        <v>126</v>
-      </c>
-      <c r="C139" s="1">
-        <v>1</v>
-      </c>
-      <c r="D139" t="s">
-        <v>127</v>
-      </c>
-      <c r="E139" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>83</v>
-      </c>
-      <c r="B140" t="s">
-        <v>107</v>
-      </c>
-      <c r="C140" s="1">
-        <v>2</v>
-      </c>
-      <c r="D140" t="s">
-        <v>128</v>
-      </c>
-      <c r="E140" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>83</v>
-      </c>
-      <c r="B141" t="s">
-        <v>129</v>
-      </c>
-      <c r="C141" s="1">
-        <v>1</v>
-      </c>
-      <c r="D141" t="s">
-        <v>130</v>
-      </c>
-      <c r="E141" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>86</v>
-      </c>
-      <c r="B142" t="s">
-        <v>82</v>
-      </c>
-      <c r="C142" s="1">
-        <v>2</v>
-      </c>
-      <c r="D142" t="s">
-        <v>158</v>
-      </c>
-      <c r="E142" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>86</v>
       </c>
       <c r="B143" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C143" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D143" t="s">
         <v>158</v>
       </c>
       <c r="E143" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>86</v>
       </c>
       <c r="B144" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C144" s="1">
         <v>1</v>
@@ -3410,92 +3407,95 @@
         <v>158</v>
       </c>
       <c r="E144" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" t="s">
+        <v>66</v>
+      </c>
+      <c r="C145" s="1">
+        <v>1</v>
+      </c>
+      <c r="D145" t="s">
+        <v>158</v>
+      </c>
+      <c r="E145" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>20</v>
-      </c>
-      <c r="B145" t="s">
-        <v>18</v>
-      </c>
-      <c r="C145" s="1">
-        <v>1</v>
-      </c>
-      <c r="D145" t="s">
-        <v>15</v>
-      </c>
-      <c r="E145" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>20</v>
       </c>
       <c r="B146" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C146" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E146" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>20</v>
       </c>
       <c r="B147" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C147" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D147" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E147" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>20</v>
       </c>
       <c r="B148" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C148" s="1">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E148" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>20</v>
       </c>
       <c r="B149" t="s">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="C149" s="1">
+        <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>150</v>
+        <v>28</v>
       </c>
       <c r="E149" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>20</v>
       </c>
@@ -3506,24 +3506,24 @@
         <v>150</v>
       </c>
       <c r="E150" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>20</v>
       </c>
       <c r="B151" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D151" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E151" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>20</v>
       </c>
@@ -3534,38 +3534,38 @@
         <v>148</v>
       </c>
       <c r="E152" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>20</v>
       </c>
       <c r="B153" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D153" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="E153" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>20</v>
       </c>
       <c r="B154" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D154" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="E154" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>20</v>
       </c>
@@ -3576,24 +3576,24 @@
         <v>145</v>
       </c>
       <c r="E155" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D156" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="E156" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>20</v>
       </c>
@@ -3604,10 +3604,10 @@
         <v>57</v>
       </c>
       <c r="E157" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>20</v>
       </c>
@@ -3618,10 +3618,10 @@
         <v>57</v>
       </c>
       <c r="E158" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>20</v>
       </c>
@@ -3632,10 +3632,10 @@
         <v>57</v>
       </c>
       <c r="E159" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>20</v>
       </c>
@@ -3646,10 +3646,10 @@
         <v>57</v>
       </c>
       <c r="E160" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>20</v>
       </c>
@@ -3660,32 +3660,29 @@
         <v>57</v>
       </c>
       <c r="E161" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>20</v>
       </c>
       <c r="B162" t="s">
-        <v>67</v>
-      </c>
-      <c r="C162" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D162" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E162" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>20</v>
       </c>
       <c r="B163" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C163" s="1">
         <v>1</v>
@@ -3694,15 +3691,15 @@
         <v>68</v>
       </c>
       <c r="E163" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>20</v>
       </c>
       <c r="B164" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -3711,10 +3708,10 @@
         <v>68</v>
       </c>
       <c r="E164" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>20</v>
       </c>
@@ -3725,35 +3722,35 @@
         <v>1</v>
       </c>
       <c r="D165" t="s">
-        <v>137</v>
+        <v>68</v>
       </c>
       <c r="E165" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>20</v>
       </c>
       <c r="B166" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C166" s="1">
         <v>1</v>
       </c>
       <c r="D166" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="E166" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>20</v>
       </c>
       <c r="B167" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
@@ -3762,41 +3759,44 @@
         <v>68</v>
       </c>
       <c r="E167" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>20</v>
       </c>
       <c r="B168" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C168" s="1">
         <v>1</v>
       </c>
       <c r="D168" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="E168" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>20</v>
       </c>
       <c r="B169" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="C169" s="1">
+        <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="E169" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>20</v>
       </c>
@@ -3807,10 +3807,10 @@
         <v>161</v>
       </c>
       <c r="E170" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>20</v>
       </c>
@@ -3821,41 +3821,38 @@
         <v>161</v>
       </c>
       <c r="E171" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>20</v>
       </c>
       <c r="B172" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D172" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="E172" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>20</v>
       </c>
       <c r="B173" t="s">
-        <v>106</v>
-      </c>
-      <c r="C173" s="1">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="D173" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E173" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>20</v>
       </c>
@@ -3863,72 +3860,72 @@
         <v>106</v>
       </c>
       <c r="C174" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D174" t="s">
         <v>105</v>
       </c>
       <c r="E174" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>20</v>
       </c>
       <c r="B175" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C175" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D175" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="E175" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>20</v>
       </c>
       <c r="B176" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C176" s="1">
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E176" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>20</v>
       </c>
       <c r="B177" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C177" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D177" t="s">
         <v>137</v>
       </c>
       <c r="E177" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>20</v>
       </c>
       <c r="B178" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C178" s="1">
         <v>1</v>
@@ -3937,24 +3934,27 @@
         <v>137</v>
       </c>
       <c r="E178" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>20</v>
       </c>
       <c r="B179" t="s">
-        <v>162</v>
+        <v>136</v>
+      </c>
+      <c r="C179" s="1">
+        <v>1</v>
       </c>
       <c r="D179" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="E179" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>20</v>
       </c>
@@ -3965,153 +3965,153 @@
         <v>164</v>
       </c>
       <c r="E180" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>20</v>
       </c>
       <c r="B181" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D181" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E181" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>20</v>
       </c>
       <c r="B182" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D182" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E182" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>20</v>
       </c>
       <c r="B183" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="D183" t="s">
-        <v>230</v>
+        <v>179</v>
       </c>
       <c r="E183" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>20</v>
       </c>
       <c r="B184" t="s">
+        <v>212</v>
+      </c>
+      <c r="D184" t="s">
+        <v>230</v>
+      </c>
+      <c r="E184" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>20</v>
+      </c>
+      <c r="B185" t="s">
         <v>224</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D185" t="s">
         <v>225</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E185" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>21</v>
-      </c>
-      <c r="B185" t="s">
-        <v>18</v>
-      </c>
-      <c r="C185" s="1">
-        <v>1</v>
-      </c>
-      <c r="D185" t="s">
-        <v>15</v>
-      </c>
-      <c r="E185" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>21</v>
       </c>
       <c r="B186" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="C186" s="1">
+        <v>1</v>
       </c>
       <c r="D186" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E186" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>21</v>
       </c>
       <c r="B187" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D187" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E187" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>21</v>
       </c>
       <c r="B188" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D188" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E188" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>21</v>
       </c>
       <c r="B189" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D189" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E189" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>21</v>
       </c>
       <c r="B190" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D190" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E190" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>21</v>
       </c>
@@ -4122,10 +4122,10 @@
         <v>57</v>
       </c>
       <c r="E191" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>21</v>
       </c>
@@ -4136,10 +4136,10 @@
         <v>57</v>
       </c>
       <c r="E192" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>21</v>
       </c>
@@ -4150,10 +4150,10 @@
         <v>57</v>
       </c>
       <c r="E193" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>21</v>
       </c>
@@ -4164,10 +4164,10 @@
         <v>57</v>
       </c>
       <c r="E194" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>21</v>
       </c>
@@ -4178,55 +4178,55 @@
         <v>57</v>
       </c>
       <c r="E195" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>21</v>
       </c>
       <c r="B196" t="s">
-        <v>76</v>
-      </c>
-      <c r="C196" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D196" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="E196" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>21</v>
       </c>
       <c r="B197" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C197" s="1">
+        <v>1</v>
       </c>
       <c r="D197" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="E197" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>21</v>
       </c>
       <c r="B198" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D198" t="s">
-        <v>161</v>
+        <v>78</v>
       </c>
       <c r="E198" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>21</v>
       </c>
@@ -4237,10 +4237,10 @@
         <v>161</v>
       </c>
       <c r="E199" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>21</v>
       </c>
@@ -4251,60 +4251,57 @@
         <v>161</v>
       </c>
       <c r="E200" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>21</v>
       </c>
       <c r="B201" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D201" t="s">
-        <v>89</v>
+        <v>161</v>
       </c>
       <c r="E201" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>21</v>
       </c>
       <c r="B202" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D202" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E202" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>21</v>
       </c>
       <c r="B203" t="s">
-        <v>101</v>
-      </c>
-      <c r="C203" s="1">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D203" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E203" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>21</v>
       </c>
       <c r="B204" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C204" s="1">
         <v>1</v>
@@ -4313,49 +4310,49 @@
         <v>103</v>
       </c>
       <c r="E204" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>21</v>
       </c>
       <c r="B205" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C205" s="1">
         <v>1</v>
       </c>
       <c r="D205" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E205" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>21</v>
       </c>
       <c r="B206" t="s">
-        <v>209</v>
+        <v>101</v>
       </c>
       <c r="C206" s="1">
         <v>1</v>
       </c>
       <c r="D206" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E206" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>21</v>
       </c>
       <c r="B207" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C207" s="1">
         <v>1</v>
@@ -4364,44 +4361,44 @@
         <v>103</v>
       </c>
       <c r="E207" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>21</v>
       </c>
       <c r="B208" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C208" s="1">
         <v>1</v>
       </c>
       <c r="D208" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E208" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>21</v>
       </c>
       <c r="B209" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="C209" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D209" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E209" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>21</v>
       </c>
@@ -4409,38 +4406,38 @@
         <v>106</v>
       </c>
       <c r="C210" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D210" t="s">
         <v>105</v>
       </c>
       <c r="E210" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>21</v>
       </c>
       <c r="B211" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
       </c>
       <c r="D211" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E211" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>21</v>
       </c>
       <c r="B212" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -4449,32 +4446,32 @@
         <v>109</v>
       </c>
       <c r="E212" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>21</v>
       </c>
       <c r="B213" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
       </c>
       <c r="D213" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E213" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>21</v>
       </c>
       <c r="B214" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
@@ -4483,15 +4480,15 @@
         <v>112</v>
       </c>
       <c r="E214" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>21</v>
       </c>
       <c r="B215" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
@@ -4500,32 +4497,32 @@
         <v>112</v>
       </c>
       <c r="E215" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>21</v>
       </c>
       <c r="B216" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
       </c>
       <c r="D216" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E216" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>21</v>
       </c>
       <c r="B217" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C217" s="1">
         <v>1</v>
@@ -4534,198 +4531,198 @@
         <v>116</v>
       </c>
       <c r="E217" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>21</v>
       </c>
       <c r="B218" t="s">
-        <v>162</v>
+        <v>117</v>
+      </c>
+      <c r="C218" s="1">
+        <v>1</v>
       </c>
       <c r="D218" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="E218" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>21</v>
       </c>
       <c r="B219" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D219" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E219" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>21</v>
       </c>
       <c r="B220" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D220" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E220" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>21</v>
       </c>
       <c r="B221" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D221" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E221" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>21</v>
       </c>
       <c r="B222" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D222" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E222" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>21</v>
       </c>
       <c r="B223" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D223" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E223" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>21</v>
       </c>
       <c r="B224" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D224" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E224" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>21</v>
       </c>
       <c r="B225" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D225" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E225" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>21</v>
       </c>
       <c r="B226" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D226" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E226" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>21</v>
       </c>
       <c r="B227" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D227" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E227" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>21</v>
       </c>
       <c r="B228" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D228" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E228" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>21</v>
       </c>
       <c r="B229" t="s">
+        <v>187</v>
+      </c>
+      <c r="D229" t="s">
+        <v>188</v>
+      </c>
+      <c r="E229" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>21</v>
+      </c>
+      <c r="B230" t="s">
         <v>222</v>
       </c>
-      <c r="C229" s="1">
-        <v>1</v>
-      </c>
-      <c r="D229" t="s">
+      <c r="C230" s="1">
+        <v>1</v>
+      </c>
+      <c r="D230" t="s">
         <v>223</v>
       </c>
-      <c r="E229" t="s">
+      <c r="E230" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>55</v>
-      </c>
-      <c r="B230" t="s">
-        <v>56</v>
-      </c>
-      <c r="C230" s="1">
-        <v>1</v>
-      </c>
-      <c r="D230" t="s">
-        <v>57</v>
-      </c>
-      <c r="E230" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>55</v>
       </c>
@@ -4739,10 +4736,10 @@
         <v>57</v>
       </c>
       <c r="E231" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>55</v>
       </c>
@@ -4756,10 +4753,10 @@
         <v>57</v>
       </c>
       <c r="E232" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>55</v>
       </c>
@@ -4773,15 +4770,15 @@
         <v>57</v>
       </c>
       <c r="E233" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>55</v>
       </c>
       <c r="B234" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C234" s="1">
         <v>1</v>
@@ -4790,15 +4787,15 @@
         <v>57</v>
       </c>
       <c r="E234" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>55</v>
       </c>
       <c r="B235" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -4807,15 +4804,15 @@
         <v>57</v>
       </c>
       <c r="E235" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>55</v>
       </c>
       <c r="B236" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -4824,49 +4821,49 @@
         <v>57</v>
       </c>
       <c r="E236" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>55</v>
+      </c>
+      <c r="B237" t="s">
+        <v>66</v>
+      </c>
+      <c r="C237" s="1">
+        <v>1</v>
+      </c>
+      <c r="D237" t="s">
+        <v>57</v>
+      </c>
+      <c r="E237" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
         <v>134</v>
-      </c>
-      <c r="B237" t="s">
-        <v>82</v>
-      </c>
-      <c r="C237" s="1">
-        <v>1</v>
-      </c>
-      <c r="D237" t="s">
-        <v>45</v>
-      </c>
-      <c r="E237" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>131</v>
       </c>
       <c r="B238" t="s">
         <v>82</v>
       </c>
       <c r="C238" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D238" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="E238" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>131</v>
       </c>
       <c r="B239" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C239" s="1">
         <v>2</v>
@@ -4875,32 +4872,32 @@
         <v>150</v>
       </c>
       <c r="E239" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>131</v>
       </c>
       <c r="B240" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C240" s="1">
         <v>2</v>
       </c>
       <c r="D240" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E240" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>131</v>
       </c>
       <c r="B241" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C241" s="1">
         <v>2</v>
@@ -4909,32 +4906,32 @@
         <v>148</v>
       </c>
       <c r="E241" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>131</v>
       </c>
       <c r="B242" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C242" s="1">
         <v>2</v>
       </c>
       <c r="D242" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E242" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>131</v>
       </c>
       <c r="B243" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C243" s="1">
         <v>2</v>
@@ -4943,32 +4940,32 @@
         <v>155</v>
       </c>
       <c r="E243" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>131</v>
       </c>
       <c r="B244" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C244" s="1">
         <v>2</v>
       </c>
       <c r="D244" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E244" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>131</v>
       </c>
       <c r="B245" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C245" s="1">
         <v>2</v>
@@ -4977,32 +4974,32 @@
         <v>152</v>
       </c>
       <c r="E245" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>131</v>
       </c>
       <c r="B246" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C246" s="1">
         <v>2</v>
       </c>
       <c r="D246" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E246" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>131</v>
       </c>
       <c r="B247" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C247" s="1">
         <v>2</v>
@@ -5011,32 +5008,32 @@
         <v>145</v>
       </c>
       <c r="E247" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>131</v>
+      </c>
+      <c r="B248" t="s">
+        <v>147</v>
+      </c>
+      <c r="C248" s="1">
+        <v>2</v>
+      </c>
+      <c r="D248" t="s">
+        <v>145</v>
+      </c>
+      <c r="E248" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>88</v>
-      </c>
-      <c r="B248" t="s">
-        <v>82</v>
-      </c>
-      <c r="C248" s="1">
-        <v>1</v>
-      </c>
-      <c r="D248" t="s">
-        <v>175</v>
-      </c>
-      <c r="E248" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>88</v>
       </c>
       <c r="B249" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C249" s="1">
         <v>1</v>
@@ -5045,24 +5042,27 @@
         <v>175</v>
       </c>
       <c r="E249" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>88</v>
+      </c>
+      <c r="B250" t="s">
+        <v>147</v>
+      </c>
+      <c r="C250" s="1">
+        <v>1</v>
+      </c>
+      <c r="D250" t="s">
+        <v>175</v>
+      </c>
+      <c r="E250" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>240</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D250" t="s">
-        <v>119</v>
-      </c>
-      <c r="E250" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>10</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>10</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>10</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>201</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>201</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>214</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>214</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>214</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>214</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>214</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>174</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>174</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>174</v>
       </c>

</xml_diff>

<commit_message>
[Outlook] Add MailboxEnums to enum names (#669)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25519"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573EEB92-EB70-4023-A64F-7D50B497C831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605E840B-88E4-453B-8FA2-3B255470EF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-90" windowWidth="38640" windowHeight="23520" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -726,31 +726,31 @@
     <t>outlook-tokens-and-service-calls-get-icaluid-as-attendee</t>
   </si>
   <si>
-    <t>AppointmentSensitivity</t>
-  </si>
-  <si>
     <t>enum</t>
   </si>
   <si>
-    <t>AttachmentContentFormat</t>
-  </si>
-  <si>
     <t>handleAttachmentsCallback</t>
   </si>
   <si>
-    <t>CategoryColor</t>
-  </si>
-  <si>
-    <t>DelegatePermissions</t>
-  </si>
-  <si>
-    <t>EntityType</t>
-  </si>
-  <si>
-    <t>LocationType</t>
-  </si>
-  <si>
-    <t>RestVersion</t>
+    <t>MailboxEnums.AppointmentSensitivity</t>
+  </si>
+  <si>
+    <t>MailboxEnums.AttachmentContentFormat</t>
+  </si>
+  <si>
+    <t>MailboxEnums.CategoryColor</t>
+  </si>
+  <si>
+    <t>MailboxEnums.DelegatePermissions</t>
+  </si>
+  <si>
+    <t>MailboxEnums.EntityType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.LocationType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.RestVersion</t>
   </si>
 </sst>
 </file>
@@ -1165,20 +1165,20 @@
   <dimension ref="A1:E263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="74.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>19</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>19</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>19</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>19</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>19</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>19</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>19</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -2599,201 +2599,213 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>232</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>233</v>
+        <v>139</v>
+      </c>
+      <c r="B95" t="s">
+        <v>140</v>
+      </c>
+      <c r="C95" s="1">
+        <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="E95" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>234</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>233</v>
+        <v>139</v>
+      </c>
+      <c r="B96" t="s">
+        <v>140</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E96" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="B97" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="C97" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="E97" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="B98" t="s">
-        <v>140</v>
+        <v>56</v>
       </c>
       <c r="C98" s="1">
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="E98" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>81</v>
       </c>
       <c r="B99" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C99" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D99" t="s">
         <v>161</v>
       </c>
       <c r="E99" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="B100" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="C100" s="1">
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="E100" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="B101" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="C101" s="1">
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="E101" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>236</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>233</v>
+        <v>14</v>
+      </c>
+      <c r="B102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>158</v>
+        <v>15</v>
       </c>
       <c r="E102" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>15</v>
+        <v>192</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="B104" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C104" s="1">
         <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>15</v>
+        <v>192</v>
       </c>
       <c r="E104" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C105" s="1">
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>15</v>
+        <v>192</v>
       </c>
       <c r="E105" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>237</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>233</v>
+        <v>133</v>
+      </c>
+      <c r="B106" t="s">
+        <v>82</v>
+      </c>
+      <c r="C106" s="1">
+        <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="E106" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="B107" t="s">
         <v>82</v>
@@ -2802,606 +2814,591 @@
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="B108" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C108" s="1">
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="E108" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="C109" s="1">
         <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="E109" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>238</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>233</v>
+        <v>197</v>
+      </c>
+      <c r="B110" t="s">
+        <v>82</v>
+      </c>
+      <c r="C110" s="1">
+        <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>109</v>
+        <v>195</v>
       </c>
       <c r="E110" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>133</v>
+        <v>197</v>
       </c>
       <c r="B111" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C111" s="1">
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
       <c r="E111" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="B112" t="s">
         <v>82</v>
       </c>
       <c r="C112" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D112" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="E112" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="B113" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="C113" s="1">
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="E113" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>227</v>
+        <v>83</v>
       </c>
       <c r="B114" t="s">
-        <v>147</v>
-      </c>
-      <c r="C114" s="1">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D114" t="s">
-        <v>225</v>
+        <v>158</v>
       </c>
       <c r="E114" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>197</v>
+        <v>83</v>
       </c>
       <c r="B115" t="s">
-        <v>82</v>
-      </c>
-      <c r="C115" s="1">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D115" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="E115" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>197</v>
+        <v>83</v>
       </c>
       <c r="B116" t="s">
-        <v>147</v>
-      </c>
-      <c r="C116" s="1">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D116" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="E116" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>190</v>
+        <v>83</v>
       </c>
       <c r="B117" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C117" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>189</v>
+        <v>94</v>
       </c>
       <c r="E117" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>190</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="E118" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>239</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>233</v>
+        <v>83</v>
+      </c>
+      <c r="B119" t="s">
+        <v>97</v>
+      </c>
+      <c r="C119" s="1">
+        <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>192</v>
+        <v>98</v>
       </c>
       <c r="E119" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>83</v>
       </c>
       <c r="B120" t="s">
-        <v>84</v>
+        <v>99</v>
+      </c>
+      <c r="C120" s="1">
+        <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="E120" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>83</v>
       </c>
       <c r="B121" t="s">
-        <v>84</v>
+        <v>205</v>
+      </c>
+      <c r="C121" s="1">
+        <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="E121" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>83</v>
       </c>
       <c r="B122" t="s">
-        <v>84</v>
+        <v>206</v>
+      </c>
+      <c r="C122" s="1">
+        <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>158</v>
+        <v>96</v>
       </c>
       <c r="E122" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>83</v>
       </c>
       <c r="B123" t="s">
-        <v>93</v>
+        <v>207</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E123" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>83</v>
       </c>
       <c r="B124" t="s">
-        <v>95</v>
+        <v>208</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E124" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>83</v>
       </c>
       <c r="B125" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="E125" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>83</v>
       </c>
       <c r="B126" t="s">
-        <v>99</v>
-      </c>
-      <c r="C126" s="1">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D126" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="E126" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>83</v>
       </c>
       <c r="B127" t="s">
-        <v>205</v>
+        <v>107</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="E127" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>83</v>
       </c>
       <c r="B128" t="s">
-        <v>206</v>
-      </c>
-      <c r="C128" s="1">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="D128" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="E128" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>207</v>
-      </c>
-      <c r="C129" s="1">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D129" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="E129" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>83</v>
       </c>
       <c r="B130" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="E130" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>83</v>
       </c>
       <c r="B131" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C131" s="1">
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E131" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>83</v>
       </c>
       <c r="B132" t="s">
-        <v>120</v>
+        <v>126</v>
+      </c>
+      <c r="C132" s="1">
+        <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>119</v>
+        <v>231</v>
       </c>
       <c r="E132" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>83</v>
       </c>
       <c r="B133" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="C133" s="1">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="E133" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>83</v>
       </c>
       <c r="B134" t="s">
-        <v>121</v>
+        <v>107</v>
+      </c>
+      <c r="C134" s="1">
+        <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E134" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>83</v>
       </c>
       <c r="B135" t="s">
-        <v>120</v>
+        <v>129</v>
+      </c>
+      <c r="C135" s="1">
+        <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="E135" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>83</v>
-      </c>
-      <c r="B136" t="s">
-        <v>118</v>
-      </c>
-      <c r="C136" s="1">
-        <v>1</v>
+        <v>234</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="D136" t="s">
-        <v>122</v>
+        <v>195</v>
       </c>
       <c r="E136" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>235</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D137" t="s">
+        <v>135</v>
+      </c>
+      <c r="E137" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>236</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D138" t="s">
+        <v>158</v>
+      </c>
+      <c r="E138" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>237</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D139" t="s">
+        <v>105</v>
+      </c>
+      <c r="E139" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>238</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D140" t="s">
+        <v>109</v>
+      </c>
+      <c r="E140" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>239</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D141" t="s">
+        <v>192</v>
+      </c>
+      <c r="E141" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>240</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D142" t="s">
+        <v>119</v>
+      </c>
+      <c r="E142" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>83</v>
-      </c>
-      <c r="B137" t="s">
-        <v>123</v>
-      </c>
-      <c r="C137" s="1">
-        <v>1</v>
-      </c>
-      <c r="D137" t="s">
-        <v>122</v>
-      </c>
-      <c r="E137" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>83</v>
-      </c>
-      <c r="B138" t="s">
-        <v>126</v>
-      </c>
-      <c r="C138" s="1">
-        <v>1</v>
-      </c>
-      <c r="D138" t="s">
-        <v>231</v>
-      </c>
-      <c r="E138" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>83</v>
-      </c>
-      <c r="B139" t="s">
-        <v>126</v>
-      </c>
-      <c r="C139" s="1">
-        <v>1</v>
-      </c>
-      <c r="D139" t="s">
-        <v>127</v>
-      </c>
-      <c r="E139" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>83</v>
-      </c>
-      <c r="B140" t="s">
-        <v>107</v>
-      </c>
-      <c r="C140" s="1">
-        <v>2</v>
-      </c>
-      <c r="D140" t="s">
-        <v>128</v>
-      </c>
-      <c r="E140" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>83</v>
-      </c>
-      <c r="B141" t="s">
-        <v>129</v>
-      </c>
-      <c r="C141" s="1">
-        <v>1</v>
-      </c>
-      <c r="D141" t="s">
-        <v>130</v>
-      </c>
-      <c r="E141" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>86</v>
-      </c>
-      <c r="B142" t="s">
-        <v>82</v>
-      </c>
-      <c r="C142" s="1">
-        <v>2</v>
-      </c>
-      <c r="D142" t="s">
-        <v>158</v>
-      </c>
-      <c r="E142" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>86</v>
       </c>
       <c r="B143" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C143" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D143" t="s">
         <v>158</v>
       </c>
       <c r="E143" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>86</v>
       </c>
       <c r="B144" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C144" s="1">
         <v>1</v>
@@ -3410,92 +3407,95 @@
         <v>158</v>
       </c>
       <c r="E144" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" t="s">
+        <v>66</v>
+      </c>
+      <c r="C145" s="1">
+        <v>1</v>
+      </c>
+      <c r="D145" t="s">
+        <v>158</v>
+      </c>
+      <c r="E145" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>20</v>
-      </c>
-      <c r="B145" t="s">
-        <v>18</v>
-      </c>
-      <c r="C145" s="1">
-        <v>1</v>
-      </c>
-      <c r="D145" t="s">
-        <v>15</v>
-      </c>
-      <c r="E145" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>20</v>
       </c>
       <c r="B146" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C146" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E146" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>20</v>
       </c>
       <c r="B147" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C147" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D147" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E147" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>20</v>
       </c>
       <c r="B148" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C148" s="1">
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E148" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>20</v>
       </c>
       <c r="B149" t="s">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="C149" s="1">
+        <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>150</v>
+        <v>28</v>
       </c>
       <c r="E149" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>20</v>
       </c>
@@ -3506,24 +3506,24 @@
         <v>150</v>
       </c>
       <c r="E150" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>20</v>
       </c>
       <c r="B151" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D151" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E151" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>20</v>
       </c>
@@ -3534,38 +3534,38 @@
         <v>148</v>
       </c>
       <c r="E152" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>20</v>
       </c>
       <c r="B153" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D153" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="E153" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>20</v>
       </c>
       <c r="B154" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D154" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="E154" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>20</v>
       </c>
@@ -3576,24 +3576,24 @@
         <v>145</v>
       </c>
       <c r="E155" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D156" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="E156" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>20</v>
       </c>
@@ -3604,10 +3604,10 @@
         <v>57</v>
       </c>
       <c r="E157" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>20</v>
       </c>
@@ -3618,10 +3618,10 @@
         <v>57</v>
       </c>
       <c r="E158" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>20</v>
       </c>
@@ -3632,10 +3632,10 @@
         <v>57</v>
       </c>
       <c r="E159" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>20</v>
       </c>
@@ -3646,10 +3646,10 @@
         <v>57</v>
       </c>
       <c r="E160" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>20</v>
       </c>
@@ -3660,32 +3660,29 @@
         <v>57</v>
       </c>
       <c r="E161" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>20</v>
       </c>
       <c r="B162" t="s">
-        <v>67</v>
-      </c>
-      <c r="C162" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D162" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E162" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>20</v>
       </c>
       <c r="B163" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C163" s="1">
         <v>1</v>
@@ -3694,15 +3691,15 @@
         <v>68</v>
       </c>
       <c r="E163" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>20</v>
       </c>
       <c r="B164" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -3711,10 +3708,10 @@
         <v>68</v>
       </c>
       <c r="E164" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>20</v>
       </c>
@@ -3725,35 +3722,35 @@
         <v>1</v>
       </c>
       <c r="D165" t="s">
-        <v>137</v>
+        <v>68</v>
       </c>
       <c r="E165" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>20</v>
       </c>
       <c r="B166" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C166" s="1">
         <v>1</v>
       </c>
       <c r="D166" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="E166" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>20</v>
       </c>
       <c r="B167" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
@@ -3762,41 +3759,44 @@
         <v>68</v>
       </c>
       <c r="E167" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>20</v>
       </c>
       <c r="B168" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C168" s="1">
         <v>1</v>
       </c>
       <c r="D168" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="E168" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>20</v>
       </c>
       <c r="B169" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="C169" s="1">
+        <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="E169" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>20</v>
       </c>
@@ -3807,10 +3807,10 @@
         <v>161</v>
       </c>
       <c r="E170" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>20</v>
       </c>
@@ -3821,41 +3821,38 @@
         <v>161</v>
       </c>
       <c r="E171" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>20</v>
       </c>
       <c r="B172" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D172" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="E172" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>20</v>
       </c>
       <c r="B173" t="s">
-        <v>106</v>
-      </c>
-      <c r="C173" s="1">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="D173" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E173" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>20</v>
       </c>
@@ -3863,72 +3860,72 @@
         <v>106</v>
       </c>
       <c r="C174" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D174" t="s">
         <v>105</v>
       </c>
       <c r="E174" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>20</v>
       </c>
       <c r="B175" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C175" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D175" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="E175" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>20</v>
       </c>
       <c r="B176" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C176" s="1">
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E176" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>20</v>
       </c>
       <c r="B177" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C177" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D177" t="s">
         <v>137</v>
       </c>
       <c r="E177" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>20</v>
       </c>
       <c r="B178" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C178" s="1">
         <v>1</v>
@@ -3937,24 +3934,27 @@
         <v>137</v>
       </c>
       <c r="E178" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>20</v>
       </c>
       <c r="B179" t="s">
-        <v>162</v>
+        <v>136</v>
+      </c>
+      <c r="C179" s="1">
+        <v>1</v>
       </c>
       <c r="D179" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="E179" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>20</v>
       </c>
@@ -3965,153 +3965,153 @@
         <v>164</v>
       </c>
       <c r="E180" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>20</v>
       </c>
       <c r="B181" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D181" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E181" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>20</v>
       </c>
       <c r="B182" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D182" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E182" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>20</v>
       </c>
       <c r="B183" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="D183" t="s">
-        <v>230</v>
+        <v>179</v>
       </c>
       <c r="E183" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>20</v>
       </c>
       <c r="B184" t="s">
+        <v>212</v>
+      </c>
+      <c r="D184" t="s">
+        <v>230</v>
+      </c>
+      <c r="E184" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>20</v>
+      </c>
+      <c r="B185" t="s">
         <v>224</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D185" t="s">
         <v>225</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E185" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>21</v>
-      </c>
-      <c r="B185" t="s">
-        <v>18</v>
-      </c>
-      <c r="C185" s="1">
-        <v>1</v>
-      </c>
-      <c r="D185" t="s">
-        <v>15</v>
-      </c>
-      <c r="E185" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>21</v>
       </c>
       <c r="B186" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="C186" s="1">
+        <v>1</v>
       </c>
       <c r="D186" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E186" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>21</v>
       </c>
       <c r="B187" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D187" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E187" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>21</v>
       </c>
       <c r="B188" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D188" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E188" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>21</v>
       </c>
       <c r="B189" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D189" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E189" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>21</v>
       </c>
       <c r="B190" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D190" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E190" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>21</v>
       </c>
@@ -4122,10 +4122,10 @@
         <v>57</v>
       </c>
       <c r="E191" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>21</v>
       </c>
@@ -4136,10 +4136,10 @@
         <v>57</v>
       </c>
       <c r="E192" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>21</v>
       </c>
@@ -4150,10 +4150,10 @@
         <v>57</v>
       </c>
       <c r="E193" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>21</v>
       </c>
@@ -4164,10 +4164,10 @@
         <v>57</v>
       </c>
       <c r="E194" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>21</v>
       </c>
@@ -4178,55 +4178,55 @@
         <v>57</v>
       </c>
       <c r="E195" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>21</v>
       </c>
       <c r="B196" t="s">
-        <v>76</v>
-      </c>
-      <c r="C196" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D196" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="E196" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>21</v>
       </c>
       <c r="B197" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C197" s="1">
+        <v>1</v>
       </c>
       <c r="D197" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="E197" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>21</v>
       </c>
       <c r="B198" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D198" t="s">
-        <v>161</v>
+        <v>78</v>
       </c>
       <c r="E198" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>21</v>
       </c>
@@ -4237,10 +4237,10 @@
         <v>161</v>
       </c>
       <c r="E199" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>21</v>
       </c>
@@ -4251,60 +4251,57 @@
         <v>161</v>
       </c>
       <c r="E200" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>21</v>
       </c>
       <c r="B201" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D201" t="s">
-        <v>89</v>
+        <v>161</v>
       </c>
       <c r="E201" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>21</v>
       </c>
       <c r="B202" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D202" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E202" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>21</v>
       </c>
       <c r="B203" t="s">
-        <v>101</v>
-      </c>
-      <c r="C203" s="1">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D203" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E203" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>21</v>
       </c>
       <c r="B204" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C204" s="1">
         <v>1</v>
@@ -4313,49 +4310,49 @@
         <v>103</v>
       </c>
       <c r="E204" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>21</v>
       </c>
       <c r="B205" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C205" s="1">
         <v>1</v>
       </c>
       <c r="D205" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E205" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>21</v>
       </c>
       <c r="B206" t="s">
-        <v>209</v>
+        <v>101</v>
       </c>
       <c r="C206" s="1">
         <v>1</v>
       </c>
       <c r="D206" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E206" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>21</v>
       </c>
       <c r="B207" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C207" s="1">
         <v>1</v>
@@ -4364,44 +4361,44 @@
         <v>103</v>
       </c>
       <c r="E207" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>21</v>
       </c>
       <c r="B208" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C208" s="1">
         <v>1</v>
       </c>
       <c r="D208" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E208" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>21</v>
       </c>
       <c r="B209" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="C209" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D209" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E209" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>21</v>
       </c>
@@ -4409,38 +4406,38 @@
         <v>106</v>
       </c>
       <c r="C210" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D210" t="s">
         <v>105</v>
       </c>
       <c r="E210" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>21</v>
       </c>
       <c r="B211" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
       </c>
       <c r="D211" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E211" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>21</v>
       </c>
       <c r="B212" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -4449,32 +4446,32 @@
         <v>109</v>
       </c>
       <c r="E212" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>21</v>
       </c>
       <c r="B213" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
       </c>
       <c r="D213" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E213" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>21</v>
       </c>
       <c r="B214" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
@@ -4483,15 +4480,15 @@
         <v>112</v>
       </c>
       <c r="E214" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>21</v>
       </c>
       <c r="B215" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
@@ -4500,32 +4497,32 @@
         <v>112</v>
       </c>
       <c r="E215" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>21</v>
       </c>
       <c r="B216" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
       </c>
       <c r="D216" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E216" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>21</v>
       </c>
       <c r="B217" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C217" s="1">
         <v>1</v>
@@ -4534,198 +4531,198 @@
         <v>116</v>
       </c>
       <c r="E217" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>21</v>
       </c>
       <c r="B218" t="s">
-        <v>162</v>
+        <v>117</v>
+      </c>
+      <c r="C218" s="1">
+        <v>1</v>
       </c>
       <c r="D218" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="E218" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>21</v>
       </c>
       <c r="B219" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D219" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E219" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>21</v>
       </c>
       <c r="B220" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D220" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E220" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>21</v>
       </c>
       <c r="B221" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D221" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E221" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>21</v>
       </c>
       <c r="B222" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D222" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E222" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>21</v>
       </c>
       <c r="B223" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D223" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E223" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>21</v>
       </c>
       <c r="B224" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D224" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E224" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>21</v>
       </c>
       <c r="B225" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D225" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E225" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>21</v>
       </c>
       <c r="B226" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D226" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E226" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>21</v>
       </c>
       <c r="B227" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D227" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E227" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>21</v>
       </c>
       <c r="B228" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D228" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E228" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>21</v>
       </c>
       <c r="B229" t="s">
+        <v>187</v>
+      </c>
+      <c r="D229" t="s">
+        <v>188</v>
+      </c>
+      <c r="E229" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>21</v>
+      </c>
+      <c r="B230" t="s">
         <v>222</v>
       </c>
-      <c r="C229" s="1">
-        <v>1</v>
-      </c>
-      <c r="D229" t="s">
+      <c r="C230" s="1">
+        <v>1</v>
+      </c>
+      <c r="D230" t="s">
         <v>223</v>
       </c>
-      <c r="E229" t="s">
+      <c r="E230" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>55</v>
-      </c>
-      <c r="B230" t="s">
-        <v>56</v>
-      </c>
-      <c r="C230" s="1">
-        <v>1</v>
-      </c>
-      <c r="D230" t="s">
-        <v>57</v>
-      </c>
-      <c r="E230" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>55</v>
       </c>
@@ -4739,10 +4736,10 @@
         <v>57</v>
       </c>
       <c r="E231" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>55</v>
       </c>
@@ -4756,10 +4753,10 @@
         <v>57</v>
       </c>
       <c r="E232" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>55</v>
       </c>
@@ -4773,15 +4770,15 @@
         <v>57</v>
       </c>
       <c r="E233" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>55</v>
       </c>
       <c r="B234" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C234" s="1">
         <v>1</v>
@@ -4790,15 +4787,15 @@
         <v>57</v>
       </c>
       <c r="E234" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>55</v>
       </c>
       <c r="B235" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -4807,15 +4804,15 @@
         <v>57</v>
       </c>
       <c r="E235" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>55</v>
       </c>
       <c r="B236" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -4824,49 +4821,49 @@
         <v>57</v>
       </c>
       <c r="E236" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>55</v>
+      </c>
+      <c r="B237" t="s">
+        <v>66</v>
+      </c>
+      <c r="C237" s="1">
+        <v>1</v>
+      </c>
+      <c r="D237" t="s">
+        <v>57</v>
+      </c>
+      <c r="E237" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
         <v>134</v>
-      </c>
-      <c r="B237" t="s">
-        <v>82</v>
-      </c>
-      <c r="C237" s="1">
-        <v>1</v>
-      </c>
-      <c r="D237" t="s">
-        <v>45</v>
-      </c>
-      <c r="E237" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>131</v>
       </c>
       <c r="B238" t="s">
         <v>82</v>
       </c>
       <c r="C238" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D238" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="E238" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>131</v>
       </c>
       <c r="B239" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C239" s="1">
         <v>2</v>
@@ -4875,32 +4872,32 @@
         <v>150</v>
       </c>
       <c r="E239" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>131</v>
       </c>
       <c r="B240" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C240" s="1">
         <v>2</v>
       </c>
       <c r="D240" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E240" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>131</v>
       </c>
       <c r="B241" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C241" s="1">
         <v>2</v>
@@ -4909,32 +4906,32 @@
         <v>148</v>
       </c>
       <c r="E241" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>131</v>
       </c>
       <c r="B242" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C242" s="1">
         <v>2</v>
       </c>
       <c r="D242" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E242" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>131</v>
       </c>
       <c r="B243" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C243" s="1">
         <v>2</v>
@@ -4943,32 +4940,32 @@
         <v>155</v>
       </c>
       <c r="E243" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>131</v>
       </c>
       <c r="B244" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C244" s="1">
         <v>2</v>
       </c>
       <c r="D244" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E244" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>131</v>
       </c>
       <c r="B245" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C245" s="1">
         <v>2</v>
@@ -4977,32 +4974,32 @@
         <v>152</v>
       </c>
       <c r="E245" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>131</v>
       </c>
       <c r="B246" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C246" s="1">
         <v>2</v>
       </c>
       <c r="D246" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E246" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>131</v>
       </c>
       <c r="B247" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C247" s="1">
         <v>2</v>
@@ -5011,32 +5008,32 @@
         <v>145</v>
       </c>
       <c r="E247" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>131</v>
+      </c>
+      <c r="B248" t="s">
+        <v>147</v>
+      </c>
+      <c r="C248" s="1">
+        <v>2</v>
+      </c>
+      <c r="D248" t="s">
+        <v>145</v>
+      </c>
+      <c r="E248" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>88</v>
-      </c>
-      <c r="B248" t="s">
-        <v>82</v>
-      </c>
-      <c r="C248" s="1">
-        <v>1</v>
-      </c>
-      <c r="D248" t="s">
-        <v>175</v>
-      </c>
-      <c r="E248" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>88</v>
       </c>
       <c r="B249" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C249" s="1">
         <v>1</v>
@@ -5045,24 +5042,27 @@
         <v>175</v>
       </c>
       <c r="E249" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>88</v>
+      </c>
+      <c r="B250" t="s">
+        <v>147</v>
+      </c>
+      <c r="C250" s="1">
+        <v>1</v>
+      </c>
+      <c r="D250" t="s">
+        <v>175</v>
+      </c>
+      <c r="E250" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>240</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D250" t="s">
-        <v>119</v>
-      </c>
-      <c r="E250" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>10</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>10</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>10</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>201</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>201</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>214</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>214</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>214</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>214</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>214</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>174</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>174</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>174</v>
       </c>

</xml_diff>

<commit_message>
[Outlook] Fix name to AppointmentSensitivityType
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25519"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25523"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605E840B-88E4-453B-8FA2-3B255470EF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65695B3E-71C4-45F0-9459-45EEA54EDADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -732,9 +732,6 @@
     <t>handleAttachmentsCallback</t>
   </si>
   <si>
-    <t>MailboxEnums.AppointmentSensitivity</t>
-  </si>
-  <si>
     <t>MailboxEnums.AttachmentContentFormat</t>
   </si>
   <si>
@@ -751,6 +748,9 @@
   </si>
   <si>
     <t>MailboxEnums.RestVersion</t>
+  </si>
+  <si>
+    <t>MailboxEnums.AppointmentSensitivityType</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1166,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A136" sqref="A136"/>
+      <selection pane="bottomLeft" activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>232</v>
@@ -3294,7 +3294,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>232</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>232</v>
@@ -3322,7 +3322,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>232</v>
@@ -3336,7 +3336,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>232</v>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>232</v>
@@ -3364,7 +3364,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
[Outlook] Fix name to AppointmentSensitivityType (#673)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25519"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25523"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605E840B-88E4-453B-8FA2-3B255470EF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65695B3E-71C4-45F0-9459-45EEA54EDADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -732,9 +732,6 @@
     <t>handleAttachmentsCallback</t>
   </si>
   <si>
-    <t>MailboxEnums.AppointmentSensitivity</t>
-  </si>
-  <si>
     <t>MailboxEnums.AttachmentContentFormat</t>
   </si>
   <si>
@@ -751,6 +748,9 @@
   </si>
   <si>
     <t>MailboxEnums.RestVersion</t>
+  </si>
+  <si>
+    <t>MailboxEnums.AppointmentSensitivityType</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1166,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A136" sqref="A136"/>
+      <selection pane="bottomLeft" activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>232</v>
@@ -3294,7 +3294,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>232</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>232</v>
@@ -3322,7 +3322,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>232</v>
@@ -3336,7 +3336,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>232</v>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>232</v>
@@ -3364,7 +3364,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
Add snippet for MailboxEnums.ComposeType and clarify getComposeType function
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25604"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65695B3E-71C4-45F0-9459-45EEA54EDADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C3332B-9EBC-4E83-806C-8533EA8BD98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="38280" yWindow="-90" windowWidth="38640" windowHeight="23520" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="242">
   <si>
     <t>Class</t>
   </si>
@@ -751,6 +751,9 @@
   </si>
   <si>
     <t>MailboxEnums.AppointmentSensitivityType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.ComposeType</t>
   </si>
 </sst>
 </file>
@@ -786,9 +789,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -829,10 +836,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E263" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E263" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E263">
-    <sortCondition ref="A1:A263"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E264" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E264" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E264">
+    <sortCondition ref="A1:A264"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="4"/>
@@ -1162,23 +1169,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E263"/>
+  <dimension ref="A1:E264"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A137" sqref="A137"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="74.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1236,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1246,7 +1253,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1280,7 +1287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1294,7 +1301,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1308,7 +1315,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1322,7 +1329,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1336,7 +1343,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1364,7 +1371,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1378,7 +1385,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1399,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1406,7 +1413,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1427,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1434,7 +1441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1451,7 +1458,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1468,7 +1475,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1485,7 +1492,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1502,7 +1509,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1519,7 +1526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1536,7 +1543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1553,7 +1560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1567,7 +1574,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1581,7 +1588,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1595,7 +1602,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1609,7 +1616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1623,7 +1630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1637,7 +1644,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1654,7 +1661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1671,7 +1678,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1688,7 +1695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1705,7 +1712,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1722,7 +1729,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1736,7 +1743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1750,7 +1757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1764,7 +1771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -1778,7 +1785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1792,7 +1799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +1813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1820,7 +1827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1834,7 +1841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1848,7 +1855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1862,7 +1869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1876,7 +1883,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1890,7 +1897,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1904,7 +1911,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1918,7 +1925,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1932,7 +1939,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -1946,7 +1953,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -1960,7 +1967,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -1977,7 +1984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1991,7 +1998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -2005,7 +2012,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -2019,7 +2026,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -2033,7 +2040,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -2047,7 +2054,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -2061,7 +2068,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -2075,7 +2082,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2089,7 +2096,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -2103,7 +2110,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -2120,7 +2127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -2134,7 +2141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -2148,7 +2155,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -2162,7 +2169,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -2176,7 +2183,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -2190,7 +2197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -2204,7 +2211,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -2221,7 +2228,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -2238,7 +2245,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -2255,7 +2262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -2272,7 +2279,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -2289,7 +2296,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -2306,7 +2313,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -2323,7 +2330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
@@ -2340,7 +2347,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -2357,7 +2364,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -2374,7 +2381,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2391,7 +2398,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>19</v>
       </c>
@@ -2408,7 +2415,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>19</v>
       </c>
@@ -2425,7 +2432,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -2442,7 +2449,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -2459,7 +2466,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -2473,7 +2480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>19</v>
       </c>
@@ -2487,7 +2494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -2501,7 +2508,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>19</v>
       </c>
@@ -2515,7 +2522,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -2529,7 +2536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -2543,7 +2550,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>19</v>
       </c>
@@ -2557,7 +2564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>19</v>
       </c>
@@ -2571,7 +2578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2585,7 +2592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -2599,7 +2606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>139</v>
       </c>
@@ -2616,7 +2623,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>139</v>
       </c>
@@ -2633,7 +2640,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>81</v>
       </c>
@@ -2650,7 +2657,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>81</v>
       </c>
@@ -2667,7 +2674,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>81</v>
       </c>
@@ -2684,7 +2691,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -2701,7 +2708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -2718,7 +2725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>14</v>
       </c>
@@ -2735,7 +2742,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>193</v>
       </c>
@@ -2752,7 +2759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -2769,7 +2776,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>193</v>
       </c>
@@ -2786,7 +2793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>133</v>
       </c>
@@ -2803,7 +2810,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>227</v>
       </c>
@@ -2820,7 +2827,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>227</v>
       </c>
@@ -2837,7 +2844,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>227</v>
       </c>
@@ -2854,7 +2861,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>197</v>
       </c>
@@ -2871,7 +2878,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>197</v>
       </c>
@@ -2888,7 +2895,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>190</v>
       </c>
@@ -2905,7 +2912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>190</v>
       </c>
@@ -2922,7 +2929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>83</v>
       </c>
@@ -2936,7 +2943,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>83</v>
       </c>
@@ -2950,7 +2957,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>83</v>
       </c>
@@ -2964,7 +2971,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>83</v>
       </c>
@@ -2981,7 +2988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>83</v>
       </c>
@@ -2998,7 +3005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>83</v>
       </c>
@@ -3015,7 +3022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>83</v>
       </c>
@@ -3032,7 +3039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>83</v>
       </c>
@@ -3049,7 +3056,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>83</v>
       </c>
@@ -3066,7 +3073,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>83</v>
       </c>
@@ -3083,7 +3090,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>83</v>
       </c>
@@ -3100,7 +3107,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>83</v>
       </c>
@@ -3117,7 +3124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>83</v>
       </c>
@@ -3131,7 +3138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>83</v>
       </c>
@@ -3148,7 +3155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>83</v>
       </c>
@@ -3162,7 +3169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>83</v>
       </c>
@@ -3176,7 +3183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>83</v>
       </c>
@@ -3193,7 +3200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>83</v>
       </c>
@@ -3210,7 +3217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>83</v>
       </c>
@@ -3227,7 +3234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>83</v>
       </c>
@@ -3244,7 +3251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>83</v>
       </c>
@@ -3261,7 +3268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>83</v>
       </c>
@@ -3278,7 +3285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>240</v>
       </c>
@@ -3292,7 +3299,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>234</v>
       </c>
@@ -3306,7 +3313,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>235</v>
       </c>
@@ -3320,102 +3327,100 @@
         <v>156</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B139" s="2"/>
+      <c r="C139" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>236</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D139" t="s">
-        <v>105</v>
-      </c>
-      <c r="E139" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>237</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D140" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E140" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D141" t="s">
-        <v>192</v>
+        <v>109</v>
       </c>
       <c r="E141" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D142" t="s">
+        <v>192</v>
+      </c>
+      <c r="E142" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>239</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D143" t="s">
         <v>119</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E143" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>86</v>
-      </c>
-      <c r="B143" t="s">
-        <v>82</v>
-      </c>
-      <c r="C143" s="1">
-        <v>2</v>
-      </c>
-      <c r="D143" t="s">
-        <v>158</v>
-      </c>
-      <c r="E143" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>86</v>
       </c>
       <c r="B144" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C144" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D144" t="s">
         <v>158</v>
       </c>
       <c r="E144" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>86</v>
       </c>
       <c r="B145" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C145" s="1">
         <v>1</v>
@@ -3424,92 +3429,95 @@
         <v>158</v>
       </c>
       <c r="E145" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>86</v>
+      </c>
+      <c r="B146" t="s">
+        <v>66</v>
+      </c>
+      <c r="C146" s="1">
+        <v>1</v>
+      </c>
+      <c r="D146" t="s">
+        <v>158</v>
+      </c>
+      <c r="E146" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>20</v>
-      </c>
-      <c r="B146" t="s">
-        <v>18</v>
-      </c>
-      <c r="C146" s="1">
-        <v>1</v>
-      </c>
-      <c r="D146" t="s">
-        <v>15</v>
-      </c>
-      <c r="E146" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>20</v>
       </c>
       <c r="B147" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C147" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E147" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>20</v>
       </c>
       <c r="B148" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C148" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D148" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E148" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>20</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C149" s="1">
         <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E149" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>20</v>
       </c>
       <c r="B150" t="s">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="C150" s="1">
+        <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>150</v>
+        <v>28</v>
       </c>
       <c r="E150" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>20</v>
       </c>
@@ -3520,24 +3528,24 @@
         <v>150</v>
       </c>
       <c r="E151" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D152" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E152" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>20</v>
       </c>
@@ -3548,38 +3556,38 @@
         <v>148</v>
       </c>
       <c r="E153" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>20</v>
       </c>
       <c r="B154" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D154" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="E154" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>20</v>
       </c>
       <c r="B155" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D155" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="E155" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>20</v>
       </c>
@@ -3590,24 +3598,24 @@
         <v>145</v>
       </c>
       <c r="E156" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>20</v>
       </c>
       <c r="B157" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D157" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="E157" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>20</v>
       </c>
@@ -3618,10 +3626,10 @@
         <v>57</v>
       </c>
       <c r="E158" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>20</v>
       </c>
@@ -3632,10 +3640,10 @@
         <v>57</v>
       </c>
       <c r="E159" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>20</v>
       </c>
@@ -3646,10 +3654,10 @@
         <v>57</v>
       </c>
       <c r="E160" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>20</v>
       </c>
@@ -3660,10 +3668,10 @@
         <v>57</v>
       </c>
       <c r="E161" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>20</v>
       </c>
@@ -3674,32 +3682,29 @@
         <v>57</v>
       </c>
       <c r="E162" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>20</v>
       </c>
       <c r="B163" t="s">
-        <v>67</v>
-      </c>
-      <c r="C163" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D163" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E163" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>20</v>
       </c>
       <c r="B164" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -3708,15 +3713,15 @@
         <v>68</v>
       </c>
       <c r="E164" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>20</v>
       </c>
       <c r="B165" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C165" s="1">
         <v>1</v>
@@ -3725,10 +3730,10 @@
         <v>68</v>
       </c>
       <c r="E165" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>20</v>
       </c>
@@ -3739,35 +3744,35 @@
         <v>1</v>
       </c>
       <c r="D166" t="s">
-        <v>137</v>
+        <v>68</v>
       </c>
       <c r="E166" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>20</v>
       </c>
       <c r="B167" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
       </c>
       <c r="D167" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="E167" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>20</v>
       </c>
       <c r="B168" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C168" s="1">
         <v>1</v>
@@ -3776,41 +3781,44 @@
         <v>68</v>
       </c>
       <c r="E168" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>20</v>
       </c>
       <c r="B169" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C169" s="1">
         <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="E169" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>20</v>
       </c>
       <c r="B170" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="C170" s="1">
+        <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="E170" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>20</v>
       </c>
@@ -3821,10 +3829,10 @@
         <v>161</v>
       </c>
       <c r="E171" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>20</v>
       </c>
@@ -3835,41 +3843,38 @@
         <v>161</v>
       </c>
       <c r="E172" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>20</v>
       </c>
       <c r="B173" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D173" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="E173" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>20</v>
       </c>
       <c r="B174" t="s">
-        <v>106</v>
-      </c>
-      <c r="C174" s="1">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="D174" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E174" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>20</v>
       </c>
@@ -3877,72 +3882,72 @@
         <v>106</v>
       </c>
       <c r="C175" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D175" t="s">
         <v>105</v>
       </c>
       <c r="E175" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>20</v>
       </c>
       <c r="B176" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C176" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D176" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="E176" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>20</v>
       </c>
       <c r="B177" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C177" s="1">
         <v>2</v>
       </c>
       <c r="D177" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E177" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>20</v>
       </c>
       <c r="B178" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C178" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D178" t="s">
         <v>137</v>
       </c>
       <c r="E178" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>20</v>
       </c>
       <c r="B179" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C179" s="1">
         <v>1</v>
@@ -3951,24 +3956,27 @@
         <v>137</v>
       </c>
       <c r="E179" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>20</v>
       </c>
       <c r="B180" t="s">
-        <v>162</v>
+        <v>136</v>
+      </c>
+      <c r="C180" s="1">
+        <v>1</v>
       </c>
       <c r="D180" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="E180" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>20</v>
       </c>
@@ -3979,153 +3987,153 @@
         <v>164</v>
       </c>
       <c r="E181" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>20</v>
       </c>
       <c r="B182" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D182" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E182" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>20</v>
       </c>
       <c r="B183" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D183" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E183" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>20</v>
       </c>
       <c r="B184" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="D184" t="s">
-        <v>230</v>
+        <v>179</v>
       </c>
       <c r="E184" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>20</v>
       </c>
       <c r="B185" t="s">
+        <v>212</v>
+      </c>
+      <c r="D185" t="s">
+        <v>230</v>
+      </c>
+      <c r="E185" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>20</v>
+      </c>
+      <c r="B186" t="s">
         <v>224</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D186" t="s">
         <v>225</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E186" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
-        <v>21</v>
-      </c>
-      <c r="B186" t="s">
-        <v>18</v>
-      </c>
-      <c r="C186" s="1">
-        <v>1</v>
-      </c>
-      <c r="D186" t="s">
-        <v>15</v>
-      </c>
-      <c r="E186" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>21</v>
       </c>
       <c r="B187" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="C187" s="1">
+        <v>1</v>
       </c>
       <c r="D187" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E187" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>21</v>
       </c>
       <c r="B188" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D188" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E188" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>21</v>
       </c>
       <c r="B189" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D189" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E189" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>21</v>
       </c>
       <c r="B190" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D190" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E190" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>21</v>
       </c>
       <c r="B191" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D191" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E191" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>21</v>
       </c>
@@ -4136,10 +4144,10 @@
         <v>57</v>
       </c>
       <c r="E192" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>21</v>
       </c>
@@ -4150,10 +4158,10 @@
         <v>57</v>
       </c>
       <c r="E193" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>21</v>
       </c>
@@ -4164,10 +4172,10 @@
         <v>57</v>
       </c>
       <c r="E194" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>21</v>
       </c>
@@ -4178,10 +4186,10 @@
         <v>57</v>
       </c>
       <c r="E195" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>21</v>
       </c>
@@ -4192,55 +4200,55 @@
         <v>57</v>
       </c>
       <c r="E196" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>21</v>
       </c>
       <c r="B197" t="s">
-        <v>76</v>
-      </c>
-      <c r="C197" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D197" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="E197" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>21</v>
       </c>
       <c r="B198" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C198" s="1">
+        <v>1</v>
       </c>
       <c r="D198" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="E198" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>21</v>
       </c>
       <c r="B199" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D199" t="s">
-        <v>161</v>
+        <v>78</v>
       </c>
       <c r="E199" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>21</v>
       </c>
@@ -4251,10 +4259,10 @@
         <v>161</v>
       </c>
       <c r="E200" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>21</v>
       </c>
@@ -4265,60 +4273,57 @@
         <v>161</v>
       </c>
       <c r="E201" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>21</v>
       </c>
       <c r="B202" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D202" t="s">
-        <v>89</v>
+        <v>161</v>
       </c>
       <c r="E202" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>21</v>
       </c>
       <c r="B203" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D203" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E203" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>21</v>
       </c>
       <c r="B204" t="s">
-        <v>101</v>
-      </c>
-      <c r="C204" s="1">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D204" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E204" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>21</v>
       </c>
       <c r="B205" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C205" s="1">
         <v>1</v>
@@ -4327,49 +4332,49 @@
         <v>103</v>
       </c>
       <c r="E205" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>21</v>
       </c>
       <c r="B206" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C206" s="1">
         <v>1</v>
       </c>
       <c r="D206" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E206" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>21</v>
       </c>
       <c r="B207" t="s">
-        <v>209</v>
+        <v>101</v>
       </c>
       <c r="C207" s="1">
         <v>1</v>
       </c>
       <c r="D207" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E207" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>21</v>
       </c>
       <c r="B208" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C208" s="1">
         <v>1</v>
@@ -4378,44 +4383,44 @@
         <v>103</v>
       </c>
       <c r="E208" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>21</v>
       </c>
       <c r="B209" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C209" s="1">
         <v>1</v>
       </c>
       <c r="D209" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E209" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>21</v>
       </c>
       <c r="B210" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="C210" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D210" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E210" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>21</v>
       </c>
@@ -4423,38 +4428,38 @@
         <v>106</v>
       </c>
       <c r="C211" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D211" t="s">
         <v>105</v>
       </c>
       <c r="E211" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>21</v>
       </c>
       <c r="B212" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
       </c>
       <c r="D212" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E212" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>21</v>
       </c>
       <c r="B213" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -4463,32 +4468,32 @@
         <v>109</v>
       </c>
       <c r="E213" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>21</v>
       </c>
       <c r="B214" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
       </c>
       <c r="D214" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E214" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>21</v>
       </c>
       <c r="B215" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
@@ -4497,15 +4502,15 @@
         <v>112</v>
       </c>
       <c r="E215" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>21</v>
       </c>
       <c r="B216" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
@@ -4514,32 +4519,32 @@
         <v>112</v>
       </c>
       <c r="E216" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>21</v>
       </c>
       <c r="B217" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C217" s="1">
         <v>1</v>
       </c>
       <c r="D217" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E217" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>21</v>
       </c>
       <c r="B218" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C218" s="1">
         <v>1</v>
@@ -4548,198 +4553,198 @@
         <v>116</v>
       </c>
       <c r="E218" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>21</v>
       </c>
       <c r="B219" t="s">
-        <v>162</v>
+        <v>117</v>
+      </c>
+      <c r="C219" s="1">
+        <v>1</v>
       </c>
       <c r="D219" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="E219" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>21</v>
       </c>
       <c r="B220" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D220" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E220" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>21</v>
       </c>
       <c r="B221" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D221" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E221" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>21</v>
       </c>
       <c r="B222" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D222" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E222" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>21</v>
       </c>
       <c r="B223" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D223" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E223" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>21</v>
       </c>
       <c r="B224" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D224" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E224" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>21</v>
       </c>
       <c r="B225" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D225" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E225" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>21</v>
       </c>
       <c r="B226" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D226" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E226" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>21</v>
       </c>
       <c r="B227" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D227" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E227" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>21</v>
       </c>
       <c r="B228" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D228" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E228" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>21</v>
       </c>
       <c r="B229" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D229" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E229" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>21</v>
       </c>
       <c r="B230" t="s">
+        <v>187</v>
+      </c>
+      <c r="D230" t="s">
+        <v>188</v>
+      </c>
+      <c r="E230" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>21</v>
+      </c>
+      <c r="B231" t="s">
         <v>222</v>
       </c>
-      <c r="C230" s="1">
-        <v>1</v>
-      </c>
-      <c r="D230" t="s">
+      <c r="C231" s="1">
+        <v>1</v>
+      </c>
+      <c r="D231" t="s">
         <v>223</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E231" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A231" t="s">
-        <v>55</v>
-      </c>
-      <c r="B231" t="s">
-        <v>56</v>
-      </c>
-      <c r="C231" s="1">
-        <v>1</v>
-      </c>
-      <c r="D231" t="s">
-        <v>57</v>
-      </c>
-      <c r="E231" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>55</v>
       </c>
@@ -4753,10 +4758,10 @@
         <v>57</v>
       </c>
       <c r="E232" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>55</v>
       </c>
@@ -4770,10 +4775,10 @@
         <v>57</v>
       </c>
       <c r="E233" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>55</v>
       </c>
@@ -4787,15 +4792,15 @@
         <v>57</v>
       </c>
       <c r="E234" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>55</v>
       </c>
       <c r="B235" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -4804,15 +4809,15 @@
         <v>57</v>
       </c>
       <c r="E235" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>55</v>
       </c>
       <c r="B236" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -4821,15 +4826,15 @@
         <v>57</v>
       </c>
       <c r="E236" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>55</v>
       </c>
       <c r="B237" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -4838,49 +4843,49 @@
         <v>57</v>
       </c>
       <c r="E237" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>55</v>
+      </c>
+      <c r="B238" t="s">
+        <v>66</v>
+      </c>
+      <c r="C238" s="1">
+        <v>1</v>
+      </c>
+      <c r="D238" t="s">
+        <v>57</v>
+      </c>
+      <c r="E238" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A238" t="s">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
         <v>134</v>
-      </c>
-      <c r="B238" t="s">
-        <v>82</v>
-      </c>
-      <c r="C238" s="1">
-        <v>1</v>
-      </c>
-      <c r="D238" t="s">
-        <v>45</v>
-      </c>
-      <c r="E238" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A239" t="s">
-        <v>131</v>
       </c>
       <c r="B239" t="s">
         <v>82</v>
       </c>
       <c r="C239" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D239" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="E239" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>131</v>
       </c>
       <c r="B240" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C240" s="1">
         <v>2</v>
@@ -4889,32 +4894,32 @@
         <v>150</v>
       </c>
       <c r="E240" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>131</v>
       </c>
       <c r="B241" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C241" s="1">
         <v>2</v>
       </c>
       <c r="D241" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E241" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>131</v>
       </c>
       <c r="B242" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C242" s="1">
         <v>2</v>
@@ -4923,32 +4928,32 @@
         <v>148</v>
       </c>
       <c r="E242" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>131</v>
       </c>
       <c r="B243" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C243" s="1">
         <v>2</v>
       </c>
       <c r="D243" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E243" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>131</v>
       </c>
       <c r="B244" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C244" s="1">
         <v>2</v>
@@ -4957,32 +4962,32 @@
         <v>155</v>
       </c>
       <c r="E244" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>131</v>
       </c>
       <c r="B245" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C245" s="1">
         <v>2</v>
       </c>
       <c r="D245" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E245" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>131</v>
       </c>
       <c r="B246" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C246" s="1">
         <v>2</v>
@@ -4991,32 +4996,32 @@
         <v>152</v>
       </c>
       <c r="E246" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>131</v>
       </c>
       <c r="B247" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C247" s="1">
         <v>2</v>
       </c>
       <c r="D247" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E247" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>131</v>
       </c>
       <c r="B248" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C248" s="1">
         <v>2</v>
@@ -5025,32 +5030,32 @@
         <v>145</v>
       </c>
       <c r="E248" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>131</v>
+      </c>
+      <c r="B249" t="s">
+        <v>147</v>
+      </c>
+      <c r="C249" s="1">
+        <v>2</v>
+      </c>
+      <c r="D249" t="s">
+        <v>145</v>
+      </c>
+      <c r="E249" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A249" t="s">
-        <v>88</v>
-      </c>
-      <c r="B249" t="s">
-        <v>82</v>
-      </c>
-      <c r="C249" s="1">
-        <v>1</v>
-      </c>
-      <c r="D249" t="s">
-        <v>175</v>
-      </c>
-      <c r="E249" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>88</v>
       </c>
       <c r="B250" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C250" s="1">
         <v>1</v>
@@ -5059,32 +5064,32 @@
         <v>175</v>
       </c>
       <c r="E250" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>88</v>
+      </c>
+      <c r="B251" t="s">
+        <v>147</v>
+      </c>
+      <c r="C251" s="1">
+        <v>1</v>
+      </c>
+      <c r="D251" t="s">
+        <v>175</v>
+      </c>
+      <c r="E251" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A251" t="s">
-        <v>10</v>
-      </c>
-      <c r="B251" t="s">
-        <v>11</v>
-      </c>
-      <c r="C251" s="1">
-        <v>1</v>
-      </c>
-      <c r="D251" t="s">
-        <v>12</v>
-      </c>
-      <c r="E251" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>10</v>
       </c>
       <c r="B252" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C252" s="1">
         <v>1</v>
@@ -5093,15 +5098,15 @@
         <v>12</v>
       </c>
       <c r="E252" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>10</v>
       </c>
       <c r="B253" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C253" s="1">
         <v>1</v>
@@ -5110,46 +5115,46 @@
         <v>12</v>
       </c>
       <c r="E253" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>10</v>
+      </c>
+      <c r="B254" t="s">
+        <v>13</v>
+      </c>
+      <c r="C254" s="1">
+        <v>1</v>
+      </c>
+      <c r="D254" t="s">
+        <v>12</v>
+      </c>
+      <c r="E254" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A254" t="s">
-        <v>201</v>
-      </c>
-      <c r="B254" t="s">
-        <v>82</v>
-      </c>
-      <c r="C254" s="1">
-        <v>2</v>
-      </c>
-      <c r="D254" t="s">
-        <v>195</v>
-      </c>
-      <c r="E254" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>201</v>
       </c>
       <c r="B255" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C255" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D255" t="s">
         <v>195</v>
       </c>
       <c r="E255" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B256" t="s">
         <v>147</v>
@@ -5158,18 +5163,18 @@
         <v>1</v>
       </c>
       <c r="D256" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="E256" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>214</v>
       </c>
       <c r="B257" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C257" s="1">
         <v>1</v>
@@ -5178,15 +5183,15 @@
         <v>230</v>
       </c>
       <c r="E257" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>214</v>
       </c>
       <c r="B258" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C258" s="1">
         <v>1</v>
@@ -5195,15 +5200,15 @@
         <v>230</v>
       </c>
       <c r="E258" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>214</v>
       </c>
       <c r="B259" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C259" s="1">
         <v>1</v>
@@ -5212,15 +5217,15 @@
         <v>230</v>
       </c>
       <c r="E259" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>214</v>
       </c>
       <c r="B260" t="s">
-        <v>218</v>
+        <v>66</v>
       </c>
       <c r="C260" s="1">
         <v>1</v>
@@ -5229,44 +5234,44 @@
         <v>230</v>
       </c>
       <c r="E260" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>214</v>
+      </c>
+      <c r="B261" t="s">
+        <v>218</v>
+      </c>
+      <c r="C261" s="1">
+        <v>1</v>
+      </c>
+      <c r="D261" t="s">
+        <v>230</v>
+      </c>
+      <c r="E261" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A261" t="s">
-        <v>174</v>
-      </c>
-      <c r="B261" t="s">
-        <v>82</v>
-      </c>
-      <c r="C261" s="1">
-        <v>2</v>
-      </c>
-      <c r="D261" t="s">
-        <v>173</v>
-      </c>
-      <c r="E261" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>174</v>
       </c>
       <c r="B262" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C262" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D262" t="s">
         <v>173</v>
       </c>
       <c r="E262" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>174</v>
       </c>
@@ -5277,9 +5282,26 @@
         <v>1</v>
       </c>
       <c r="D263" t="s">
+        <v>173</v>
+      </c>
+      <c r="E263" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>174</v>
+      </c>
+      <c r="B264" t="s">
+        <v>147</v>
+      </c>
+      <c r="C264" s="1">
+        <v>1</v>
+      </c>
+      <c r="D264" t="s">
         <v>186</v>
       </c>
-      <c r="E263" t="s">
+      <c r="E264" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add snippets for ComposeType, Days, ItemNotificationMessageType, RecipientType, RecurrenceTimeZone, and RecurrenceType
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25606"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C3332B-9EBC-4E83-806C-8533EA8BD98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6DC717-9E1D-4B2F-83E8-19A7671833A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-90" windowWidth="38640" windowHeight="23520" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="1725" yWindow="3000" windowWidth="28800" windowHeight="17145" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="247">
   <si>
     <t>Class</t>
   </si>
@@ -754,6 +755,21 @@
   </si>
   <si>
     <t>MailboxEnums.ComposeType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.Days</t>
+  </si>
+  <si>
+    <t>MailboxEnums.ItemNotificationMessageType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.RecipientType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.RecurrenceTimeZone</t>
+  </si>
+  <si>
+    <t>MailboxEnums.RecurrenceType</t>
   </si>
 </sst>
 </file>
@@ -836,10 +852,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E264" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E264" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E264">
-    <sortCondition ref="A1:A264"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E269" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E269" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E269">
+    <sortCondition ref="A1:A269"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="4"/>
@@ -1169,11 +1185,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E264"/>
+  <dimension ref="A1:E269"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B139" sqref="B139"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,207 +3344,197 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
+      <c r="A139" t="s">
         <v>241</v>
       </c>
-      <c r="B139" s="2"/>
-      <c r="C139" s="3" t="s">
+      <c r="C139" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D139" s="2" t="s">
+      <c r="D139" t="s">
         <v>137</v>
       </c>
-      <c r="E139" s="2" t="s">
+      <c r="E139" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D140" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="E140" t="s">
-        <v>220</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D141" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E141" t="s">
-        <v>110</v>
+        <v>220</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D142" t="s">
-        <v>192</v>
+        <v>109</v>
       </c>
       <c r="E142" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D143" t="s">
-        <v>119</v>
+        <v>57</v>
       </c>
       <c r="E143" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>86</v>
-      </c>
-      <c r="B144" t="s">
-        <v>82</v>
-      </c>
-      <c r="C144" s="1">
-        <v>2</v>
+        <v>238</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="D144" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="E144" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>86</v>
-      </c>
-      <c r="B145" t="s">
-        <v>56</v>
-      </c>
-      <c r="C145" s="1">
-        <v>1</v>
-      </c>
-      <c r="D145" t="s">
-        <v>158</v>
-      </c>
-      <c r="E145" t="s">
-        <v>156</v>
+      <c r="A145" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B145" s="2"/>
+      <c r="C145" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>86</v>
-      </c>
-      <c r="B146" t="s">
-        <v>66</v>
-      </c>
-      <c r="C146" s="1">
-        <v>1</v>
-      </c>
-      <c r="D146" t="s">
-        <v>158</v>
-      </c>
-      <c r="E146" t="s">
-        <v>157</v>
+      <c r="A146" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B146" s="2"/>
+      <c r="C146" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>20</v>
-      </c>
-      <c r="B147" t="s">
-        <v>18</v>
-      </c>
-      <c r="C147" s="1">
-        <v>1</v>
-      </c>
-      <c r="D147" t="s">
-        <v>15</v>
-      </c>
-      <c r="E147" t="s">
-        <v>5</v>
+      <c r="A147" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B147" s="2"/>
+      <c r="C147" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>20</v>
-      </c>
-      <c r="B148" t="s">
-        <v>22</v>
-      </c>
-      <c r="C148" s="1">
-        <v>2</v>
+        <v>239</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="D148" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="E148" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B149" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="C149" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D149" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E149" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B150" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="C150" s="1">
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="E150" t="s">
-        <v>4</v>
+        <v>156</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B151" t="s">
-        <v>30</v>
+        <v>66</v>
+      </c>
+      <c r="C151" s="1">
+        <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E151" t="s">
-        <v>31</v>
+        <v>157</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3536,13 +3542,16 @@
         <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>30</v>
+        <v>18</v>
+      </c>
+      <c r="C152" s="1">
+        <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="E152" t="s">
-        <v>151</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3550,13 +3559,16 @@
         <v>20</v>
       </c>
       <c r="B153" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="C153" s="1">
+        <v>2</v>
       </c>
       <c r="D153" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="E153" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -3564,13 +3576,16 @@
         <v>20</v>
       </c>
       <c r="B154" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="C154" s="1">
+        <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>148</v>
+        <v>26</v>
       </c>
       <c r="E154" t="s">
-        <v>149</v>
+        <v>27</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,13 +3593,16 @@
         <v>20</v>
       </c>
       <c r="B155" t="s">
-        <v>35</v>
+        <v>7</v>
+      </c>
+      <c r="C155" s="1">
+        <v>1</v>
       </c>
       <c r="D155" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E155" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -3592,13 +3610,13 @@
         <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D156" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E156" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -3606,13 +3624,13 @@
         <v>20</v>
       </c>
       <c r="B157" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D157" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E157" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3620,13 +3638,13 @@
         <v>20</v>
       </c>
       <c r="B158" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="D158" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="E158" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -3634,13 +3652,13 @@
         <v>20</v>
       </c>
       <c r="B159" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="D159" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="E159" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -3648,13 +3666,13 @@
         <v>20</v>
       </c>
       <c r="B160" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
       <c r="D160" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="E160" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -3662,13 +3680,13 @@
         <v>20</v>
       </c>
       <c r="B161" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D161" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="E161" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -3676,13 +3694,13 @@
         <v>20</v>
       </c>
       <c r="B162" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D162" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="E162" t="s">
-        <v>65</v>
+        <v>146</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -3696,7 +3714,7 @@
         <v>57</v>
       </c>
       <c r="E163" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -3704,16 +3722,13 @@
         <v>20</v>
       </c>
       <c r="B164" t="s">
-        <v>67</v>
-      </c>
-      <c r="C164" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D164" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E164" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -3721,16 +3736,13 @@
         <v>20</v>
       </c>
       <c r="B165" t="s">
-        <v>70</v>
-      </c>
-      <c r="C165" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D165" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E165" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -3738,16 +3750,13 @@
         <v>20</v>
       </c>
       <c r="B166" t="s">
-        <v>72</v>
-      </c>
-      <c r="C166" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D166" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E166" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -3755,16 +3764,13 @@
         <v>20</v>
       </c>
       <c r="B167" t="s">
-        <v>72</v>
-      </c>
-      <c r="C167" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D167" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="E167" t="s">
-        <v>203</v>
+        <v>65</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -3772,16 +3778,13 @@
         <v>20</v>
       </c>
       <c r="B168" t="s">
-        <v>74</v>
-      </c>
-      <c r="C168" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D168" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E168" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -3789,7 +3792,7 @@
         <v>20</v>
       </c>
       <c r="B169" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C169" s="1">
         <v>1</v>
@@ -3798,7 +3801,7 @@
         <v>68</v>
       </c>
       <c r="E169" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -3806,16 +3809,16 @@
         <v>20</v>
       </c>
       <c r="B170" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C170" s="1">
         <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="E170" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -3823,13 +3826,16 @@
         <v>20</v>
       </c>
       <c r="B171" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="C171" s="1">
+        <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>161</v>
+        <v>68</v>
       </c>
       <c r="E171" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -3837,13 +3843,16 @@
         <v>20</v>
       </c>
       <c r="B172" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="C172" s="1">
+        <v>1</v>
       </c>
       <c r="D172" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="E172" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -3851,13 +3860,16 @@
         <v>20</v>
       </c>
       <c r="B173" t="s">
-        <v>79</v>
+        <v>74</v>
+      </c>
+      <c r="C173" s="1">
+        <v>1</v>
       </c>
       <c r="D173" t="s">
-        <v>161</v>
+        <v>68</v>
       </c>
       <c r="E173" t="s">
-        <v>160</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -3865,13 +3877,16 @@
         <v>20</v>
       </c>
       <c r="B174" t="s">
-        <v>90</v>
+        <v>75</v>
+      </c>
+      <c r="C174" s="1">
+        <v>1</v>
       </c>
       <c r="D174" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="E174" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -3879,16 +3894,16 @@
         <v>20</v>
       </c>
       <c r="B175" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="C175" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D175" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="E175" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -3896,16 +3911,13 @@
         <v>20</v>
       </c>
       <c r="B176" t="s">
-        <v>106</v>
-      </c>
-      <c r="C176" s="1">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D176" t="s">
-        <v>105</v>
+        <v>161</v>
       </c>
       <c r="E176" t="s">
-        <v>221</v>
+        <v>80</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -3913,16 +3925,13 @@
         <v>20</v>
       </c>
       <c r="B177" t="s">
-        <v>124</v>
-      </c>
-      <c r="C177" s="1">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D177" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="E177" t="s">
-        <v>4</v>
+        <v>159</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -3930,16 +3939,13 @@
         <v>20</v>
       </c>
       <c r="B178" t="s">
-        <v>141</v>
-      </c>
-      <c r="C178" s="1">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D178" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="E178" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -3947,16 +3953,13 @@
         <v>20</v>
       </c>
       <c r="B179" t="s">
-        <v>143</v>
-      </c>
-      <c r="C179" s="1">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D179" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="E179" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -3964,16 +3967,16 @@
         <v>20</v>
       </c>
       <c r="B180" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="C180" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D180" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="E180" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -3981,13 +3984,16 @@
         <v>20</v>
       </c>
       <c r="B181" t="s">
-        <v>162</v>
+        <v>106</v>
+      </c>
+      <c r="C181" s="1">
+        <v>1</v>
       </c>
       <c r="D181" t="s">
-        <v>164</v>
+        <v>105</v>
       </c>
       <c r="E181" t="s">
-        <v>11</v>
+        <v>221</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -3995,13 +4001,16 @@
         <v>20</v>
       </c>
       <c r="B182" t="s">
-        <v>162</v>
+        <v>124</v>
+      </c>
+      <c r="C182" s="1">
+        <v>2</v>
       </c>
       <c r="D182" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="E182" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -4009,13 +4018,16 @@
         <v>20</v>
       </c>
       <c r="B183" t="s">
-        <v>169</v>
+        <v>141</v>
+      </c>
+      <c r="C183" s="1">
+        <v>2</v>
       </c>
       <c r="D183" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="E183" t="s">
-        <v>11</v>
+        <v>142</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -4023,13 +4035,16 @@
         <v>20</v>
       </c>
       <c r="B184" t="s">
-        <v>178</v>
+        <v>143</v>
+      </c>
+      <c r="C184" s="1">
+        <v>1</v>
       </c>
       <c r="D184" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
       <c r="E184" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4037,13 +4052,16 @@
         <v>20</v>
       </c>
       <c r="B185" t="s">
-        <v>212</v>
+        <v>136</v>
+      </c>
+      <c r="C185" s="1">
+        <v>1</v>
       </c>
       <c r="D185" t="s">
-        <v>230</v>
+        <v>137</v>
       </c>
       <c r="E185" t="s">
-        <v>213</v>
+        <v>138</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4051,86 +4069,83 @@
         <v>20</v>
       </c>
       <c r="B186" t="s">
-        <v>224</v>
+        <v>162</v>
       </c>
       <c r="D186" t="s">
-        <v>225</v>
+        <v>164</v>
       </c>
       <c r="E186" t="s">
-        <v>226</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B187" t="s">
-        <v>18</v>
-      </c>
-      <c r="C187" s="1">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="D187" t="s">
-        <v>15</v>
+        <v>164</v>
       </c>
       <c r="E187" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B188" t="s">
-        <v>32</v>
+        <v>169</v>
       </c>
       <c r="D188" t="s">
-        <v>34</v>
+        <v>170</v>
       </c>
       <c r="E188" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B189" t="s">
-        <v>35</v>
+        <v>178</v>
       </c>
       <c r="D189" t="s">
-        <v>38</v>
+        <v>179</v>
       </c>
       <c r="E189" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B190" t="s">
-        <v>49</v>
+        <v>212</v>
       </c>
       <c r="D190" t="s">
-        <v>50</v>
+        <v>230</v>
       </c>
       <c r="E190" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B191" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="D191" t="s">
-        <v>54</v>
+        <v>225</v>
       </c>
       <c r="E191" t="s">
-        <v>53</v>
+        <v>226</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -4138,13 +4153,16 @@
         <v>21</v>
       </c>
       <c r="B192" t="s">
-        <v>132</v>
+        <v>18</v>
+      </c>
+      <c r="C192" s="1">
+        <v>1</v>
       </c>
       <c r="D192" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="E192" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -4152,13 +4170,13 @@
         <v>21</v>
       </c>
       <c r="B193" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="D193" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="E193" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -4166,13 +4184,13 @@
         <v>21</v>
       </c>
       <c r="B194" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
       <c r="D194" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E194" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -4180,13 +4198,13 @@
         <v>21</v>
       </c>
       <c r="B195" t="s">
-        <v>132</v>
+        <v>49</v>
       </c>
       <c r="D195" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E195" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -4194,13 +4212,13 @@
         <v>21</v>
       </c>
       <c r="B196" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D196" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E196" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4214,7 +4232,7 @@
         <v>57</v>
       </c>
       <c r="E197" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -4222,16 +4240,13 @@
         <v>21</v>
       </c>
       <c r="B198" t="s">
-        <v>76</v>
-      </c>
-      <c r="C198" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D198" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="E198" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -4239,13 +4254,13 @@
         <v>21</v>
       </c>
       <c r="B199" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
       <c r="D199" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="E199" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -4253,13 +4268,13 @@
         <v>21</v>
       </c>
       <c r="B200" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="D200" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="E200" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -4267,13 +4282,13 @@
         <v>21</v>
       </c>
       <c r="B201" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="D201" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="E201" t="s">
-        <v>159</v>
+        <v>65</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -4281,13 +4296,13 @@
         <v>21</v>
       </c>
       <c r="B202" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="D202" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="E202" t="s">
-        <v>160</v>
+        <v>16</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -4295,13 +4310,16 @@
         <v>21</v>
       </c>
       <c r="B203" t="s">
-        <v>87</v>
+        <v>76</v>
+      </c>
+      <c r="C203" s="1">
+        <v>1</v>
       </c>
       <c r="D203" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="E203" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -4309,13 +4327,13 @@
         <v>21</v>
       </c>
       <c r="B204" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D204" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E204" t="s">
-        <v>92</v>
+        <v>4</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -4323,16 +4341,13 @@
         <v>21</v>
       </c>
       <c r="B205" t="s">
-        <v>101</v>
-      </c>
-      <c r="C205" s="1">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D205" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="E205" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -4340,16 +4355,13 @@
         <v>21</v>
       </c>
       <c r="B206" t="s">
-        <v>102</v>
-      </c>
-      <c r="C206" s="1">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D206" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="E206" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -4357,16 +4369,13 @@
         <v>21</v>
       </c>
       <c r="B207" t="s">
-        <v>101</v>
-      </c>
-      <c r="C207" s="1">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D207" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
       <c r="E207" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -4374,16 +4383,13 @@
         <v>21</v>
       </c>
       <c r="B208" t="s">
-        <v>209</v>
-      </c>
-      <c r="C208" s="1">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D208" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E208" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -4391,16 +4397,13 @@
         <v>21</v>
       </c>
       <c r="B209" t="s">
-        <v>210</v>
-      </c>
-      <c r="C209" s="1">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D209" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E209" t="s">
-        <v>210</v>
+        <v>92</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -4408,16 +4411,16 @@
         <v>21</v>
       </c>
       <c r="B210" t="s">
-        <v>209</v>
+        <v>101</v>
       </c>
       <c r="C210" s="1">
         <v>1</v>
       </c>
       <c r="D210" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E210" t="s">
-        <v>211</v>
+        <v>101</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -4425,16 +4428,16 @@
         <v>21</v>
       </c>
       <c r="B211" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C211" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D211" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E211" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -4442,16 +4445,16 @@
         <v>21</v>
       </c>
       <c r="B212" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
       </c>
       <c r="D212" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E212" t="s">
-        <v>221</v>
+        <v>4</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -4459,16 +4462,16 @@
         <v>21</v>
       </c>
       <c r="B213" t="s">
-        <v>108</v>
+        <v>209</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
       </c>
       <c r="D213" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E213" t="s">
-        <v>108</v>
+        <v>209</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -4476,16 +4479,16 @@
         <v>21</v>
       </c>
       <c r="B214" t="s">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
       </c>
       <c r="D214" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E214" t="s">
-        <v>110</v>
+        <v>210</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -4493,16 +4496,16 @@
         <v>21</v>
       </c>
       <c r="B215" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
       </c>
       <c r="D215" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E215" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -4510,16 +4513,16 @@
         <v>21</v>
       </c>
       <c r="B216" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C216" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D216" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E216" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -4527,16 +4530,16 @@
         <v>21</v>
       </c>
       <c r="B217" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C217" s="1">
         <v>1</v>
       </c>
       <c r="D217" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E217" t="s">
-        <v>114</v>
+        <v>221</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -4544,16 +4547,16 @@
         <v>21</v>
       </c>
       <c r="B218" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C218" s="1">
         <v>1</v>
       </c>
       <c r="D218" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E218" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -4561,16 +4564,16 @@
         <v>21</v>
       </c>
       <c r="B219" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C219" s="1">
         <v>1</v>
       </c>
       <c r="D219" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E219" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -4578,13 +4581,16 @@
         <v>21</v>
       </c>
       <c r="B220" t="s">
-        <v>162</v>
+        <v>111</v>
+      </c>
+      <c r="C220" s="1">
+        <v>1</v>
       </c>
       <c r="D220" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="E220" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -4592,13 +4598,16 @@
         <v>21</v>
       </c>
       <c r="B221" t="s">
-        <v>165</v>
+        <v>113</v>
+      </c>
+      <c r="C221" s="1">
+        <v>1</v>
       </c>
       <c r="D221" t="s">
-        <v>166</v>
+        <v>112</v>
       </c>
       <c r="E221" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -4606,13 +4615,16 @@
         <v>21</v>
       </c>
       <c r="B222" t="s">
-        <v>167</v>
+        <v>114</v>
+      </c>
+      <c r="C222" s="1">
+        <v>1</v>
       </c>
       <c r="D222" t="s">
-        <v>168</v>
+        <v>112</v>
       </c>
       <c r="E222" t="s">
-        <v>11</v>
+        <v>114</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -4620,13 +4632,16 @@
         <v>21</v>
       </c>
       <c r="B223" t="s">
-        <v>169</v>
+        <v>115</v>
+      </c>
+      <c r="C223" s="1">
+        <v>1</v>
       </c>
       <c r="D223" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="E223" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -4634,13 +4649,16 @@
         <v>21</v>
       </c>
       <c r="B224" t="s">
-        <v>171</v>
+        <v>117</v>
+      </c>
+      <c r="C224" s="1">
+        <v>1</v>
       </c>
       <c r="D224" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="E224" t="s">
-        <v>11</v>
+        <v>117</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -4648,10 +4666,10 @@
         <v>21</v>
       </c>
       <c r="B225" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="D225" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="E225" t="s">
         <v>11</v>
@@ -4662,10 +4680,10 @@
         <v>21</v>
       </c>
       <c r="B226" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="D226" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="E226" t="s">
         <v>11</v>
@@ -4676,10 +4694,10 @@
         <v>21</v>
       </c>
       <c r="B227" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="D227" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="E227" t="s">
         <v>11</v>
@@ -4690,10 +4708,10 @@
         <v>21</v>
       </c>
       <c r="B228" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D228" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="E228" t="s">
         <v>11</v>
@@ -4704,10 +4722,10 @@
         <v>21</v>
       </c>
       <c r="B229" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D229" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="E229" t="s">
         <v>11</v>
@@ -4718,10 +4736,10 @@
         <v>21</v>
       </c>
       <c r="B230" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D230" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="E230" t="s">
         <v>11</v>
@@ -4732,101 +4750,86 @@
         <v>21</v>
       </c>
       <c r="B231" t="s">
-        <v>222</v>
-      </c>
-      <c r="C231" s="1">
-        <v>1</v>
+        <v>178</v>
       </c>
       <c r="D231" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
       <c r="E231" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B232" t="s">
-        <v>56</v>
-      </c>
-      <c r="C232" s="1">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="D232" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="E232" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B233" t="s">
-        <v>56</v>
-      </c>
-      <c r="C233" s="1">
-        <v>1</v>
+        <v>182</v>
       </c>
       <c r="D233" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="E233" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B234" t="s">
-        <v>56</v>
-      </c>
-      <c r="C234" s="1">
-        <v>1</v>
+        <v>184</v>
       </c>
       <c r="D234" t="s">
-        <v>57</v>
+        <v>185</v>
       </c>
       <c r="E234" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B235" t="s">
-        <v>56</v>
-      </c>
-      <c r="C235" s="1">
-        <v>1</v>
+        <v>187</v>
       </c>
       <c r="D235" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="E235" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B236" t="s">
-        <v>62</v>
+        <v>222</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
       </c>
       <c r="D236" t="s">
-        <v>57</v>
+        <v>223</v>
       </c>
       <c r="E236" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -4834,7 +4837,7 @@
         <v>55</v>
       </c>
       <c r="B237" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -4843,7 +4846,7 @@
         <v>57</v>
       </c>
       <c r="E237" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -4851,7 +4854,7 @@
         <v>55</v>
       </c>
       <c r="B238" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C238" s="1">
         <v>1</v>
@@ -4860,109 +4863,109 @@
         <v>57</v>
       </c>
       <c r="E238" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>134</v>
+        <v>55</v>
       </c>
       <c r="B239" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="C239" s="1">
         <v>1</v>
       </c>
       <c r="D239" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E239" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B240" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="C240" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D240" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="E240" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B241" t="s">
-        <v>147</v>
+        <v>62</v>
       </c>
       <c r="C241" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D241" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="E241" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B242" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C242" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D242" t="s">
-        <v>148</v>
+        <v>57</v>
       </c>
       <c r="E242" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B243" t="s">
-        <v>147</v>
+        <v>66</v>
       </c>
       <c r="C243" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D243" t="s">
-        <v>148</v>
+        <v>57</v>
       </c>
       <c r="E243" t="s">
-        <v>149</v>
+        <v>16</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B244" t="s">
         <v>82</v>
       </c>
       <c r="C244" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D244" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="E244" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -4970,16 +4973,16 @@
         <v>131</v>
       </c>
       <c r="B245" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C245" s="1">
         <v>2</v>
       </c>
       <c r="D245" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E245" t="s">
-        <v>154</v>
+        <v>31</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -4987,16 +4990,16 @@
         <v>131</v>
       </c>
       <c r="B246" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C246" s="1">
         <v>2</v>
       </c>
       <c r="D246" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E246" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -5004,16 +5007,16 @@
         <v>131</v>
       </c>
       <c r="B247" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C247" s="1">
         <v>2</v>
       </c>
       <c r="D247" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E247" t="s">
-        <v>153</v>
+        <v>33</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -5021,16 +5024,16 @@
         <v>131</v>
       </c>
       <c r="B248" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C248" s="1">
         <v>2</v>
       </c>
       <c r="D248" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E248" t="s">
-        <v>53</v>
+        <v>149</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -5038,123 +5041,123 @@
         <v>131</v>
       </c>
       <c r="B249" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C249" s="1">
         <v>2</v>
       </c>
       <c r="D249" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E249" t="s">
-        <v>146</v>
+        <v>41</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="B250" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C250" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D250" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="E250" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="B251" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C251" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D251" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="E251" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="B252" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C252" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D252" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E252" t="s">
-        <v>11</v>
+        <v>153</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="B253" t="s">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="C253" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D253" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="E253" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="B254" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="C254" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="E254" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>201</v>
+        <v>88</v>
       </c>
       <c r="B255" t="s">
         <v>82</v>
       </c>
       <c r="C255" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D255" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="E255" t="s">
-        <v>200</v>
+        <v>11</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>201</v>
+        <v>88</v>
       </c>
       <c r="B256" t="s">
         <v>147</v>
@@ -5163,145 +5166,230 @@
         <v>1</v>
       </c>
       <c r="D256" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="E256" t="s">
-        <v>202</v>
+        <v>3</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="B257" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="C257" s="1">
         <v>1</v>
       </c>
       <c r="D257" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="E257" t="s">
-        <v>215</v>
+        <v>11</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="B258" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="C258" s="1">
         <v>1</v>
       </c>
       <c r="D258" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="E258" t="s">
-        <v>216</v>
+        <v>3</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="B259" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C259" s="1">
         <v>1</v>
       </c>
       <c r="D259" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="E259" t="s">
-        <v>213</v>
+        <v>6</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B260" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="C260" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D260" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="E260" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B261" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="C261" s="1">
         <v>1</v>
       </c>
       <c r="D261" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="E261" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="B262" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C262" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D262" t="s">
-        <v>173</v>
+        <v>230</v>
       </c>
       <c r="E262" t="s">
-        <v>11</v>
+        <v>215</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="B263" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C263" s="1">
         <v>1</v>
       </c>
       <c r="D263" t="s">
-        <v>173</v>
+        <v>230</v>
       </c>
       <c r="E263" t="s">
-        <v>3</v>
+        <v>216</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
+        <v>214</v>
+      </c>
+      <c r="B264" t="s">
+        <v>62</v>
+      </c>
+      <c r="C264" s="1">
+        <v>1</v>
+      </c>
+      <c r="D264" t="s">
+        <v>230</v>
+      </c>
+      <c r="E264" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>214</v>
+      </c>
+      <c r="B265" t="s">
+        <v>66</v>
+      </c>
+      <c r="C265" s="1">
+        <v>1</v>
+      </c>
+      <c r="D265" t="s">
+        <v>230</v>
+      </c>
+      <c r="E265" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>214</v>
+      </c>
+      <c r="B266" t="s">
+        <v>218</v>
+      </c>
+      <c r="C266" s="1">
+        <v>1</v>
+      </c>
+      <c r="D266" t="s">
+        <v>230</v>
+      </c>
+      <c r="E266" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
         <v>174</v>
       </c>
-      <c r="B264" t="s">
+      <c r="B267" t="s">
+        <v>82</v>
+      </c>
+      <c r="C267" s="1">
+        <v>2</v>
+      </c>
+      <c r="D267" t="s">
+        <v>173</v>
+      </c>
+      <c r="E267" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>174</v>
+      </c>
+      <c r="B268" t="s">
         <v>147</v>
       </c>
-      <c r="C264" s="1">
-        <v>1</v>
-      </c>
-      <c r="D264" t="s">
+      <c r="C268" s="1">
+        <v>1</v>
+      </c>
+      <c r="D268" t="s">
+        <v>173</v>
+      </c>
+      <c r="E268" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>174</v>
+      </c>
+      <c r="B269" t="s">
+        <v>147</v>
+      </c>
+      <c r="C269" s="1">
+        <v>1</v>
+      </c>
+      <c r="D269" t="s">
         <v>186</v>
       </c>
-      <c r="E264" t="s">
+      <c r="E269" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Outlook] (enum) Add Script Lab samples to MailboxEnums (#685)
* Add snippet for MailboxEnums.ComposeType and clarify getComposeType function

* Add snippets for ComposeType, Days, ItemNotificationMessageType, RecipientType, RecurrenceTimeZone, and RecurrenceType

* Apply suggestion from review
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25606"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65695B3E-71C4-45F0-9459-45EEA54EDADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6DC717-9E1D-4B2F-83E8-19A7671833A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="1725" yWindow="3000" windowWidth="28800" windowHeight="17145" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="247">
   <si>
     <t>Class</t>
   </si>
@@ -751,6 +752,24 @@
   </si>
   <si>
     <t>MailboxEnums.AppointmentSensitivityType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.ComposeType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.Days</t>
+  </si>
+  <si>
+    <t>MailboxEnums.ItemNotificationMessageType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.RecipientType</t>
+  </si>
+  <si>
+    <t>MailboxEnums.RecurrenceTimeZone</t>
+  </si>
+  <si>
+    <t>MailboxEnums.RecurrenceType</t>
   </si>
 </sst>
 </file>
@@ -786,9 +805,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -829,10 +852,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E263" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E263" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E263">
-    <sortCondition ref="A1:A263"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E269" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E269" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E269">
+    <sortCondition ref="A1:A269"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="4"/>
@@ -1162,23 +1185,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E263"/>
+  <dimension ref="A1:E269"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A137" sqref="A137"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="74.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1212,7 +1235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1252,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1246,7 +1269,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1263,7 +1286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1280,7 +1303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1294,7 +1317,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1308,7 +1331,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1322,7 +1345,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1336,7 +1359,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1350,7 +1373,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1364,7 +1387,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1378,7 +1401,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1415,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1406,7 +1429,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1443,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1434,7 +1457,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1451,7 +1474,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1468,7 +1491,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1485,7 +1508,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1502,7 +1525,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1519,7 +1542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1536,7 +1559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1553,7 +1576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1567,7 +1590,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1581,7 +1604,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1595,7 +1618,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1609,7 +1632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1623,7 +1646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1637,7 +1660,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1654,7 +1677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1671,7 +1694,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1688,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1705,7 +1728,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1722,7 +1745,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1736,7 +1759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1750,7 +1773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1764,7 +1787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -1778,7 +1801,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1792,7 +1815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +1829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1820,7 +1843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1834,7 +1857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1848,7 +1871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1862,7 +1885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1876,7 +1899,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1890,7 +1913,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1904,7 +1927,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1918,7 +1941,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1932,7 +1955,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -1946,7 +1969,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -1960,7 +1983,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -1977,7 +2000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1991,7 +2014,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -2005,7 +2028,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -2019,7 +2042,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -2033,7 +2056,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -2047,7 +2070,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -2061,7 +2084,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -2075,7 +2098,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2089,7 +2112,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -2103,7 +2126,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -2120,7 +2143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -2134,7 +2157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -2148,7 +2171,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -2162,7 +2185,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -2176,7 +2199,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -2190,7 +2213,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -2204,7 +2227,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -2221,7 +2244,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -2238,7 +2261,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -2255,7 +2278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -2272,7 +2295,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -2289,7 +2312,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -2306,7 +2329,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -2323,7 +2346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
@@ -2340,7 +2363,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -2357,7 +2380,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -2374,7 +2397,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2391,7 +2414,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>19</v>
       </c>
@@ -2408,7 +2431,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>19</v>
       </c>
@@ -2425,7 +2448,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -2442,7 +2465,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -2459,7 +2482,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -2473,7 +2496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>19</v>
       </c>
@@ -2487,7 +2510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -2501,7 +2524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>19</v>
       </c>
@@ -2515,7 +2538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -2529,7 +2552,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -2543,7 +2566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>19</v>
       </c>
@@ -2557,7 +2580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>19</v>
       </c>
@@ -2571,7 +2594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2585,7 +2608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -2599,7 +2622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>139</v>
       </c>
@@ -2616,7 +2639,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>139</v>
       </c>
@@ -2633,7 +2656,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>81</v>
       </c>
@@ -2650,7 +2673,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>81</v>
       </c>
@@ -2667,7 +2690,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>81</v>
       </c>
@@ -2684,7 +2707,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -2701,7 +2724,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -2718,7 +2741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>14</v>
       </c>
@@ -2735,7 +2758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>193</v>
       </c>
@@ -2752,7 +2775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -2769,7 +2792,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>193</v>
       </c>
@@ -2786,7 +2809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>133</v>
       </c>
@@ -2803,7 +2826,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>227</v>
       </c>
@@ -2820,7 +2843,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>227</v>
       </c>
@@ -2837,7 +2860,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>227</v>
       </c>
@@ -2854,7 +2877,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>197</v>
       </c>
@@ -2871,7 +2894,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>197</v>
       </c>
@@ -2888,7 +2911,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>190</v>
       </c>
@@ -2905,7 +2928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>190</v>
       </c>
@@ -2922,7 +2945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>83</v>
       </c>
@@ -2936,7 +2959,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>83</v>
       </c>
@@ -2950,7 +2973,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>83</v>
       </c>
@@ -2964,7 +2987,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>83</v>
       </c>
@@ -2981,7 +3004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>83</v>
       </c>
@@ -2998,7 +3021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>83</v>
       </c>
@@ -3015,7 +3038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>83</v>
       </c>
@@ -3032,7 +3055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>83</v>
       </c>
@@ -3049,7 +3072,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>83</v>
       </c>
@@ -3066,7 +3089,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>83</v>
       </c>
@@ -3083,7 +3106,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>83</v>
       </c>
@@ -3100,7 +3123,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>83</v>
       </c>
@@ -3117,7 +3140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>83</v>
       </c>
@@ -3131,7 +3154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>83</v>
       </c>
@@ -3148,7 +3171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>83</v>
       </c>
@@ -3162,7 +3185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>83</v>
       </c>
@@ -3176,7 +3199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>83</v>
       </c>
@@ -3193,7 +3216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>83</v>
       </c>
@@ -3210,7 +3233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>83</v>
       </c>
@@ -3227,7 +3250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>83</v>
       </c>
@@ -3244,7 +3267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>83</v>
       </c>
@@ -3261,7 +3284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>83</v>
       </c>
@@ -3278,7 +3301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>240</v>
       </c>
@@ -3292,7 +3315,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>234</v>
       </c>
@@ -3306,7 +3329,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>235</v>
       </c>
@@ -3320,1516 +3343,1501 @@
         <v>156</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D139" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="E139" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D140" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
       <c r="E140" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D141" t="s">
-        <v>192</v>
+        <v>105</v>
       </c>
       <c r="E141" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D142" t="s">
+        <v>109</v>
+      </c>
+      <c r="E142" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>243</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D143" t="s">
+        <v>57</v>
+      </c>
+      <c r="E143" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>238</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D144" t="s">
+        <v>192</v>
+      </c>
+      <c r="E144" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B145" s="2"/>
+      <c r="C145" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B146" s="2"/>
+      <c r="C146" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B147" s="2"/>
+      <c r="C147" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>239</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D148" t="s">
         <v>119</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E148" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>86</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B149" t="s">
         <v>82</v>
       </c>
-      <c r="C143" s="1">
+      <c r="C149" s="1">
         <v>2</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D149" t="s">
         <v>158</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E149" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>86</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B150" t="s">
         <v>56</v>
       </c>
-      <c r="C144" s="1">
-        <v>1</v>
-      </c>
-      <c r="D144" t="s">
+      <c r="C150" s="1">
+        <v>1</v>
+      </c>
+      <c r="D150" t="s">
         <v>158</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E150" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>86</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B151" t="s">
         <v>66</v>
       </c>
-      <c r="C145" s="1">
-        <v>1</v>
-      </c>
-      <c r="D145" t="s">
+      <c r="C151" s="1">
+        <v>1</v>
+      </c>
+      <c r="D151" t="s">
         <v>158</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E151" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>20</v>
-      </c>
-      <c r="B146" t="s">
-        <v>18</v>
-      </c>
-      <c r="C146" s="1">
-        <v>1</v>
-      </c>
-      <c r="D146" t="s">
-        <v>15</v>
-      </c>
-      <c r="E146" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>20</v>
-      </c>
-      <c r="B147" t="s">
-        <v>22</v>
-      </c>
-      <c r="C147" s="1">
-        <v>2</v>
-      </c>
-      <c r="D147" t="s">
-        <v>23</v>
-      </c>
-      <c r="E147" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>20</v>
-      </c>
-      <c r="B148" t="s">
-        <v>25</v>
-      </c>
-      <c r="C148" s="1">
-        <v>1</v>
-      </c>
-      <c r="D148" t="s">
-        <v>26</v>
-      </c>
-      <c r="E148" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>20</v>
-      </c>
-      <c r="B149" t="s">
-        <v>7</v>
-      </c>
-      <c r="C149" s="1">
-        <v>1</v>
-      </c>
-      <c r="D149" t="s">
-        <v>28</v>
-      </c>
-      <c r="E149" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>20</v>
-      </c>
-      <c r="B150" t="s">
-        <v>30</v>
-      </c>
-      <c r="D150" t="s">
-        <v>150</v>
-      </c>
-      <c r="E150" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>20</v>
-      </c>
-      <c r="B151" t="s">
-        <v>30</v>
-      </c>
-      <c r="D151" t="s">
-        <v>150</v>
-      </c>
-      <c r="E151" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="C152" s="1">
+        <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>148</v>
+        <v>15</v>
       </c>
       <c r="E152" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>20</v>
       </c>
       <c r="B153" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="C153" s="1">
+        <v>2</v>
       </c>
       <c r="D153" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="E153" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>20</v>
       </c>
       <c r="B154" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="C154" s="1">
+        <v>1</v>
       </c>
       <c r="D154" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E154" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>20</v>
       </c>
       <c r="B155" t="s">
-        <v>52</v>
+        <v>7</v>
+      </c>
+      <c r="C155" s="1">
+        <v>1</v>
       </c>
       <c r="D155" t="s">
-        <v>145</v>
+        <v>28</v>
       </c>
       <c r="E155" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D156" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E156" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>20</v>
       </c>
       <c r="B157" t="s">
-        <v>132</v>
+        <v>30</v>
       </c>
       <c r="D157" t="s">
-        <v>57</v>
+        <v>150</v>
       </c>
       <c r="E157" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>20</v>
       </c>
       <c r="B158" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="D158" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="E158" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>20</v>
       </c>
       <c r="B159" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="D159" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="E159" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>20</v>
       </c>
       <c r="B160" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
       <c r="D160" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="E160" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>20</v>
       </c>
       <c r="B161" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D161" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="E161" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>20</v>
       </c>
       <c r="B162" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D162" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="E162" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>20</v>
       </c>
       <c r="B163" t="s">
-        <v>67</v>
-      </c>
-      <c r="C163" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D163" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E163" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>20</v>
       </c>
       <c r="B164" t="s">
-        <v>70</v>
-      </c>
-      <c r="C164" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D164" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E164" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>20</v>
       </c>
       <c r="B165" t="s">
-        <v>72</v>
-      </c>
-      <c r="C165" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D165" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E165" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>20</v>
       </c>
       <c r="B166" t="s">
-        <v>72</v>
-      </c>
-      <c r="C166" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D166" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="E166" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>20</v>
       </c>
       <c r="B167" t="s">
-        <v>74</v>
-      </c>
-      <c r="C167" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D167" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E167" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>20</v>
       </c>
       <c r="B168" t="s">
-        <v>75</v>
-      </c>
-      <c r="C168" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D168" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E168" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>20</v>
       </c>
       <c r="B169" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C169" s="1">
         <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="E169" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>20</v>
       </c>
       <c r="B170" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="C170" s="1">
+        <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>161</v>
+        <v>68</v>
       </c>
       <c r="E170" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>20</v>
       </c>
       <c r="B171" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="C171" s="1">
+        <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>161</v>
+        <v>68</v>
       </c>
       <c r="E171" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>20</v>
       </c>
       <c r="B172" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="C172" s="1">
+        <v>1</v>
       </c>
       <c r="D172" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="E172" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>20</v>
       </c>
       <c r="B173" t="s">
-        <v>90</v>
+        <v>74</v>
+      </c>
+      <c r="C173" s="1">
+        <v>1</v>
       </c>
       <c r="D173" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="E173" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>20</v>
       </c>
       <c r="B174" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C174" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D174" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="E174" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>20</v>
       </c>
       <c r="B175" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="C175" s="1">
         <v>1</v>
       </c>
       <c r="D175" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="E175" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>20</v>
       </c>
       <c r="B176" t="s">
-        <v>124</v>
-      </c>
-      <c r="C176" s="1">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D176" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="E176" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>20</v>
       </c>
       <c r="B177" t="s">
-        <v>141</v>
-      </c>
-      <c r="C177" s="1">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D177" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="E177" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>20</v>
       </c>
       <c r="B178" t="s">
-        <v>143</v>
-      </c>
-      <c r="C178" s="1">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D178" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="E178" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>20</v>
       </c>
       <c r="B179" t="s">
-        <v>136</v>
-      </c>
-      <c r="C179" s="1">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D179" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="E179" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>20</v>
       </c>
       <c r="B180" t="s">
-        <v>162</v>
+        <v>106</v>
+      </c>
+      <c r="C180" s="1">
+        <v>2</v>
       </c>
       <c r="D180" t="s">
-        <v>164</v>
+        <v>105</v>
       </c>
       <c r="E180" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>20</v>
       </c>
       <c r="B181" t="s">
-        <v>162</v>
+        <v>106</v>
+      </c>
+      <c r="C181" s="1">
+        <v>1</v>
       </c>
       <c r="D181" t="s">
-        <v>164</v>
+        <v>105</v>
       </c>
       <c r="E181" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>20</v>
       </c>
       <c r="B182" t="s">
-        <v>169</v>
+        <v>124</v>
+      </c>
+      <c r="C182" s="1">
+        <v>2</v>
       </c>
       <c r="D182" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="E182" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>20</v>
       </c>
       <c r="B183" t="s">
-        <v>178</v>
+        <v>141</v>
+      </c>
+      <c r="C183" s="1">
+        <v>2</v>
       </c>
       <c r="D183" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
       <c r="E183" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>20</v>
       </c>
       <c r="B184" t="s">
-        <v>212</v>
+        <v>143</v>
+      </c>
+      <c r="C184" s="1">
+        <v>1</v>
       </c>
       <c r="D184" t="s">
-        <v>230</v>
+        <v>137</v>
       </c>
       <c r="E184" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>20</v>
       </c>
       <c r="B185" t="s">
+        <v>136</v>
+      </c>
+      <c r="C185" s="1">
+        <v>1</v>
+      </c>
+      <c r="D185" t="s">
+        <v>137</v>
+      </c>
+      <c r="E185" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>20</v>
+      </c>
+      <c r="B186" t="s">
+        <v>162</v>
+      </c>
+      <c r="D186" t="s">
+        <v>164</v>
+      </c>
+      <c r="E186" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>20</v>
+      </c>
+      <c r="B187" t="s">
+        <v>162</v>
+      </c>
+      <c r="D187" t="s">
+        <v>164</v>
+      </c>
+      <c r="E187" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>20</v>
+      </c>
+      <c r="B188" t="s">
+        <v>169</v>
+      </c>
+      <c r="D188" t="s">
+        <v>170</v>
+      </c>
+      <c r="E188" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>20</v>
+      </c>
+      <c r="B189" t="s">
+        <v>178</v>
+      </c>
+      <c r="D189" t="s">
+        <v>179</v>
+      </c>
+      <c r="E189" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>20</v>
+      </c>
+      <c r="B190" t="s">
+        <v>212</v>
+      </c>
+      <c r="D190" t="s">
+        <v>230</v>
+      </c>
+      <c r="E190" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>20</v>
+      </c>
+      <c r="B191" t="s">
         <v>224</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D191" t="s">
         <v>225</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E191" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
-        <v>21</v>
-      </c>
-      <c r="B186" t="s">
-        <v>18</v>
-      </c>
-      <c r="C186" s="1">
-        <v>1</v>
-      </c>
-      <c r="D186" t="s">
-        <v>15</v>
-      </c>
-      <c r="E186" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
-        <v>21</v>
-      </c>
-      <c r="B187" t="s">
-        <v>32</v>
-      </c>
-      <c r="D187" t="s">
-        <v>34</v>
-      </c>
-      <c r="E187" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
-        <v>21</v>
-      </c>
-      <c r="B188" t="s">
-        <v>35</v>
-      </c>
-      <c r="D188" t="s">
-        <v>38</v>
-      </c>
-      <c r="E188" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
-        <v>21</v>
-      </c>
-      <c r="B189" t="s">
-        <v>49</v>
-      </c>
-      <c r="D189" t="s">
-        <v>50</v>
-      </c>
-      <c r="E189" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
-        <v>21</v>
-      </c>
-      <c r="B190" t="s">
-        <v>52</v>
-      </c>
-      <c r="D190" t="s">
-        <v>54</v>
-      </c>
-      <c r="E190" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
-        <v>21</v>
-      </c>
-      <c r="B191" t="s">
-        <v>132</v>
-      </c>
-      <c r="D191" t="s">
-        <v>57</v>
-      </c>
-      <c r="E191" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>21</v>
       </c>
       <c r="B192" t="s">
-        <v>132</v>
+        <v>18</v>
+      </c>
+      <c r="C192" s="1">
+        <v>1</v>
       </c>
       <c r="D192" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="E192" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>21</v>
       </c>
       <c r="B193" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="D193" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="E193" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>21</v>
       </c>
       <c r="B194" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
       <c r="D194" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E194" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>21</v>
       </c>
       <c r="B195" t="s">
-        <v>132</v>
+        <v>49</v>
       </c>
       <c r="D195" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E195" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>21</v>
       </c>
       <c r="B196" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D196" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E196" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>21</v>
       </c>
       <c r="B197" t="s">
-        <v>76</v>
-      </c>
-      <c r="C197" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D197" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="E197" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>21</v>
       </c>
       <c r="B198" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
       <c r="D198" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="E198" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>21</v>
       </c>
       <c r="B199" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="D199" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="E199" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>21</v>
       </c>
       <c r="B200" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="D200" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="E200" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>21</v>
       </c>
       <c r="B201" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="D201" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="E201" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>21</v>
       </c>
       <c r="B202" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="D202" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="E202" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>21</v>
       </c>
       <c r="B203" t="s">
-        <v>90</v>
+        <v>76</v>
+      </c>
+      <c r="C203" s="1">
+        <v>1</v>
       </c>
       <c r="D203" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="E203" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>21</v>
       </c>
       <c r="B204" t="s">
-        <v>101</v>
-      </c>
-      <c r="C204" s="1">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="D204" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="E204" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>21</v>
       </c>
       <c r="B205" t="s">
-        <v>102</v>
-      </c>
-      <c r="C205" s="1">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D205" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="E205" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>21</v>
       </c>
       <c r="B206" t="s">
-        <v>101</v>
-      </c>
-      <c r="C206" s="1">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D206" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
       <c r="E206" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>21</v>
       </c>
       <c r="B207" t="s">
-        <v>209</v>
-      </c>
-      <c r="C207" s="1">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D207" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="E207" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>21</v>
       </c>
       <c r="B208" t="s">
-        <v>210</v>
-      </c>
-      <c r="C208" s="1">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D208" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E208" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>21</v>
       </c>
       <c r="B209" t="s">
-        <v>209</v>
-      </c>
-      <c r="C209" s="1">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D209" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E209" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>21</v>
       </c>
       <c r="B210" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C210" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D210" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E210" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>21</v>
       </c>
       <c r="B211" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
       </c>
       <c r="D211" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E211" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>21</v>
       </c>
       <c r="B212" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
       </c>
       <c r="D212" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E212" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>21</v>
       </c>
       <c r="B213" t="s">
-        <v>110</v>
+        <v>209</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
       </c>
       <c r="D213" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E213" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>21</v>
       </c>
       <c r="B214" t="s">
-        <v>111</v>
+        <v>210</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
       </c>
       <c r="D214" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E214" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>21</v>
       </c>
       <c r="B215" t="s">
-        <v>113</v>
+        <v>209</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
       </c>
       <c r="D215" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E215" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>21</v>
       </c>
       <c r="B216" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C216" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D216" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E216" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>21</v>
       </c>
       <c r="B217" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C217" s="1">
         <v>1</v>
       </c>
       <c r="D217" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E217" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>21</v>
       </c>
       <c r="B218" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C218" s="1">
         <v>1</v>
       </c>
       <c r="D218" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E218" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>21</v>
       </c>
       <c r="B219" t="s">
-        <v>162</v>
+        <v>110</v>
+      </c>
+      <c r="C219" s="1">
+        <v>1</v>
       </c>
       <c r="D219" t="s">
-        <v>163</v>
+        <v>109</v>
       </c>
       <c r="E219" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>21</v>
       </c>
       <c r="B220" t="s">
-        <v>165</v>
+        <v>111</v>
+      </c>
+      <c r="C220" s="1">
+        <v>1</v>
       </c>
       <c r="D220" t="s">
-        <v>166</v>
+        <v>112</v>
       </c>
       <c r="E220" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>21</v>
       </c>
       <c r="B221" t="s">
-        <v>167</v>
+        <v>113</v>
+      </c>
+      <c r="C221" s="1">
+        <v>1</v>
       </c>
       <c r="D221" t="s">
-        <v>168</v>
+        <v>112</v>
       </c>
       <c r="E221" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>21</v>
       </c>
       <c r="B222" t="s">
-        <v>169</v>
+        <v>114</v>
+      </c>
+      <c r="C222" s="1">
+        <v>1</v>
       </c>
       <c r="D222" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="E222" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>21</v>
       </c>
       <c r="B223" t="s">
-        <v>171</v>
+        <v>115</v>
+      </c>
+      <c r="C223" s="1">
+        <v>1</v>
       </c>
       <c r="D223" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="E223" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>21</v>
       </c>
       <c r="B224" t="s">
-        <v>176</v>
+        <v>117</v>
+      </c>
+      <c r="C224" s="1">
+        <v>1</v>
       </c>
       <c r="D224" t="s">
-        <v>177</v>
+        <v>116</v>
       </c>
       <c r="E224" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>21</v>
       </c>
       <c r="B225" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="D225" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="E225" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>21</v>
       </c>
       <c r="B226" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D226" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E226" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>21</v>
       </c>
       <c r="B227" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="D227" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="E227" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>21</v>
       </c>
       <c r="B228" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D228" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="E228" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>21</v>
       </c>
       <c r="B229" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="D229" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="E229" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>21</v>
       </c>
       <c r="B230" t="s">
+        <v>176</v>
+      </c>
+      <c r="D230" t="s">
+        <v>177</v>
+      </c>
+      <c r="E230" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>21</v>
+      </c>
+      <c r="B231" t="s">
+        <v>178</v>
+      </c>
+      <c r="D231" t="s">
+        <v>179</v>
+      </c>
+      <c r="E231" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>21</v>
+      </c>
+      <c r="B232" t="s">
+        <v>180</v>
+      </c>
+      <c r="D232" t="s">
+        <v>181</v>
+      </c>
+      <c r="E232" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>21</v>
+      </c>
+      <c r="B233" t="s">
+        <v>182</v>
+      </c>
+      <c r="D233" t="s">
+        <v>183</v>
+      </c>
+      <c r="E233" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>21</v>
+      </c>
+      <c r="B234" t="s">
+        <v>184</v>
+      </c>
+      <c r="D234" t="s">
+        <v>185</v>
+      </c>
+      <c r="E234" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>21</v>
+      </c>
+      <c r="B235" t="s">
+        <v>187</v>
+      </c>
+      <c r="D235" t="s">
+        <v>188</v>
+      </c>
+      <c r="E235" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>21</v>
+      </c>
+      <c r="B236" t="s">
         <v>222</v>
       </c>
-      <c r="C230" s="1">
-        <v>1</v>
-      </c>
-      <c r="D230" t="s">
+      <c r="C236" s="1">
+        <v>1</v>
+      </c>
+      <c r="D236" t="s">
         <v>223</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E236" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A231" t="s">
-        <v>55</v>
-      </c>
-      <c r="B231" t="s">
-        <v>56</v>
-      </c>
-      <c r="C231" s="1">
-        <v>1</v>
-      </c>
-      <c r="D231" t="s">
-        <v>57</v>
-      </c>
-      <c r="E231" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A232" t="s">
-        <v>55</v>
-      </c>
-      <c r="B232" t="s">
-        <v>56</v>
-      </c>
-      <c r="C232" s="1">
-        <v>1</v>
-      </c>
-      <c r="D232" t="s">
-        <v>57</v>
-      </c>
-      <c r="E232" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A233" t="s">
-        <v>55</v>
-      </c>
-      <c r="B233" t="s">
-        <v>56</v>
-      </c>
-      <c r="C233" s="1">
-        <v>1</v>
-      </c>
-      <c r="D233" t="s">
-        <v>57</v>
-      </c>
-      <c r="E233" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A234" t="s">
-        <v>55</v>
-      </c>
-      <c r="B234" t="s">
-        <v>56</v>
-      </c>
-      <c r="C234" s="1">
-        <v>1</v>
-      </c>
-      <c r="D234" t="s">
-        <v>57</v>
-      </c>
-      <c r="E234" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A235" t="s">
-        <v>55</v>
-      </c>
-      <c r="B235" t="s">
-        <v>62</v>
-      </c>
-      <c r="C235" s="1">
-        <v>1</v>
-      </c>
-      <c r="D235" t="s">
-        <v>57</v>
-      </c>
-      <c r="E235" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A236" t="s">
-        <v>55</v>
-      </c>
-      <c r="B236" t="s">
-        <v>64</v>
-      </c>
-      <c r="C236" s="1">
-        <v>1</v>
-      </c>
-      <c r="D236" t="s">
-        <v>57</v>
-      </c>
-      <c r="E236" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>55</v>
       </c>
       <c r="B237" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -4838,129 +4846,129 @@
         <v>57</v>
       </c>
       <c r="E237" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>55</v>
+      </c>
+      <c r="B238" t="s">
+        <v>56</v>
+      </c>
+      <c r="C238" s="1">
+        <v>1</v>
+      </c>
+      <c r="D238" t="s">
+        <v>57</v>
+      </c>
+      <c r="E238" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>55</v>
+      </c>
+      <c r="B239" t="s">
+        <v>56</v>
+      </c>
+      <c r="C239" s="1">
+        <v>1</v>
+      </c>
+      <c r="D239" t="s">
+        <v>57</v>
+      </c>
+      <c r="E239" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>55</v>
+      </c>
+      <c r="B240" t="s">
+        <v>56</v>
+      </c>
+      <c r="C240" s="1">
+        <v>1</v>
+      </c>
+      <c r="D240" t="s">
+        <v>57</v>
+      </c>
+      <c r="E240" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>55</v>
+      </c>
+      <c r="B241" t="s">
+        <v>62</v>
+      </c>
+      <c r="C241" s="1">
+        <v>1</v>
+      </c>
+      <c r="D241" t="s">
+        <v>57</v>
+      </c>
+      <c r="E241" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>55</v>
+      </c>
+      <c r="B242" t="s">
+        <v>64</v>
+      </c>
+      <c r="C242" s="1">
+        <v>1</v>
+      </c>
+      <c r="D242" t="s">
+        <v>57</v>
+      </c>
+      <c r="E242" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>55</v>
+      </c>
+      <c r="B243" t="s">
+        <v>66</v>
+      </c>
+      <c r="C243" s="1">
+        <v>1</v>
+      </c>
+      <c r="D243" t="s">
+        <v>57</v>
+      </c>
+      <c r="E243" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A238" t="s">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
         <v>134</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B244" t="s">
         <v>82</v>
       </c>
-      <c r="C238" s="1">
-        <v>1</v>
-      </c>
-      <c r="D238" t="s">
+      <c r="C244" s="1">
+        <v>1</v>
+      </c>
+      <c r="D244" t="s">
         <v>45</v>
       </c>
-      <c r="E238" t="s">
+      <c r="E244" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A239" t="s">
-        <v>131</v>
-      </c>
-      <c r="B239" t="s">
-        <v>82</v>
-      </c>
-      <c r="C239" s="1">
-        <v>2</v>
-      </c>
-      <c r="D239" t="s">
-        <v>150</v>
-      </c>
-      <c r="E239" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A240" t="s">
-        <v>131</v>
-      </c>
-      <c r="B240" t="s">
-        <v>147</v>
-      </c>
-      <c r="C240" s="1">
-        <v>2</v>
-      </c>
-      <c r="D240" t="s">
-        <v>150</v>
-      </c>
-      <c r="E240" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A241" t="s">
-        <v>131</v>
-      </c>
-      <c r="B241" t="s">
-        <v>82</v>
-      </c>
-      <c r="C241" s="1">
-        <v>2</v>
-      </c>
-      <c r="D241" t="s">
-        <v>148</v>
-      </c>
-      <c r="E241" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A242" t="s">
-        <v>131</v>
-      </c>
-      <c r="B242" t="s">
-        <v>147</v>
-      </c>
-      <c r="C242" s="1">
-        <v>2</v>
-      </c>
-      <c r="D242" t="s">
-        <v>148</v>
-      </c>
-      <c r="E242" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A243" t="s">
-        <v>131</v>
-      </c>
-      <c r="B243" t="s">
-        <v>82</v>
-      </c>
-      <c r="C243" s="1">
-        <v>2</v>
-      </c>
-      <c r="D243" t="s">
-        <v>155</v>
-      </c>
-      <c r="E243" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A244" t="s">
-        <v>131</v>
-      </c>
-      <c r="B244" t="s">
-        <v>147</v>
-      </c>
-      <c r="C244" s="1">
-        <v>2</v>
-      </c>
-      <c r="D244" t="s">
-        <v>155</v>
-      </c>
-      <c r="E244" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>131</v>
       </c>
@@ -4971,13 +4979,13 @@
         <v>2</v>
       </c>
       <c r="D245" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E245" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>131</v>
       </c>
@@ -4988,13 +4996,13 @@
         <v>2</v>
       </c>
       <c r="D246" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E246" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>131</v>
       </c>
@@ -5005,13 +5013,13 @@
         <v>2</v>
       </c>
       <c r="D247" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E247" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>131</v>
       </c>
@@ -5022,134 +5030,134 @@
         <v>2</v>
       </c>
       <c r="D248" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E248" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="B249" t="s">
         <v>82</v>
       </c>
       <c r="C249" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D249" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="E249" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="B250" t="s">
         <v>147</v>
       </c>
       <c r="C250" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D250" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="E250" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="B251" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C251" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D251" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E251" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="B252" t="s">
-        <v>3</v>
+        <v>147</v>
       </c>
       <c r="C252" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D252" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E252" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="B253" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="C253" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D253" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="E253" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>201</v>
+        <v>131</v>
       </c>
       <c r="B254" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C254" s="1">
         <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="E254" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>201</v>
+        <v>88</v>
       </c>
       <c r="B255" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="C255" s="1">
         <v>1</v>
       </c>
       <c r="D255" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="E255" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>214</v>
+        <v>88</v>
       </c>
       <c r="B256" t="s">
         <v>147</v>
@@ -5158,100 +5166,100 @@
         <v>1</v>
       </c>
       <c r="D256" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
       <c r="E256" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
+        <v>10</v>
+      </c>
+      <c r="B257" t="s">
+        <v>11</v>
+      </c>
+      <c r="C257" s="1">
+        <v>1</v>
+      </c>
+      <c r="D257" t="s">
+        <v>12</v>
+      </c>
+      <c r="E257" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>10</v>
+      </c>
+      <c r="B258" t="s">
+        <v>3</v>
+      </c>
+      <c r="C258" s="1">
+        <v>1</v>
+      </c>
+      <c r="D258" t="s">
+        <v>12</v>
+      </c>
+      <c r="E258" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>10</v>
+      </c>
+      <c r="B259" t="s">
+        <v>13</v>
+      </c>
+      <c r="C259" s="1">
+        <v>1</v>
+      </c>
+      <c r="D259" t="s">
+        <v>12</v>
+      </c>
+      <c r="E259" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>201</v>
+      </c>
+      <c r="B260" t="s">
+        <v>82</v>
+      </c>
+      <c r="C260" s="1">
+        <v>2</v>
+      </c>
+      <c r="D260" t="s">
+        <v>195</v>
+      </c>
+      <c r="E260" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>201</v>
+      </c>
+      <c r="B261" t="s">
+        <v>147</v>
+      </c>
+      <c r="C261" s="1">
+        <v>1</v>
+      </c>
+      <c r="D261" t="s">
+        <v>195</v>
+      </c>
+      <c r="E261" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
         <v>214</v>
-      </c>
-      <c r="B257" t="s">
-        <v>82</v>
-      </c>
-      <c r="C257" s="1">
-        <v>1</v>
-      </c>
-      <c r="D257" t="s">
-        <v>230</v>
-      </c>
-      <c r="E257" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A258" t="s">
-        <v>214</v>
-      </c>
-      <c r="B258" t="s">
-        <v>62</v>
-      </c>
-      <c r="C258" s="1">
-        <v>1</v>
-      </c>
-      <c r="D258" t="s">
-        <v>230</v>
-      </c>
-      <c r="E258" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A259" t="s">
-        <v>214</v>
-      </c>
-      <c r="B259" t="s">
-        <v>66</v>
-      </c>
-      <c r="C259" s="1">
-        <v>1</v>
-      </c>
-      <c r="D259" t="s">
-        <v>230</v>
-      </c>
-      <c r="E259" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A260" t="s">
-        <v>214</v>
-      </c>
-      <c r="B260" t="s">
-        <v>218</v>
-      </c>
-      <c r="C260" s="1">
-        <v>1</v>
-      </c>
-      <c r="D260" t="s">
-        <v>230</v>
-      </c>
-      <c r="E260" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A261" t="s">
-        <v>174</v>
-      </c>
-      <c r="B261" t="s">
-        <v>82</v>
-      </c>
-      <c r="C261" s="1">
-        <v>2</v>
-      </c>
-      <c r="D261" t="s">
-        <v>173</v>
-      </c>
-      <c r="E261" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A262" t="s">
-        <v>174</v>
       </c>
       <c r="B262" t="s">
         <v>147</v>
@@ -5260,26 +5268,128 @@
         <v>1</v>
       </c>
       <c r="D262" t="s">
+        <v>230</v>
+      </c>
+      <c r="E262" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>214</v>
+      </c>
+      <c r="B263" t="s">
+        <v>82</v>
+      </c>
+      <c r="C263" s="1">
+        <v>1</v>
+      </c>
+      <c r="D263" t="s">
+        <v>230</v>
+      </c>
+      <c r="E263" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>214</v>
+      </c>
+      <c r="B264" t="s">
+        <v>62</v>
+      </c>
+      <c r="C264" s="1">
+        <v>1</v>
+      </c>
+      <c r="D264" t="s">
+        <v>230</v>
+      </c>
+      <c r="E264" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>214</v>
+      </c>
+      <c r="B265" t="s">
+        <v>66</v>
+      </c>
+      <c r="C265" s="1">
+        <v>1</v>
+      </c>
+      <c r="D265" t="s">
+        <v>230</v>
+      </c>
+      <c r="E265" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>214</v>
+      </c>
+      <c r="B266" t="s">
+        <v>218</v>
+      </c>
+      <c r="C266" s="1">
+        <v>1</v>
+      </c>
+      <c r="D266" t="s">
+        <v>230</v>
+      </c>
+      <c r="E266" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>174</v>
+      </c>
+      <c r="B267" t="s">
+        <v>82</v>
+      </c>
+      <c r="C267" s="1">
+        <v>2</v>
+      </c>
+      <c r="D267" t="s">
         <v>173</v>
       </c>
-      <c r="E262" t="s">
+      <c r="E267" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>174</v>
+      </c>
+      <c r="B268" t="s">
+        <v>147</v>
+      </c>
+      <c r="C268" s="1">
+        <v>1</v>
+      </c>
+      <c r="D268" t="s">
+        <v>173</v>
+      </c>
+      <c r="E268" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A263" t="s">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
         <v>174</v>
       </c>
-      <c r="B263" t="s">
+      <c r="B269" t="s">
         <v>147</v>
       </c>
-      <c r="C263" s="1">
-        <v>1</v>
-      </c>
-      <c r="D263" t="s">
+      <c r="C269" s="1">
+        <v>1</v>
+      </c>
+      <c r="D269" t="s">
         <v>186</v>
       </c>
-      <c r="E263" t="s">
+      <c r="E269" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Apply suggestions from code review
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25619"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36BB872-DAAB-478B-ADE9-4DD2AE6E7AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F065C9B6-936A-4534-B404-0666C5341433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-90" windowWidth="38640" windowHeight="23520" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -11,7 +11,6 @@
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="260">
   <si>
     <t>Class</t>
   </si>
@@ -788,9 +787,6 @@
   </si>
   <si>
     <t>MailboxEnums.AttachmentType</t>
-  </si>
-  <si>
-    <t>getAttachmentTypeMessage</t>
   </si>
   <si>
     <t>MailboxEnums.ItemType</t>
@@ -847,13 +843,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1229,7 +1221,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
+      <selection pane="bottomLeft" activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3861,7 +3853,7 @@
         <v>68</v>
       </c>
       <c r="F138" t="s">
-        <v>253</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -3971,7 +3963,7 @@
         <v>248</v>
       </c>
       <c r="B145" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>232</v>
@@ -4021,18 +4013,17 @@
       <c r="A148" t="s">
         <v>248</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B148" t="s">
+        <v>257</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E148" t="s">
         <v>258</v>
       </c>
-      <c r="C148" s="2"/>
-      <c r="D148" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E148" s="2" t="s">
+      <c r="F148" t="s">
         <v>259</v>
-      </c>
-      <c r="F148" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -4091,16 +4082,16 @@
         <v>248</v>
       </c>
       <c r="B152" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E152" t="s">
+        <v>255</v>
+      </c>
+      <c r="F152" t="s">
         <v>256</v>
-      </c>
-      <c r="F152" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create Script Lab snippets for Office.Body
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/outlook.xlsx
+++ b/snippet-extractor-metadata/outlook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25619"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25627"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F065C9B6-936A-4534-B404-0666C5341433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA95726-83A3-4C48-9DA1-39E9FA84AA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-90" windowWidth="38640" windowHeight="23520" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-30" yWindow="75" windowWidth="20430" windowHeight="20835" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="273">
   <si>
     <t>Class</t>
   </si>
@@ -808,6 +808,45 @@
   </si>
   <si>
     <t>getDiagnostics</t>
+  </si>
+  <si>
+    <t>getTypeAsync</t>
+  </si>
+  <si>
+    <t>outlook-item-body-get-body-format</t>
+  </si>
+  <si>
+    <t>getBodyFormat</t>
+  </si>
+  <si>
+    <t>appendOnSendAsync</t>
+  </si>
+  <si>
+    <t>outlook-item-body-append-text-on-send</t>
+  </si>
+  <si>
+    <t>appendOnSend</t>
+  </si>
+  <si>
+    <t>outlook-item-body-add-inline-base64-image</t>
+  </si>
+  <si>
+    <t>addImage</t>
+  </si>
+  <si>
+    <t>prependAsync</t>
+  </si>
+  <si>
+    <t>outlook-item-body-prepend-text-to-item-body</t>
+  </si>
+  <si>
+    <t>prependText</t>
+  </si>
+  <si>
+    <t>outlook-item-body-replace-selected-text</t>
+  </si>
+  <si>
+    <t>replaceSelection</t>
   </si>
 </sst>
 </file>
@@ -843,9 +882,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -886,8 +929,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F276" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F276" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F282" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F282" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{EFF7BB35-6FE7-4943-B8A3-9C5F576D40BA}" name="Package"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="4"/>
@@ -1217,11 +1260,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F276"/>
+  <dimension ref="A1:F282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E138" sqref="E138"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3005,16 +3048,16 @@
         <v>139</v>
       </c>
       <c r="C95" t="s">
-        <v>140</v>
+        <v>263</v>
       </c>
       <c r="D95" s="1">
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>137</v>
+        <v>264</v>
       </c>
       <c r="F95" t="s">
-        <v>203</v>
+        <v>265</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3025,16 +3068,16 @@
         <v>139</v>
       </c>
       <c r="C96" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="D96" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>137</v>
+        <v>266</v>
       </c>
       <c r="F96" t="s">
-        <v>204</v>
+        <v>267</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3042,19 +3085,19 @@
         <v>248</v>
       </c>
       <c r="B97" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="C97" t="s">
-        <v>82</v>
+        <v>260</v>
       </c>
       <c r="D97" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>161</v>
+        <v>261</v>
       </c>
       <c r="F97" t="s">
-        <v>80</v>
+        <v>262</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3062,19 +3105,19 @@
         <v>248</v>
       </c>
       <c r="B98" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="C98" t="s">
-        <v>56</v>
+        <v>268</v>
       </c>
       <c r="D98" s="1">
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>161</v>
+        <v>269</v>
       </c>
       <c r="F98" t="s">
-        <v>159</v>
+        <v>270</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3082,39 +3125,39 @@
         <v>248</v>
       </c>
       <c r="B99" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="D99" s="1">
         <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>161</v>
+        <v>266</v>
       </c>
       <c r="F99" t="s">
-        <v>160</v>
+        <v>267</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>248</v>
       </c>
-      <c r="B100" t="s">
-        <v>14</v>
-      </c>
-      <c r="C100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D100" s="1">
-        <v>1</v>
-      </c>
-      <c r="E100" t="s">
-        <v>15</v>
-      </c>
-      <c r="F100" t="s">
-        <v>11</v>
+      <c r="B100" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D100" s="3">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3122,19 +3165,19 @@
         <v>248</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
       <c r="C101" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="F101" t="s">
-        <v>3</v>
+        <v>203</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3142,19 +3185,19 @@
         <v>248</v>
       </c>
       <c r="B102" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
       <c r="C102" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="F102" t="s">
-        <v>16</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,19 +3205,19 @@
         <v>248</v>
       </c>
       <c r="B103" t="s">
-        <v>193</v>
+        <v>81</v>
       </c>
       <c r="C103" t="s">
         <v>82</v>
       </c>
       <c r="D103" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E103" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="F103" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3182,7 +3225,7 @@
         <v>248</v>
       </c>
       <c r="B104" t="s">
-        <v>193</v>
+        <v>81</v>
       </c>
       <c r="C104" t="s">
         <v>56</v>
@@ -3191,10 +3234,10 @@
         <v>1</v>
       </c>
       <c r="E104" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="F104" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3202,7 +3245,7 @@
         <v>248</v>
       </c>
       <c r="B105" t="s">
-        <v>193</v>
+        <v>81</v>
       </c>
       <c r="C105" t="s">
         <v>66</v>
@@ -3211,10 +3254,10 @@
         <v>1</v>
       </c>
       <c r="E105" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="F105" t="s">
-        <v>16</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3222,19 +3265,19 @@
         <v>248</v>
       </c>
       <c r="B106" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="C106" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="D106" s="1">
         <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="F106" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3242,19 +3285,19 @@
         <v>248</v>
       </c>
       <c r="B107" t="s">
-        <v>227</v>
+        <v>14</v>
       </c>
       <c r="C107" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="D107" s="1">
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>225</v>
+        <v>15</v>
       </c>
       <c r="F107" t="s">
-        <v>226</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3262,19 +3305,19 @@
         <v>248</v>
       </c>
       <c r="B108" t="s">
-        <v>227</v>
+        <v>14</v>
       </c>
       <c r="C108" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D108" s="1">
         <v>1</v>
       </c>
       <c r="E108" t="s">
-        <v>225</v>
+        <v>15</v>
       </c>
       <c r="F108" t="s">
-        <v>228</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3282,19 +3325,19 @@
         <v>248</v>
       </c>
       <c r="B109" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="C109" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="D109" s="1">
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
       <c r="F109" t="s">
-        <v>229</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3302,19 +3345,19 @@
         <v>248</v>
       </c>
       <c r="B110" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C110" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="D110" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E110" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F110" t="s">
-        <v>194</v>
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3322,19 +3365,19 @@
         <v>248</v>
       </c>
       <c r="B111" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C111" t="s">
-        <v>147</v>
+        <v>66</v>
       </c>
       <c r="D111" s="1">
         <v>1</v>
       </c>
       <c r="E111" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F111" t="s">
-        <v>198</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -3342,19 +3385,19 @@
         <v>248</v>
       </c>
       <c r="B112" t="s">
-        <v>190</v>
+        <v>133</v>
       </c>
       <c r="C112" t="s">
         <v>82</v>
       </c>
       <c r="D112" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E112" t="s">
-        <v>189</v>
+        <v>36</v>
       </c>
       <c r="F112" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3362,19 +3405,19 @@
         <v>248</v>
       </c>
       <c r="B113" t="s">
-        <v>190</v>
+        <v>227</v>
       </c>
       <c r="C113" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="D113" s="1">
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="F113" t="s">
-        <v>3</v>
+        <v>226</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3382,17 +3425,19 @@
         <v>248</v>
       </c>
       <c r="B114" t="s">
-        <v>83</v>
+        <v>227</v>
       </c>
       <c r="C114" t="s">
-        <v>84</v>
-      </c>
-      <c r="D114" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1</v>
+      </c>
       <c r="E114" t="s">
-        <v>158</v>
+        <v>225</v>
       </c>
       <c r="F114" t="s">
-        <v>85</v>
+        <v>228</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3400,17 +3445,19 @@
         <v>248</v>
       </c>
       <c r="B115" t="s">
-        <v>83</v>
+        <v>227</v>
       </c>
       <c r="C115" t="s">
-        <v>84</v>
-      </c>
-      <c r="D115" s="1"/>
+        <v>147</v>
+      </c>
+      <c r="D115" s="1">
+        <v>1</v>
+      </c>
       <c r="E115" t="s">
-        <v>158</v>
+        <v>225</v>
       </c>
       <c r="F115" t="s">
-        <v>156</v>
+        <v>229</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3418,17 +3465,19 @@
         <v>248</v>
       </c>
       <c r="B116" t="s">
-        <v>83</v>
+        <v>197</v>
       </c>
       <c r="C116" t="s">
-        <v>84</v>
-      </c>
-      <c r="D116" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D116" s="1">
+        <v>2</v>
+      </c>
       <c r="E116" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
       <c r="F116" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3436,19 +3485,19 @@
         <v>248</v>
       </c>
       <c r="B117" t="s">
-        <v>83</v>
+        <v>197</v>
       </c>
       <c r="C117" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
       <c r="D117" s="1">
         <v>1</v>
       </c>
       <c r="E117" t="s">
-        <v>94</v>
+        <v>195</v>
       </c>
       <c r="F117" t="s">
-        <v>4</v>
+        <v>198</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3456,19 +3505,19 @@
         <v>248</v>
       </c>
       <c r="B118" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
       <c r="C118" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D118" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E118" t="s">
-        <v>96</v>
+        <v>189</v>
       </c>
       <c r="F118" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3476,19 +3525,19 @@
         <v>248</v>
       </c>
       <c r="B119" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
       <c r="C119" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="D119" s="1">
         <v>1</v>
       </c>
       <c r="E119" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="F119" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3499,16 +3548,14 @@
         <v>83</v>
       </c>
       <c r="C120" t="s">
-        <v>99</v>
-      </c>
-      <c r="D120" s="1">
-        <v>1</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="D120" s="1"/>
       <c r="E120" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="F120" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3519,16 +3566,14 @@
         <v>83</v>
       </c>
       <c r="C121" t="s">
-        <v>205</v>
-      </c>
-      <c r="D121" s="1">
-        <v>1</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="D121" s="1"/>
       <c r="E121" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
       <c r="F121" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3539,16 +3584,14 @@
         <v>83</v>
       </c>
       <c r="C122" t="s">
-        <v>206</v>
-      </c>
-      <c r="D122" s="1">
-        <v>1</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="D122" s="1"/>
       <c r="E122" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="F122" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3559,16 +3602,16 @@
         <v>83</v>
       </c>
       <c r="C123" t="s">
-        <v>207</v>
+        <v>93</v>
       </c>
       <c r="D123" s="1">
         <v>1</v>
       </c>
       <c r="E123" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F123" t="s">
-        <v>211</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3579,16 +3622,16 @@
         <v>83</v>
       </c>
       <c r="C124" t="s">
-        <v>208</v>
+        <v>95</v>
       </c>
       <c r="D124" s="1">
         <v>1</v>
       </c>
       <c r="E124" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F124" t="s">
-        <v>211</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3599,13 +3642,13 @@
         <v>83</v>
       </c>
       <c r="C125" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="D125" s="1">
         <v>1</v>
       </c>
       <c r="E125" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="F125" t="s">
         <v>4</v>
@@ -3619,11 +3662,13 @@
         <v>83</v>
       </c>
       <c r="C126" t="s">
-        <v>120</v>
-      </c>
-      <c r="D126" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="D126" s="1">
+        <v>1</v>
+      </c>
       <c r="E126" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="F126" t="s">
         <v>4</v>
@@ -3637,16 +3682,16 @@
         <v>83</v>
       </c>
       <c r="C127" t="s">
-        <v>107</v>
+        <v>205</v>
       </c>
       <c r="D127" s="1">
         <v>1</v>
       </c>
       <c r="E127" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="F127" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3657,14 +3702,16 @@
         <v>83</v>
       </c>
       <c r="C128" t="s">
-        <v>121</v>
-      </c>
-      <c r="D128" s="1"/>
+        <v>206</v>
+      </c>
+      <c r="D128" s="1">
+        <v>1</v>
+      </c>
       <c r="E128" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F128" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3675,14 +3722,16 @@
         <v>83</v>
       </c>
       <c r="C129" t="s">
-        <v>120</v>
-      </c>
-      <c r="D129" s="1"/>
+        <v>207</v>
+      </c>
+      <c r="D129" s="1">
+        <v>1</v>
+      </c>
       <c r="E129" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="F129" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -3693,16 +3742,16 @@
         <v>83</v>
       </c>
       <c r="C130" t="s">
-        <v>118</v>
+        <v>208</v>
       </c>
       <c r="D130" s="1">
         <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="F130" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -3713,13 +3762,13 @@
         <v>83</v>
       </c>
       <c r="C131" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D131" s="1">
         <v>1</v>
       </c>
       <c r="E131" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F131" t="s">
         <v>4</v>
@@ -3733,13 +3782,11 @@
         <v>83</v>
       </c>
       <c r="C132" t="s">
-        <v>126</v>
-      </c>
-      <c r="D132" s="1">
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D132" s="1"/>
       <c r="E132" t="s">
-        <v>231</v>
+        <v>119</v>
       </c>
       <c r="F132" t="s">
         <v>4</v>
@@ -3753,13 +3800,13 @@
         <v>83</v>
       </c>
       <c r="C133" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="D133" s="1">
         <v>1</v>
       </c>
       <c r="E133" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F133" t="s">
         <v>4</v>
@@ -3773,13 +3820,11 @@
         <v>83</v>
       </c>
       <c r="C134" t="s">
-        <v>107</v>
-      </c>
-      <c r="D134" s="1">
-        <v>2</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="D134" s="1"/>
       <c r="E134" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F134" t="s">
         <v>4</v>
@@ -3793,13 +3838,11 @@
         <v>83</v>
       </c>
       <c r="C135" t="s">
-        <v>129</v>
-      </c>
-      <c r="D135" s="1">
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D135" s="1"/>
       <c r="E135" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F135" t="s">
         <v>4</v>
@@ -3810,16 +3853,19 @@
         <v>248</v>
       </c>
       <c r="B136" t="s">
-        <v>240</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>232</v>
+        <v>83</v>
+      </c>
+      <c r="C136" t="s">
+        <v>118</v>
+      </c>
+      <c r="D136" s="1">
+        <v>1</v>
       </c>
       <c r="E136" t="s">
-        <v>195</v>
+        <v>122</v>
       </c>
       <c r="F136" t="s">
-        <v>202</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -3827,16 +3873,19 @@
         <v>248</v>
       </c>
       <c r="B137" t="s">
-        <v>234</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>232</v>
+        <v>83</v>
+      </c>
+      <c r="C137" t="s">
+        <v>123</v>
+      </c>
+      <c r="D137" s="1">
+        <v>1</v>
       </c>
       <c r="E137" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="F137" t="s">
-        <v>233</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -3844,16 +3893,19 @@
         <v>248</v>
       </c>
       <c r="B138" t="s">
-        <v>252</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>232</v>
+        <v>83</v>
+      </c>
+      <c r="C138" t="s">
+        <v>126</v>
+      </c>
+      <c r="D138" s="1">
+        <v>1</v>
       </c>
       <c r="E138" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="F138" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -3861,16 +3913,19 @@
         <v>248</v>
       </c>
       <c r="B139" t="s">
-        <v>235</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>232</v>
+        <v>83</v>
+      </c>
+      <c r="C139" t="s">
+        <v>126</v>
+      </c>
+      <c r="D139" s="1">
+        <v>1</v>
       </c>
       <c r="E139" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="F139" t="s">
-        <v>156</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -3878,16 +3933,19 @@
         <v>248</v>
       </c>
       <c r="B140" t="s">
-        <v>241</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>232</v>
+        <v>83</v>
+      </c>
+      <c r="C140" t="s">
+        <v>107</v>
+      </c>
+      <c r="D140" s="1">
+        <v>2</v>
       </c>
       <c r="E140" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F140" t="s">
-        <v>142</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -3895,16 +3953,19 @@
         <v>248</v>
       </c>
       <c r="B141" t="s">
-        <v>242</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>232</v>
+        <v>83</v>
+      </c>
+      <c r="C141" t="s">
+        <v>129</v>
+      </c>
+      <c r="D141" s="1">
+        <v>1</v>
       </c>
       <c r="E141" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="F141" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -3912,16 +3973,16 @@
         <v>248</v>
       </c>
       <c r="B142" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E142" t="s">
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="F142" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -3929,16 +3990,16 @@
         <v>248</v>
       </c>
       <c r="B143" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E143" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="F143" t="s">
-        <v>110</v>
+        <v>233</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -3946,16 +4007,16 @@
         <v>248</v>
       </c>
       <c r="B144" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E144" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F144" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -3963,16 +4024,16 @@
         <v>248</v>
       </c>
       <c r="B145" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E145" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F145" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -3980,16 +4041,16 @@
         <v>248</v>
       </c>
       <c r="B146" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E146" t="s">
-        <v>192</v>
+        <v>137</v>
       </c>
       <c r="F146" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -3997,7 +4058,7 @@
         <v>248</v>
       </c>
       <c r="B147" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>232</v>
@@ -4014,16 +4075,16 @@
         <v>248</v>
       </c>
       <c r="B148" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E148" t="s">
-        <v>258</v>
+        <v>105</v>
       </c>
       <c r="F148" t="s">
-        <v>259</v>
+        <v>220</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -4031,16 +4092,16 @@
         <v>248</v>
       </c>
       <c r="B149" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E149" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="F149" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -4048,16 +4109,16 @@
         <v>248</v>
       </c>
       <c r="B150" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E150" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="F150" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4065,16 +4126,16 @@
         <v>248</v>
       </c>
       <c r="B151" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E151" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F151" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4082,16 +4143,16 @@
         <v>248</v>
       </c>
       <c r="B152" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E152" t="s">
-        <v>255</v>
+        <v>192</v>
       </c>
       <c r="F152" t="s">
-        <v>256</v>
+        <v>69</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4099,16 +4160,16 @@
         <v>248</v>
       </c>
       <c r="B153" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E153" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="F153" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,16 +4177,16 @@
         <v>248</v>
       </c>
       <c r="B154" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E154" t="s">
-        <v>23</v>
+        <v>258</v>
       </c>
       <c r="F154" t="s">
-        <v>24</v>
+        <v>259</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4133,16 +4194,16 @@
         <v>248</v>
       </c>
       <c r="B155" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E155" t="s">
-        <v>175</v>
+        <v>54</v>
       </c>
       <c r="F155" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4150,19 +4211,16 @@
         <v>248</v>
       </c>
       <c r="B156" t="s">
-        <v>86</v>
-      </c>
-      <c r="C156" t="s">
-        <v>82</v>
-      </c>
-      <c r="D156" s="1">
-        <v>2</v>
+        <v>245</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E156" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="F156" t="s">
-        <v>85</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4170,19 +4228,16 @@
         <v>248</v>
       </c>
       <c r="B157" t="s">
-        <v>86</v>
-      </c>
-      <c r="C157" t="s">
-        <v>56</v>
-      </c>
-      <c r="D157" s="1">
-        <v>1</v>
+        <v>246</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E157" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="F157" t="s">
-        <v>156</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4190,19 +4245,16 @@
         <v>248</v>
       </c>
       <c r="B158" t="s">
-        <v>86</v>
-      </c>
-      <c r="C158" t="s">
-        <v>66</v>
-      </c>
-      <c r="D158" s="1">
-        <v>1</v>
+        <v>254</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E158" t="s">
-        <v>158</v>
+        <v>255</v>
       </c>
       <c r="F158" t="s">
-        <v>157</v>
+        <v>256</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4210,19 +4262,16 @@
         <v>248</v>
       </c>
       <c r="B159" t="s">
-        <v>20</v>
-      </c>
-      <c r="C159" t="s">
-        <v>18</v>
-      </c>
-      <c r="D159" s="1">
-        <v>1</v>
+        <v>239</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E159" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="F159" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4230,13 +4279,10 @@
         <v>248</v>
       </c>
       <c r="B160" t="s">
-        <v>20</v>
-      </c>
-      <c r="C160" t="s">
-        <v>22</v>
-      </c>
-      <c r="D160" s="1">
-        <v>2</v>
+        <v>251</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E160" t="s">
         <v>23</v>
@@ -4250,19 +4296,16 @@
         <v>248</v>
       </c>
       <c r="B161" t="s">
-        <v>20</v>
-      </c>
-      <c r="C161" t="s">
-        <v>25</v>
-      </c>
-      <c r="D161" s="1">
-        <v>1</v>
+        <v>250</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E161" t="s">
-        <v>26</v>
+        <v>175</v>
       </c>
       <c r="F161" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -4270,19 +4313,19 @@
         <v>248</v>
       </c>
       <c r="B162" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C162" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="D162" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E162" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="F162" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -4290,17 +4333,19 @@
         <v>248</v>
       </c>
       <c r="B163" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C163" t="s">
-        <v>30</v>
-      </c>
-      <c r="D163" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="D163" s="1">
+        <v>1</v>
+      </c>
       <c r="E163" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F163" t="s">
-        <v>31</v>
+        <v>156</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -4308,17 +4353,19 @@
         <v>248</v>
       </c>
       <c r="B164" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C164" t="s">
-        <v>30</v>
-      </c>
-      <c r="D164" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="D164" s="1">
+        <v>1</v>
+      </c>
       <c r="E164" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F164" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -4329,14 +4376,16 @@
         <v>20</v>
       </c>
       <c r="C165" t="s">
-        <v>32</v>
-      </c>
-      <c r="D165" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="D165" s="1">
+        <v>1</v>
+      </c>
       <c r="E165" t="s">
-        <v>148</v>
+        <v>15</v>
       </c>
       <c r="F165" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -4347,14 +4396,16 @@
         <v>20</v>
       </c>
       <c r="C166" t="s">
-        <v>32</v>
-      </c>
-      <c r="D166" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="D166" s="1">
+        <v>2</v>
+      </c>
       <c r="E166" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="F166" t="s">
-        <v>149</v>
+        <v>24</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -4365,14 +4416,16 @@
         <v>20</v>
       </c>
       <c r="C167" t="s">
-        <v>35</v>
-      </c>
-      <c r="D167" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="D167" s="1">
+        <v>1